<commit_message>
updted complementary feeding intervention so that fraction poor is the same as fraction food insecure
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Bangladesh/2017Aug/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38420" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="10"/>
+    <workbookView xWindow="-69620" yWindow="-4060" windowWidth="26380" windowHeight="16040" tabRatio="500" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -28,13 +23,13 @@
     <sheet name="Interventions for children" sheetId="28" r:id="rId14"/>
     <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -3077,9 +3072,6 @@
     <t>ID anaemia prevalence</t>
   </si>
   <si>
-    <t>Complementary feeding (food insecure with promotion and supplementation) no iron</t>
-  </si>
-  <si>
     <t>Complementary feeding (food insecure with promotion and supplementation) with iron</t>
   </si>
   <si>
@@ -3123,6 +3115,9 @@
   </si>
   <si>
     <t>Mortality rates</t>
+  </si>
+  <si>
+    <t>Complementary feeding (food insecure with promotion and supplementation)</t>
   </si>
 </sst>
 </file>
@@ -5705,16 +5700,16 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="16" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>125</v>
       </c>
@@ -5725,7 +5720,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>65</v>
       </c>
@@ -5736,7 +5731,7 @@
         <v>15204000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
@@ -5744,15 +5739,15 @@
         <v>3118117</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="B4" s="34" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C4" s="61">
         <v>171684000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
@@ -5761,7 +5756,7 @@
         <v>3677298.8269880489</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="B6" s="34" t="s">
         <v>75</v>
       </c>
@@ -5769,7 +5764,7 @@
         <v>0.35199999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1">
       <c r="B7" s="4" t="s">
         <v>74</v>
       </c>
@@ -5777,7 +5772,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1">
       <c r="B8" s="34" t="s">
         <v>76</v>
       </c>
@@ -5785,13 +5780,13 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1">
       <c r="B10" s="11"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1">
       <c r="A11" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B11" t="s">
         <v>81</v>
@@ -5800,51 +5795,51 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1">
       <c r="B12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C12" s="20">
         <v>0.13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1">
       <c r="B13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C13" s="20">
         <v>25.36</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1">
       <c r="B14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C14" s="20">
         <v>25.4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1">
       <c r="B15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C15" s="20">
         <v>34.68</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1">
       <c r="B16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C16" s="20">
         <v>39.32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1">
       <c r="B18" s="11"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1">
       <c r="A19" s="11" t="s">
         <v>78</v>
       </c>
@@ -5855,7 +5850,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1">
       <c r="B20" s="34" t="s">
         <v>115</v>
       </c>
@@ -5863,7 +5858,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1">
       <c r="B21" s="34" t="s">
         <v>116</v>
       </c>
@@ -5871,7 +5866,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1">
       <c r="B22" s="34" t="s">
         <v>117</v>
       </c>
@@ -5879,7 +5874,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="B23" s="34" t="s">
         <v>79</v>
       </c>
@@ -5887,12 +5882,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1">
       <c r="B25" s="34"/>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="A26" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B26" s="58" t="s">
         <v>85</v>
@@ -5901,35 +5896,35 @@
         <v>8634000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="15" customHeight="1">
       <c r="B27" s="58" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C27" s="59">
         <v>13550000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1">
       <c r="B28" s="58" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C28" s="59">
         <v>12394000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1">
       <c r="B29" s="58" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C29" s="59">
         <v>9148000</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1">
       <c r="B30" s="58"/>
       <c r="C30" s="60"/>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="A32" s="11" t="s">
         <v>139</v>
       </c>
@@ -5940,25 +5935,25 @@
         <v>0.29978973218277538</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" ht="15.75" customHeight="1">
       <c r="B33" s="57" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C33" s="48">
         <v>0.52556568434139284</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:3" ht="15.75" customHeight="1">
       <c r="B34" s="57" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C34" s="48">
         <v>0.16210210664201097</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:3" ht="15.75" customHeight="1">
       <c r="B35" s="57" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C35" s="48">
         <v>1.2542476833820825E-2</v>
@@ -5968,6 +5963,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5982,12 +5982,12 @@
       <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -6004,7 +6004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="14">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
@@ -6021,14 +6021,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -6037,6 +6037,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6044,11 +6049,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="43.33203125" customWidth="1"/>
@@ -6059,7 +6064,7 @@
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>89</v>
       </c>
@@ -6089,7 +6094,7 @@
       </c>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>83</v>
       </c>
@@ -6118,7 +6123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1">
       <c r="B3" s="4" t="s">
         <v>51</v>
       </c>
@@ -6144,7 +6149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1">
       <c r="B4" s="4" t="s">
         <v>58</v>
       </c>
@@ -6170,7 +6175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>87</v>
       </c>
@@ -6198,7 +6203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>88</v>
       </c>
@@ -6226,7 +6231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1">
       <c r="B7" s="4" t="s">
         <v>86</v>
       </c>
@@ -6253,7 +6258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1">
       <c r="A9" s="11" t="s">
         <v>84</v>
       </c>
@@ -6283,7 +6288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1">
       <c r="B10" t="s">
         <v>60</v>
       </c>
@@ -6309,7 +6314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1">
       <c r="B11" s="4" t="s">
         <v>90</v>
       </c>
@@ -6335,7 +6340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1">
       <c r="B12" t="s">
         <v>102</v>
       </c>
@@ -6362,7 +6367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="11" t="s">
         <v>101</v>
       </c>
@@ -6392,7 +6397,7 @@
         <v>6.9170848887586636E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="B15" s="4" t="s">
         <v>93</v>
       </c>
@@ -6419,7 +6424,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="B16" s="4" t="s">
         <v>94</v>
       </c>
@@ -6446,7 +6451,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1">
       <c r="B17" s="4" t="s">
         <v>95</v>
       </c>
@@ -6473,11 +6478,11 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1">
       <c r="A19" s="11" t="s">
         <v>96</v>
       </c>
@@ -6511,7 +6516,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1">
       <c r="B20" s="4" t="s">
         <v>98</v>
       </c>
@@ -6542,7 +6547,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1">
       <c r="B21" s="4" t="s">
         <v>99</v>
       </c>
@@ -6573,7 +6578,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1">
       <c r="B22" s="4" t="s">
         <v>120</v>
       </c>
@@ -6599,7 +6604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1">
       <c r="B23" s="4" t="s">
         <v>91</v>
       </c>
@@ -6632,7 +6637,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
     </row>
@@ -6640,6 +6645,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6654,14 +6664,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -6681,7 +6691,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -6701,7 +6711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="B3" t="s">
         <v>55</v>
       </c>
@@ -6718,7 +6728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -6738,7 +6748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="B5" t="s">
         <v>55</v>
       </c>
@@ -6755,7 +6765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -6775,7 +6785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="B7" t="s">
         <v>55</v>
       </c>
@@ -6796,6 +6806,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6810,7 +6825,7 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
@@ -6819,7 +6834,7 @@
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -6848,7 +6863,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -6877,7 +6892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9">
       <c r="B3" t="s">
         <v>55</v>
       </c>
@@ -6904,7 +6919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
         <v>90</v>
       </c>
@@ -6933,7 +6948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9">
       <c r="B5" t="s">
         <v>55</v>
       </c>
@@ -6960,7 +6975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9">
       <c r="A6" s="4" t="s">
         <v>92</v>
       </c>
@@ -6989,7 +7004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9">
       <c r="B7" t="s">
         <v>55</v>
       </c>
@@ -7017,7 +7032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
         <v>93</v>
       </c>
@@ -7046,7 +7061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9">
       <c r="B9" t="s">
         <v>55</v>
       </c>
@@ -7073,7 +7088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9">
       <c r="A10" s="4" t="s">
         <v>94</v>
       </c>
@@ -7102,7 +7117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9">
       <c r="B11" t="s">
         <v>55</v>
       </c>
@@ -7129,7 +7144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9">
       <c r="A12" s="4" t="s">
         <v>95</v>
       </c>
@@ -7158,7 +7173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9">
       <c r="B13" t="s">
         <v>55</v>
       </c>
@@ -7185,7 +7200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -7214,7 +7229,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9">
       <c r="B15" t="s">
         <v>55</v>
       </c>
@@ -7244,7 +7259,7 @@
         <v>0.17934</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>118</v>
       </c>
@@ -7273,7 +7288,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9">
       <c r="B17" t="s">
         <v>55</v>
       </c>
@@ -7303,7 +7318,7 @@
         <v>0.17934</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -7332,7 +7347,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9">
       <c r="B19" t="s">
         <v>55</v>
       </c>
@@ -7362,7 +7377,7 @@
         <v>0.17934</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9">
       <c r="A20" s="4" t="s">
         <v>88</v>
       </c>
@@ -7387,7 +7402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9">
       <c r="B21" t="s">
         <v>55</v>
       </c>
@@ -7415,7 +7430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -7444,7 +7459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9">
       <c r="B23" t="s">
         <v>55</v>
       </c>
@@ -7470,7 +7485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9">
       <c r="A24" s="4" t="s">
         <v>91</v>
       </c>
@@ -7484,7 +7499,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9">
       <c r="B25" t="s">
         <v>55</v>
       </c>
@@ -7499,6 +7514,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7513,7 +7533,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="27.5" customWidth="1"/>
     <col min="3" max="3" width="38.1640625" customWidth="1"/>
@@ -7523,7 +7543,7 @@
     <col min="8" max="8" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -7549,7 +7569,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>51</v>
       </c>
@@ -7575,7 +7595,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="C3" t="s">
         <v>71</v>
       </c>
@@ -7595,7 +7615,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -7617,7 +7637,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -7625,6 +7645,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7636,7 +7661,7 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="43.83203125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -7644,7 +7669,7 @@
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -7658,7 +7683,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
@@ -7675,7 +7700,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>51</v>
       </c>
@@ -7692,7 +7717,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>58</v>
       </c>
@@ -7709,7 +7734,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>87</v>
       </c>
@@ -7726,7 +7751,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>88</v>
       </c>
@@ -7737,7 +7762,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="34" t="s">
         <v>86</v>
       </c>
@@ -7748,7 +7773,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -7765,7 +7790,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -7782,7 +7807,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>90</v>
       </c>
@@ -7793,7 +7818,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" t="s">
         <v>102</v>
       </c>
@@ -7804,7 +7829,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>92</v>
       </c>
@@ -7815,7 +7840,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>93</v>
       </c>
@@ -7826,7 +7851,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>94</v>
       </c>
@@ -7834,7 +7859,7 @@
       <c r="C14" s="35"/>
       <c r="D14" s="14"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="4" t="s">
         <v>95</v>
       </c>
@@ -7842,7 +7867,7 @@
       <c r="C15" s="14"/>
       <c r="D15" s="35"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="4" t="s">
         <v>97</v>
       </c>
@@ -7850,7 +7875,7 @@
       <c r="C16" s="14"/>
       <c r="D16" s="35"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1">
       <c r="A17" s="4" t="s">
         <v>98</v>
       </c>
@@ -7858,7 +7883,7 @@
       <c r="C17" s="14"/>
       <c r="D17" s="35"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="A18" s="4" t="s">
         <v>99</v>
       </c>
@@ -7866,7 +7891,7 @@
       <c r="C18" s="14"/>
       <c r="D18" s="35"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
         <v>120</v>
       </c>
@@ -7874,7 +7899,7 @@
       <c r="C19" s="14"/>
       <c r="D19" s="35"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1">
       <c r="A20" s="4" t="s">
         <v>91</v>
       </c>
@@ -7882,27 +7907,27 @@
       <c r="C20" s="14"/>
       <c r="D20" s="35"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
     </row>
@@ -7910,6 +7935,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7924,7 +7954,7 @@
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
@@ -7932,7 +7962,7 @@
     <col min="11" max="11" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7946,13 +7976,13 @@
         <v>67</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>150</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>151</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>68</v>
@@ -7967,10 +7997,10 @@
         <v>100</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1">
       <c r="A2" s="3">
         <v>2017</v>
       </c>
@@ -8012,7 +8042,7 @@
         <v>173766200</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1">
       <c r="A3" s="3">
         <v>2018</v>
       </c>
@@ -8054,7 +8084,7 @@
         <v>175848400</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1">
       <c r="A4" s="3">
         <v>2019</v>
       </c>
@@ -8096,7 +8126,7 @@
         <v>177930600</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1">
       <c r="A5" s="3">
         <v>2020</v>
       </c>
@@ -8138,7 +8168,7 @@
         <v>180012800</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1">
       <c r="A6" s="3">
         <v>2021</v>
       </c>
@@ -8180,7 +8210,7 @@
         <v>182095000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1">
       <c r="A7" s="3">
         <v>2022</v>
       </c>
@@ -8222,7 +8252,7 @@
         <v>183822800</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="A8" s="3">
         <v>2023</v>
       </c>
@@ -8264,7 +8294,7 @@
         <v>185550600</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1">
       <c r="A9" s="3">
         <v>2024</v>
       </c>
@@ -8306,7 +8336,7 @@
         <v>187278400</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1">
       <c r="A10" s="3">
         <v>2025</v>
       </c>
@@ -8348,7 +8378,7 @@
         <v>189006200</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1">
       <c r="A11" s="3">
         <v>2026</v>
       </c>
@@ -8390,7 +8420,7 @@
         <v>190734000</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1">
       <c r="A12" s="3">
         <v>2027</v>
       </c>
@@ -8432,7 +8462,7 @@
         <v>192287600</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1">
       <c r="A13" s="3">
         <v>2028</v>
       </c>
@@ -8474,7 +8504,7 @@
         <v>193841200</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1">
       <c r="A14" s="3">
         <v>2029</v>
       </c>
@@ -8516,7 +8546,7 @@
         <v>195394800</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1">
       <c r="A15" s="3">
         <v>2030</v>
       </c>
@@ -8562,6 +8592,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8573,12 +8608,12 @@
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -8601,7 +8636,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -8624,7 +8659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -8647,7 +8682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -8670,7 +8705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -8693,7 +8728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -8716,7 +8751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -8739,7 +8774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -8762,7 +8797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -8785,7 +8820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -8808,7 +8843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -8831,7 +8866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -8854,7 +8889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -8877,7 +8912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -8900,7 +8935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -8923,7 +8958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -8946,7 +8981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -8969,7 +9004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -8992,7 +9027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" t="s">
         <v>106</v>
       </c>
@@ -9015,7 +9050,7 @@
         <v>2.5899999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" t="s">
         <v>107</v>
       </c>
@@ -9038,7 +9073,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" t="s">
         <v>108</v>
       </c>
@@ -9061,7 +9096,7 @@
         <v>0.25590000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" t="s">
         <v>109</v>
       </c>
@@ -9084,7 +9119,7 @@
         <v>0.1464</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" t="s">
         <v>110</v>
       </c>
@@ -9107,7 +9142,7 @@
         <v>1.7600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -9130,7 +9165,7 @@
         <v>1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" t="s">
         <v>112</v>
       </c>
@@ -9153,7 +9188,7 @@
         <v>1.14E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" t="s">
         <v>113</v>
       </c>
@@ -9176,7 +9211,7 @@
         <v>0.15129999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -9206,6 +9241,11 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9217,9 +9257,9 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
@@ -9239,7 +9279,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>29</v>
       </c>
@@ -9259,7 +9299,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" t="s">
         <v>138</v>
       </c>
@@ -9279,7 +9319,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
@@ -9302,6 +9342,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9316,7 +9361,7 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
@@ -9325,7 +9370,7 @@
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5">
       <c r="A1" s="11" t="s">
         <v>127</v>
       </c>
@@ -9342,7 +9387,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5">
       <c r="A2" s="11" t="s">
         <v>103</v>
       </c>
@@ -9357,7 +9402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5">
       <c r="A3" s="11"/>
       <c r="B3" t="s">
         <v>7</v>
@@ -9370,7 +9415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5">
       <c r="A4" s="11"/>
       <c r="B4" t="s">
         <v>8</v>
@@ -9385,7 +9430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5">
       <c r="A5" s="11"/>
       <c r="B5" t="s">
         <v>9</v>
@@ -9400,7 +9445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5">
       <c r="A6" s="11"/>
       <c r="B6" t="s">
         <v>10</v>
@@ -9415,7 +9460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="A7" s="11"/>
       <c r="B7" t="s">
         <v>85</v>
@@ -9430,10 +9475,10 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5">
       <c r="A8" s="11"/>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C8" s="20">
         <v>0</v>
@@ -9445,10 +9490,10 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C9" s="20">
         <v>0</v>
@@ -9460,10 +9505,10 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C10" s="20">
         <v>0</v>
@@ -9475,13 +9520,13 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5">
       <c r="A11" s="11"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5">
       <c r="A12" s="11"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5">
       <c r="A13" s="11" t="s">
         <v>104</v>
       </c>
@@ -9496,7 +9541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -9508,7 +9553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5">
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -9522,7 +9567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5">
       <c r="B16" t="s">
         <v>9</v>
       </c>
@@ -9536,7 +9581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -9550,7 +9595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5">
       <c r="B18" t="s">
         <v>85</v>
       </c>
@@ -9564,9 +9609,9 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5">
       <c r="B19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C19" s="20">
         <v>0</v>
@@ -9578,9 +9623,9 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5">
       <c r="B20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C20" s="20">
         <v>0</v>
@@ -9592,9 +9637,9 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5">
       <c r="B21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C21" s="20">
         <v>0</v>
@@ -9606,7 +9651,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5">
       <c r="A24" s="11" t="s">
         <v>122</v>
       </c>
@@ -9627,6 +9672,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9638,9 +9688,9 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -9663,7 +9713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
@@ -9686,7 +9736,7 @@
         <v>25.35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
         <v>24</v>
@@ -9707,7 +9757,7 @@
         <v>33.25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="12"/>
       <c r="B4" s="13" t="s">
         <v>27</v>
@@ -9728,7 +9778,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="12"/>
       <c r="B5" s="13" t="s">
         <v>28</v>
@@ -9749,7 +9799,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
@@ -9772,7 +9822,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
@@ -9792,7 +9842,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
@@ -9812,7 +9862,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
@@ -9832,7 +9882,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
@@ -9855,7 +9905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
@@ -9875,7 +9925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="4" t="s">
         <v>42</v>
       </c>
@@ -9895,7 +9945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1">
       <c r="B17" s="4" t="s">
         <v>43</v>
       </c>
@@ -9920,6 +9970,11 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9931,12 +9986,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>128</v>
       </c>
@@ -9956,7 +10011,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>12</v>
       </c>
@@ -9977,7 +10032,7 @@
         <v>3.1128200000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="B3" t="s">
         <v>124</v>
       </c>
@@ -9992,7 +10047,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="B4" t="s">
         <v>63</v>
       </c>
@@ -10009,14 +10064,14 @@
         <v>46.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="11"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="11"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="B7" s="11" t="s">
         <v>5</v>
       </c>
@@ -10025,7 +10080,7 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="11" t="s">
         <v>61</v>
       </c>
@@ -10045,7 +10100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
@@ -10062,7 +10117,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
@@ -10079,7 +10134,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
@@ -10096,7 +10151,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
@@ -10113,7 +10168,7 @@
         <v>999.99</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1">
       <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
@@ -10130,7 +10185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
       <c r="B14" s="5" t="s">
         <v>46</v>
       </c>
@@ -10147,7 +10202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
@@ -10168,6 +10223,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10182,7 +10242,7 @@
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
@@ -10190,7 +10250,7 @@
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" s="11" t="s">
         <v>61</v>
       </c>
@@ -10219,7 +10279,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
@@ -10248,7 +10308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9">
       <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
@@ -10271,7 +10331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9">
       <c r="C4" s="4" t="s">
         <v>27</v>
       </c>
@@ -10294,7 +10354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9">
       <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
@@ -10317,7 +10377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9">
       <c r="B6" t="s">
         <v>31</v>
       </c>
@@ -10343,7 +10403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9">
       <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
@@ -10366,7 +10426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9">
       <c r="C8" s="4" t="s">
         <v>27</v>
       </c>
@@ -10389,7 +10449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9">
       <c r="C9" s="4" t="s">
         <v>28</v>
       </c>
@@ -10412,7 +10472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9">
       <c r="B10" t="s">
         <v>33</v>
       </c>
@@ -10438,7 +10498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9">
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
@@ -10461,7 +10521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9">
       <c r="C12" s="4" t="s">
         <v>27</v>
       </c>
@@ -10484,7 +10544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9">
       <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
@@ -10507,7 +10567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9">
       <c r="B14" t="s">
         <v>34</v>
       </c>
@@ -10533,7 +10593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9">
       <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
@@ -10556,7 +10616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9">
       <c r="C16" s="4" t="s">
         <v>27</v>
       </c>
@@ -10579,7 +10639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9">
       <c r="C17" s="4" t="s">
         <v>28</v>
       </c>
@@ -10602,7 +10662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9">
       <c r="B18" t="s">
         <v>38</v>
       </c>
@@ -10628,7 +10688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9">
       <c r="C19" s="4" t="s">
         <v>24</v>
       </c>
@@ -10651,7 +10711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9">
       <c r="C20" s="4" t="s">
         <v>27</v>
       </c>
@@ -10674,7 +10734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9">
       <c r="C21" s="4" t="s">
         <v>28</v>
       </c>
@@ -10697,7 +10757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9">
       <c r="A24" s="11" t="s">
         <v>30</v>
       </c>
@@ -10726,7 +10786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9">
       <c r="C25" s="4" t="s">
         <v>24</v>
       </c>
@@ -10749,7 +10809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9">
       <c r="C26" s="4" t="s">
         <v>27</v>
       </c>
@@ -10772,7 +10832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9">
       <c r="C27" s="4" t="s">
         <v>28</v>
       </c>
@@ -10795,7 +10855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9">
       <c r="B28" t="s">
         <v>31</v>
       </c>
@@ -10821,7 +10881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9">
       <c r="C29" s="4" t="s">
         <v>24</v>
       </c>
@@ -10844,7 +10904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9">
       <c r="C30" s="4" t="s">
         <v>27</v>
       </c>
@@ -10867,7 +10927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9">
       <c r="C31" s="4" t="s">
         <v>28</v>
       </c>
@@ -10890,7 +10950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9">
       <c r="B32" t="s">
         <v>33</v>
       </c>
@@ -10916,7 +10976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9">
       <c r="C33" s="4" t="s">
         <v>24</v>
       </c>
@@ -10939,7 +10999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:9">
       <c r="C34" s="4" t="s">
         <v>27</v>
       </c>
@@ -10962,7 +11022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:9">
       <c r="C35" s="4" t="s">
         <v>28</v>
       </c>
@@ -10985,7 +11045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:9">
       <c r="B36" t="s">
         <v>34</v>
       </c>
@@ -11011,7 +11071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:9">
       <c r="C37" s="4" t="s">
         <v>24</v>
       </c>
@@ -11034,7 +11094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:9">
       <c r="C38" s="4" t="s">
         <v>27</v>
       </c>
@@ -11057,7 +11117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:9">
       <c r="C39" s="4" t="s">
         <v>28</v>
       </c>
@@ -11080,7 +11140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:9">
       <c r="B40" t="s">
         <v>38</v>
       </c>
@@ -11106,7 +11166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:9">
       <c r="C41" s="4" t="s">
         <v>24</v>
       </c>
@@ -11129,7 +11189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:9">
       <c r="C42" s="4" t="s">
         <v>27</v>
       </c>
@@ -11152,7 +11212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:9">
       <c r="C43" s="4" t="s">
         <v>28</v>
       </c>
@@ -11175,7 +11235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:9">
       <c r="A46" s="11" t="s">
         <v>39</v>
       </c>
@@ -11204,7 +11264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:9">
       <c r="C47" s="4" t="s">
         <v>41</v>
       </c>
@@ -11227,7 +11287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:9">
       <c r="C48" s="4" t="s">
         <v>42</v>
       </c>
@@ -11250,7 +11310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:9">
       <c r="C49" s="4" t="s">
         <v>43</v>
       </c>
@@ -11273,7 +11333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:9">
       <c r="B50" t="s">
         <v>16</v>
       </c>
@@ -11299,7 +11359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="51" spans="2:9">
       <c r="C51" s="4" t="s">
         <v>41</v>
       </c>
@@ -11322,7 +11382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:9">
       <c r="C52" s="4" t="s">
         <v>42</v>
       </c>
@@ -11345,7 +11405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="53" spans="2:9">
       <c r="C53" s="4" t="s">
         <v>43</v>
       </c>
@@ -11368,7 +11428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="54" spans="2:9">
       <c r="B54" t="s">
         <v>17</v>
       </c>
@@ -11394,7 +11454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="55" spans="2:9">
       <c r="C55" s="4" t="s">
         <v>41</v>
       </c>
@@ -11417,7 +11477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="56" spans="2:9">
       <c r="C56" s="4" t="s">
         <v>42</v>
       </c>
@@ -11440,7 +11500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="57" spans="2:9">
       <c r="C57" s="4" t="s">
         <v>43</v>
       </c>
@@ -11463,7 +11523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="58" spans="2:9">
       <c r="B58" t="s">
         <v>22</v>
       </c>
@@ -11489,7 +11549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="59" spans="2:9">
       <c r="C59" s="4" t="s">
         <v>41</v>
       </c>
@@ -11512,7 +11572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="60" spans="2:9">
       <c r="C60" s="4" t="s">
         <v>42</v>
       </c>
@@ -11535,7 +11595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="61" spans="2:9">
       <c r="C61" s="4" t="s">
         <v>43</v>
       </c>
@@ -11558,7 +11618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="62" spans="2:9">
       <c r="B62" t="s">
         <v>29</v>
       </c>
@@ -11584,7 +11644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="63" spans="2:9">
       <c r="C63" s="4" t="s">
         <v>41</v>
       </c>
@@ -11607,7 +11667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="64" spans="2:9">
       <c r="C64" s="4" t="s">
         <v>42</v>
       </c>
@@ -11630,7 +11690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:9">
       <c r="C65" s="4" t="s">
         <v>43</v>
       </c>
@@ -11653,7 +11713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:9">
       <c r="B66" t="s">
         <v>31</v>
       </c>
@@ -11679,7 +11739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:9">
       <c r="C67" s="4" t="s">
         <v>41</v>
       </c>
@@ -11702,7 +11762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:9">
       <c r="C68" s="4" t="s">
         <v>42</v>
       </c>
@@ -11725,7 +11785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:9">
       <c r="C69" s="4" t="s">
         <v>43</v>
       </c>
@@ -11748,7 +11808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:9">
       <c r="B70" t="s">
         <v>32</v>
       </c>
@@ -11774,7 +11834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:9">
       <c r="C71" s="4" t="s">
         <v>41</v>
       </c>
@@ -11797,7 +11857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:9">
       <c r="C72" s="4" t="s">
         <v>42</v>
       </c>
@@ -11820,7 +11880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:9">
       <c r="C73" s="4" t="s">
         <v>43</v>
       </c>
@@ -11843,7 +11903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:9">
       <c r="A76" s="11" t="s">
         <v>140</v>
       </c>
@@ -11872,7 +11932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:9">
       <c r="C77" s="4" t="s">
         <v>130</v>
       </c>
@@ -11895,7 +11955,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:9">
       <c r="B78" t="s">
         <v>107</v>
       </c>
@@ -11921,7 +11981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:9">
       <c r="C79" s="4" t="s">
         <v>130</v>
       </c>
@@ -11944,7 +12004,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:9">
       <c r="B80" t="s">
         <v>108</v>
       </c>
@@ -11970,7 +12030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:9">
       <c r="C81" s="4" t="s">
         <v>130</v>
       </c>
@@ -11993,7 +12053,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:9">
       <c r="A84" s="11" t="s">
         <v>121</v>
       </c>
@@ -12022,7 +12082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:9">
       <c r="C85" s="4" t="s">
         <v>41</v>
       </c>
@@ -12045,7 +12105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:9">
       <c r="C86" s="4" t="s">
         <v>42</v>
       </c>
@@ -12068,7 +12128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:9">
       <c r="C87" s="4" t="s">
         <v>43</v>
       </c>
@@ -12091,7 +12151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:9">
       <c r="A90" s="11" t="s">
         <v>141</v>
       </c>
@@ -12102,6 +12162,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -12112,11 +12177,11 @@
   </sheetPr>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="36.6640625" customWidth="1"/>
     <col min="2" max="2" width="64.5" customWidth="1"/>
@@ -12126,7 +12191,7 @@
     <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
         <v>52</v>
       </c>
@@ -12149,7 +12214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2" s="11" t="s">
         <v>132</v>
       </c>
@@ -12170,7 +12235,7 @@
         <v>174.7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="B3" s="4" t="s">
         <v>29</v>
       </c>
@@ -12190,7 +12255,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" s="11" t="s">
         <v>131</v>
       </c>
@@ -12213,7 +12278,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7">
       <c r="B6" s="4" t="s">
         <v>48</v>
       </c>
@@ -12233,7 +12298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7">
       <c r="B7" s="4" t="s">
         <v>49</v>
       </c>
@@ -12253,9 +12318,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7">
       <c r="B8" s="4" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -12273,9 +12338,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7">
       <c r="B9" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -12293,7 +12358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7">
       <c r="B10" s="4" t="s">
         <v>50</v>
       </c>
@@ -12313,7 +12378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="14">
       <c r="A12" s="11" t="s">
         <v>133</v>
       </c>
@@ -12336,7 +12401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="14">
       <c r="B13" s="4" t="s">
         <v>58</v>
       </c>
@@ -12360,5 +12425,10 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated spreadsheet Interventions anemia tab to a suggestion of how it should look
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-69620" yWindow="-4060" windowWidth="26380" windowHeight="16040" tabRatio="500" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="-69620" yWindow="-4220" windowWidth="26380" windowHeight="16040" tabRatio="500" firstSheet="10" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -338,7 +338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A15" authorId="0">
+    <comment ref="A18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1706,10 +1706,11 @@
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Ruth</author>
     <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="E17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1718,7 +1719,7 @@
             <color indexed="81"/>
             <rFont val="Arial"/>
           </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
+          <t>Ruth:</t>
         </r>
         <r>
           <rPr>
@@ -1727,601 +1728,8 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Impact on decreasing prevalence of anemia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-From RR in the book</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Severe Fe-deficiency anemia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Pregnant women with iron deficiency anemia; AF should really be age dependent</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-not sure</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Severe Fe-deficiency anemia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Pregnant women with iron deficiency anemia; AF should really be age dependent</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Severe Fe-deficiency anemia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Pregnant women with iron deficiency anemia; AF should really be age dependent</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Non-pregnant with iron deficiency anemia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Severe Fe-deficiency anemia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Pregnant women with iron deficiency anemia; AF should really be age dependent</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B11" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Severe Fe-deficiency anemia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C11" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Pregnant women with iron deficiency anemia; AF should really be age dependent</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A12" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-There is no unit cost for this to impact the budget.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B13" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Severe Fe-deficiency anemia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C13" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Pregnant women with iron deficiency anemia; AF should really be age dependent</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G14" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Guess</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H14" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Guess</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I14" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Guess</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B15" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Severe Fe-deficiency anemia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C15" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Pregnant women with iron deficiency anemia; AF should really be age dependent</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G16" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Guess</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H16" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Guess</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I16" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Guess</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B17" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Severe Fe-deficiency anemia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C17" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Pregnant women with iron deficiency anemia; AF should really be age dependent</t>
+made this number up
+</t>
         </r>
       </text>
     </comment>
@@ -2334,7 +1742,7 @@
             <color indexed="81"/>
             <rFont val="Arial"/>
           </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
+          <t>Ruth:</t>
         </r>
         <r>
           <rPr>
@@ -2343,11 +1751,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Guess</t>
+mader this number up</t>
         </r>
       </text>
     </comment>
-    <comment ref="H18" authorId="0">
+    <comment ref="B19" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2365,11 +1773,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Guess</t>
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
         </r>
       </text>
     </comment>
-    <comment ref="I18" authorId="0">
+    <comment ref="L19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2378,7 +1786,7 @@
             <color indexed="81"/>
             <rFont val="Arial"/>
           </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
+          <t>Ruth:</t>
         </r>
         <r>
           <rPr>
@@ -2387,11 +1795,12 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Guess</t>
+made this number up
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="B19" authorId="0">
+    <comment ref="B31" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2409,11 +1818,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Baseline year</t>
+Also brestfeeding women up to 6 months?</t>
         </r>
       </text>
     </comment>
-    <comment ref="C19" authorId="0">
+    <comment ref="B35" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2431,205 +1840,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Pregnant women with iron deficiency anemia; AF should really be age dependent</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B21" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Baseline year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A22" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-prevents malaria, IFAS or AMS can be given only with this where there is malaria risk. IFAS &amp; AMS will help with anemia only where IPTp or nets are effective</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C22" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-All anemia in malaria-risk</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B23" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Severe Fe-deficiency anemia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C23" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-All target pop, i.e. pregnant at risk of malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C24" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-All anemia in malaria-risk</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B25" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Severe Fe-deficiency anemia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C25" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-All target pop, i.e. pregnant at risk of malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D25" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-All target pop, i.e. non-pregnant at risk of malaria</t>
+There is no unit cost for this to impact the budget.</t>
         </r>
       </text>
     </comment>
@@ -2638,7 +1849,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="178">
   <si>
     <t>year</t>
   </si>
@@ -2994,12 +2205,6 @@
     <t>fraction eating maize</t>
   </si>
   <si>
-    <t>Iron fortification of flour</t>
-  </si>
-  <si>
-    <t>fortification of maize</t>
-  </si>
-  <si>
     <t>Iron and iodine fortification of salt</t>
   </si>
   <si>
@@ -3118,6 +2323,66 @@
   </si>
   <si>
     <t>Complementary feeding (food insecure with promotion and supplementation)</t>
+  </si>
+  <si>
+    <t>WRA: 15-19 years</t>
+  </si>
+  <si>
+    <t>WRA: 20-29 years</t>
+  </si>
+  <si>
+    <t>WRA: 30-39 years</t>
+  </si>
+  <si>
+    <t>WRA: 40-49 years</t>
+  </si>
+  <si>
+    <t>PW: 15-19 years</t>
+  </si>
+  <si>
+    <t>PW: 20-29 years</t>
+  </si>
+  <si>
+    <t>PW: 30-39 years</t>
+  </si>
+  <si>
+    <t>PW: 40-49 years</t>
+  </si>
+  <si>
+    <t>IPTp</t>
+  </si>
+  <si>
+    <t>Relative Risks</t>
+  </si>
+  <si>
+    <t>Odds Ratios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprinkles </t>
+  </si>
+  <si>
+    <t>IFAS poor: school</t>
+  </si>
+  <si>
+    <t>IFAS poor: community</t>
+  </si>
+  <si>
+    <t>IFAS poor: hospital</t>
+  </si>
+  <si>
+    <t>IFAS not poor: school</t>
+  </si>
+  <si>
+    <t>IFAS not poor: community</t>
+  </si>
+  <si>
+    <t>IFAS not poor: hospital</t>
+  </si>
+  <si>
+    <t>IFAS not poor: retailer</t>
+  </si>
+  <si>
+    <t>Public provision of complementary foods</t>
   </si>
 </sst>
 </file>
@@ -3291,7 +2556,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="501">
+  <cellStyleXfs count="509">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3793,8 +3058,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3868,10 +3141,8 @@
     <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="14" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3884,16 +3155,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="14" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="14" fillId="2" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="501">
+  <cellStyles count="509">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -4144,6 +3415,10 @@
     <cellStyle name="Followed Hyperlink" xfId="496" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="498" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="500" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="502" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="504" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="506" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="508" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4393,6 +3668,10 @@
     <cellStyle name="Hyperlink" xfId="495" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="497" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="499" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="501" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="503" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="505" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="507" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -5711,13 +4990,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>64</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
@@ -5741,9 +5020,9 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="B4" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4" s="61">
+        <v>150</v>
+      </c>
+      <c r="C4" s="57">
         <v>171684000</v>
       </c>
     </row>
@@ -5786,7 +5065,7 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1">
       <c r="A11" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B11" t="s">
         <v>81</v>
@@ -5797,7 +5076,7 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1">
       <c r="B12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C12" s="20">
         <v>0.13</v>
@@ -5805,7 +5084,7 @@
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1">
       <c r="B13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C13" s="20">
         <v>25.36</v>
@@ -5813,7 +5092,7 @@
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1">
       <c r="B14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C14" s="20">
         <v>25.4</v>
@@ -5821,7 +5100,7 @@
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1">
       <c r="B15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C15" s="20">
         <v>34.68</v>
@@ -5829,7 +5108,7 @@
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1">
       <c r="B16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C16" s="20">
         <v>39.32</v>
@@ -5846,7 +5125,7 @@
       <c r="B19" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="49">
+      <c r="C19" s="47">
         <v>0.3</v>
       </c>
     </row>
@@ -5854,7 +5133,7 @@
       <c r="B20" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="C20" s="49">
+      <c r="C20" s="47">
         <v>0.8</v>
       </c>
     </row>
@@ -5862,7 +5141,7 @@
       <c r="B21" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="C21" s="49">
+      <c r="C21" s="47">
         <v>0.12</v>
       </c>
     </row>
@@ -5870,7 +5149,7 @@
       <c r="B22" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="C22" s="49">
+      <c r="C22" s="47">
         <v>0.05</v>
       </c>
     </row>
@@ -5878,7 +5157,7 @@
       <c r="B23" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="49">
+      <c r="C23" s="47">
         <v>0.05</v>
       </c>
     </row>
@@ -5887,75 +5166,75 @@
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="A26" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="B26" s="58" t="s">
+        <v>149</v>
+      </c>
+      <c r="B26" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="59">
+      <c r="C26" s="55">
         <v>8634000</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1">
-      <c r="B27" s="58" t="s">
+      <c r="B27" s="54" t="s">
+        <v>143</v>
+      </c>
+      <c r="C27" s="55">
+        <v>13550000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B28" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="55">
+        <v>12394000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B29" s="54" t="s">
         <v>145</v>
       </c>
-      <c r="C27" s="59">
-        <v>13550000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B28" s="58" t="s">
-        <v>146</v>
-      </c>
-      <c r="C28" s="59">
-        <v>12394000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B29" s="58" t="s">
-        <v>147</v>
-      </c>
-      <c r="C29" s="59">
+      <c r="C29" s="55">
         <v>9148000</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B30" s="58"/>
-      <c r="C30" s="60"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="56"/>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="A32" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="B32" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="C32" s="48">
+      <c r="C32" s="46">
         <v>0.29978973218277538</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B33" s="57" t="s">
+      <c r="B33" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" s="46">
+        <v>0.52556568434139284</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B34" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="C34" s="46">
+        <v>0.16210210664201097</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B35" s="53" t="s">
         <v>145</v>
       </c>
-      <c r="C33" s="48">
-        <v>0.52556568434139284</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B34" s="57" t="s">
-        <v>146</v>
-      </c>
-      <c r="C34" s="48">
-        <v>0.16210210664201097</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B35" s="57" t="s">
-        <v>147</v>
-      </c>
-      <c r="C35" s="48">
+      <c r="C35" s="46">
         <v>1.2542476833820825E-2</v>
       </c>
     </row>
@@ -6580,7 +5859,7 @@
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1">
       <c r="B22" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
@@ -6767,15 +6046,15 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="51">
+      <c r="C6" s="49">
         <v>0.15</v>
       </c>
-      <c r="D6" s="51">
+      <c r="D6" s="49">
         <v>0.15</v>
       </c>
       <c r="E6" s="10">
@@ -6789,10 +6068,10 @@
       <c r="B7" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="51">
-        <v>1</v>
-      </c>
-      <c r="D7" s="51">
+      <c r="C7" s="49">
+        <v>1</v>
+      </c>
+      <c r="D7" s="49">
         <v>1</v>
       </c>
       <c r="E7" s="10">
@@ -6819,696 +6098,761 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="45" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" customWidth="1"/>
     <col min="3" max="3" width="18.83203125" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15">
+      <c r="B1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>52</v>
-      </c>
       <c r="C1" s="11" t="s">
-        <v>84</v>
+        <v>6</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>9</v>
+        <v>158</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" t="s">
         <v>60</v>
       </c>
-      <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="39">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
         <v>0.3</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="B3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="42">
-        <f>'Prevalence of anemia'!$E$18</f>
-        <v>0.23580000000000001</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="4" t="s">
+      <c r="M3">
+        <v>0.3</v>
+      </c>
+      <c r="N3">
+        <v>0.3</v>
+      </c>
+      <c r="O3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="B4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0.83</v>
+      </c>
+      <c r="M4">
+        <v>0.83</v>
+      </c>
+      <c r="N4">
+        <v>0.83</v>
+      </c>
+      <c r="O4">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="B5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0.73</v>
+      </c>
+      <c r="I5">
+        <v>0.73</v>
+      </c>
+      <c r="J5">
+        <v>0.73</v>
+      </c>
+      <c r="K5">
+        <v>0.73</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="B6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0.73</v>
+      </c>
+      <c r="I6">
+        <v>0.73</v>
+      </c>
+      <c r="J6">
+        <v>0.73</v>
+      </c>
+      <c r="K6">
+        <v>0.73</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="B7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0.73</v>
+      </c>
+      <c r="I7">
+        <v>0.73</v>
+      </c>
+      <c r="J7">
+        <v>0.73</v>
+      </c>
+      <c r="K7">
+        <v>0.73</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="B8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0.73</v>
+      </c>
+      <c r="I8">
+        <v>0.73</v>
+      </c>
+      <c r="J8">
+        <v>0.73</v>
+      </c>
+      <c r="K8">
+        <v>0.73</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="B9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0.73</v>
+      </c>
+      <c r="I9">
+        <v>0.73</v>
+      </c>
+      <c r="J9">
+        <v>0.73</v>
+      </c>
+      <c r="K9">
+        <v>0.73</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="B10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0.73</v>
+      </c>
+      <c r="I10">
+        <v>0.73</v>
+      </c>
+      <c r="J10">
+        <v>0.73</v>
+      </c>
+      <c r="K10">
+        <v>0.73</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="B11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0.73</v>
+      </c>
+      <c r="I11">
+        <v>0.73</v>
+      </c>
+      <c r="J11">
+        <v>0.73</v>
+      </c>
+      <c r="K11">
+        <v>0.73</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="B14" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="F14" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="G14" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="H14" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="I14" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="J14" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="K14" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="L14" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="M14" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="N14" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="O14" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="B15" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="F15" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="G15" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="H15" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="I15" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="J15" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="K15" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="L15" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="M15" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="N15" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="O15" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="B16" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="F16" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="G16" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="H16" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="I16" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="J16" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="K16" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="L16" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="M16" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="N16" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="O16" s="59">
+        <v>0.97599999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15">
+      <c r="B17" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="60">
+        <v>0.9</v>
+      </c>
+      <c r="F17" s="60">
+        <v>0.9</v>
+      </c>
+      <c r="G17" s="60">
+        <v>0.9</v>
+      </c>
+      <c r="H17" s="60">
+        <v>0.9</v>
+      </c>
+      <c r="I17" s="60">
+        <v>0.9</v>
+      </c>
+      <c r="J17" s="60">
+        <v>0.9</v>
+      </c>
+      <c r="K17" s="60">
+        <v>0.9</v>
+      </c>
+      <c r="L17" s="60">
+        <v>0.9</v>
+      </c>
+      <c r="M17" s="60">
+        <v>0.9</v>
+      </c>
+      <c r="N17" s="60">
+        <v>0.9</v>
+      </c>
+      <c r="O17" s="60">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15">
+      <c r="B18" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="59">
+        <v>1</v>
+      </c>
+      <c r="F18" s="59">
+        <v>1</v>
+      </c>
+      <c r="G18" s="60">
+        <v>0.8</v>
+      </c>
+      <c r="H18" s="59">
+        <v>1</v>
+      </c>
+      <c r="I18" s="59">
+        <v>1</v>
+      </c>
+      <c r="J18" s="59">
+        <v>1</v>
+      </c>
+      <c r="K18" s="59">
+        <v>1</v>
+      </c>
+      <c r="L18" s="59">
+        <v>1</v>
+      </c>
+      <c r="M18" s="59">
+        <v>1</v>
+      </c>
+      <c r="N18" s="59">
+        <v>1</v>
+      </c>
+      <c r="O18" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15">
+      <c r="B19" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="39">
-        <v>0.83</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="42">
-        <f>'Prevalence of anemia'!$E$18</f>
-        <v>0.23580000000000001</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0.61</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="B7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="42">
-        <f>'Prevalence of anemia'!$E$18</f>
-        <v>0.23580000000000001</v>
-      </c>
-      <c r="D7" s="42">
-        <f>'Prevalence of anemia'!$D$18</f>
-        <v>0.2238</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0.61</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="B9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="42">
-        <f>'Prevalence of anemia'!$E$18</f>
-        <v>0.23580000000000001</v>
-      </c>
-      <c r="D9" s="42">
-        <v>0.2238</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0.61</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="B11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="42">
-        <f>'Prevalence of anemia'!$E$18</f>
-        <v>0.23580000000000001</v>
-      </c>
-      <c r="D11" s="42">
-        <v>0.2238</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0.61</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="B13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="42">
-        <f>'Prevalence of anemia'!$E$18</f>
-        <v>0.23580000000000001</v>
-      </c>
-      <c r="D13" s="42">
-        <v>0.2238</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>99</v>
-      </c>
-      <c r="B14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14">
-        <v>0.67</v>
-      </c>
-      <c r="D14">
-        <v>0.61</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14" s="39">
-        <v>0.3</v>
-      </c>
-      <c r="H14" s="39">
-        <v>0.61</v>
-      </c>
-      <c r="I14" s="39">
-        <v>0.61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="B15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="42">
-        <f>'Prevalence of anemia'!$E$18</f>
-        <v>0.23580000000000001</v>
-      </c>
-      <c r="D15" s="42">
-        <v>0.2238</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15" s="55">
-        <f>'Prevalence of anemia'!$C$15</f>
-        <v>0.31079999999999997</v>
-      </c>
-      <c r="H15" s="55">
-        <f>'Prevalence of anemia'!$C$16</f>
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="I15" s="55">
-        <f>'Prevalence of anemia'!$C$17</f>
-        <v>0.17934</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>118</v>
-      </c>
-      <c r="B16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16">
-        <v>0.67</v>
-      </c>
-      <c r="D16">
-        <v>0.61</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16" s="39">
-        <v>0.3</v>
-      </c>
-      <c r="H16" s="39">
-        <v>0.61</v>
-      </c>
-      <c r="I16" s="39">
-        <v>0.61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="B17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="42">
-        <f>'Prevalence of anemia'!$E$18</f>
-        <v>0.23580000000000001</v>
-      </c>
-      <c r="D17" s="42">
-        <v>0.2238</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17" s="55">
-        <f>'Prevalence of anemia'!$C$15</f>
-        <v>0.31079999999999997</v>
-      </c>
-      <c r="H17" s="55">
-        <f>'Prevalence of anemia'!$C$16</f>
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="I17" s="55">
-        <f>'Prevalence of anemia'!$C$17</f>
-        <v>0.17934</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" t="s">
-        <v>119</v>
-      </c>
-      <c r="B18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18">
-        <v>0.67</v>
-      </c>
-      <c r="D18">
-        <v>0.61</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18" s="39">
-        <v>0.3</v>
-      </c>
-      <c r="H18" s="39">
-        <v>0.61</v>
-      </c>
-      <c r="I18" s="39">
-        <v>0.61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="B19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="42">
-        <f>'Prevalence of anemia'!$E$18</f>
-        <v>0.23580000000000001</v>
-      </c>
-      <c r="D19" s="42">
-        <v>0.2238</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19" s="55">
-        <f>'Prevalence of anemia'!$C$15</f>
-        <v>0.31079999999999997</v>
-      </c>
-      <c r="H19" s="56">
-        <f>'Prevalence of anemia'!$C$16</f>
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="I19" s="56">
-        <f>'Prevalence of anemia'!$C$17</f>
-        <v>0.17934</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="B21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21" s="55">
-        <f>'Prevalence of anemia'!$C$15</f>
-        <v>0.31079999999999997</v>
-      </c>
-      <c r="H21" s="55">
-        <f>'Prevalence of anemia'!$C$16</f>
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="I21" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22">
-        <v>0.17</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="B23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24">
-        <v>0.17</v>
-      </c>
-      <c r="D24">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="B25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="59">
+        <v>1</v>
+      </c>
+      <c r="F19" s="59">
+        <v>1</v>
+      </c>
+      <c r="G19" s="59">
+        <v>1</v>
+      </c>
+      <c r="H19" s="59">
+        <v>1</v>
+      </c>
+      <c r="I19" s="59">
+        <v>1</v>
+      </c>
+      <c r="J19" s="59">
+        <v>1</v>
+      </c>
+      <c r="K19" s="59">
+        <v>1</v>
+      </c>
+      <c r="L19" s="60">
+        <v>0.9</v>
+      </c>
+      <c r="M19" s="60">
+        <v>0.9</v>
+      </c>
+      <c r="N19" s="60">
+        <v>0.9</v>
+      </c>
+      <c r="O19" s="60">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15"/>
+    <row r="32" spans="2:15">
+      <c r="B32" s="4"/>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="4"/>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="4"/>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7577,7 +6921,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
@@ -7655,10 +6999,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -7674,13 +7018,13 @@
         <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
@@ -7736,7 +7080,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>87</v>
+        <v>177</v>
       </c>
       <c r="B5" s="15">
         <v>0</v>
@@ -7820,7 +7164,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>166</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="35"/>
@@ -7830,8 +7174,8 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A12" s="4" t="s">
-        <v>92</v>
+      <c r="A12" t="s">
+        <v>170</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="35"/>
@@ -7841,8 +7185,8 @@
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>93</v>
+      <c r="A13" t="s">
+        <v>171</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="35"/>
@@ -7852,40 +7196,46 @@
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A14" s="4" t="s">
-        <v>94</v>
+      <c r="A14" t="s">
+        <v>172</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="35"/>
       <c r="D14" s="14"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A15" s="4" t="s">
-        <v>95</v>
+      <c r="A15" t="s">
+        <v>173</v>
       </c>
       <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A16" s="4" t="s">
-        <v>97</v>
+      <c r="A16" t="s">
+        <v>174</v>
       </c>
       <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="14"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A17" s="4" t="s">
-        <v>98</v>
+      <c r="A17" t="s">
+        <v>175</v>
       </c>
       <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="14"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A18" s="4" t="s">
-        <v>99</v>
+      <c r="A18" t="s">
+        <v>176</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -7893,7 +7243,7 @@
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -7901,23 +7251,35 @@
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="35"/>
     </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A21" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="35"/>
+    </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1">
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="A22" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="35"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
+      <c r="A23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="35"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1">
       <c r="B25" s="4"/>
@@ -7930,6 +7292,18 @@
     <row r="27" spans="1:4" ht="15.75" customHeight="1">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7976,13 +7350,13 @@
         <v>67</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>148</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>150</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>68</v>
@@ -7997,7 +7371,7 @@
         <v>100</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1">
@@ -8038,7 +7412,7 @@
         <f>H2-I2</f>
         <v>41058509.531465083</v>
       </c>
-      <c r="L2" s="62">
+      <c r="L2" s="58">
         <v>173766200</v>
       </c>
     </row>
@@ -8080,7 +7454,7 @@
         <f t="shared" ref="K3:K15" si="3">H3-I3</f>
         <v>42070162.3670066</v>
       </c>
-      <c r="L3" s="62">
+      <c r="L3" s="58">
         <v>175848400</v>
       </c>
     </row>
@@ -8122,7 +7496,7 @@
         <f t="shared" si="3"/>
         <v>43083946.257598445</v>
       </c>
-      <c r="L4" s="62">
+      <c r="L4" s="58">
         <v>177930600</v>
       </c>
     </row>
@@ -8164,7 +7538,7 @@
         <f t="shared" si="3"/>
         <v>44100038.10321714</v>
       </c>
-      <c r="L5" s="62">
+      <c r="L5" s="58">
         <v>180012800</v>
       </c>
     </row>
@@ -8206,7 +7580,7 @@
         <f t="shared" si="3"/>
         <v>45114495.393052891</v>
       </c>
-      <c r="L6" s="62">
+      <c r="L6" s="58">
         <v>182095000</v>
       </c>
     </row>
@@ -8248,7 +7622,7 @@
         <f t="shared" si="3"/>
         <v>45617945.306584187</v>
       </c>
-      <c r="L7" s="62">
+      <c r="L7" s="58">
         <v>183822800</v>
       </c>
     </row>
@@ -8290,7 +7664,7 @@
         <f t="shared" si="3"/>
         <v>46123716.147807248</v>
       </c>
-      <c r="L8" s="62">
+      <c r="L8" s="58">
         <v>185550600</v>
       </c>
     </row>
@@ -8332,7 +7706,7 @@
         <f t="shared" si="3"/>
         <v>46631712.390734792</v>
       </c>
-      <c r="L9" s="62">
+      <c r="L9" s="58">
         <v>187278400</v>
       </c>
     </row>
@@ -8374,7 +7748,7 @@
         <f t="shared" si="3"/>
         <v>47141901.014037848</v>
       </c>
-      <c r="L10" s="62">
+      <c r="L10" s="58">
         <v>189006200</v>
       </c>
     </row>
@@ -8416,7 +7790,7 @@
         <f t="shared" si="3"/>
         <v>47645743.645516977</v>
       </c>
-      <c r="L11" s="62">
+      <c r="L11" s="58">
         <v>190734000</v>
       </c>
     </row>
@@ -8458,7 +7832,7 @@
         <f t="shared" si="3"/>
         <v>48024732.420057721</v>
       </c>
-      <c r="L12" s="62">
+      <c r="L12" s="58">
         <v>192287600</v>
       </c>
     </row>
@@ -8500,7 +7874,7 @@
         <f t="shared" si="3"/>
         <v>48405730.778331593</v>
       </c>
-      <c r="L13" s="62">
+      <c r="L13" s="58">
         <v>193841200</v>
       </c>
     </row>
@@ -8542,7 +7916,7 @@
         <f t="shared" si="3"/>
         <v>48788684.471012466</v>
       </c>
-      <c r="L14" s="62">
+      <c r="L14" s="58">
         <v>195394800</v>
       </c>
     </row>
@@ -8584,7 +7958,7 @@
         <f t="shared" si="3"/>
         <v>49173572.270103149</v>
       </c>
-      <c r="L15" s="62">
+      <c r="L15" s="58">
         <v>196948400</v>
       </c>
     </row>
@@ -9046,7 +8420,7 @@
       <c r="F19" s="20">
         <v>0</v>
       </c>
-      <c r="G19" s="41">
+      <c r="G19" s="40">
         <v>2.5899999999999999E-2</v>
       </c>
     </row>
@@ -9069,7 +8443,7 @@
       <c r="F20" s="20">
         <v>0</v>
       </c>
-      <c r="G20" s="41">
+      <c r="G20" s="40">
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
@@ -9092,7 +8466,7 @@
       <c r="F21" s="20">
         <v>0</v>
       </c>
-      <c r="G21" s="41">
+      <c r="G21" s="40">
         <v>0.25590000000000002</v>
       </c>
     </row>
@@ -9115,7 +8489,7 @@
       <c r="F22" s="20">
         <v>0</v>
       </c>
-      <c r="G22" s="41">
+      <c r="G22" s="40">
         <v>0.1464</v>
       </c>
     </row>
@@ -9138,7 +8512,7 @@
       <c r="F23" s="20">
         <v>0</v>
       </c>
-      <c r="G23" s="41">
+      <c r="G23" s="40">
         <v>1.7600000000000001E-2</v>
       </c>
     </row>
@@ -9161,7 +8535,7 @@
       <c r="F24" s="20">
         <v>0</v>
       </c>
-      <c r="G24" s="41">
+      <c r="G24" s="40">
         <v>1.8100000000000002E-2</v>
       </c>
     </row>
@@ -9184,7 +8558,7 @@
       <c r="F25" s="20">
         <v>0</v>
       </c>
-      <c r="G25" s="41">
+      <c r="G25" s="40">
         <v>1.14E-2</v>
       </c>
     </row>
@@ -9207,7 +8581,7 @@
       <c r="F26" s="20">
         <v>0</v>
       </c>
-      <c r="G26" s="41">
+      <c r="G26" s="40">
         <v>0.15129999999999999</v>
       </c>
     </row>
@@ -9230,7 +8604,7 @@
       <c r="F27" s="20">
         <v>0</v>
       </c>
-      <c r="G27" s="41">
+      <c r="G27" s="40">
         <v>0.36630000000000001</v>
       </c>
     </row>
@@ -9301,7 +8675,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B3" s="35">
         <v>5.1999999999999998E-2</v>
@@ -9372,7 +8746,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>82</v>
@@ -9394,7 +8768,7 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="52"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="20">
         <v>0</v>
       </c>
@@ -9407,7 +8781,7 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="53"/>
+      <c r="C3" s="51"/>
       <c r="D3" s="20">
         <v>0</v>
       </c>
@@ -9420,7 +8794,7 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="43">
+      <c r="C4" s="41">
         <v>0.74</v>
       </c>
       <c r="D4" s="20">
@@ -9435,7 +8809,7 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="41">
         <v>0.55000000000000004</v>
       </c>
       <c r="D5" s="20">
@@ -9450,7 +8824,7 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="44">
         <v>0.42699999999999999</v>
       </c>
       <c r="D6" s="20">
@@ -9468,55 +8842,55 @@
       <c r="C7" s="20">
         <v>0</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="39">
         <v>0.43469999999999998</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="39">
         <v>0.48149999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="11"/>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C8" s="20">
         <v>0</v>
       </c>
-      <c r="D8" s="40">
+      <c r="D8" s="39">
         <v>0.43469999999999998</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8" s="39">
         <v>0.48149999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C9" s="20">
         <v>0</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="39">
         <v>0.43469999999999998</v>
       </c>
-      <c r="E9" s="40">
+      <c r="E9" s="39">
         <v>0.48149999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C10" s="20">
         <v>0</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="39">
         <v>0.43469999999999998</v>
       </c>
-      <c r="E10" s="40">
+      <c r="E10" s="39">
         <v>0.48149999999999998</v>
       </c>
     </row>
@@ -9533,7 +8907,7 @@
       <c r="B13" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="52"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="20">
         <v>0</v>
       </c>
@@ -9545,7 +8919,7 @@
       <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="54"/>
+      <c r="C14" s="52"/>
       <c r="D14" s="20">
         <v>0</v>
       </c>
@@ -9557,7 +8931,7 @@
       <c r="B15" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="44">
+      <c r="C15" s="42">
         <v>0.31079999999999997</v>
       </c>
       <c r="D15" s="20">
@@ -9571,7 +8945,7 @@
       <c r="B16" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="42">
         <v>0.23100000000000001</v>
       </c>
       <c r="D16" s="20">
@@ -9585,7 +8959,7 @@
       <c r="B17" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="44">
+      <c r="C17" s="42">
         <v>0.17934</v>
       </c>
       <c r="D17" s="20">
@@ -9602,69 +8976,69 @@
       <c r="C18" s="20">
         <v>0</v>
       </c>
-      <c r="D18" s="40">
+      <c r="D18" s="39">
         <v>0.2238</v>
       </c>
-      <c r="E18" s="40">
+      <c r="E18" s="39">
         <v>0.23580000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="B19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C19" s="20">
         <v>0</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="39">
         <v>0.2238</v>
       </c>
-      <c r="E19" s="40">
+      <c r="E19" s="39">
         <v>0.23580000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C20" s="20">
         <v>0</v>
       </c>
-      <c r="D20" s="40">
+      <c r="D20" s="39">
         <v>0.2238</v>
       </c>
-      <c r="E20" s="40">
+      <c r="E20" s="39">
         <v>0.23580000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="B21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C21" s="20">
         <v>0</v>
       </c>
-      <c r="D21" s="40">
+      <c r="D21" s="39">
         <v>0.2238</v>
       </c>
-      <c r="E21" s="40">
+      <c r="E21" s="39">
         <v>0.23580000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B24" t="s">
-        <v>123</v>
-      </c>
-      <c r="C24" s="45">
+        <v>121</v>
+      </c>
+      <c r="C24" s="43">
         <v>0.01</v>
       </c>
-      <c r="D24" s="45">
-        <v>0</v>
-      </c>
-      <c r="E24" s="45">
+      <c r="D24" s="43">
+        <v>0</v>
+      </c>
+      <c r="E24" s="43">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
@@ -9993,7 +9367,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>64</v>
@@ -10034,9 +9408,9 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="B3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="50"/>
+        <v>122</v>
+      </c>
+      <c r="C3" s="48"/>
       <c r="D3" s="12">
         <v>1.53</v>
       </c>
@@ -11905,13 +11279,13 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B76" t="s">
         <v>106</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D76" s="4">
         <v>1</v>
@@ -11934,7 +11308,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="C77" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D77" s="4">
         <v>1</v>
@@ -11960,7 +11334,7 @@
         <v>107</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D78" s="4">
         <v>1</v>
@@ -11983,7 +11357,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="C79" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D79" s="4">
         <v>1</v>
@@ -12009,7 +11383,7 @@
         <v>108</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D80" s="4">
         <v>1</v>
@@ -12032,7 +11406,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="C81" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D81" s="4">
         <v>1</v>
@@ -12055,7 +11429,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B84" s="12" t="s">
         <v>73</v>
@@ -12153,10 +11527,10 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B90" t="s">
         <v>141</v>
-      </c>
-      <c r="B90" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -12177,7 +11551,7 @@
   </sheetPr>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -12216,7 +11590,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
         <v>69</v>
@@ -12257,7 +11631,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>56</v>
@@ -12320,7 +11694,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="B8" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -12340,7 +11714,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="B9" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -12380,7 +11754,7 @@
     </row>
     <row r="12" spans="1:7" ht="14">
       <c r="A12" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
updated spreadsheet to keep anemia intervention names consistent across tabs
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-69620" yWindow="-4220" windowWidth="26380" windowHeight="16040" tabRatio="500" firstSheet="10" activeTab="12"/>
+    <workbookView xWindow="-69620" yWindow="-4220" windowWidth="26380" windowHeight="16040" tabRatio="500" firstSheet="10" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -1161,7 +1161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="1">
+    <comment ref="E22" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1179,11 +1179,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-There is no unit cost for this to impact the budget.</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
-    <comment ref="E19" authorId="1">
+    <comment ref="F22" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1205,7 +1205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F19" authorId="1">
+    <comment ref="G22" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1227,7 +1227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G19" authorId="1">
+    <comment ref="H22" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1249,7 +1249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H19" authorId="1">
+    <comment ref="I22" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1268,292 +1268,6 @@
           </rPr>
           <t xml:space="preserve">
 Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I19" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E20" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F20" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G20" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H20" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I20" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E21" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F21" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G21" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H21" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I21" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C23" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D23" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
         </r>
       </text>
     </comment>
@@ -1575,7 +1289,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-At risk from malaria</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1597,7 +1311,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-At risk from malaria</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1619,7 +1333,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-At risk from malaria</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1641,11 +1355,275 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-At risk from malaria</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
     <comment ref="I23" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E24" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F24" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G24" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H24" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I24" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C26" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D26" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E26" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F26" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G26" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H26" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I26" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1849,7 +1827,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="172">
   <si>
     <t>year</t>
   </si>
@@ -2112,9 +2090,6 @@
     <t>Sprinkles</t>
   </si>
   <si>
-    <t>Public provision of complementary foods no iron</t>
-  </si>
-  <si>
     <t>Public provision of complementary foods with iron</t>
   </si>
   <si>
@@ -2127,18 +2102,6 @@
     <t>Long-lasting insecticide-treated bednets</t>
   </si>
   <si>
-    <t>IFAS for WRA school delivery</t>
-  </si>
-  <si>
-    <t>IFAS for WRA community-based delivery</t>
-  </si>
-  <si>
-    <t>IFAS for WRA hospital delivery</t>
-  </si>
-  <si>
-    <t>IFAS for WRA private retail</t>
-  </si>
-  <si>
     <t>General population</t>
   </si>
   <si>
@@ -2155,9 +2118,6 @@
   </si>
   <si>
     <t>Non-pregnant WRA</t>
-  </si>
-  <si>
-    <t>Intermittent preventive treatment in pregnancy</t>
   </si>
   <si>
     <t>All anemia</t>
@@ -2556,7 +2516,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="509">
+  <cellStyleXfs count="515">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2568,6 +2528,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3135,12 +3101,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="14" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3163,8 +3123,14 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="509">
+  <cellStyles count="515">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3419,6 +3385,9 @@
     <cellStyle name="Followed Hyperlink" xfId="504" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="506" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="508" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="510" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="512" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3672,6 +3641,9 @@
     <cellStyle name="Hyperlink" xfId="503" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="505" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="507" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="509" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="511" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -4990,13 +4962,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>64</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
@@ -5020,9 +4992,9 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="B4" s="34" t="s">
-        <v>150</v>
-      </c>
-      <c r="C4" s="57">
+        <v>144</v>
+      </c>
+      <c r="C4" s="55">
         <v>171684000</v>
       </c>
     </row>
@@ -5065,7 +5037,7 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1">
       <c r="A11" s="11" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B11" t="s">
         <v>81</v>
@@ -5076,7 +5048,7 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1">
       <c r="B12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C12" s="20">
         <v>0.13</v>
@@ -5084,7 +5056,7 @@
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1">
       <c r="B13" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C13" s="20">
         <v>25.36</v>
@@ -5092,7 +5064,7 @@
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1">
       <c r="B14" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C14" s="20">
         <v>25.4</v>
@@ -5100,7 +5072,7 @@
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1">
       <c r="B15" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C15" s="20">
         <v>34.68</v>
@@ -5108,7 +5080,7 @@
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1">
       <c r="B16" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C16" s="20">
         <v>39.32</v>
@@ -5125,31 +5097,31 @@
       <c r="B19" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="47">
+      <c r="C19" s="45">
         <v>0.3</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
       <c r="B20" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="C20" s="47">
+        <v>109</v>
+      </c>
+      <c r="C20" s="45">
         <v>0.8</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1">
       <c r="B21" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="C21" s="47">
+        <v>110</v>
+      </c>
+      <c r="C21" s="45">
         <v>0.12</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
       <c r="B22" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="C22" s="47">
+        <v>111</v>
+      </c>
+      <c r="C22" s="45">
         <v>0.05</v>
       </c>
     </row>
@@ -5157,7 +5129,7 @@
       <c r="B23" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="47">
+      <c r="C23" s="45">
         <v>0.05</v>
       </c>
     </row>
@@ -5166,75 +5138,75 @@
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="A26" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="B26" s="54" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="55">
+      <c r="C26" s="53">
         <v>8634000</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1">
-      <c r="B27" s="54" t="s">
-        <v>143</v>
-      </c>
-      <c r="C27" s="55">
+      <c r="B27" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" s="53">
         <v>13550000</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B28" s="54" t="s">
-        <v>144</v>
-      </c>
-      <c r="C28" s="55">
+      <c r="B28" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" s="53">
         <v>12394000</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B29" s="54" t="s">
-        <v>145</v>
-      </c>
-      <c r="C29" s="55">
+      <c r="B29" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="53">
         <v>9148000</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B30" s="54"/>
-      <c r="C30" s="56"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="54"/>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="A32" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="44">
+        <v>0.29978973218277538</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B33" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="B32" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="C32" s="46">
-        <v>0.29978973218277538</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B33" s="53" t="s">
-        <v>143</v>
-      </c>
-      <c r="C33" s="46">
+      <c r="C33" s="44">
         <v>0.52556568434139284</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B34" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="C34" s="46">
+      <c r="B34" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="C34" s="44">
         <v>0.16210210664201097</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B35" s="53" t="s">
-        <v>145</v>
-      </c>
-      <c r="C35" s="46">
+      <c r="B35" s="51" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="44">
         <v>1.2542476833820825E-2</v>
       </c>
     </row>
@@ -5326,10 +5298,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5345,7 +5317,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>47</v>
@@ -5369,7 +5341,7 @@
         <v>84</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J1" s="4"/>
     </row>
@@ -5456,7 +5428,7 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1">
       <c r="B5" s="4" t="s">
-        <v>87</v>
+        <v>171</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
@@ -5484,7 +5456,7 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -5595,7 +5567,7 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1">
       <c r="B11" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" s="3">
         <v>0</v>
@@ -5621,7 +5593,7 @@
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1">
       <c r="B12" t="s">
-        <v>102</v>
+        <v>160</v>
       </c>
       <c r="C12" s="3">
         <v>0</v>
@@ -5648,277 +5620,351 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B14" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1">
+      <c r="B15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1">
+      <c r="B16" t="s">
+        <v>166</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B18" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+      <c r="I18" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B19" t="s">
+        <v>169</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B20" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+      <c r="I20" s="60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A22" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3">
-        <v>0</v>
-      </c>
-      <c r="I14" s="38">
-        <f>'Demographic projections'!$J$2 * 'Baseline year demographics'!$C$6</f>
-        <v>6.9170848887586636E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B15" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0</v>
-      </c>
-      <c r="H15" s="3">
-        <v>0</v>
-      </c>
-      <c r="I15" s="31">
-        <f>'Baseline year demographics'!$C$7</f>
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B16" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0</v>
-      </c>
-      <c r="H16" s="3">
-        <v>0</v>
-      </c>
-      <c r="I16" s="31">
-        <f>'Baseline year demographics'!$C$7</f>
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B17" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0</v>
-      </c>
-      <c r="H17" s="3">
-        <v>0</v>
-      </c>
-      <c r="I17" s="37">
-        <f xml:space="preserve"> 1-'Baseline year demographics'!$C$7</f>
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A19" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0</v>
-      </c>
-      <c r="E19" s="36">
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="F19" s="36">
+      <c r="F22" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="G19" s="36">
+      <c r="G22" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="H19" s="36">
+      <c r="H22" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="I19" s="36">
+      <c r="I22" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B20" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0</v>
-      </c>
-      <c r="D20" s="3">
-        <v>0</v>
-      </c>
-      <c r="E20" s="3">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B23" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F23" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G23" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H23" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I23" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B21" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0</v>
-      </c>
-      <c r="E21" s="3">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B24" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F24" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G24" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H24" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I24" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B22" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C22" s="3">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0</v>
-      </c>
-      <c r="E22" s="36">
-        <v>1</v>
-      </c>
-      <c r="F22" s="36">
-        <v>1</v>
-      </c>
-      <c r="G22" s="36">
-        <v>1</v>
-      </c>
-      <c r="H22" s="36">
-        <v>1</v>
-      </c>
-      <c r="I22" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B23" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" s="36">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B25" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="36">
+        <v>1</v>
+      </c>
+      <c r="F25" s="36">
+        <v>1</v>
+      </c>
+      <c r="G25" s="36">
+        <v>1</v>
+      </c>
+      <c r="H25" s="36">
+        <v>1</v>
+      </c>
+      <c r="I25" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B26" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="D23" s="36">
+      <c r="D26" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="E23" s="36">
+      <c r="E26" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="F23" s="36">
+      <c r="F26" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="G23" s="36">
+      <c r="G26" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="H23" s="36">
+      <c r="H26" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="I23" s="36">
+      <c r="I26" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6046,15 +6092,15 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="47">
         <v>0.15</v>
       </c>
-      <c r="D6" s="49">
+      <c r="D6" s="47">
         <v>0.15</v>
       </c>
       <c r="E6" s="10">
@@ -6068,10 +6114,10 @@
       <c r="B7" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="49">
-        <v>1</v>
-      </c>
-      <c r="D7" s="49">
+      <c r="C7" s="47">
+        <v>1</v>
+      </c>
+      <c r="D7" s="47">
         <v>1</v>
       </c>
       <c r="E7" s="10">
@@ -6100,8 +6146,8 @@
   </sheetPr>
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -6133,28 +6179,28 @@
         <v>10</v>
       </c>
       <c r="H1" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="N1" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -6175,7 +6221,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="11" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B3" t="s">
         <v>60</v>
@@ -6222,7 +6268,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="B4" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -6266,7 +6312,7 @@
     </row>
     <row r="5" spans="1:15">
       <c r="B5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -6310,7 +6356,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="B6" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -6354,7 +6400,7 @@
     </row>
     <row r="7" spans="1:15">
       <c r="B7" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -6398,7 +6444,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="B8" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -6442,7 +6488,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="B9" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -6486,7 +6532,7 @@
     </row>
     <row r="10" spans="1:15">
       <c r="B10" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -6530,7 +6576,7 @@
     </row>
     <row r="11" spans="1:15">
       <c r="B11" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -6574,12 +6620,12 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="11" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="B14" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -6587,43 +6633,43 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" s="59">
+      <c r="E14" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="F14" s="59">
+      <c r="F14" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="G14" s="59">
+      <c r="G14" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="H14" s="59">
+      <c r="H14" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="I14" s="59">
+      <c r="I14" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="J14" s="59">
+      <c r="J14" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="K14" s="59">
+      <c r="K14" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="L14" s="59">
+      <c r="L14" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="M14" s="59">
+      <c r="M14" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="N14" s="59">
+      <c r="N14" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="O14" s="59">
+      <c r="O14" s="57">
         <v>0.97599999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="B15" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -6631,43 +6677,43 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="59">
+      <c r="E15" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="F15" s="59">
+      <c r="F15" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="G15" s="59">
+      <c r="G15" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="H15" s="59">
+      <c r="H15" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="I15" s="59">
+      <c r="I15" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="J15" s="59">
+      <c r="J15" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="K15" s="59">
+      <c r="K15" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="L15" s="59">
+      <c r="L15" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="M15" s="59">
+      <c r="M15" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="N15" s="59">
+      <c r="N15" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="O15" s="59">
+      <c r="O15" s="57">
         <v>0.97599999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="B16" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -6675,43 +6721,43 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16" s="59">
+      <c r="E16" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="F16" s="59">
+      <c r="F16" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="G16" s="59">
+      <c r="G16" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="H16" s="59">
+      <c r="H16" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="I16" s="59">
+      <c r="I16" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="J16" s="59">
+      <c r="J16" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="K16" s="59">
+      <c r="K16" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="L16" s="59">
+      <c r="L16" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="M16" s="59">
+      <c r="M16" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="N16" s="59">
+      <c r="N16" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="O16" s="59">
+      <c r="O16" s="57">
         <v>0.97599999999999998</v>
       </c>
     </row>
     <row r="17" spans="2:15">
       <c r="B17" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -6719,43 +6765,43 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17" s="60">
+      <c r="E17" s="58">
         <v>0.9</v>
       </c>
-      <c r="F17" s="60">
+      <c r="F17" s="58">
         <v>0.9</v>
       </c>
-      <c r="G17" s="60">
+      <c r="G17" s="58">
         <v>0.9</v>
       </c>
-      <c r="H17" s="60">
+      <c r="H17" s="58">
         <v>0.9</v>
       </c>
-      <c r="I17" s="60">
+      <c r="I17" s="58">
         <v>0.9</v>
       </c>
-      <c r="J17" s="60">
+      <c r="J17" s="58">
         <v>0.9</v>
       </c>
-      <c r="K17" s="60">
+      <c r="K17" s="58">
         <v>0.9</v>
       </c>
-      <c r="L17" s="60">
+      <c r="L17" s="58">
         <v>0.9</v>
       </c>
-      <c r="M17" s="60">
+      <c r="M17" s="58">
         <v>0.9</v>
       </c>
-      <c r="N17" s="60">
+      <c r="N17" s="58">
         <v>0.9</v>
       </c>
-      <c r="O17" s="60">
+      <c r="O17" s="58">
         <v>0.9</v>
       </c>
     </row>
     <row r="18" spans="2:15">
       <c r="B18" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -6763,43 +6809,43 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18" s="59">
-        <v>1</v>
-      </c>
-      <c r="F18" s="59">
-        <v>1</v>
-      </c>
-      <c r="G18" s="60">
+      <c r="E18" s="57">
+        <v>1</v>
+      </c>
+      <c r="F18" s="57">
+        <v>1</v>
+      </c>
+      <c r="G18" s="58">
         <v>0.8</v>
       </c>
-      <c r="H18" s="59">
-        <v>1</v>
-      </c>
-      <c r="I18" s="59">
-        <v>1</v>
-      </c>
-      <c r="J18" s="59">
-        <v>1</v>
-      </c>
-      <c r="K18" s="59">
-        <v>1</v>
-      </c>
-      <c r="L18" s="59">
-        <v>1</v>
-      </c>
-      <c r="M18" s="59">
-        <v>1</v>
-      </c>
-      <c r="N18" s="59">
-        <v>1</v>
-      </c>
-      <c r="O18" s="59">
+      <c r="H18" s="57">
+        <v>1</v>
+      </c>
+      <c r="I18" s="57">
+        <v>1</v>
+      </c>
+      <c r="J18" s="57">
+        <v>1</v>
+      </c>
+      <c r="K18" s="57">
+        <v>1</v>
+      </c>
+      <c r="L18" s="57">
+        <v>1</v>
+      </c>
+      <c r="M18" s="57">
+        <v>1</v>
+      </c>
+      <c r="N18" s="57">
+        <v>1</v>
+      </c>
+      <c r="O18" s="57">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:15">
       <c r="B19" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -6807,37 +6853,37 @@
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="E19" s="59">
-        <v>1</v>
-      </c>
-      <c r="F19" s="59">
-        <v>1</v>
-      </c>
-      <c r="G19" s="59">
-        <v>1</v>
-      </c>
-      <c r="H19" s="59">
-        <v>1</v>
-      </c>
-      <c r="I19" s="59">
-        <v>1</v>
-      </c>
-      <c r="J19" s="59">
-        <v>1</v>
-      </c>
-      <c r="K19" s="59">
-        <v>1</v>
-      </c>
-      <c r="L19" s="60">
+      <c r="E19" s="57">
+        <v>1</v>
+      </c>
+      <c r="F19" s="57">
+        <v>1</v>
+      </c>
+      <c r="G19" s="57">
+        <v>1</v>
+      </c>
+      <c r="H19" s="57">
+        <v>1</v>
+      </c>
+      <c r="I19" s="57">
+        <v>1</v>
+      </c>
+      <c r="J19" s="57">
+        <v>1</v>
+      </c>
+      <c r="K19" s="57">
+        <v>1</v>
+      </c>
+      <c r="L19" s="58">
         <v>0.9</v>
       </c>
-      <c r="M19" s="60">
+      <c r="M19" s="58">
         <v>0.9</v>
       </c>
-      <c r="N19" s="60">
+      <c r="N19" s="58">
         <v>0.9</v>
       </c>
-      <c r="O19" s="60">
+      <c r="O19" s="58">
         <v>0.9</v>
       </c>
     </row>
@@ -6921,7 +6967,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
@@ -7002,7 +7048,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -7018,13 +7064,13 @@
         <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
@@ -7080,7 +7126,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B5" s="15">
         <v>0</v>
@@ -7097,7 +7143,7 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="35"/>
       <c r="C6" s="35"/>
@@ -7153,7 +7199,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="35"/>
@@ -7164,7 +7210,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="35"/>
@@ -7175,7 +7221,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="35"/>
@@ -7186,7 +7232,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="35"/>
@@ -7197,7 +7243,7 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="35"/>
@@ -7208,7 +7254,7 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="35"/>
@@ -7219,7 +7265,7 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="35"/>
@@ -7227,7 +7273,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1">
       <c r="A17" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="35"/>
@@ -7235,7 +7281,7 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="A18" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -7243,7 +7289,7 @@
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -7251,7 +7297,7 @@
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -7259,7 +7305,7 @@
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -7267,7 +7313,7 @@
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -7275,7 +7321,7 @@
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -7350,13 +7396,13 @@
         <v>67</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>68</v>
@@ -7368,10 +7414,10 @@
         <v>77</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1">
@@ -7412,7 +7458,7 @@
         <f>H2-I2</f>
         <v>41058509.531465083</v>
       </c>
-      <c r="L2" s="58">
+      <c r="L2" s="56">
         <v>173766200</v>
       </c>
     </row>
@@ -7454,7 +7500,7 @@
         <f t="shared" ref="K3:K15" si="3">H3-I3</f>
         <v>42070162.3670066</v>
       </c>
-      <c r="L3" s="58">
+      <c r="L3" s="56">
         <v>175848400</v>
       </c>
     </row>
@@ -7496,7 +7542,7 @@
         <f t="shared" si="3"/>
         <v>43083946.257598445</v>
       </c>
-      <c r="L4" s="58">
+      <c r="L4" s="56">
         <v>177930600</v>
       </c>
     </row>
@@ -7538,7 +7584,7 @@
         <f t="shared" si="3"/>
         <v>44100038.10321714</v>
       </c>
-      <c r="L5" s="58">
+      <c r="L5" s="56">
         <v>180012800</v>
       </c>
     </row>
@@ -7580,7 +7626,7 @@
         <f t="shared" si="3"/>
         <v>45114495.393052891</v>
       </c>
-      <c r="L6" s="58">
+      <c r="L6" s="56">
         <v>182095000</v>
       </c>
     </row>
@@ -7622,7 +7668,7 @@
         <f t="shared" si="3"/>
         <v>45617945.306584187</v>
       </c>
-      <c r="L7" s="58">
+      <c r="L7" s="56">
         <v>183822800</v>
       </c>
     </row>
@@ -7664,7 +7710,7 @@
         <f t="shared" si="3"/>
         <v>46123716.147807248</v>
       </c>
-      <c r="L8" s="58">
+      <c r="L8" s="56">
         <v>185550600</v>
       </c>
     </row>
@@ -7706,7 +7752,7 @@
         <f t="shared" si="3"/>
         <v>46631712.390734792</v>
       </c>
-      <c r="L9" s="58">
+      <c r="L9" s="56">
         <v>187278400</v>
       </c>
     </row>
@@ -7748,7 +7794,7 @@
         <f t="shared" si="3"/>
         <v>47141901.014037848</v>
       </c>
-      <c r="L10" s="58">
+      <c r="L10" s="56">
         <v>189006200</v>
       </c>
     </row>
@@ -7790,7 +7836,7 @@
         <f t="shared" si="3"/>
         <v>47645743.645516977</v>
       </c>
-      <c r="L11" s="58">
+      <c r="L11" s="56">
         <v>190734000</v>
       </c>
     </row>
@@ -7832,7 +7878,7 @@
         <f t="shared" si="3"/>
         <v>48024732.420057721</v>
       </c>
-      <c r="L12" s="58">
+      <c r="L12" s="56">
         <v>192287600</v>
       </c>
     </row>
@@ -7874,7 +7920,7 @@
         <f t="shared" si="3"/>
         <v>48405730.778331593</v>
       </c>
-      <c r="L13" s="58">
+      <c r="L13" s="56">
         <v>193841200</v>
       </c>
     </row>
@@ -7916,7 +7962,7 @@
         <f t="shared" si="3"/>
         <v>48788684.471012466</v>
       </c>
-      <c r="L14" s="58">
+      <c r="L14" s="56">
         <v>195394800</v>
       </c>
     </row>
@@ -7958,7 +8004,7 @@
         <f t="shared" si="3"/>
         <v>49173572.270103149</v>
       </c>
-      <c r="L15" s="58">
+      <c r="L15" s="56">
         <v>196948400</v>
       </c>
     </row>
@@ -8403,7 +8449,7 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B19" s="20">
         <v>0</v>
@@ -8420,13 +8466,13 @@
       <c r="F19" s="20">
         <v>0</v>
       </c>
-      <c r="G19" s="40">
+      <c r="G19" s="38">
         <v>2.5899999999999999E-2</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B20" s="20">
         <v>0</v>
@@ -8443,13 +8489,13 @@
       <c r="F20" s="20">
         <v>0</v>
       </c>
-      <c r="G20" s="40">
+      <c r="G20" s="38">
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B21" s="20">
         <v>0</v>
@@ -8466,13 +8512,13 @@
       <c r="F21" s="20">
         <v>0</v>
       </c>
-      <c r="G21" s="40">
+      <c r="G21" s="38">
         <v>0.25590000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B22" s="20">
         <v>0</v>
@@ -8489,13 +8535,13 @@
       <c r="F22" s="20">
         <v>0</v>
       </c>
-      <c r="G22" s="40">
+      <c r="G22" s="38">
         <v>0.1464</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B23" s="20">
         <v>0</v>
@@ -8512,13 +8558,13 @@
       <c r="F23" s="20">
         <v>0</v>
       </c>
-      <c r="G23" s="40">
+      <c r="G23" s="38">
         <v>1.7600000000000001E-2</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B24" s="20">
         <v>0</v>
@@ -8535,13 +8581,13 @@
       <c r="F24" s="20">
         <v>0</v>
       </c>
-      <c r="G24" s="40">
+      <c r="G24" s="38">
         <v>1.8100000000000002E-2</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B25" s="20">
         <v>0</v>
@@ -8558,13 +8604,13 @@
       <c r="F25" s="20">
         <v>0</v>
       </c>
-      <c r="G25" s="40">
+      <c r="G25" s="38">
         <v>1.14E-2</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B26" s="20">
         <v>0</v>
@@ -8581,13 +8627,13 @@
       <c r="F26" s="20">
         <v>0</v>
       </c>
-      <c r="G26" s="40">
+      <c r="G26" s="38">
         <v>0.15129999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B27" s="20">
         <v>0</v>
@@ -8604,7 +8650,7 @@
       <c r="F27" s="20">
         <v>0</v>
       </c>
-      <c r="G27" s="40">
+      <c r="G27" s="38">
         <v>0.36630000000000001</v>
       </c>
     </row>
@@ -8675,7 +8721,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B3" s="35">
         <v>5.1999999999999998E-2</v>
@@ -8746,7 +8792,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="11" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>82</v>
@@ -8755,7 +8801,7 @@
         <v>83</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>84</v>
@@ -8763,12 +8809,12 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="11" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="50"/>
+      <c r="C2" s="48"/>
       <c r="D2" s="20">
         <v>0</v>
       </c>
@@ -8781,7 +8827,7 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="51"/>
+      <c r="C3" s="49"/>
       <c r="D3" s="20">
         <v>0</v>
       </c>
@@ -8794,7 +8840,7 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="39">
         <v>0.74</v>
       </c>
       <c r="D4" s="20">
@@ -8809,7 +8855,7 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="39">
         <v>0.55000000000000004</v>
       </c>
       <c r="D5" s="20">
@@ -8824,7 +8870,7 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="44">
+      <c r="C6" s="42">
         <v>0.42699999999999999</v>
       </c>
       <c r="D6" s="20">
@@ -8842,55 +8888,55 @@
       <c r="C7" s="20">
         <v>0</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D7" s="37">
         <v>0.43469999999999998</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="37">
         <v>0.48149999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="11"/>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C8" s="20">
         <v>0</v>
       </c>
-      <c r="D8" s="39">
+      <c r="D8" s="37">
         <v>0.43469999999999998</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="37">
         <v>0.48149999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C9" s="20">
         <v>0</v>
       </c>
-      <c r="D9" s="39">
+      <c r="D9" s="37">
         <v>0.43469999999999998</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="37">
         <v>0.48149999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C10" s="20">
         <v>0</v>
       </c>
-      <c r="D10" s="39">
+      <c r="D10" s="37">
         <v>0.43469999999999998</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="37">
         <v>0.48149999999999998</v>
       </c>
     </row>
@@ -8902,12 +8948,12 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="50"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="20">
         <v>0</v>
       </c>
@@ -8919,7 +8965,7 @@
       <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="52"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="20">
         <v>0</v>
       </c>
@@ -8931,7 +8977,7 @@
       <c r="B15" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="42">
+      <c r="C15" s="40">
         <v>0.31079999999999997</v>
       </c>
       <c r="D15" s="20">
@@ -8945,7 +8991,7 @@
       <c r="B16" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="42">
+      <c r="C16" s="40">
         <v>0.23100000000000001</v>
       </c>
       <c r="D16" s="20">
@@ -8959,7 +9005,7 @@
       <c r="B17" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="42">
+      <c r="C17" s="40">
         <v>0.17934</v>
       </c>
       <c r="D17" s="20">
@@ -8976,69 +9022,69 @@
       <c r="C18" s="20">
         <v>0</v>
       </c>
-      <c r="D18" s="39">
+      <c r="D18" s="37">
         <v>0.2238</v>
       </c>
-      <c r="E18" s="39">
+      <c r="E18" s="37">
         <v>0.23580000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="B19" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C19" s="20">
         <v>0</v>
       </c>
-      <c r="D19" s="39">
+      <c r="D19" s="37">
         <v>0.2238</v>
       </c>
-      <c r="E19" s="39">
+      <c r="E19" s="37">
         <v>0.23580000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C20" s="20">
         <v>0</v>
       </c>
-      <c r="D20" s="39">
+      <c r="D20" s="37">
         <v>0.2238</v>
       </c>
-      <c r="E20" s="39">
+      <c r="E20" s="37">
         <v>0.23580000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="B21" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C21" s="20">
         <v>0</v>
       </c>
-      <c r="D21" s="39">
+      <c r="D21" s="37">
         <v>0.2238</v>
       </c>
-      <c r="E21" s="39">
+      <c r="E21" s="37">
         <v>0.23580000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="11" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B24" t="s">
-        <v>121</v>
-      </c>
-      <c r="C24" s="43">
+        <v>115</v>
+      </c>
+      <c r="C24" s="41">
         <v>0.01</v>
       </c>
-      <c r="D24" s="43">
-        <v>0</v>
-      </c>
-      <c r="E24" s="43">
+      <c r="D24" s="41">
+        <v>0</v>
+      </c>
+      <c r="E24" s="41">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
@@ -9367,7 +9413,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>64</v>
@@ -9408,9 +9454,9 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="B3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C3" s="48"/>
+        <v>116</v>
+      </c>
+      <c r="C3" s="46"/>
       <c r="D3" s="12">
         <v>1.53</v>
       </c>
@@ -11279,13 +11325,13 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="11" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B76" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D76" s="4">
         <v>1</v>
@@ -11308,7 +11354,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="C77" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D77" s="4">
         <v>1</v>
@@ -11331,10 +11377,10 @@
     </row>
     <row r="78" spans="1:9">
       <c r="B78" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D78" s="4">
         <v>1</v>
@@ -11357,7 +11403,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="C79" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D79" s="4">
         <v>1</v>
@@ -11380,10 +11426,10 @@
     </row>
     <row r="80" spans="1:9">
       <c r="B80" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D80" s="4">
         <v>1</v>
@@ -11406,7 +11452,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="C81" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D81" s="4">
         <v>1</v>
@@ -11429,7 +11475,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="11" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B84" s="12" t="s">
         <v>73</v>
@@ -11527,10 +11573,10 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="11" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B90" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -11590,7 +11636,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="11" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
         <v>69</v>
@@ -11631,7 +11677,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="11" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>56</v>
@@ -11694,7 +11740,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="B8" s="4" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -11714,7 +11760,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="B9" s="4" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -11754,7 +11800,7 @@
     </row>
     <row r="12" spans="1:7" ht="14">
       <c r="A12" s="11" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
Fixed typo in spreadsheet
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Bangladesh/2017Aug/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-69620" yWindow="-4220" windowWidth="26380" windowHeight="16040" tabRatio="500" firstSheet="10" activeTab="10"/>
+    <workbookView xWindow="-34100" yWindow="-20540" windowWidth="25460" windowHeight="20540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -23,13 +28,13 @@
     <sheet name="Interventions for children" sheetId="28" r:id="rId14"/>
     <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -2030,9 +2035,6 @@
     <t>children under 5</t>
   </si>
   <si>
-    <t>women 15-19</t>
-  </si>
-  <si>
     <t>total WRA</t>
   </si>
   <si>
@@ -2343,6 +2345,9 @@
   </si>
   <si>
     <t>Public provision of complementary foods</t>
+  </si>
+  <si>
+    <t>women 15-19 years</t>
   </si>
 </sst>
 </file>
@@ -4954,24 +4959,24 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" customHeight="1">
+    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>64</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>65</v>
       </c>
@@ -4982,7 +4987,7 @@
         <v>15204000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
@@ -4990,15 +4995,15 @@
         <v>3118117</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C4" s="55">
         <v>171684000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
@@ -5007,204 +5012,204 @@
         <v>3677298.8269880489</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="20">
         <v>0.35199999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="18">
         <v>0.36</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" s="20">
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="11"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" s="20">
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C12" s="20">
         <v>0.13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C13" s="20">
         <v>25.36</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C14" s="20">
         <v>25.4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C15" s="20">
         <v>34.68</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" s="20">
         <v>39.32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="11"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" s="45">
         <v>0.3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C20" s="45">
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" s="45">
         <v>0.12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C22" s="45">
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" s="45">
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="34"/>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B26" s="52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26" s="53">
         <v>8634000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="52" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C27" s="53">
         <v>13550000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="52" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C28" s="53">
         <v>12394000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="52" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C29" s="53">
         <v>9148000</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="52"/>
       <c r="C30" s="54"/>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B32" s="43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C32" s="44">
         <v>0.29978973218277538</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="15.75" customHeight="1">
+    <row r="33" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C33" s="44">
         <v>0.52556568434139284</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="15.75" customHeight="1">
+    <row r="34" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C34" s="44">
         <v>0.16210210664201097</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="15.75" customHeight="1">
+    <row r="35" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C35" s="44">
         <v>1.2542476833820825E-2</v>
@@ -5214,11 +5219,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5233,12 +5233,12 @@
       <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
@@ -5272,14 +5272,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -5288,11 +5288,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5300,11 +5295,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D16" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="43.33203125" customWidth="1"/>
@@ -5315,9 +5310,9 @@
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>47</v>
@@ -5338,16 +5333,16 @@
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>57</v>
@@ -5374,7 +5369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
         <v>51</v>
       </c>
@@ -5400,7 +5395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4" t="s">
         <v>58</v>
       </c>
@@ -5426,9 +5421,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
@@ -5454,9 +5449,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -5482,9 +5477,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" s="3">
         <v>0</v>
@@ -5509,9 +5504,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
         <v>59</v>
@@ -5539,7 +5534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>60</v>
       </c>
@@ -5565,9 +5560,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C11" s="3">
         <v>0</v>
@@ -5591,9 +5586,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C12" s="3">
         <v>0</v>
@@ -5618,169 +5613,169 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" t="s">
         <v>164</v>
       </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3">
-        <v>0</v>
-      </c>
-      <c r="I14" s="59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B15" t="s">
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" t="s">
         <v>165</v>
       </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0</v>
-      </c>
-      <c r="H15" s="3">
-        <v>0</v>
-      </c>
-      <c r="I15" s="59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B16" t="s">
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
         <v>166</v>
       </c>
-      <c r="C16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0</v>
-      </c>
-      <c r="H16" s="3">
-        <v>0</v>
-      </c>
-      <c r="I16" s="59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B17" t="s">
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" t="s">
         <v>167</v>
       </c>
-      <c r="C17" s="3">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0</v>
-      </c>
-      <c r="H17" s="3">
-        <v>0</v>
-      </c>
-      <c r="I17" s="59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B18" t="s">
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+      <c r="I18" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" t="s">
         <v>168</v>
       </c>
-      <c r="C18" s="3">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3">
-        <v>0</v>
-      </c>
-      <c r="I18" s="59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B19" t="s">
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" t="s">
         <v>169</v>
       </c>
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0</v>
-      </c>
-      <c r="E19" s="3">
-        <v>0</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0</v>
-      </c>
-      <c r="H19" s="3">
-        <v>0</v>
-      </c>
-      <c r="I19" s="59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B20" t="s">
-        <v>170</v>
-      </c>
       <c r="C20" s="3">
         <v>0</v>
       </c>
@@ -5803,16 +5798,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
@@ -5841,9 +5836,9 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
@@ -5872,9 +5867,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
@@ -5903,9 +5898,9 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C25" s="3">
         <v>0</v>
@@ -5929,9 +5924,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C26" s="36">
         <f>'Baseline year demographics'!$C$8</f>
@@ -5962,7 +5957,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
     </row>
@@ -5970,11 +5965,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5989,14 +5979,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -6016,7 +6006,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -6036,7 +6026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>55</v>
       </c>
@@ -6053,7 +6043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -6073,7 +6063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>55</v>
       </c>
@@ -6090,9 +6080,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B6" t="s">
         <v>53</v>
@@ -6110,7 +6100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>55</v>
       </c>
@@ -6131,11 +6121,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6150,7 +6135,7 @@
       <selection activeCell="B5" sqref="B5:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="42.6640625" customWidth="1"/>
@@ -6159,7 +6144,7 @@
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B1" s="11" t="s">
         <v>47</v>
       </c>
@@ -6179,31 +6164,31 @@
         <v>10</v>
       </c>
       <c r="H1" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="O1" s="11" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -6219,9 +6204,9 @@
       <c r="N2" s="11"/>
       <c r="O2" s="11"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s">
         <v>60</v>
@@ -6266,9 +6251,9 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -6310,9 +6295,9 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -6354,9 +6339,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -6398,9 +6383,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -6442,9 +6427,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -6486,9 +6471,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -6530,9 +6515,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -6574,9 +6559,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -6618,14 +6603,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13" s="11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B14" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -6667,9 +6652,9 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B15" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -6711,9 +6696,9 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B16" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -6755,9 +6740,9 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="17" spans="2:15">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B17" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -6799,9 +6784,9 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="18" spans="2:15">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -6843,9 +6828,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:15">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B19" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -6887,28 +6872,23 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="31" spans="2:15"/>
-    <row r="32" spans="2:15">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.15"/>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="2:2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="2:2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B35" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6923,7 +6903,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="27.5" customWidth="1"/>
     <col min="3" max="3" width="38.1640625" customWidth="1"/>
@@ -6933,7 +6913,7 @@
     <col min="8" max="8" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -6959,7 +6939,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>51</v>
       </c>
@@ -6967,7 +6947,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
@@ -6985,9 +6965,9 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -7005,11 +6985,11 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
@@ -7027,7 +7007,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -7035,11 +7015,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7051,7 +7026,7 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="43.83203125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -7059,21 +7034,21 @@
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
@@ -7090,7 +7065,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>51</v>
       </c>
@@ -7107,7 +7082,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>58</v>
       </c>
@@ -7124,9 +7099,9 @@
       <c r="F4" s="9"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B5" s="15">
         <v>0</v>
@@ -7141,9 +7116,9 @@
       <c r="F5" s="9"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="35"/>
       <c r="C6" s="35"/>
@@ -7152,9 +7127,9 @@
       <c r="F6" s="9"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="35"/>
       <c r="C7" s="35"/>
@@ -7163,7 +7138,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -7180,7 +7155,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -7197,9 +7172,9 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="35"/>
@@ -7208,9 +7183,9 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="35"/>
@@ -7219,9 +7194,9 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="35"/>
@@ -7230,9 +7205,9 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="35"/>
@@ -7241,9 +7216,9 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="35"/>
@@ -7252,9 +7227,9 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="35"/>
@@ -7263,91 +7238,91 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="35"/>
       <c r="D16" s="14"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="35"/>
       <c r="D17" s="14"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="35"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="35"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="35"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="35"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="35"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
       <c r="D23" s="35"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1">
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
     </row>
@@ -7355,11 +7330,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7370,11 +7340,11 @@
   </sheetPr>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
@@ -7382,7 +7352,7 @@
     <col min="11" max="11" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7393,34 +7363,34 @@
         <v>66</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>67</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>68</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>54</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>2017</v>
       </c>
@@ -7462,7 +7432,7 @@
         <v>173766200</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>2018</v>
       </c>
@@ -7504,7 +7474,7 @@
         <v>175848400</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>2019</v>
       </c>
@@ -7546,7 +7516,7 @@
         <v>177930600</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>2020</v>
       </c>
@@ -7588,7 +7558,7 @@
         <v>180012800</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>2021</v>
       </c>
@@ -7630,7 +7600,7 @@
         <v>182095000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>2022</v>
       </c>
@@ -7672,7 +7642,7 @@
         <v>183822800</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>2023</v>
       </c>
@@ -7714,7 +7684,7 @@
         <v>185550600</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>2024</v>
       </c>
@@ -7756,7 +7726,7 @@
         <v>187278400</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>2025</v>
       </c>
@@ -7798,7 +7768,7 @@
         <v>189006200</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>2026</v>
       </c>
@@ -7840,7 +7810,7 @@
         <v>190734000</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>2027</v>
       </c>
@@ -7882,7 +7852,7 @@
         <v>192287600</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>2028</v>
       </c>
@@ -7924,7 +7894,7 @@
         <v>193841200</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>2029</v>
       </c>
@@ -7966,7 +7936,7 @@
         <v>195394800</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>2030</v>
       </c>
@@ -8012,11 +7982,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8028,12 +7993,12 @@
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -8053,10 +8018,10 @@
         <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -8079,7 +8044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -8102,7 +8067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -8125,7 +8090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -8148,7 +8113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -8171,7 +8136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -8194,7 +8159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -8217,7 +8182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -8240,7 +8205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -8263,7 +8228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -8286,7 +8251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -8309,7 +8274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -8332,7 +8297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -8355,7 +8320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -8378,7 +8343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -8401,7 +8366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -8424,7 +8389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -8447,9 +8412,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19" s="20">
         <v>0</v>
@@ -8470,9 +8435,9 @@
         <v>2.5899999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20" s="20">
         <v>0</v>
@@ -8493,9 +8458,9 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B21" s="20">
         <v>0</v>
@@ -8516,9 +8481,9 @@
         <v>0.25590000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B22" s="20">
         <v>0</v>
@@ -8539,9 +8504,9 @@
         <v>0.1464</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B23" s="20">
         <v>0</v>
@@ -8562,9 +8527,9 @@
         <v>1.7600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B24" s="20">
         <v>0</v>
@@ -8585,9 +8550,9 @@
         <v>1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B25" s="20">
         <v>0</v>
@@ -8608,9 +8573,9 @@
         <v>1.14E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B26" s="20">
         <v>0</v>
@@ -8631,9 +8596,9 @@
         <v>0.15129999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B27" s="20">
         <v>0</v>
@@ -8661,11 +8626,6 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8677,9 +8637,9 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
@@ -8699,7 +8659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>29</v>
       </c>
@@ -8719,9 +8679,9 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" s="35">
         <v>5.1999999999999998E-2</v>
@@ -8739,7 +8699,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
@@ -8762,11 +8722,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8781,7 +8736,7 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
@@ -8790,26 +8745,26 @@
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -8822,7 +8777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="11"/>
       <c r="B3" t="s">
         <v>7</v>
@@ -8835,7 +8790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="11"/>
       <c r="B4" t="s">
         <v>8</v>
@@ -8850,7 +8805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="11"/>
       <c r="B5" t="s">
         <v>9</v>
@@ -8865,7 +8820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="11"/>
       <c r="B6" t="s">
         <v>10</v>
@@ -8880,10 +8835,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="11"/>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" s="20">
         <v>0</v>
@@ -8895,10 +8850,10 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="11"/>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C8" s="20">
         <v>0</v>
@@ -8910,10 +8865,10 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C9" s="20">
         <v>0</v>
@@ -8925,10 +8880,10 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C10" s="20">
         <v>0</v>
@@ -8940,15 +8895,15 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="11"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="11"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -8961,7 +8916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -8973,7 +8928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -8987,7 +8942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>9</v>
       </c>
@@ -9001,7 +8956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -9015,9 +8970,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C18" s="20">
         <v>0</v>
@@ -9029,9 +8984,9 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C19" s="20">
         <v>0</v>
@@ -9043,9 +8998,9 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C20" s="20">
         <v>0</v>
@@ -9057,9 +9012,9 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C21" s="20">
         <v>0</v>
@@ -9071,12 +9026,12 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" t="s">
         <v>114</v>
-      </c>
-      <c r="B24" t="s">
-        <v>115</v>
       </c>
       <c r="C24" s="41">
         <v>0.01</v>
@@ -9092,11 +9047,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9108,9 +9058,9 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -9133,7 +9083,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
@@ -9156,7 +9106,7 @@
         <v>25.35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
         <v>24</v>
@@ -9177,7 +9127,7 @@
         <v>33.25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="12"/>
       <c r="B4" s="13" t="s">
         <v>27</v>
@@ -9198,7 +9148,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="12"/>
       <c r="B5" s="13" t="s">
         <v>28</v>
@@ -9219,7 +9169,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
@@ -9242,7 +9192,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
@@ -9262,7 +9212,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
@@ -9282,7 +9232,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
@@ -9302,7 +9252,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
@@ -9325,7 +9275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
@@ -9345,7 +9295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="4" t="s">
         <v>42</v>
       </c>
@@ -9365,7 +9315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="4" t="s">
         <v>43</v>
       </c>
@@ -9390,11 +9340,6 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9406,14 +9351,14 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>64</v>
@@ -9431,7 +9376,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
         <v>12</v>
       </c>
@@ -9452,9 +9397,9 @@
         <v>3.1128200000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" s="46"/>
       <c r="D3" s="12">
@@ -9467,7 +9412,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>63</v>
       </c>
@@ -9484,14 +9429,14 @@
         <v>46.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="11"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="11"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="11" t="s">
         <v>5</v>
       </c>
@@ -9500,7 +9445,7 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
         <v>61</v>
       </c>
@@ -9520,7 +9465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
@@ -9537,7 +9482,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
@@ -9554,7 +9499,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
@@ -9571,7 +9516,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
@@ -9588,7 +9533,7 @@
         <v>999.99</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
@@ -9605,7 +9550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>46</v>
       </c>
@@ -9622,7 +9567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
@@ -9643,11 +9588,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9662,7 +9602,7 @@
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
@@ -9670,7 +9610,7 @@
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>61</v>
       </c>
@@ -9696,10 +9636,10 @@
         <v>10</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
@@ -9728,7 +9668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
@@ -9751,7 +9691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C4" s="4" t="s">
         <v>27</v>
       </c>
@@ -9774,7 +9714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
@@ -9797,7 +9737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>31</v>
       </c>
@@ -9823,7 +9763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
@@ -9846,7 +9786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C8" s="4" t="s">
         <v>27</v>
       </c>
@@ -9869,7 +9809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C9" s="4" t="s">
         <v>28</v>
       </c>
@@ -9892,7 +9832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>33</v>
       </c>
@@ -9918,7 +9858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
@@ -9941,7 +9881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C12" s="4" t="s">
         <v>27</v>
       </c>
@@ -9964,7 +9904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
@@ -9987,7 +9927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>34</v>
       </c>
@@ -10013,7 +9953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
@@ -10036,7 +9976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C16" s="4" t="s">
         <v>27</v>
       </c>
@@ -10059,7 +9999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C17" s="4" t="s">
         <v>28</v>
       </c>
@@ -10082,7 +10022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>38</v>
       </c>
@@ -10108,7 +10048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C19" s="4" t="s">
         <v>24</v>
       </c>
@@ -10131,7 +10071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C20" s="4" t="s">
         <v>27</v>
       </c>
@@ -10154,7 +10094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C21" s="4" t="s">
         <v>28</v>
       </c>
@@ -10177,7 +10117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="11" t="s">
         <v>30</v>
       </c>
@@ -10206,7 +10146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C25" s="4" t="s">
         <v>24</v>
       </c>
@@ -10229,7 +10169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C26" s="4" t="s">
         <v>27</v>
       </c>
@@ -10252,7 +10192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C27" s="4" t="s">
         <v>28</v>
       </c>
@@ -10275,7 +10215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
         <v>31</v>
       </c>
@@ -10301,7 +10241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C29" s="4" t="s">
         <v>24</v>
       </c>
@@ -10324,7 +10264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C30" s="4" t="s">
         <v>27</v>
       </c>
@@ -10347,7 +10287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C31" s="4" t="s">
         <v>28</v>
       </c>
@@ -10370,7 +10310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>33</v>
       </c>
@@ -10396,7 +10336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C33" s="4" t="s">
         <v>24</v>
       </c>
@@ -10419,7 +10359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C34" s="4" t="s">
         <v>27</v>
       </c>
@@ -10442,7 +10382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C35" s="4" t="s">
         <v>28</v>
       </c>
@@ -10465,7 +10405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B36" t="s">
         <v>34</v>
       </c>
@@ -10491,7 +10431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C37" s="4" t="s">
         <v>24</v>
       </c>
@@ -10514,7 +10454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C38" s="4" t="s">
         <v>27</v>
       </c>
@@ -10537,7 +10477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C39" s="4" t="s">
         <v>28</v>
       </c>
@@ -10560,7 +10500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B40" t="s">
         <v>38</v>
       </c>
@@ -10586,7 +10526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C41" s="4" t="s">
         <v>24</v>
       </c>
@@ -10609,7 +10549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C42" s="4" t="s">
         <v>27</v>
       </c>
@@ -10632,7 +10572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C43" s="4" t="s">
         <v>28</v>
       </c>
@@ -10655,7 +10595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="11" t="s">
         <v>39</v>
       </c>
@@ -10684,7 +10624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C47" s="4" t="s">
         <v>41</v>
       </c>
@@ -10707,7 +10647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C48" s="4" t="s">
         <v>42</v>
       </c>
@@ -10730,7 +10670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:9">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C49" s="4" t="s">
         <v>43</v>
       </c>
@@ -10753,7 +10693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:9">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B50" t="s">
         <v>16</v>
       </c>
@@ -10779,7 +10719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:9">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C51" s="4" t="s">
         <v>41</v>
       </c>
@@ -10802,7 +10742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:9">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C52" s="4" t="s">
         <v>42</v>
       </c>
@@ -10825,7 +10765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:9">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C53" s="4" t="s">
         <v>43</v>
       </c>
@@ -10848,7 +10788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:9">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B54" t="s">
         <v>17</v>
       </c>
@@ -10874,7 +10814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:9">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C55" s="4" t="s">
         <v>41</v>
       </c>
@@ -10897,7 +10837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:9">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C56" s="4" t="s">
         <v>42</v>
       </c>
@@ -10920,7 +10860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:9">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C57" s="4" t="s">
         <v>43</v>
       </c>
@@ -10943,7 +10883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:9">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B58" t="s">
         <v>22</v>
       </c>
@@ -10969,7 +10909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:9">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C59" s="4" t="s">
         <v>41</v>
       </c>
@@ -10992,7 +10932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:9">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C60" s="4" t="s">
         <v>42</v>
       </c>
@@ -11015,7 +10955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:9">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C61" s="4" t="s">
         <v>43</v>
       </c>
@@ -11038,7 +10978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:9">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B62" t="s">
         <v>29</v>
       </c>
@@ -11064,7 +11004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:9">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C63" s="4" t="s">
         <v>41</v>
       </c>
@@ -11087,7 +11027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:9">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C64" s="4" t="s">
         <v>42</v>
       </c>
@@ -11110,7 +11050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C65" s="4" t="s">
         <v>43</v>
       </c>
@@ -11133,7 +11073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B66" t="s">
         <v>31</v>
       </c>
@@ -11159,7 +11099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C67" s="4" t="s">
         <v>41</v>
       </c>
@@ -11182,7 +11122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C68" s="4" t="s">
         <v>42</v>
       </c>
@@ -11205,7 +11145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C69" s="4" t="s">
         <v>43</v>
       </c>
@@ -11228,7 +11168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B70" t="s">
         <v>32</v>
       </c>
@@ -11254,7 +11194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C71" s="4" t="s">
         <v>41</v>
       </c>
@@ -11277,7 +11217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C72" s="4" t="s">
         <v>42</v>
       </c>
@@ -11300,7 +11240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C73" s="4" t="s">
         <v>43</v>
       </c>
@@ -11323,38 +11263,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A76" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B76" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C76" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D76" s="4">
+        <v>1</v>
+      </c>
+      <c r="E76" s="4">
+        <v>1</v>
+      </c>
+      <c r="F76" s="4">
+        <v>1</v>
+      </c>
+      <c r="G76" s="4">
+        <v>1</v>
+      </c>
+      <c r="H76" s="4">
+        <v>1</v>
+      </c>
+      <c r="I76" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C77" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="D76" s="4">
-        <v>1</v>
-      </c>
-      <c r="E76" s="4">
-        <v>1</v>
-      </c>
-      <c r="F76" s="4">
-        <v>1</v>
-      </c>
-      <c r="G76" s="4">
-        <v>1</v>
-      </c>
-      <c r="H76" s="4">
-        <v>1</v>
-      </c>
-      <c r="I76" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9">
-      <c r="C77" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="D77" s="4">
         <v>1</v>
@@ -11375,35 +11315,35 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B78" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C78" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D78" s="4">
+        <v>1</v>
+      </c>
+      <c r="E78" s="4">
+        <v>1</v>
+      </c>
+      <c r="F78" s="4">
+        <v>1</v>
+      </c>
+      <c r="G78" s="4">
+        <v>1</v>
+      </c>
+      <c r="H78" s="4">
+        <v>1</v>
+      </c>
+      <c r="I78" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C79" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="D78" s="4">
-        <v>1</v>
-      </c>
-      <c r="E78" s="4">
-        <v>1</v>
-      </c>
-      <c r="F78" s="4">
-        <v>1</v>
-      </c>
-      <c r="G78" s="4">
-        <v>1</v>
-      </c>
-      <c r="H78" s="4">
-        <v>1</v>
-      </c>
-      <c r="I78" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9">
-      <c r="C79" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="D79" s="4">
         <v>1</v>
@@ -11424,35 +11364,35 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B80" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C80" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D80" s="4">
+        <v>1</v>
+      </c>
+      <c r="E80" s="4">
+        <v>1</v>
+      </c>
+      <c r="F80" s="4">
+        <v>1</v>
+      </c>
+      <c r="G80" s="4">
+        <v>1</v>
+      </c>
+      <c r="H80" s="4">
+        <v>1</v>
+      </c>
+      <c r="I80" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C81" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="D80" s="4">
-        <v>1</v>
-      </c>
-      <c r="E80" s="4">
-        <v>1</v>
-      </c>
-      <c r="F80" s="4">
-        <v>1</v>
-      </c>
-      <c r="G80" s="4">
-        <v>1</v>
-      </c>
-      <c r="H80" s="4">
-        <v>1</v>
-      </c>
-      <c r="I80" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9">
-      <c r="C81" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="D81" s="4">
         <v>1</v>
@@ -11473,12 +11413,12 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A84" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>40</v>
@@ -11502,7 +11442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C85" s="4" t="s">
         <v>41</v>
       </c>
@@ -11525,7 +11465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C86" s="4" t="s">
         <v>42</v>
       </c>
@@ -11548,7 +11488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C87" s="4" t="s">
         <v>43</v>
       </c>
@@ -11571,22 +11511,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A90" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B90" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -11601,7 +11536,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="36.6640625" customWidth="1"/>
     <col min="2" max="2" width="64.5" customWidth="1"/>
@@ -11611,12 +11546,12 @@
     <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>6</v>
@@ -11634,12 +11569,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="4">
@@ -11655,7 +11590,7 @@
         <v>174.7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
         <v>29</v>
       </c>
@@ -11675,9 +11610,9 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>56</v>
@@ -11698,7 +11633,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>48</v>
       </c>
@@ -11718,7 +11653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>49</v>
       </c>
@@ -11738,9 +11673,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B8" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -11758,9 +11693,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -11778,7 +11713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>50</v>
       </c>
@@ -11798,9 +11733,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>57</v>
@@ -11821,7 +11756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14">
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>58</v>
       </c>
@@ -11845,10 +11780,5 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Small change to subheading
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-34100" yWindow="-20540" windowWidth="25460" windowHeight="20540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-34100" yWindow="-20540" windowWidth="25460" windowHeight="20540" tabRatio="500" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -1693,7 +1693,7 @@
     <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="E17" authorId="0">
+    <comment ref="E16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1716,7 +1716,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G18" authorId="0">
+    <comment ref="G17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1738,7 +1738,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B19" authorId="1">
+    <comment ref="B18" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1760,7 +1760,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L19" authorId="0">
+    <comment ref="L18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1783,7 +1783,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B31" authorId="1">
+    <comment ref="B30" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1805,7 +1805,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B35" authorId="1">
+    <comment ref="B34" authorId="1">
       <text>
         <r>
           <rPr>
@@ -5295,7 +5295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="D16" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -6129,10 +6129,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6607,10 +6607,52 @@
       <c r="A13" s="11" t="s">
         <v>161</v>
       </c>
+      <c r="B13" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="F13" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="G13" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="H13" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="I13" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="J13" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="K13" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="L13" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="M13" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="N13" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="O13" s="57">
+        <v>0.97599999999999998</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B14" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -6654,7 +6696,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B15" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -6698,7 +6740,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B16" s="4" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -6706,43 +6748,43 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="F16" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="G16" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="H16" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="I16" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="J16" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="K16" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="L16" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="M16" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="N16" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="O16" s="57">
-        <v>0.97599999999999998</v>
+      <c r="E16" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="F16" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="G16" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="H16" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="I16" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="J16" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="K16" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="L16" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="M16" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="N16" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="O16" s="58">
+        <v>0.9</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B17" s="4" t="s">
-        <v>111</v>
+      <c r="B17" t="s">
+        <v>162</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -6750,129 +6792,88 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17" s="58">
+      <c r="E17" s="57">
+        <v>1</v>
+      </c>
+      <c r="F17" s="57">
+        <v>1</v>
+      </c>
+      <c r="G17" s="58">
+        <v>0.8</v>
+      </c>
+      <c r="H17" s="57">
+        <v>1</v>
+      </c>
+      <c r="I17" s="57">
+        <v>1</v>
+      </c>
+      <c r="J17" s="57">
+        <v>1</v>
+      </c>
+      <c r="K17" s="57">
+        <v>1</v>
+      </c>
+      <c r="L17" s="57">
+        <v>1</v>
+      </c>
+      <c r="M17" s="57">
+        <v>1</v>
+      </c>
+      <c r="N17" s="57">
+        <v>1</v>
+      </c>
+      <c r="O17" s="57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B18" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="57">
+        <v>1</v>
+      </c>
+      <c r="F18" s="57">
+        <v>1</v>
+      </c>
+      <c r="G18" s="57">
+        <v>1</v>
+      </c>
+      <c r="H18" s="57">
+        <v>1</v>
+      </c>
+      <c r="I18" s="57">
+        <v>1</v>
+      </c>
+      <c r="J18" s="57">
+        <v>1</v>
+      </c>
+      <c r="K18" s="57">
+        <v>1</v>
+      </c>
+      <c r="L18" s="58">
         <v>0.9</v>
       </c>
-      <c r="F17" s="58">
+      <c r="M18" s="58">
         <v>0.9</v>
       </c>
-      <c r="G17" s="58">
+      <c r="N18" s="58">
         <v>0.9</v>
       </c>
-      <c r="H17" s="58">
+      <c r="O18" s="58">
         <v>0.9</v>
       </c>
-      <c r="I17" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="J17" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="K17" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="L17" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="M17" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="N17" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="O17" s="58">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B18" t="s">
-        <v>162</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" s="57">
-        <v>1</v>
-      </c>
-      <c r="F18" s="57">
-        <v>1</v>
-      </c>
-      <c r="G18" s="58">
-        <v>0.8</v>
-      </c>
-      <c r="H18" s="57">
-        <v>1</v>
-      </c>
-      <c r="I18" s="57">
-        <v>1</v>
-      </c>
-      <c r="J18" s="57">
-        <v>1</v>
-      </c>
-      <c r="K18" s="57">
-        <v>1</v>
-      </c>
-      <c r="L18" s="57">
-        <v>1</v>
-      </c>
-      <c r="M18" s="57">
-        <v>1</v>
-      </c>
-      <c r="N18" s="57">
-        <v>1</v>
-      </c>
-      <c r="O18" s="57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B19" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="57">
-        <v>1</v>
-      </c>
-      <c r="F19" s="57">
-        <v>1</v>
-      </c>
-      <c r="G19" s="57">
-        <v>1</v>
-      </c>
-      <c r="H19" s="57">
-        <v>1</v>
-      </c>
-      <c r="I19" s="57">
-        <v>1</v>
-      </c>
-      <c r="J19" s="57">
-        <v>1</v>
-      </c>
-      <c r="K19" s="57">
-        <v>1</v>
-      </c>
-      <c r="L19" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="M19" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="N19" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="O19" s="58">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.15"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.15"/>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B31" s="4"/>
+    </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B32" s="4"/>
     </row>
@@ -6881,9 +6882,6 @@
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B34" s="4"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B35" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7340,7 +7338,7 @@
   </sheetPr>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update to anaemia by intervention sheet
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -1693,7 +1693,7 @@
     <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="E16" authorId="0">
+    <comment ref="E15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1716,7 +1716,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G17" authorId="0">
+    <comment ref="G16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1738,7 +1738,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="1">
+    <comment ref="B17" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1760,7 +1760,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L18" authorId="0">
+    <comment ref="L17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1783,7 +1783,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B30" authorId="1">
+    <comment ref="B29" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1805,7 +1805,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B34" authorId="1">
+    <comment ref="B33" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1832,7 +1832,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="172">
   <si>
     <t>year</t>
   </si>
@@ -6129,10 +6129,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6144,7 +6144,10 @@
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="11" t="s">
+        <v>52</v>
+      </c>
       <c r="B1" s="11" t="s">
         <v>47</v>
       </c>
@@ -6189,27 +6192,55 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
+      <c r="A2" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0.3</v>
+      </c>
+      <c r="M2">
+        <v>0.3</v>
+      </c>
+      <c r="N2">
+        <v>0.3</v>
+      </c>
+      <c r="O2">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A3" s="11" t="s">
-        <v>160</v>
-      </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>159</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -6239,21 +6270,21 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.3</v>
+        <v>0.83</v>
       </c>
       <c r="M3">
-        <v>0.3</v>
+        <v>0.83</v>
       </c>
       <c r="N3">
-        <v>0.3</v>
+        <v>0.83</v>
       </c>
       <c r="O3">
-        <v>0.3</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -6271,33 +6302,33 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0.73</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0.73</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0.73</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0.73</v>
       </c>
       <c r="L4">
-        <v>0.83</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>0.83</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>0.83</v>
+        <v>1</v>
       </c>
       <c r="O4">
-        <v>0.83</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -6341,7 +6372,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -6385,7 +6416,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -6429,7 +6460,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -6473,7 +6504,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -6517,7 +6548,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -6559,56 +6590,56 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B11" t="s">
-        <v>169</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>0.73</v>
-      </c>
-      <c r="I11">
-        <v>0.73</v>
-      </c>
-      <c r="J11">
-        <v>0.73</v>
-      </c>
-      <c r="K11">
-        <v>0.73</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-      <c r="O11">
-        <v>1</v>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A12" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="F12" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="G12" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="H12" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="I12" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="J12" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="K12" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="L12" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="M12" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="N12" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="O12" s="57">
+        <v>0.97599999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A13" s="11" t="s">
-        <v>161</v>
-      </c>
       <c r="B13" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -6652,7 +6683,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B14" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -6696,7 +6727,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B15" s="4" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -6704,43 +6735,43 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="F15" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="G15" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="H15" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="I15" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="J15" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="K15" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="L15" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="M15" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="N15" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="O15" s="57">
-        <v>0.97599999999999998</v>
+      <c r="E15" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="F15" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="G15" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="H15" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="I15" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="J15" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="K15" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="L15" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="M15" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="N15" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="O15" s="58">
+        <v>0.9</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B16" s="4" t="s">
-        <v>111</v>
+      <c r="B16" t="s">
+        <v>162</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -6748,129 +6779,88 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16" s="58">
+      <c r="E16" s="57">
+        <v>1</v>
+      </c>
+      <c r="F16" s="57">
+        <v>1</v>
+      </c>
+      <c r="G16" s="58">
+        <v>0.8</v>
+      </c>
+      <c r="H16" s="57">
+        <v>1</v>
+      </c>
+      <c r="I16" s="57">
+        <v>1</v>
+      </c>
+      <c r="J16" s="57">
+        <v>1</v>
+      </c>
+      <c r="K16" s="57">
+        <v>1</v>
+      </c>
+      <c r="L16" s="57">
+        <v>1</v>
+      </c>
+      <c r="M16" s="57">
+        <v>1</v>
+      </c>
+      <c r="N16" s="57">
+        <v>1</v>
+      </c>
+      <c r="O16" s="57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B17" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="57">
+        <v>1</v>
+      </c>
+      <c r="F17" s="57">
+        <v>1</v>
+      </c>
+      <c r="G17" s="57">
+        <v>1</v>
+      </c>
+      <c r="H17" s="57">
+        <v>1</v>
+      </c>
+      <c r="I17" s="57">
+        <v>1</v>
+      </c>
+      <c r="J17" s="57">
+        <v>1</v>
+      </c>
+      <c r="K17" s="57">
+        <v>1</v>
+      </c>
+      <c r="L17" s="58">
         <v>0.9</v>
       </c>
-      <c r="F16" s="58">
+      <c r="M17" s="58">
         <v>0.9</v>
       </c>
-      <c r="G16" s="58">
+      <c r="N17" s="58">
         <v>0.9</v>
       </c>
-      <c r="H16" s="58">
+      <c r="O17" s="58">
         <v>0.9</v>
       </c>
-      <c r="I16" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="J16" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="K16" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="L16" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="M16" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="N16" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="O16" s="58">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B17" t="s">
-        <v>162</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" s="57">
-        <v>1</v>
-      </c>
-      <c r="F17" s="57">
-        <v>1</v>
-      </c>
-      <c r="G17" s="58">
-        <v>0.8</v>
-      </c>
-      <c r="H17" s="57">
-        <v>1</v>
-      </c>
-      <c r="I17" s="57">
-        <v>1</v>
-      </c>
-      <c r="J17" s="57">
-        <v>1</v>
-      </c>
-      <c r="K17" s="57">
-        <v>1</v>
-      </c>
-      <c r="L17" s="57">
-        <v>1</v>
-      </c>
-      <c r="M17" s="57">
-        <v>1</v>
-      </c>
-      <c r="N17" s="57">
-        <v>1</v>
-      </c>
-      <c r="O17" s="57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B18" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" s="57">
-        <v>1</v>
-      </c>
-      <c r="F18" s="57">
-        <v>1</v>
-      </c>
-      <c r="G18" s="57">
-        <v>1</v>
-      </c>
-      <c r="H18" s="57">
-        <v>1</v>
-      </c>
-      <c r="I18" s="57">
-        <v>1</v>
-      </c>
-      <c r="J18" s="57">
-        <v>1</v>
-      </c>
-      <c r="K18" s="57">
-        <v>1</v>
-      </c>
-      <c r="L18" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="M18" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="N18" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="O18" s="58">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.15"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.15"/>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B30" s="4"/>
+    </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B31" s="4"/>
     </row>
@@ -6879,9 +6869,6 @@
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Removed space from intervention name
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -1832,7 +1832,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="171">
   <si>
     <t>year</t>
   </si>
@@ -2318,9 +2318,6 @@
   </si>
   <si>
     <t>Odds Ratios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprinkles </t>
   </si>
   <si>
     <t>IFAS poor: school</t>
@@ -5423,7 +5420,7 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
@@ -5618,7 +5615,7 @@
         <v>95</v>
       </c>
       <c r="B14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
@@ -5644,7 +5641,7 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C15" s="3">
         <v>0</v>
@@ -5670,7 +5667,7 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -5696,7 +5693,7 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C17" s="3">
         <v>0</v>
@@ -5722,7 +5719,7 @@
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
@@ -5748,7 +5745,7 @@
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -5774,7 +5771,7 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
@@ -6132,7 +6129,7 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6284,7 +6281,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -6328,7 +6325,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -6372,7 +6369,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -6416,7 +6413,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -6460,7 +6457,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -6504,7 +6501,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -6548,7 +6545,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -6771,7 +6768,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
-        <v>162</v>
+        <v>85</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -7086,7 +7083,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B5" s="15">
         <v>0</v>
@@ -7181,7 +7178,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="35"/>
@@ -7192,7 +7189,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="35"/>
@@ -7203,7 +7200,7 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="35"/>
@@ -7214,7 +7211,7 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="35"/>
@@ -7225,7 +7222,7 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="35"/>
@@ -7233,7 +7230,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="35"/>
@@ -7241,7 +7238,7 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -7348,7 +7345,7 @@
         <v>66</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>139</v>

</xml_diff>

<commit_message>
Added 'severe diarrhea' to the interventions for children tab
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-34100" yWindow="-20540" windowWidth="25460" windowHeight="20540" tabRatio="500" firstSheet="8" activeTab="12"/>
+    <workbookView xWindow="-34100" yWindow="-20540" windowWidth="25460" windowHeight="20540" tabRatio="500" firstSheet="8" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -1832,7 +1832,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="172">
   <si>
     <t>year</t>
   </si>
@@ -2345,6 +2345,9 @@
   </si>
   <si>
     <t>women 15-19 years</t>
+  </si>
+  <si>
+    <t>Severe diarrhea</t>
   </si>
 </sst>
 </file>
@@ -6128,7 +6131,7 @@
   </sheetPr>
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -6881,8 +6884,8 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6987,6 +6990,29 @@
       </c>
       <c r="H4" s="4">
         <v>0.62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G5" s="32">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H5" s="32">
+        <v>0.33500000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Highlighted uncertain cells in yellow
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-34100" yWindow="-20540" windowWidth="25460" windowHeight="20540" tabRatio="500" firstSheet="8" activeTab="13"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="8" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3038,7 +3038,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3133,6 +3133,11 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="515">
@@ -6885,7 +6890,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6993,25 +6998,26 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B5" t="s">
+      <c r="A5" s="61"/>
+      <c r="B5" s="61" t="s">
         <v>171</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="D5" s="62">
+        <v>0</v>
+      </c>
+      <c r="E5" s="62">
+        <v>0</v>
+      </c>
+      <c r="F5" s="62">
         <v>0.33500000000000002</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="63">
         <v>0.33500000000000002</v>
       </c>
-      <c r="H5" s="32">
+      <c r="H5" s="63">
         <v>0.33500000000000002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added multiple micronutrient supplementation as a separate intervention
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="8" activeTab="13"/>
+    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -1034,7 +1034,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H9" authorId="0">
+    <comment ref="E8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1056,7 +1056,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="1">
+    <comment ref="F8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1065,7 +1065,7 @@
             <color indexed="81"/>
             <rFont val="Arial"/>
           </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
+          <t>Janka Petravic:</t>
         </r>
         <r>
           <rPr>
@@ -1074,7 +1074,29 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+food insecure - default poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+food insecure - default poor</t>
         </r>
       </text>
     </comment>
@@ -1096,11 +1118,33 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Also brestfeeding women up to 6 months?</t>
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="1">
+    <comment ref="B13" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Also brestfeeding women up to 6 months?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1122,7 +1166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I14" authorId="1">
+    <comment ref="I15" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1144,7 +1188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I15" authorId="0">
+    <comment ref="I16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1163,116 +1207,6 @@
           </rPr>
           <t xml:space="preserve">
 food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E22" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F22" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G22" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H22" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I22" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1294,7 +1228,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1316,7 +1250,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1338,7 +1272,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1360,7 +1294,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1382,7 +1316,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1404,7 +1338,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1426,7 +1360,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1448,7 +1382,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1470,7 +1404,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1492,11 +1426,121 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
-    <comment ref="C26" authorId="1">
+    <comment ref="E25" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F25" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G25" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H25" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I25" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C27" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1518,7 +1562,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D26" authorId="1">
+    <comment ref="D27" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1540,7 +1584,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E26" authorId="1">
+    <comment ref="E27" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1562,7 +1606,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F26" authorId="1">
+    <comment ref="F27" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1584,7 +1628,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G26" authorId="1">
+    <comment ref="G27" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1606,7 +1650,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H26" authorId="1">
+    <comment ref="H27" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1628,7 +1672,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I26" authorId="1">
+    <comment ref="I27" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1693,7 +1737,7 @@
     <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="E15" authorId="0">
+    <comment ref="E16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1716,7 +1760,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G16" authorId="0">
+    <comment ref="G17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1738,7 +1782,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="1">
+    <comment ref="B18" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1760,7 +1804,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L17" authorId="0">
+    <comment ref="L18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1783,7 +1827,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B29" authorId="1">
+    <comment ref="B30" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1805,7 +1849,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B33" authorId="1">
+    <comment ref="B34" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1832,7 +1876,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="173">
   <si>
     <t>year</t>
   </si>
@@ -2348,6 +2392,9 @@
   </si>
   <si>
     <t>Severe diarrhea</t>
+  </si>
+  <si>
+    <t>Multiple micronutrient supplementation</t>
   </si>
 </sst>
 </file>
@@ -2521,7 +2568,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="515">
+  <cellStyleXfs count="517">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2533,6 +2580,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3140,7 +3189,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="515">
+  <cellStyles count="517">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3398,6 +3447,7 @@
     <cellStyle name="Followed Hyperlink" xfId="510" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="512" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="516" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3654,6 +3704,7 @@
     <cellStyle name="Hyperlink" xfId="509" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="511" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="515" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -5298,10 +5349,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5509,147 +5560,149 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="31">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="31">
         <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
-      <c r="I9" s="3">
+      <c r="F8" s="31">
+        <f>'Baseline year demographics'!$C$7</f>
+        <v>0.36</v>
+      </c>
+      <c r="G8" s="31">
+        <v>0</v>
+      </c>
+      <c r="H8" s="31">
+        <v>0</v>
+      </c>
+      <c r="I8" s="31">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="11" t="s">
+        <v>83</v>
+      </c>
       <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="31">
+        <f>'Baseline year demographics'!$C$7</f>
+        <v>0.36</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3">
-        <v>1</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="36">
-        <v>1</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" t="s">
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="36">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" t="s">
         <v>159</v>
       </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0</v>
-      </c>
-      <c r="G12" s="3">
-        <v>0</v>
-      </c>
-      <c r="H12" s="36">
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="I12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="11" t="s">
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>162</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3">
-        <v>0</v>
-      </c>
-      <c r="I14" s="59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" t="s">
-        <v>163</v>
       </c>
       <c r="C15" s="3">
         <v>0</v>
@@ -5675,7 +5728,7 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -5701,7 +5754,7 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C17" s="3">
         <v>0</v>
@@ -5727,7 +5780,7 @@
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
@@ -5753,7 +5806,7 @@
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -5779,192 +5832,218 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+      <c r="I20" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" t="s">
         <v>168</v>
       </c>
-      <c r="C20" s="3">
-        <v>0</v>
-      </c>
-      <c r="D20" s="3">
-        <v>0</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0</v>
-      </c>
-      <c r="H20" s="3">
-        <v>0</v>
-      </c>
-      <c r="I20" s="60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+      <c r="I21" s="60">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="11" t="s">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="3">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0</v>
-      </c>
-      <c r="E22" s="36">
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="F22" s="36">
+      <c r="F23" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="G22" s="36">
+      <c r="G23" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="H22" s="36">
+      <c r="H23" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="I22" s="36">
+      <c r="I23" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="4" t="s">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="3">
-        <v>0</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0</v>
-      </c>
-      <c r="E23" s="3">
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F24" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G24" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H24" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I24" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="4" t="s">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C24" s="3">
-        <v>0</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0</v>
-      </c>
-      <c r="E24" s="3">
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F25" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G25" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H25" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I25" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C25" s="3">
-        <v>0</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0</v>
-      </c>
-      <c r="E25" s="36">
-        <v>1</v>
-      </c>
-      <c r="F25" s="36">
-        <v>1</v>
-      </c>
-      <c r="G25" s="36">
-        <v>1</v>
-      </c>
-      <c r="H25" s="36">
-        <v>1</v>
-      </c>
-      <c r="I25" s="36">
-        <v>1</v>
-      </c>
-    </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="36">
+        <v>1</v>
+      </c>
+      <c r="F26" s="36">
+        <v>1</v>
+      </c>
+      <c r="G26" s="36">
+        <v>1</v>
+      </c>
+      <c r="H26" s="36">
+        <v>1</v>
+      </c>
+      <c r="I26" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="36">
+      <c r="C27" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="D26" s="36">
+      <c r="D27" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="E26" s="36">
+      <c r="E27" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="F26" s="36">
+      <c r="F27" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="G26" s="36">
+      <c r="G27" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="H26" s="36">
+      <c r="H27" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="I26" s="36">
+      <c r="I27" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6134,10 +6213,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6595,56 +6674,56 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A12" s="11" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B11" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="61">
+        <v>1</v>
+      </c>
+      <c r="F11" s="61">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A13" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="F12" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="G12" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="H12" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="I12" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="J12" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="K12" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="L12" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="M12" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="N12" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="O12" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B13" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -6688,7 +6767,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B14" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -6732,140 +6811,181 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B15" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="F15" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="G15" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="H15" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="I15" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="J15" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="K15" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="L15" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="M15" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="N15" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="O15" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B16" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="58">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="58">
         <v>0.9</v>
       </c>
-      <c r="F15" s="58">
+      <c r="F16" s="58">
         <v>0.9</v>
       </c>
-      <c r="G15" s="58">
+      <c r="G16" s="58">
         <v>0.9</v>
       </c>
-      <c r="H15" s="58">
+      <c r="H16" s="58">
         <v>0.9</v>
       </c>
-      <c r="I15" s="58">
+      <c r="I16" s="58">
         <v>0.9</v>
       </c>
-      <c r="J15" s="58">
+      <c r="J16" s="58">
         <v>0.9</v>
       </c>
-      <c r="K15" s="58">
+      <c r="K16" s="58">
         <v>0.9</v>
       </c>
-      <c r="L15" s="58">
+      <c r="L16" s="58">
         <v>0.9</v>
       </c>
-      <c r="M15" s="58">
+      <c r="M16" s="58">
         <v>0.9</v>
       </c>
-      <c r="N15" s="58">
+      <c r="N16" s="58">
         <v>0.9</v>
       </c>
-      <c r="O15" s="58">
+      <c r="O16" s="58">
         <v>0.9</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B16" t="s">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
         <v>85</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="57">
-        <v>1</v>
-      </c>
-      <c r="F16" s="57">
-        <v>1</v>
-      </c>
-      <c r="G16" s="58">
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="57">
+        <v>1</v>
+      </c>
+      <c r="F17" s="57">
+        <v>1</v>
+      </c>
+      <c r="G17" s="58">
         <v>0.8</v>
       </c>
-      <c r="H16" s="57">
-        <v>1</v>
-      </c>
-      <c r="I16" s="57">
-        <v>1</v>
-      </c>
-      <c r="J16" s="57">
-        <v>1</v>
-      </c>
-      <c r="K16" s="57">
-        <v>1</v>
-      </c>
-      <c r="L16" s="57">
-        <v>1</v>
-      </c>
-      <c r="M16" s="57">
-        <v>1</v>
-      </c>
-      <c r="N16" s="57">
-        <v>1</v>
-      </c>
-      <c r="O16" s="57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B17" s="4" t="s">
+      <c r="H17" s="57">
+        <v>1</v>
+      </c>
+      <c r="I17" s="57">
+        <v>1</v>
+      </c>
+      <c r="J17" s="57">
+        <v>1</v>
+      </c>
+      <c r="K17" s="57">
+        <v>1</v>
+      </c>
+      <c r="L17" s="57">
+        <v>1</v>
+      </c>
+      <c r="M17" s="57">
+        <v>1</v>
+      </c>
+      <c r="N17" s="57">
+        <v>1</v>
+      </c>
+      <c r="O17" s="57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B18" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" s="57">
-        <v>1</v>
-      </c>
-      <c r="F17" s="57">
-        <v>1</v>
-      </c>
-      <c r="G17" s="57">
-        <v>1</v>
-      </c>
-      <c r="H17" s="57">
-        <v>1</v>
-      </c>
-      <c r="I17" s="57">
-        <v>1</v>
-      </c>
-      <c r="J17" s="57">
-        <v>1</v>
-      </c>
-      <c r="K17" s="57">
-        <v>1</v>
-      </c>
-      <c r="L17" s="58">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="57">
+        <v>1</v>
+      </c>
+      <c r="F18" s="57">
+        <v>1</v>
+      </c>
+      <c r="G18" s="57">
+        <v>1</v>
+      </c>
+      <c r="H18" s="57">
+        <v>1</v>
+      </c>
+      <c r="I18" s="57">
+        <v>1</v>
+      </c>
+      <c r="J18" s="57">
+        <v>1</v>
+      </c>
+      <c r="K18" s="57">
+        <v>1</v>
+      </c>
+      <c r="L18" s="58">
         <v>0.9</v>
       </c>
-      <c r="M17" s="58">
+      <c r="M18" s="58">
         <v>0.9</v>
       </c>
-      <c r="N17" s="58">
+      <c r="N18" s="58">
         <v>0.9</v>
       </c>
-      <c r="O17" s="58">
+      <c r="O18" s="58">
         <v>0.9</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.15"/>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B30" s="4"/>
-    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.15"/>
     <row r="31" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B31" s="4"/>
     </row>
@@ -6874,6 +6994,9 @@
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B33" s="4"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6889,7 +7012,7 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -7037,7 +7160,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7315,6 +7438,14 @@
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
       <c r="D23" s="35"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>172</v>
+      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="35"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="4"/>
@@ -9068,8 +9199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Removed MMS, added PPCF + iron to anemia tab
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -1034,7 +1034,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0">
+    <comment ref="H9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1056,7 +1056,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0">
+    <comment ref="B11" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1065,7 +1065,7 @@
             <color indexed="81"/>
             <rFont val="Arial"/>
           </rPr>
-          <t>Janka Petravic:</t>
+          <t xml:space="preserve"> Janka Petravic:</t>
         </r>
         <r>
           <rPr>
@@ -1074,29 +1074,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H10" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-food insecure - default poor</t>
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
         </r>
       </text>
     </comment>
@@ -1118,11 +1096,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+Also brestfeeding women up to 6 months?</t>
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="1">
+    <comment ref="A14" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1140,11 +1118,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Also brestfeeding women up to 6 months?</t>
+Coverage of these interventions is mutually exclusive</t>
         </r>
       </text>
     </comment>
-    <comment ref="A15" authorId="1">
+    <comment ref="I14" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1162,11 +1140,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Coverage of these interventions is mutually exclusive</t>
+In baseline year, assuming only non-pregnant go to school</t>
         </r>
       </text>
     </comment>
-    <comment ref="I15" authorId="1">
+    <comment ref="I15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1175,7 +1153,7 @@
             <color indexed="81"/>
             <rFont val="Arial"/>
           </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
+          <t>Janka Petravic:</t>
         </r>
         <r>
           <rPr>
@@ -1184,11 +1162,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-In baseline year, assuming only non-pregnant go to school</t>
+food insecure - default poor</t>
         </r>
       </text>
     </comment>
-    <comment ref="I16" authorId="0">
+    <comment ref="E22" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1197,7 +1175,7 @@
             <color indexed="81"/>
             <rFont val="Arial"/>
           </rPr>
-          <t>Janka Petravic:</t>
+          <t xml:space="preserve"> Janka Petravic:</t>
         </r>
         <r>
           <rPr>
@@ -1206,7 +1184,95 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-food insecure - default poor</t>
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F22" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G22" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H22" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I22" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1228,7 +1294,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating wheat</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1250,7 +1316,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating wheat</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1272,7 +1338,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating wheat</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1294,7 +1360,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating wheat</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1316,7 +1382,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating wheat</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1338,7 +1404,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+fraction eating rice</t>
         </r>
       </text>
     </comment>
@@ -1360,7 +1426,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+fraction eating rice</t>
         </r>
       </text>
     </comment>
@@ -1382,7 +1448,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+fraction eating rice</t>
         </r>
       </text>
     </comment>
@@ -1404,7 +1470,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+fraction eating rice</t>
         </r>
       </text>
     </comment>
@@ -1426,11 +1492,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+fraction eating rice</t>
         </r>
       </text>
     </comment>
-    <comment ref="E25" authorId="1">
+    <comment ref="C26" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1448,11 +1514,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+At risk from malaria</t>
         </r>
       </text>
     </comment>
-    <comment ref="F25" authorId="1">
+    <comment ref="D26" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1470,11 +1536,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+At risk from malaria</t>
         </r>
       </text>
     </comment>
-    <comment ref="G25" authorId="1">
+    <comment ref="E26" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1492,11 +1558,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+At risk from malaria</t>
         </r>
       </text>
     </comment>
-    <comment ref="H25" authorId="1">
+    <comment ref="F26" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1514,11 +1580,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+At risk from malaria</t>
         </r>
       </text>
     </comment>
-    <comment ref="I25" authorId="1">
+    <comment ref="G26" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1536,11 +1602,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+At risk from malaria</t>
         </r>
       </text>
     </comment>
-    <comment ref="C27" authorId="1">
+    <comment ref="H26" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1562,117 +1628,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D27" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E27" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F27" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G27" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H27" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I27" authorId="1">
+    <comment ref="I26" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1876,7 +1832,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="172">
   <si>
     <t>year</t>
   </si>
@@ -2392,9 +2348,6 @@
   </si>
   <si>
     <t>Severe diarrhea</t>
-  </si>
-  <si>
-    <t>Multiple micronutrient supplementation</t>
   </si>
 </sst>
 </file>
@@ -5349,10 +5302,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5560,40 +5513,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" t="s">
-        <v>172</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="31">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="31">
         <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
-      <c r="F8" s="31">
-        <f>'Baseline year demographics'!$C$7</f>
-        <v>0.36</v>
-      </c>
-      <c r="G8" s="31">
-        <v>0</v>
-      </c>
-      <c r="H8" s="31">
-        <v>0</v>
-      </c>
-      <c r="I8" s="31">
+      <c r="I9" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="11" t="s">
-        <v>83</v>
-      </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
@@ -5610,17 +5562,16 @@
       <c r="G10" s="3">
         <v>0</v>
       </c>
-      <c r="H10" s="31">
-        <f>'Baseline year demographics'!$C$7</f>
-        <v>0.36</v>
+      <c r="H10" s="3">
+        <v>1</v>
       </c>
       <c r="I10" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" t="s">
-        <v>60</v>
+      <c r="B11" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="C11" s="3">
         <v>0</v>
@@ -5637,7 +5588,7 @@
       <c r="G11" s="3">
         <v>0</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="36">
         <v>1</v>
       </c>
       <c r="I11" s="3">
@@ -5645,8 +5596,8 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="4" t="s">
-        <v>88</v>
+      <c r="B12" t="s">
+        <v>159</v>
       </c>
       <c r="C12" s="3">
         <v>0</v>
@@ -5664,45 +5615,45 @@
         <v>0</v>
       </c>
       <c r="H12" s="36">
-        <v>1</v>
-      </c>
-      <c r="I12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" t="s">
-        <v>159</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0</v>
-      </c>
-      <c r="H13" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="I13" s="3">
-        <v>0</v>
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="59">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="11" t="s">
-        <v>95</v>
-      </c>
       <c r="B15" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C15" s="3">
         <v>0</v>
@@ -5728,7 +5679,7 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -5754,7 +5705,7 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C17" s="3">
         <v>0</v>
@@ -5780,7 +5731,7 @@
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
@@ -5806,7 +5757,7 @@
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -5832,7 +5783,7 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
@@ -5852,77 +5803,82 @@
       <c r="H20" s="3">
         <v>0</v>
       </c>
-      <c r="I20" s="59">
+      <c r="I20" s="60">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" t="s">
-        <v>168</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0</v>
-      </c>
-      <c r="E21" s="3">
-        <v>0</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0</v>
-      </c>
-      <c r="G21" s="3">
-        <v>0</v>
-      </c>
-      <c r="H21" s="3">
-        <v>0</v>
-      </c>
-      <c r="I21" s="60">
-        <v>1</v>
-      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="11" t="s">
+      <c r="A22" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="3">
-        <v>0</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0</v>
-      </c>
-      <c r="E23" s="36">
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="F23" s="36">
+      <c r="F22" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="G23" s="36">
+      <c r="G22" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="H23" s="36">
+      <c r="H22" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="I23" s="36">
+      <c r="I22" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
     </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <f>'Baseline year demographics'!$C$22</f>
+        <v>0.05</v>
+      </c>
+      <c r="F23" s="3">
+        <f>'Baseline year demographics'!$C$22</f>
+        <v>0.05</v>
+      </c>
+      <c r="G23" s="3">
+        <f>'Baseline year demographics'!$C$22</f>
+        <v>0.05</v>
+      </c>
+      <c r="H23" s="3">
+        <f>'Baseline year demographics'!$C$22</f>
+        <v>0.05</v>
+      </c>
+      <c r="I23" s="3">
+        <f>'Baseline year demographics'!$C$22</f>
+        <v>0.05</v>
+      </c>
+    </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
@@ -5931,29 +5887,29 @@
         <v>0</v>
       </c>
       <c r="E24" s="3">
-        <f>'Baseline year demographics'!$C$22</f>
-        <v>0.05</v>
+        <f>'Baseline year demographics'!$C$20</f>
+        <v>0.8</v>
       </c>
       <c r="F24" s="3">
-        <f>'Baseline year demographics'!$C$22</f>
-        <v>0.05</v>
+        <f>'Baseline year demographics'!$C$20</f>
+        <v>0.8</v>
       </c>
       <c r="G24" s="3">
-        <f>'Baseline year demographics'!$C$22</f>
-        <v>0.05</v>
+        <f>'Baseline year demographics'!$C$20</f>
+        <v>0.8</v>
       </c>
       <c r="H24" s="3">
-        <f>'Baseline year demographics'!$C$22</f>
-        <v>0.05</v>
+        <f>'Baseline year demographics'!$C$20</f>
+        <v>0.8</v>
       </c>
       <c r="I24" s="3">
-        <f>'Baseline year demographics'!$C$22</f>
-        <v>0.05</v>
+        <f>'Baseline year demographics'!$C$20</f>
+        <v>0.8</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="4" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C25" s="3">
         <v>0</v>
@@ -5961,89 +5917,58 @@
       <c r="D25" s="3">
         <v>0</v>
       </c>
-      <c r="E25" s="3">
-        <f>'Baseline year demographics'!$C$20</f>
-        <v>0.8</v>
-      </c>
-      <c r="F25" s="3">
-        <f>'Baseline year demographics'!$C$20</f>
-        <v>0.8</v>
-      </c>
-      <c r="G25" s="3">
-        <f>'Baseline year demographics'!$C$20</f>
-        <v>0.8</v>
-      </c>
-      <c r="H25" s="3">
-        <f>'Baseline year demographics'!$C$20</f>
-        <v>0.8</v>
-      </c>
-      <c r="I25" s="3">
-        <f>'Baseline year demographics'!$C$20</f>
-        <v>0.8</v>
+      <c r="E25" s="36">
+        <v>1</v>
+      </c>
+      <c r="F25" s="36">
+        <v>1</v>
+      </c>
+      <c r="G25" s="36">
+        <v>1</v>
+      </c>
+      <c r="H25" s="36">
+        <v>1</v>
+      </c>
+      <c r="I25" s="36">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C26" s="3">
-        <v>0</v>
-      </c>
-      <c r="D26" s="3">
-        <v>0</v>
-      </c>
-      <c r="E26" s="36">
-        <v>1</v>
-      </c>
-      <c r="F26" s="36">
-        <v>1</v>
-      </c>
-      <c r="G26" s="36">
-        <v>1</v>
-      </c>
-      <c r="H26" s="36">
-        <v>1</v>
-      </c>
-      <c r="I26" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="36">
+      <c r="C26" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="D27" s="36">
+      <c r="D26" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E26" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="F27" s="36">
+      <c r="F26" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="G27" s="36">
+      <c r="G26" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="H27" s="36">
+      <c r="H26" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="I27" s="36">
+      <c r="I26" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6675,8 +6600,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B11" t="s">
-        <v>172</v>
+      <c r="B11" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -7013,7 +6938,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7121,7 +7046,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" s="61"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="61" t="s">
         <v>171</v>
       </c>
@@ -7157,10 +7082,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7440,12 +7365,8 @@
       <c r="D23" s="35"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
-        <v>172</v>
-      </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="35"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="4"/>
@@ -7466,10 +7387,6 @@
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7485,7 +7402,7 @@
   </sheetPr>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -9199,7 +9116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added food fortification interventions: correct target pop, saturation in spreadsheet, and actual coverage accounting for subsistence farming in params.py
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Bangladesh/2017Aug/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24300" windowHeight="13420" tabRatio="500" firstSheet="12" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -28,13 +23,13 @@
     <sheet name="Interventions for children" sheetId="28" r:id="rId14"/>
     <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -297,6 +292,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author xml:space="preserve"> Janka Petravic</author>
+    <author>Ruth</author>
   </authors>
   <commentList>
     <comment ref="A10" authorId="0">
@@ -362,6 +358,28 @@
           </rPr>
           <t xml:space="preserve">
 There is no unit cost for this to impact the budget.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C21" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+This is the fraction of the population eating these staples and belongs here.</t>
         </r>
       </text>
     </comment>
@@ -4968,13 +4986,13 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="16" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>116</v>
       </c>
@@ -4985,7 +5003,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>65</v>
       </c>
@@ -4996,7 +5014,7 @@
         <v>15204000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
@@ -5004,7 +5022,7 @@
         <v>3118117</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="B4" s="34" t="s">
         <v>143</v>
       </c>
@@ -5012,7 +5030,7 @@
         <v>171684000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
@@ -5021,7 +5039,7 @@
         <v>3677298.8269880489</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="B6" s="34" t="s">
         <v>74</v>
       </c>
@@ -5029,7 +5047,7 @@
         <v>0.35199999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1">
       <c r="B7" s="4" t="s">
         <v>73</v>
       </c>
@@ -5037,7 +5055,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1">
       <c r="B8" s="34" t="s">
         <v>75</v>
       </c>
@@ -5045,11 +5063,11 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1">
       <c r="B10" s="11"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1">
       <c r="A11" s="11" t="s">
         <v>149</v>
       </c>
@@ -5060,7 +5078,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1">
       <c r="B12" t="s">
         <v>144</v>
       </c>
@@ -5068,7 +5086,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1">
       <c r="B13" t="s">
         <v>145</v>
       </c>
@@ -5076,7 +5094,7 @@
         <v>25.36</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1">
       <c r="B14" t="s">
         <v>146</v>
       </c>
@@ -5084,7 +5102,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1">
       <c r="B15" t="s">
         <v>147</v>
       </c>
@@ -5092,7 +5110,7 @@
         <v>34.68</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1">
       <c r="B16" t="s">
         <v>148</v>
       </c>
@@ -5100,11 +5118,11 @@
         <v>39.32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1">
       <c r="B18" s="11"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1">
       <c r="A19" s="11" t="s">
         <v>77</v>
       </c>
@@ -5115,7 +5133,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1">
       <c r="B20" s="34" t="s">
         <v>108</v>
       </c>
@@ -5123,7 +5141,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1">
       <c r="B21" s="34" t="s">
         <v>109</v>
       </c>
@@ -5131,7 +5149,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1">
       <c r="B22" s="34" t="s">
         <v>110</v>
       </c>
@@ -5139,7 +5157,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="B23" s="34" t="s">
         <v>78</v>
       </c>
@@ -5147,10 +5165,10 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1">
       <c r="B25" s="34"/>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="A26" s="11" t="s">
         <v>142</v>
       </c>
@@ -5161,7 +5179,7 @@
         <v>8634000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="15" customHeight="1">
       <c r="B27" s="52" t="s">
         <v>136</v>
       </c>
@@ -5169,7 +5187,7 @@
         <v>13550000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1">
       <c r="B28" s="52" t="s">
         <v>137</v>
       </c>
@@ -5177,7 +5195,7 @@
         <v>12394000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1">
       <c r="B29" s="52" t="s">
         <v>138</v>
       </c>
@@ -5185,11 +5203,11 @@
         <v>9148000</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1">
       <c r="B30" s="52"/>
       <c r="C30" s="54"/>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="A32" s="11" t="s">
         <v>130</v>
       </c>
@@ -5200,7 +5218,7 @@
         <v>0.29978973218277538</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" ht="15.75" customHeight="1">
       <c r="B33" s="51" t="s">
         <v>136</v>
       </c>
@@ -5208,7 +5226,7 @@
         <v>0.52556568434139284</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:3" ht="15.75" customHeight="1">
       <c r="B34" s="51" t="s">
         <v>137</v>
       </c>
@@ -5216,7 +5234,7 @@
         <v>0.16210210664201097</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:3" ht="15.75" customHeight="1">
       <c r="B35" s="51" t="s">
         <v>138</v>
       </c>
@@ -5228,6 +5246,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5242,12 +5265,12 @@
       <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -5264,7 +5287,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="14">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
@@ -5281,14 +5304,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -5297,6 +5320,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5305,10 +5333,10 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="43.33203125" customWidth="1"/>
@@ -5319,7 +5347,7 @@
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>87</v>
       </c>
@@ -5349,7 +5377,7 @@
       </c>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>82</v>
       </c>
@@ -5378,7 +5406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1">
       <c r="B3" s="4" t="s">
         <v>51</v>
       </c>
@@ -5404,7 +5432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1">
       <c r="B4" s="4" t="s">
         <v>58</v>
       </c>
@@ -5430,7 +5458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>169</v>
       </c>
@@ -5458,7 +5486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>86</v>
       </c>
@@ -5486,7 +5514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1">
       <c r="B7" s="4" t="s">
         <v>85</v>
       </c>
@@ -5513,7 +5541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1">
       <c r="A9" s="11" t="s">
         <v>83</v>
       </c>
@@ -5543,7 +5571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1">
       <c r="B10" t="s">
         <v>60</v>
       </c>
@@ -5569,7 +5597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1">
       <c r="B11" s="4" t="s">
         <v>88</v>
       </c>
@@ -5595,7 +5623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1">
       <c r="B12" t="s">
         <v>159</v>
       </c>
@@ -5622,7 +5650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="11" t="s">
         <v>95</v>
       </c>
@@ -5651,7 +5679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="B15" t="s">
         <v>163</v>
       </c>
@@ -5677,7 +5705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="B16" t="s">
         <v>164</v>
       </c>
@@ -5703,7 +5731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1">
       <c r="B17" t="s">
         <v>165</v>
       </c>
@@ -5729,7 +5757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1">
       <c r="B18" t="s">
         <v>166</v>
       </c>
@@ -5755,7 +5783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1">
       <c r="B19" t="s">
         <v>167</v>
       </c>
@@ -5781,7 +5809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1">
       <c r="B20" t="s">
         <v>168</v>
       </c>
@@ -5807,11 +5835,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1">
       <c r="A22" s="11" t="s">
         <v>90</v>
       </c>
@@ -5845,7 +5873,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1">
       <c r="B23" s="4" t="s">
         <v>92</v>
       </c>
@@ -5876,7 +5904,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1">
       <c r="B24" s="4" t="s">
         <v>93</v>
       </c>
@@ -5907,7 +5935,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1">
       <c r="B25" s="4" t="s">
         <v>111</v>
       </c>
@@ -5933,7 +5961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1">
       <c r="B26" s="4" t="s">
         <v>89</v>
       </c>
@@ -5966,7 +5994,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
     </row>
@@ -5974,6 +6002,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5988,14 +6021,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -6015,7 +6048,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -6035,7 +6068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="B3" t="s">
         <v>55</v>
       </c>
@@ -6052,7 +6085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -6072,7 +6105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="B5" t="s">
         <v>55</v>
       </c>
@@ -6089,7 +6122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>133</v>
       </c>
@@ -6109,7 +6142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="B7" t="s">
         <v>55</v>
       </c>
@@ -6130,6 +6163,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6144,7 +6182,7 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="42.6640625" customWidth="1"/>
@@ -6153,7 +6191,7 @@
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="14" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>52</v>
       </c>
@@ -6200,7 +6238,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15">
       <c r="A2" s="11" t="s">
         <v>160</v>
       </c>
@@ -6247,7 +6285,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15">
       <c r="B3" t="s">
         <v>159</v>
       </c>
@@ -6291,7 +6329,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15">
       <c r="B4" t="s">
         <v>162</v>
       </c>
@@ -6335,7 +6373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15">
       <c r="B5" t="s">
         <v>163</v>
       </c>
@@ -6379,7 +6417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15">
       <c r="B6" t="s">
         <v>164</v>
       </c>
@@ -6423,7 +6461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15">
       <c r="B7" t="s">
         <v>165</v>
       </c>
@@ -6467,7 +6505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15">
       <c r="B8" t="s">
         <v>166</v>
       </c>
@@ -6511,7 +6549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15">
       <c r="B9" t="s">
         <v>167</v>
       </c>
@@ -6555,7 +6593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15">
       <c r="B10" t="s">
         <v>168</v>
       </c>
@@ -6599,7 +6637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15">
       <c r="B11" s="4" t="s">
         <v>86</v>
       </c>
@@ -6643,7 +6681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15">
       <c r="A13" s="11" t="s">
         <v>161</v>
       </c>
@@ -6690,7 +6728,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15">
       <c r="B14" s="4" t="s">
         <v>92</v>
       </c>
@@ -6734,7 +6772,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15">
       <c r="B15" s="4" t="s">
         <v>93</v>
       </c>
@@ -6778,7 +6816,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15">
       <c r="B16" s="4" t="s">
         <v>111</v>
       </c>
@@ -6822,7 +6860,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:15">
       <c r="B17" t="s">
         <v>85</v>
       </c>
@@ -6866,7 +6904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:15">
       <c r="B18" s="4" t="s">
         <v>88</v>
       </c>
@@ -6910,23 +6948,28 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.15"/>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:15"/>
+    <row r="31" spans="2:15">
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:15">
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:2">
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:2">
       <c r="B34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6941,7 +6984,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="27.5" customWidth="1"/>
     <col min="3" max="3" width="38.1640625" customWidth="1"/>
@@ -6951,7 +6994,7 @@
     <col min="8" max="8" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -6977,7 +7020,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>51</v>
       </c>
@@ -7003,7 +7046,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="C3" t="s">
         <v>70</v>
       </c>
@@ -7023,7 +7066,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -7045,7 +7088,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8">
       <c r="A5" s="12"/>
       <c r="B5" s="61" t="s">
         <v>171</v>
@@ -7069,7 +7112,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -7077,6 +7120,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7084,11 +7132,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="43.83203125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -7096,7 +7144,7 @@
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -7110,7 +7158,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
@@ -7127,7 +7175,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>51</v>
       </c>
@@ -7144,7 +7192,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>58</v>
       </c>
@@ -7161,7 +7209,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>169</v>
       </c>
@@ -7178,7 +7226,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>86</v>
       </c>
@@ -7189,7 +7237,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="34" t="s">
         <v>85</v>
       </c>
@@ -7200,7 +7248,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -7217,7 +7265,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -7234,7 +7282,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>88</v>
       </c>
@@ -7245,7 +7293,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" t="s">
         <v>159</v>
       </c>
@@ -7256,7 +7304,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" t="s">
         <v>162</v>
       </c>
@@ -7267,7 +7315,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" t="s">
         <v>163</v>
       </c>
@@ -7278,7 +7326,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>164</v>
       </c>
@@ -7289,7 +7337,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" t="s">
         <v>165</v>
       </c>
@@ -7300,7 +7348,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" t="s">
         <v>166</v>
       </c>
@@ -7308,7 +7356,7 @@
       <c r="C16" s="35"/>
       <c r="D16" s="14"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1">
       <c r="A17" t="s">
         <v>167</v>
       </c>
@@ -7316,7 +7364,7 @@
       <c r="C17" s="35"/>
       <c r="D17" s="14"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>168</v>
       </c>
@@ -7324,31 +7372,37 @@
       <c r="C18" s="14"/>
       <c r="D18" s="35"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
         <v>91</v>
       </c>
       <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
+      <c r="C19" s="15">
+        <v>0.12</v>
+      </c>
       <c r="D19" s="35"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1">
       <c r="A20" s="4" t="s">
         <v>92</v>
       </c>
       <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
+      <c r="C20" s="15">
+        <v>0.05</v>
+      </c>
       <c r="D20" s="35"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
         <v>93</v>
       </c>
       <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
+      <c r="C21" s="15">
+        <v>0.8</v>
+      </c>
       <c r="D21" s="35"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1">
       <c r="A22" s="4" t="s">
         <v>111</v>
       </c>
@@ -7356,7 +7410,7 @@
       <c r="C22" s="14"/>
       <c r="D22" s="35"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1">
       <c r="A23" s="4" t="s">
         <v>89</v>
       </c>
@@ -7364,27 +7418,27 @@
       <c r="C23" s="14"/>
       <c r="D23" s="35"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
     </row>
@@ -7392,6 +7446,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7402,11 +7461,11 @@
   </sheetPr>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
@@ -7414,7 +7473,7 @@
     <col min="11" max="11" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7452,7 +7511,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1">
       <c r="A2" s="3">
         <v>2017</v>
       </c>
@@ -7494,7 +7553,7 @@
         <v>173766200</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1">
       <c r="A3" s="3">
         <v>2018</v>
       </c>
@@ -7536,7 +7595,7 @@
         <v>175848400</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1">
       <c r="A4" s="3">
         <v>2019</v>
       </c>
@@ -7578,7 +7637,7 @@
         <v>177930600</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1">
       <c r="A5" s="3">
         <v>2020</v>
       </c>
@@ -7620,7 +7679,7 @@
         <v>180012800</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1">
       <c r="A6" s="3">
         <v>2021</v>
       </c>
@@ -7662,7 +7721,7 @@
         <v>182095000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1">
       <c r="A7" s="3">
         <v>2022</v>
       </c>
@@ -7704,7 +7763,7 @@
         <v>183822800</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="A8" s="3">
         <v>2023</v>
       </c>
@@ -7746,7 +7805,7 @@
         <v>185550600</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1">
       <c r="A9" s="3">
         <v>2024</v>
       </c>
@@ -7788,7 +7847,7 @@
         <v>187278400</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1">
       <c r="A10" s="3">
         <v>2025</v>
       </c>
@@ -7830,7 +7889,7 @@
         <v>189006200</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1">
       <c r="A11" s="3">
         <v>2026</v>
       </c>
@@ -7872,7 +7931,7 @@
         <v>190734000</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1">
       <c r="A12" s="3">
         <v>2027</v>
       </c>
@@ -7914,7 +7973,7 @@
         <v>192287600</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1">
       <c r="A13" s="3">
         <v>2028</v>
       </c>
@@ -7956,7 +8015,7 @@
         <v>193841200</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1">
       <c r="A14" s="3">
         <v>2029</v>
       </c>
@@ -7998,7 +8057,7 @@
         <v>195394800</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1">
       <c r="A15" s="3">
         <v>2030</v>
       </c>
@@ -8044,6 +8103,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8055,12 +8119,12 @@
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -8083,7 +8147,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -8106,7 +8170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -8129,7 +8193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -8152,7 +8216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -8175,7 +8239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -8198,7 +8262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -8221,7 +8285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -8244,7 +8308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -8267,7 +8331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -8290,7 +8354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -8313,7 +8377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -8336,7 +8400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -8359,7 +8423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -8382,7 +8446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -8405,7 +8469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -8428,7 +8492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -8451,7 +8515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -8474,7 +8538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -8497,7 +8561,7 @@
         <v>2.5899999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -8520,7 +8584,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" t="s">
         <v>101</v>
       </c>
@@ -8543,7 +8607,7 @@
         <v>0.25590000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -8566,7 +8630,7 @@
         <v>0.1464</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -8589,7 +8653,7 @@
         <v>1.7600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -8612,7 +8676,7 @@
         <v>1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -8635,7 +8699,7 @@
         <v>1.14E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" t="s">
         <v>106</v>
       </c>
@@ -8658,7 +8722,7 @@
         <v>0.15129999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -8688,6 +8752,11 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8699,9 +8768,9 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
@@ -8721,7 +8790,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>29</v>
       </c>
@@ -8741,7 +8810,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -8761,7 +8830,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
@@ -8784,6 +8853,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8798,7 +8872,7 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
@@ -8807,7 +8881,7 @@
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5">
       <c r="A1" s="11" t="s">
         <v>118</v>
       </c>
@@ -8824,7 +8898,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5">
       <c r="A2" s="11" t="s">
         <v>96</v>
       </c>
@@ -8839,7 +8913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5">
       <c r="A3" s="11"/>
       <c r="B3" t="s">
         <v>7</v>
@@ -8852,7 +8926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5">
       <c r="A4" s="11"/>
       <c r="B4" t="s">
         <v>8</v>
@@ -8867,7 +8941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5">
       <c r="A5" s="11"/>
       <c r="B5" t="s">
         <v>9</v>
@@ -8882,7 +8956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5">
       <c r="A6" s="11"/>
       <c r="B6" t="s">
         <v>10</v>
@@ -8897,7 +8971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="A7" s="11"/>
       <c r="B7" t="s">
         <v>84</v>
@@ -8912,7 +8986,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5">
       <c r="A8" s="11"/>
       <c r="B8" t="s">
         <v>136</v>
@@ -8927,7 +9001,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>137</v>
@@ -8942,7 +9016,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>138</v>
@@ -8957,13 +9031,13 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5">
       <c r="A11" s="11"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5">
       <c r="A12" s="11"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5">
       <c r="A13" s="11" t="s">
         <v>97</v>
       </c>
@@ -8978,7 +9052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -8990,7 +9064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5">
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -9004,7 +9078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5">
       <c r="B16" t="s">
         <v>9</v>
       </c>
@@ -9018,7 +9092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -9032,7 +9106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5">
       <c r="B18" t="s">
         <v>84</v>
       </c>
@@ -9046,7 +9120,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5">
       <c r="B19" t="s">
         <v>136</v>
       </c>
@@ -9060,7 +9134,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5">
       <c r="B20" t="s">
         <v>137</v>
       </c>
@@ -9074,7 +9148,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5">
       <c r="B21" t="s">
         <v>138</v>
       </c>
@@ -9088,7 +9162,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5">
       <c r="A24" s="11" t="s">
         <v>113</v>
       </c>
@@ -9109,6 +9183,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9120,9 +9199,9 @@
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -9145,7 +9224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
@@ -9168,7 +9247,7 @@
         <v>25.35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
         <v>24</v>
@@ -9189,7 +9268,7 @@
         <v>33.25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="12"/>
       <c r="B4" s="13" t="s">
         <v>27</v>
@@ -9210,7 +9289,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="12"/>
       <c r="B5" s="13" t="s">
         <v>28</v>
@@ -9231,7 +9310,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
@@ -9254,7 +9333,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
@@ -9274,7 +9353,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
@@ -9294,7 +9373,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
@@ -9314,7 +9393,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
@@ -9337,7 +9416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
@@ -9357,7 +9436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="4" t="s">
         <v>42</v>
       </c>
@@ -9377,7 +9456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1">
       <c r="B17" s="4" t="s">
         <v>43</v>
       </c>
@@ -9402,6 +9481,11 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9413,12 +9497,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>119</v>
       </c>
@@ -9438,7 +9522,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>12</v>
       </c>
@@ -9459,7 +9543,7 @@
         <v>3.1128200000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="B3" t="s">
         <v>115</v>
       </c>
@@ -9474,7 +9558,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="B4" t="s">
         <v>63</v>
       </c>
@@ -9491,14 +9575,14 @@
         <v>46.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="11"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="11"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="B7" s="11" t="s">
         <v>5</v>
       </c>
@@ -9507,7 +9591,7 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="11" t="s">
         <v>61</v>
       </c>
@@ -9527,7 +9611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
@@ -9544,7 +9628,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
@@ -9561,7 +9645,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
@@ -9578,7 +9662,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
@@ -9595,7 +9679,7 @@
         <v>999.99</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1">
       <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
@@ -9612,7 +9696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
       <c r="B14" s="5" t="s">
         <v>46</v>
       </c>
@@ -9629,7 +9713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
@@ -9650,6 +9734,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9664,7 +9753,7 @@
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
@@ -9672,7 +9761,7 @@
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" s="11" t="s">
         <v>61</v>
       </c>
@@ -9701,7 +9790,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
@@ -9730,7 +9819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9">
       <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
@@ -9753,7 +9842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9">
       <c r="C4" s="4" t="s">
         <v>27</v>
       </c>
@@ -9776,7 +9865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9">
       <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
@@ -9799,7 +9888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9">
       <c r="B6" t="s">
         <v>31</v>
       </c>
@@ -9825,7 +9914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9">
       <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
@@ -9848,7 +9937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9">
       <c r="C8" s="4" t="s">
         <v>27</v>
       </c>
@@ -9871,7 +9960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9">
       <c r="C9" s="4" t="s">
         <v>28</v>
       </c>
@@ -9894,7 +9983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9">
       <c r="B10" t="s">
         <v>33</v>
       </c>
@@ -9920,7 +10009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9">
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
@@ -9943,7 +10032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9">
       <c r="C12" s="4" t="s">
         <v>27</v>
       </c>
@@ -9966,7 +10055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9">
       <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
@@ -9989,7 +10078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9">
       <c r="B14" t="s">
         <v>34</v>
       </c>
@@ -10015,7 +10104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9">
       <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
@@ -10038,7 +10127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9">
       <c r="C16" s="4" t="s">
         <v>27</v>
       </c>
@@ -10061,7 +10150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9">
       <c r="C17" s="4" t="s">
         <v>28</v>
       </c>
@@ -10084,7 +10173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9">
       <c r="B18" t="s">
         <v>38</v>
       </c>
@@ -10110,7 +10199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9">
       <c r="C19" s="4" t="s">
         <v>24</v>
       </c>
@@ -10133,7 +10222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9">
       <c r="C20" s="4" t="s">
         <v>27</v>
       </c>
@@ -10156,7 +10245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9">
       <c r="C21" s="4" t="s">
         <v>28</v>
       </c>
@@ -10179,7 +10268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9">
       <c r="A24" s="11" t="s">
         <v>30</v>
       </c>
@@ -10208,7 +10297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9">
       <c r="C25" s="4" t="s">
         <v>24</v>
       </c>
@@ -10231,7 +10320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9">
       <c r="C26" s="4" t="s">
         <v>27</v>
       </c>
@@ -10254,7 +10343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9">
       <c r="C27" s="4" t="s">
         <v>28</v>
       </c>
@@ -10277,7 +10366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9">
       <c r="B28" t="s">
         <v>31</v>
       </c>
@@ -10303,7 +10392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9">
       <c r="C29" s="4" t="s">
         <v>24</v>
       </c>
@@ -10326,7 +10415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9">
       <c r="C30" s="4" t="s">
         <v>27</v>
       </c>
@@ -10349,7 +10438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9">
       <c r="C31" s="4" t="s">
         <v>28</v>
       </c>
@@ -10372,7 +10461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9">
       <c r="B32" t="s">
         <v>33</v>
       </c>
@@ -10398,7 +10487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9">
       <c r="C33" s="4" t="s">
         <v>24</v>
       </c>
@@ -10421,7 +10510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:9">
       <c r="C34" s="4" t="s">
         <v>27</v>
       </c>
@@ -10444,7 +10533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:9">
       <c r="C35" s="4" t="s">
         <v>28</v>
       </c>
@@ -10467,7 +10556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:9">
       <c r="B36" t="s">
         <v>34</v>
       </c>
@@ -10493,7 +10582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:9">
       <c r="C37" s="4" t="s">
         <v>24</v>
       </c>
@@ -10516,7 +10605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:9">
       <c r="C38" s="4" t="s">
         <v>27</v>
       </c>
@@ -10539,7 +10628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:9">
       <c r="C39" s="4" t="s">
         <v>28</v>
       </c>
@@ -10562,7 +10651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:9">
       <c r="B40" t="s">
         <v>38</v>
       </c>
@@ -10588,7 +10677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:9">
       <c r="C41" s="4" t="s">
         <v>24</v>
       </c>
@@ -10611,7 +10700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:9">
       <c r="C42" s="4" t="s">
         <v>27</v>
       </c>
@@ -10634,7 +10723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:9">
       <c r="C43" s="4" t="s">
         <v>28</v>
       </c>
@@ -10657,7 +10746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:9">
       <c r="A46" s="11" t="s">
         <v>39</v>
       </c>
@@ -10686,7 +10775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:9">
       <c r="C47" s="4" t="s">
         <v>41</v>
       </c>
@@ -10709,7 +10798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:9">
       <c r="C48" s="4" t="s">
         <v>42</v>
       </c>
@@ -10732,7 +10821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:9">
       <c r="C49" s="4" t="s">
         <v>43</v>
       </c>
@@ -10755,7 +10844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:9">
       <c r="B50" t="s">
         <v>16</v>
       </c>
@@ -10781,7 +10870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="51" spans="2:9">
       <c r="C51" s="4" t="s">
         <v>41</v>
       </c>
@@ -10804,7 +10893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:9">
       <c r="C52" s="4" t="s">
         <v>42</v>
       </c>
@@ -10827,7 +10916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="53" spans="2:9">
       <c r="C53" s="4" t="s">
         <v>43</v>
       </c>
@@ -10850,7 +10939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="54" spans="2:9">
       <c r="B54" t="s">
         <v>17</v>
       </c>
@@ -10876,7 +10965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="55" spans="2:9">
       <c r="C55" s="4" t="s">
         <v>41</v>
       </c>
@@ -10899,7 +10988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="56" spans="2:9">
       <c r="C56" s="4" t="s">
         <v>42</v>
       </c>
@@ -10922,7 +11011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="57" spans="2:9">
       <c r="C57" s="4" t="s">
         <v>43</v>
       </c>
@@ -10945,7 +11034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="58" spans="2:9">
       <c r="B58" t="s">
         <v>22</v>
       </c>
@@ -10971,7 +11060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="59" spans="2:9">
       <c r="C59" s="4" t="s">
         <v>41</v>
       </c>
@@ -10994,7 +11083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="60" spans="2:9">
       <c r="C60" s="4" t="s">
         <v>42</v>
       </c>
@@ -11017,7 +11106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="61" spans="2:9">
       <c r="C61" s="4" t="s">
         <v>43</v>
       </c>
@@ -11040,7 +11129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="62" spans="2:9">
       <c r="B62" t="s">
         <v>29</v>
       </c>
@@ -11066,7 +11155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="63" spans="2:9">
       <c r="C63" s="4" t="s">
         <v>41</v>
       </c>
@@ -11089,7 +11178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="64" spans="2:9">
       <c r="C64" s="4" t="s">
         <v>42</v>
       </c>
@@ -11112,7 +11201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:9">
       <c r="C65" s="4" t="s">
         <v>43</v>
       </c>
@@ -11135,7 +11224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:9">
       <c r="B66" t="s">
         <v>31</v>
       </c>
@@ -11161,7 +11250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:9">
       <c r="C67" s="4" t="s">
         <v>41</v>
       </c>
@@ -11184,7 +11273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:9">
       <c r="C68" s="4" t="s">
         <v>42</v>
       </c>
@@ -11207,7 +11296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:9">
       <c r="C69" s="4" t="s">
         <v>43</v>
       </c>
@@ -11230,7 +11319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:9">
       <c r="B70" t="s">
         <v>32</v>
       </c>
@@ -11256,7 +11345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:9">
       <c r="C71" s="4" t="s">
         <v>41</v>
       </c>
@@ -11279,7 +11368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:9">
       <c r="C72" s="4" t="s">
         <v>42</v>
       </c>
@@ -11302,7 +11391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:9">
       <c r="C73" s="4" t="s">
         <v>43</v>
       </c>
@@ -11325,7 +11414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:9">
       <c r="A76" s="11" t="s">
         <v>131</v>
       </c>
@@ -11354,7 +11443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:9">
       <c r="C77" s="4" t="s">
         <v>121</v>
       </c>
@@ -11377,7 +11466,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:9">
       <c r="B78" t="s">
         <v>100</v>
       </c>
@@ -11403,7 +11492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:9">
       <c r="C79" s="4" t="s">
         <v>121</v>
       </c>
@@ -11426,7 +11515,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:9">
       <c r="B80" t="s">
         <v>101</v>
       </c>
@@ -11452,7 +11541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:9">
       <c r="C81" s="4" t="s">
         <v>121</v>
       </c>
@@ -11475,7 +11564,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:9">
       <c r="A84" s="11" t="s">
         <v>112</v>
       </c>
@@ -11504,7 +11593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:9">
       <c r="C85" s="4" t="s">
         <v>41</v>
       </c>
@@ -11527,7 +11616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:9">
       <c r="C86" s="4" t="s">
         <v>42</v>
       </c>
@@ -11550,7 +11639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:9">
       <c r="C87" s="4" t="s">
         <v>43</v>
       </c>
@@ -11573,7 +11662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:9">
       <c r="A90" s="11" t="s">
         <v>132</v>
       </c>
@@ -11584,6 +11673,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -11598,7 +11692,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="36.6640625" customWidth="1"/>
     <col min="2" max="2" width="64.5" customWidth="1"/>
@@ -11608,7 +11702,7 @@
     <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
         <v>52</v>
       </c>
@@ -11631,7 +11725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2" s="11" t="s">
         <v>123</v>
       </c>
@@ -11652,7 +11746,7 @@
         <v>174.7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="B3" s="4" t="s">
         <v>29</v>
       </c>
@@ -11672,7 +11766,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" s="11" t="s">
         <v>122</v>
       </c>
@@ -11695,7 +11789,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7">
       <c r="B6" s="4" t="s">
         <v>48</v>
       </c>
@@ -11715,7 +11809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7">
       <c r="B7" s="4" t="s">
         <v>49</v>
       </c>
@@ -11735,7 +11829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7">
       <c r="B8" s="4" t="s">
         <v>150</v>
       </c>
@@ -11755,7 +11849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7">
       <c r="B9" s="4" t="s">
         <v>135</v>
       </c>
@@ -11775,7 +11869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7">
       <c r="B10" s="4" t="s">
         <v>50</v>
       </c>
@@ -11795,7 +11889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="14">
       <c r="A12" s="11" t="s">
         <v>124</v>
       </c>
@@ -11818,7 +11912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="14">
       <c r="B13" s="4" t="s">
         <v>58</v>
       </c>
@@ -11842,5 +11936,10 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added IFAS interventions for malaria areas to spreadsheet
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Bangladesh/2017Aug/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24300" windowHeight="13420" tabRatio="500" firstSheet="12" activeTab="14"/>
+    <workbookView xWindow="2920" yWindow="-18500" windowWidth="24480" windowHeight="18500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -23,13 +28,13 @@
     <sheet name="Interventions for children" sheetId="28" r:id="rId14"/>
     <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -1184,7 +1189,51 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="1">
+    <comment ref="I21" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+In baseline year, assuming only non-pregnant go to school</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+food insecure - default poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E29" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1206,7 +1255,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="1">
+    <comment ref="F29" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1228,7 +1277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="1">
+    <comment ref="G29" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1250,7 +1299,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H22" authorId="1">
+    <comment ref="H29" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1272,7 +1321,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I22" authorId="1">
+    <comment ref="I29" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1294,7 +1343,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E23" authorId="1">
+    <comment ref="E30" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1316,7 +1365,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F23" authorId="1">
+    <comment ref="F30" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1338,7 +1387,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G23" authorId="1">
+    <comment ref="G30" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1360,7 +1409,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H23" authorId="1">
+    <comment ref="H30" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1382,7 +1431,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I23" authorId="1">
+    <comment ref="I30" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1404,7 +1453,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E24" authorId="1">
+    <comment ref="E31" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1426,7 +1475,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F24" authorId="1">
+    <comment ref="F31" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1448,7 +1497,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G24" authorId="1">
+    <comment ref="G31" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1470,7 +1519,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H24" authorId="1">
+    <comment ref="H31" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1492,7 +1541,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I24" authorId="1">
+    <comment ref="I31" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1514,7 +1563,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C26" authorId="1">
+    <comment ref="C33" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1536,7 +1585,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D26" authorId="1">
+    <comment ref="D33" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1558,7 +1607,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E26" authorId="1">
+    <comment ref="E33" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1580,7 +1629,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F26" authorId="1">
+    <comment ref="F33" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1602,7 +1651,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G26" authorId="1">
+    <comment ref="G33" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1624,7 +1673,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H26" authorId="1">
+    <comment ref="H33" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1646,7 +1695,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I26" authorId="1">
+    <comment ref="I33" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1711,7 +1760,7 @@
     <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="E16" authorId="0">
+    <comment ref="E23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1734,7 +1783,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G17" authorId="0">
+    <comment ref="G24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1756,7 +1805,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="1">
+    <comment ref="B25" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1778,7 +1827,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L18" authorId="0">
+    <comment ref="L25" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1801,7 +1850,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B30" authorId="1">
+    <comment ref="B37" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1823,7 +1872,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B34" authorId="1">
+    <comment ref="B41" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1850,7 +1899,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="179">
   <si>
     <t>year</t>
   </si>
@@ -2366,6 +2415,27 @@
   </si>
   <si>
     <t>Severe diarrhea</t>
+  </si>
+  <si>
+    <t>IFAS poor: school (malaria area)</t>
+  </si>
+  <si>
+    <t>IFAS poor: community (malaria area)</t>
+  </si>
+  <si>
+    <t>IFAS poor: hospital (malaria area)</t>
+  </si>
+  <si>
+    <t>IFAS not poor: school (malaria area)</t>
+  </si>
+  <si>
+    <t>IFAS not poor: community (malaria area)</t>
+  </si>
+  <si>
+    <t>IFAS not poor: hospital (malaria area)</t>
+  </si>
+  <si>
+    <t>IFAS not poor: retailer (malaria area)</t>
   </si>
 </sst>
 </file>
@@ -4977,22 +5047,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor rgb="FF7030A0"/>
-  </sheetPr>
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" customHeight="1">
+    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>116</v>
       </c>
@@ -5003,7 +5070,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>65</v>
       </c>
@@ -5014,7 +5081,7 @@
         <v>15204000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
@@ -5022,7 +5089,7 @@
         <v>3118117</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="34" t="s">
         <v>143</v>
       </c>
@@ -5030,7 +5097,7 @@
         <v>171684000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
@@ -5039,7 +5106,7 @@
         <v>3677298.8269880489</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="34" t="s">
         <v>74</v>
       </c>
@@ -5047,7 +5114,7 @@
         <v>0.35199999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>73</v>
       </c>
@@ -5055,7 +5122,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="34" t="s">
         <v>75</v>
       </c>
@@ -5063,11 +5130,11 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="11"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="11" t="s">
         <v>149</v>
       </c>
@@ -5078,7 +5145,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>144</v>
       </c>
@@ -5086,7 +5153,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>145</v>
       </c>
@@ -5094,7 +5161,7 @@
         <v>25.36</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>146</v>
       </c>
@@ -5102,7 +5169,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>147</v>
       </c>
@@ -5110,7 +5177,7 @@
         <v>34.68</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>148</v>
       </c>
@@ -5118,11 +5185,11 @@
         <v>39.32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="11"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
         <v>77</v>
       </c>
@@ -5133,7 +5200,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="34" t="s">
         <v>108</v>
       </c>
@@ -5141,7 +5208,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="34" t="s">
         <v>109</v>
       </c>
@@ -5149,7 +5216,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="34" t="s">
         <v>110</v>
       </c>
@@ -5157,7 +5224,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="34" t="s">
         <v>78</v>
       </c>
@@ -5165,10 +5232,10 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="34"/>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>142</v>
       </c>
@@ -5179,7 +5246,7 @@
         <v>8634000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="52" t="s">
         <v>136</v>
       </c>
@@ -5187,7 +5254,7 @@
         <v>13550000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="52" t="s">
         <v>137</v>
       </c>
@@ -5195,7 +5262,7 @@
         <v>12394000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="52" t="s">
         <v>138</v>
       </c>
@@ -5203,11 +5270,11 @@
         <v>9148000</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="52"/>
       <c r="C30" s="54"/>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>130</v>
       </c>
@@ -5218,7 +5285,7 @@
         <v>0.29978973218277538</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="15.75" customHeight="1">
+    <row r="33" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="51" t="s">
         <v>136</v>
       </c>
@@ -5226,7 +5293,7 @@
         <v>0.52556568434139284</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="15.75" customHeight="1">
+    <row r="34" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="51" t="s">
         <v>137</v>
       </c>
@@ -5234,7 +5301,7 @@
         <v>0.16210210664201097</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="15.75" customHeight="1">
+    <row r="35" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="51" t="s">
         <v>138</v>
       </c>
@@ -5246,11 +5313,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5265,12 +5327,12 @@
       <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -5287,7 +5349,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
@@ -5304,14 +5366,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -5320,23 +5382,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="43.33203125" customWidth="1"/>
@@ -5347,7 +5404,7 @@
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>87</v>
       </c>
@@ -5377,7 +5434,7 @@
       </c>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
         <v>82</v>
       </c>
@@ -5406,7 +5463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
         <v>51</v>
       </c>
@@ -5432,7 +5489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4" t="s">
         <v>58</v>
       </c>
@@ -5458,7 +5515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
         <v>169</v>
       </c>
@@ -5486,7 +5543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>86</v>
       </c>
@@ -5514,7 +5571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>85</v>
       </c>
@@ -5541,7 +5598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
         <v>83</v>
       </c>
@@ -5571,7 +5628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>60</v>
       </c>
@@ -5597,7 +5654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>88</v>
       </c>
@@ -5623,7 +5680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>159</v>
       </c>
@@ -5650,7 +5707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="11" t="s">
         <v>95</v>
       </c>
@@ -5679,7 +5736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>163</v>
       </c>
@@ -5705,7 +5762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>164</v>
       </c>
@@ -5731,7 +5788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>165</v>
       </c>
@@ -5757,7 +5814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>166</v>
       </c>
@@ -5783,7 +5840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>167</v>
       </c>
@@ -5809,7 +5866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>168</v>
       </c>
@@ -5835,178 +5892,356 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A22" s="11" t="s">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="11"/>
+      <c r="B21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+      <c r="I21" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" t="s">
+        <v>173</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+      <c r="I22" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" t="s">
+        <v>174</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" t="s">
+        <v>175</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" t="s">
+        <v>176</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" t="s">
+        <v>177</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
+      <c r="I26" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" t="s">
+        <v>178</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+      <c r="I27" s="60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="3">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0</v>
-      </c>
-      <c r="E22" s="36">
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="F22" s="36">
+      <c r="F29" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="G22" s="36">
+      <c r="G29" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="H22" s="36">
+      <c r="H29" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="I22" s="36">
+      <c r="I29" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B23" s="4" t="s">
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B30" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="3">
-        <v>0</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0</v>
-      </c>
-      <c r="E23" s="3">
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F30" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G30" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H30" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I30" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B24" s="4" t="s">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B31" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C24" s="3">
-        <v>0</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0</v>
-      </c>
-      <c r="E24" s="3">
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F31" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G31" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H31" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I31" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B25" s="4" t="s">
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B32" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C25" s="3">
-        <v>0</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0</v>
-      </c>
-      <c r="E25" s="36">
-        <v>1</v>
-      </c>
-      <c r="F25" s="36">
-        <v>1</v>
-      </c>
-      <c r="G25" s="36">
-        <v>1</v>
-      </c>
-      <c r="H25" s="36">
-        <v>1</v>
-      </c>
-      <c r="I25" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B26" s="4" t="s">
+      <c r="C32" s="3">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0</v>
+      </c>
+      <c r="E32" s="36">
+        <v>1</v>
+      </c>
+      <c r="F32" s="36">
+        <v>1</v>
+      </c>
+      <c r="G32" s="36">
+        <v>1</v>
+      </c>
+      <c r="H32" s="36">
+        <v>1</v>
+      </c>
+      <c r="I32" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B33" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="36">
+      <c r="C33" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="D26" s="36">
+      <c r="D33" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="E26" s="36">
+      <c r="E33" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="F26" s="36">
+      <c r="F33" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="G26" s="36">
+      <c r="G33" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="H26" s="36">
+      <c r="H33" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="I26" s="36">
+      <c r="I33" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
+    <row r="35" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6021,14 +6256,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -6048,7 +6283,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -6068,7 +6303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>55</v>
       </c>
@@ -6085,7 +6320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -6105,7 +6340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>55</v>
       </c>
@@ -6122,7 +6357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>133</v>
       </c>
@@ -6142,7 +6377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>55</v>
       </c>
@@ -6163,11 +6398,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6176,13 +6406,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A11" sqref="A11:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="42.6640625" customWidth="1"/>
@@ -6191,7 +6421,7 @@
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="14" customHeight="1">
+    <row r="1" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>52</v>
       </c>
@@ -6238,7 +6468,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
         <v>160</v>
       </c>
@@ -6285,7 +6515,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>159</v>
       </c>
@@ -6329,7 +6559,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>162</v>
       </c>
@@ -6373,7 +6603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>163</v>
       </c>
@@ -6417,7 +6647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>164</v>
       </c>
@@ -6461,7 +6691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>165</v>
       </c>
@@ -6505,7 +6735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
         <v>166</v>
       </c>
@@ -6549,7 +6779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
         <v>167</v>
       </c>
@@ -6593,7 +6823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>168</v>
       </c>
@@ -6637,339 +6867,642 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B11" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0.73</v>
+      </c>
+      <c r="I11">
+        <v>0.73</v>
+      </c>
+      <c r="J11">
+        <v>0.73</v>
+      </c>
+      <c r="K11">
+        <v>0.73</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0.73</v>
+      </c>
+      <c r="I12">
+        <v>0.73</v>
+      </c>
+      <c r="J12">
+        <v>0.73</v>
+      </c>
+      <c r="K12">
+        <v>0.73</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0.73</v>
+      </c>
+      <c r="I13">
+        <v>0.73</v>
+      </c>
+      <c r="J13">
+        <v>0.73</v>
+      </c>
+      <c r="K13">
+        <v>0.73</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0.73</v>
+      </c>
+      <c r="I14">
+        <v>0.73</v>
+      </c>
+      <c r="J14">
+        <v>0.73</v>
+      </c>
+      <c r="K14">
+        <v>0.73</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0.73</v>
+      </c>
+      <c r="I15">
+        <v>0.73</v>
+      </c>
+      <c r="J15">
+        <v>0.73</v>
+      </c>
+      <c r="K15">
+        <v>0.73</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B16" t="s">
+        <v>177</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0.73</v>
+      </c>
+      <c r="I16">
+        <v>0.73</v>
+      </c>
+      <c r="J16">
+        <v>0.73</v>
+      </c>
+      <c r="K16">
+        <v>0.73</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0.73</v>
+      </c>
+      <c r="I17">
+        <v>0.73</v>
+      </c>
+      <c r="J17">
+        <v>0.73</v>
+      </c>
+      <c r="K17">
+        <v>0.73</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B18" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" s="61">
-        <v>1</v>
-      </c>
-      <c r="F11" s="61">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-      <c r="O11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="11" t="s">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="61">
+        <v>1</v>
+      </c>
+      <c r="F18" s="61">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A20" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="57">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="F13" s="57">
+      <c r="F20" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="G13" s="57">
+      <c r="G20" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="H13" s="57">
+      <c r="H20" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="I13" s="57">
+      <c r="I20" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="J13" s="57">
+      <c r="J20" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="K13" s="57">
+      <c r="K20" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="L13" s="57">
+      <c r="L20" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="M13" s="57">
+      <c r="M20" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="N13" s="57">
+      <c r="N20" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="O13" s="57">
+      <c r="O20" s="57">
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
-      <c r="B14" s="4" t="s">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B21" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" s="57">
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="F14" s="57">
+      <c r="F21" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="G14" s="57">
+      <c r="G21" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="H14" s="57">
+      <c r="H21" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="I14" s="57">
+      <c r="I21" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="J14" s="57">
+      <c r="J21" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="K14" s="57">
+      <c r="K21" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="L14" s="57">
+      <c r="L21" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="M14" s="57">
+      <c r="M21" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="N14" s="57">
+      <c r="N21" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="O14" s="57">
+      <c r="O21" s="57">
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
-      <c r="B15" s="4" t="s">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B22" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="57">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="F15" s="57">
+      <c r="F22" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="G15" s="57">
+      <c r="G22" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="H15" s="57">
+      <c r="H22" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="I15" s="57">
+      <c r="I22" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="J15" s="57">
+      <c r="J22" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="K15" s="57">
+      <c r="K22" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="L15" s="57">
+      <c r="L22" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="M15" s="57">
+      <c r="M22" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="N15" s="57">
+      <c r="N22" s="57">
         <v>0.97599999999999998</v>
       </c>
-      <c r="O15" s="57">
+      <c r="O22" s="57">
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
-      <c r="B16" s="4" t="s">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B23" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="58">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="58">
         <v>0.9</v>
       </c>
-      <c r="F16" s="58">
+      <c r="F23" s="58">
         <v>0.9</v>
       </c>
-      <c r="G16" s="58">
+      <c r="G23" s="58">
         <v>0.9</v>
       </c>
-      <c r="H16" s="58">
+      <c r="H23" s="58">
         <v>0.9</v>
       </c>
-      <c r="I16" s="58">
+      <c r="I23" s="58">
         <v>0.9</v>
       </c>
-      <c r="J16" s="58">
+      <c r="J23" s="58">
         <v>0.9</v>
       </c>
-      <c r="K16" s="58">
+      <c r="K23" s="58">
         <v>0.9</v>
       </c>
-      <c r="L16" s="58">
+      <c r="L23" s="58">
         <v>0.9</v>
       </c>
-      <c r="M16" s="58">
+      <c r="M23" s="58">
         <v>0.9</v>
       </c>
-      <c r="N16" s="58">
+      <c r="N23" s="58">
         <v>0.9</v>
       </c>
-      <c r="O16" s="58">
+      <c r="O23" s="58">
         <v>0.9</v>
       </c>
     </row>
-    <row r="17" spans="2:15">
-      <c r="B17" t="s">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B24" t="s">
         <v>85</v>
       </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" s="57">
-        <v>1</v>
-      </c>
-      <c r="F17" s="57">
-        <v>1</v>
-      </c>
-      <c r="G17" s="58">
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="57">
+        <v>1</v>
+      </c>
+      <c r="F24" s="57">
+        <v>1</v>
+      </c>
+      <c r="G24" s="58">
         <v>0.8</v>
       </c>
-      <c r="H17" s="57">
-        <v>1</v>
-      </c>
-      <c r="I17" s="57">
-        <v>1</v>
-      </c>
-      <c r="J17" s="57">
-        <v>1</v>
-      </c>
-      <c r="K17" s="57">
-        <v>1</v>
-      </c>
-      <c r="L17" s="57">
-        <v>1</v>
-      </c>
-      <c r="M17" s="57">
-        <v>1</v>
-      </c>
-      <c r="N17" s="57">
-        <v>1</v>
-      </c>
-      <c r="O17" s="57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15">
-      <c r="B18" s="4" t="s">
+      <c r="H24" s="57">
+        <v>1</v>
+      </c>
+      <c r="I24" s="57">
+        <v>1</v>
+      </c>
+      <c r="J24" s="57">
+        <v>1</v>
+      </c>
+      <c r="K24" s="57">
+        <v>1</v>
+      </c>
+      <c r="L24" s="57">
+        <v>1</v>
+      </c>
+      <c r="M24" s="57">
+        <v>1</v>
+      </c>
+      <c r="N24" s="57">
+        <v>1</v>
+      </c>
+      <c r="O24" s="57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B25" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" s="57">
-        <v>1</v>
-      </c>
-      <c r="F18" s="57">
-        <v>1</v>
-      </c>
-      <c r="G18" s="57">
-        <v>1</v>
-      </c>
-      <c r="H18" s="57">
-        <v>1</v>
-      </c>
-      <c r="I18" s="57">
-        <v>1</v>
-      </c>
-      <c r="J18" s="57">
-        <v>1</v>
-      </c>
-      <c r="K18" s="57">
-        <v>1</v>
-      </c>
-      <c r="L18" s="58">
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="57">
+        <v>1</v>
+      </c>
+      <c r="F25" s="57">
+        <v>1</v>
+      </c>
+      <c r="G25" s="57">
+        <v>1</v>
+      </c>
+      <c r="H25" s="57">
+        <v>1</v>
+      </c>
+      <c r="I25" s="57">
+        <v>1</v>
+      </c>
+      <c r="J25" s="57">
+        <v>1</v>
+      </c>
+      <c r="K25" s="57">
+        <v>1</v>
+      </c>
+      <c r="L25" s="58">
         <v>0.9</v>
       </c>
-      <c r="M18" s="58">
+      <c r="M25" s="58">
         <v>0.9</v>
       </c>
-      <c r="N18" s="58">
+      <c r="N25" s="58">
         <v>0.9</v>
       </c>
-      <c r="O18" s="58">
+      <c r="O25" s="58">
         <v>0.9</v>
       </c>
     </row>
-    <row r="30" spans="2:15"/>
-    <row r="31" spans="2:15">
-      <c r="B31" s="4"/>
-    </row>
-    <row r="32" spans="2:15">
-      <c r="B32" s="4"/>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" s="4"/>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.15"/>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B38" s="4"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B39" s="4"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B40" s="4"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B41" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6984,7 +7517,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="27.5" customWidth="1"/>
     <col min="3" max="3" width="38.1640625" customWidth="1"/>
@@ -6994,7 +7527,7 @@
     <col min="8" max="8" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -7020,7 +7553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>51</v>
       </c>
@@ -7046,7 +7579,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C3" t="s">
         <v>70</v>
       </c>
@@ -7066,7 +7599,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -7088,7 +7621,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="12"/>
       <c r="B5" s="61" t="s">
         <v>171</v>
@@ -7112,7 +7645,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -7120,11 +7653,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7132,11 +7660,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="43.83203125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -7144,7 +7672,7 @@
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -7158,7 +7686,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
@@ -7175,7 +7703,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>51</v>
       </c>
@@ -7192,7 +7720,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>58</v>
       </c>
@@ -7209,7 +7737,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>169</v>
       </c>
@@ -7226,7 +7754,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>86</v>
       </c>
@@ -7237,7 +7765,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="34" t="s">
         <v>85</v>
       </c>
@@ -7248,7 +7776,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -7265,7 +7793,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -7282,7 +7810,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>88</v>
       </c>
@@ -7293,7 +7821,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>159</v>
       </c>
@@ -7304,7 +7832,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>162</v>
       </c>
@@ -7315,7 +7843,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>163</v>
       </c>
@@ -7326,7 +7854,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>164</v>
       </c>
@@ -7337,7 +7865,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>165</v>
       </c>
@@ -7348,7 +7876,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>166</v>
       </c>
@@ -7356,7 +7884,7 @@
       <c r="C16" s="35"/>
       <c r="D16" s="14"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>167</v>
       </c>
@@ -7364,7 +7892,7 @@
       <c r="C17" s="35"/>
       <c r="D17" s="14"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>168</v>
       </c>
@@ -7372,7 +7900,7 @@
       <c r="C18" s="14"/>
       <c r="D18" s="35"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>91</v>
       </c>
@@ -7382,7 +7910,7 @@
       </c>
       <c r="D19" s="35"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>92</v>
       </c>
@@ -7392,7 +7920,7 @@
       </c>
       <c r="D20" s="35"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>93</v>
       </c>
@@ -7402,7 +7930,7 @@
       </c>
       <c r="D21" s="35"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
         <v>111</v>
       </c>
@@ -7410,7 +7938,7 @@
       <c r="C22" s="14"/>
       <c r="D22" s="35"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
         <v>89</v>
       </c>
@@ -7418,27 +7946,27 @@
       <c r="C23" s="14"/>
       <c r="D23" s="35"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
     </row>
@@ -7446,26 +7974,18 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor rgb="FF7030A0"/>
-  </sheetPr>
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
@@ -7473,7 +7993,7 @@
     <col min="11" max="11" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7511,7 +8031,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>2017</v>
       </c>
@@ -7553,7 +8073,7 @@
         <v>173766200</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>2018</v>
       </c>
@@ -7595,7 +8115,7 @@
         <v>175848400</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>2019</v>
       </c>
@@ -7637,7 +8157,7 @@
         <v>177930600</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>2020</v>
       </c>
@@ -7679,7 +8199,7 @@
         <v>180012800</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>2021</v>
       </c>
@@ -7721,7 +8241,7 @@
         <v>182095000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>2022</v>
       </c>
@@ -7763,7 +8283,7 @@
         <v>183822800</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>2023</v>
       </c>
@@ -7805,7 +8325,7 @@
         <v>185550600</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>2024</v>
       </c>
@@ -7847,7 +8367,7 @@
         <v>187278400</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>2025</v>
       </c>
@@ -7889,7 +8409,7 @@
         <v>189006200</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>2026</v>
       </c>
@@ -7931,7 +8451,7 @@
         <v>190734000</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>2027</v>
       </c>
@@ -7973,7 +8493,7 @@
         <v>192287600</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>2028</v>
       </c>
@@ -8015,7 +8535,7 @@
         <v>193841200</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>2029</v>
       </c>
@@ -8057,7 +8577,7 @@
         <v>195394800</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>2030</v>
       </c>
@@ -8103,11 +8623,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8119,12 +8634,12 @@
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -8147,7 +8662,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -8170,7 +8685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -8193,7 +8708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -8216,7 +8731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -8239,7 +8754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -8262,7 +8777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -8285,7 +8800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -8308,7 +8823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -8331,7 +8846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -8354,7 +8869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -8377,7 +8892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -8400,7 +8915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -8423,7 +8938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -8446,7 +8961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -8469,7 +8984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -8492,7 +9007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -8515,7 +9030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -8538,7 +9053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -8561,7 +9076,7 @@
         <v>2.5899999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -8584,7 +9099,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>101</v>
       </c>
@@ -8607,7 +9122,7 @@
         <v>0.25590000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -8630,7 +9145,7 @@
         <v>0.1464</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -8653,7 +9168,7 @@
         <v>1.7600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -8676,7 +9191,7 @@
         <v>1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -8699,7 +9214,7 @@
         <v>1.14E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>106</v>
       </c>
@@ -8722,7 +9237,7 @@
         <v>0.15129999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -8752,11 +9267,6 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8768,9 +9278,9 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
@@ -8790,7 +9300,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>29</v>
       </c>
@@ -8810,7 +9320,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -8830,7 +9340,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
@@ -8853,26 +9363,18 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor rgb="FF7030A0"/>
-  </sheetPr>
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
@@ -8881,7 +9383,7 @@
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>118</v>
       </c>
@@ -8898,7 +9400,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
         <v>96</v>
       </c>
@@ -8913,7 +9415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="11"/>
       <c r="B3" t="s">
         <v>7</v>
@@ -8926,7 +9428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="11"/>
       <c r="B4" t="s">
         <v>8</v>
@@ -8941,7 +9443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="11"/>
       <c r="B5" t="s">
         <v>9</v>
@@ -8956,7 +9458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="11"/>
       <c r="B6" t="s">
         <v>10</v>
@@ -8971,7 +9473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="11"/>
       <c r="B7" t="s">
         <v>84</v>
@@ -8986,7 +9488,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="11"/>
       <c r="B8" t="s">
         <v>136</v>
@@ -9001,7 +9503,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>137</v>
@@ -9016,7 +9518,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>138</v>
@@ -9031,13 +9533,13 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="11"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="11"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="11" t="s">
         <v>97</v>
       </c>
@@ -9052,7 +9554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -9064,7 +9566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -9078,7 +9580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>9</v>
       </c>
@@ -9092,7 +9594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -9106,7 +9608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>84</v>
       </c>
@@ -9120,7 +9622,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>136</v>
       </c>
@@ -9134,7 +9636,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>137</v>
       </c>
@@ -9148,7 +9650,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
         <v>138</v>
       </c>
@@ -9162,7 +9664,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="11" t="s">
         <v>113</v>
       </c>
@@ -9183,11 +9685,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9199,9 +9696,9 @@
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -9224,7 +9721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
@@ -9247,7 +9744,7 @@
         <v>25.35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
         <v>24</v>
@@ -9268,7 +9765,7 @@
         <v>33.25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="12"/>
       <c r="B4" s="13" t="s">
         <v>27</v>
@@ -9289,7 +9786,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="12"/>
       <c r="B5" s="13" t="s">
         <v>28</v>
@@ -9310,7 +9807,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
@@ -9333,7 +9830,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
@@ -9353,7 +9850,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
@@ -9373,7 +9870,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
@@ -9393,7 +9890,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
@@ -9416,7 +9913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
@@ -9436,7 +9933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="4" t="s">
         <v>42</v>
       </c>
@@ -9456,7 +9953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="4" t="s">
         <v>43</v>
       </c>
@@ -9481,11 +9978,6 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9497,12 +9989,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>119</v>
       </c>
@@ -9522,7 +10014,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
         <v>12</v>
       </c>
@@ -9543,7 +10035,7 @@
         <v>3.1128200000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>115</v>
       </c>
@@ -9558,7 +10050,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>63</v>
       </c>
@@ -9575,14 +10067,14 @@
         <v>46.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="11"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="11"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="11" t="s">
         <v>5</v>
       </c>
@@ -9591,7 +10083,7 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
         <v>61</v>
       </c>
@@ -9611,7 +10103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
@@ -9628,7 +10120,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
@@ -9645,7 +10137,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
@@ -9662,7 +10154,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
@@ -9679,7 +10171,7 @@
         <v>999.99</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
@@ -9696,7 +10188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>46</v>
       </c>
@@ -9713,7 +10205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
@@ -9734,11 +10226,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9753,7 +10240,7 @@
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
@@ -9761,7 +10248,7 @@
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>61</v>
       </c>
@@ -9790,7 +10277,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
@@ -9819,7 +10306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
@@ -9842,7 +10329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C4" s="4" t="s">
         <v>27</v>
       </c>
@@ -9865,7 +10352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
@@ -9888,7 +10375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>31</v>
       </c>
@@ -9914,7 +10401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
@@ -9937,7 +10424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C8" s="4" t="s">
         <v>27</v>
       </c>
@@ -9960,7 +10447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C9" s="4" t="s">
         <v>28</v>
       </c>
@@ -9983,7 +10470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>33</v>
       </c>
@@ -10009,7 +10496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
@@ -10032,7 +10519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C12" s="4" t="s">
         <v>27</v>
       </c>
@@ -10055,7 +10542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
@@ -10078,7 +10565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>34</v>
       </c>
@@ -10104,7 +10591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
@@ -10127,7 +10614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C16" s="4" t="s">
         <v>27</v>
       </c>
@@ -10150,7 +10637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C17" s="4" t="s">
         <v>28</v>
       </c>
@@ -10173,7 +10660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>38</v>
       </c>
@@ -10199,7 +10686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C19" s="4" t="s">
         <v>24</v>
       </c>
@@ -10222,7 +10709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C20" s="4" t="s">
         <v>27</v>
       </c>
@@ -10245,7 +10732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C21" s="4" t="s">
         <v>28</v>
       </c>
@@ -10268,7 +10755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="11" t="s">
         <v>30</v>
       </c>
@@ -10297,7 +10784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C25" s="4" t="s">
         <v>24</v>
       </c>
@@ -10320,7 +10807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C26" s="4" t="s">
         <v>27</v>
       </c>
@@ -10343,7 +10830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C27" s="4" t="s">
         <v>28</v>
       </c>
@@ -10366,7 +10853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
         <v>31</v>
       </c>
@@ -10392,7 +10879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C29" s="4" t="s">
         <v>24</v>
       </c>
@@ -10415,7 +10902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C30" s="4" t="s">
         <v>27</v>
       </c>
@@ -10438,7 +10925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C31" s="4" t="s">
         <v>28</v>
       </c>
@@ -10461,7 +10948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>33</v>
       </c>
@@ -10487,7 +10974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C33" s="4" t="s">
         <v>24</v>
       </c>
@@ -10510,7 +10997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C34" s="4" t="s">
         <v>27</v>
       </c>
@@ -10533,7 +11020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C35" s="4" t="s">
         <v>28</v>
       </c>
@@ -10556,7 +11043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B36" t="s">
         <v>34</v>
       </c>
@@ -10582,7 +11069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C37" s="4" t="s">
         <v>24</v>
       </c>
@@ -10605,7 +11092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C38" s="4" t="s">
         <v>27</v>
       </c>
@@ -10628,7 +11115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C39" s="4" t="s">
         <v>28</v>
       </c>
@@ -10651,7 +11138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B40" t="s">
         <v>38</v>
       </c>
@@ -10677,7 +11164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C41" s="4" t="s">
         <v>24</v>
       </c>
@@ -10700,7 +11187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C42" s="4" t="s">
         <v>27</v>
       </c>
@@ -10723,7 +11210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C43" s="4" t="s">
         <v>28</v>
       </c>
@@ -10746,7 +11233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="11" t="s">
         <v>39</v>
       </c>
@@ -10775,7 +11262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C47" s="4" t="s">
         <v>41</v>
       </c>
@@ -10798,7 +11285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C48" s="4" t="s">
         <v>42</v>
       </c>
@@ -10821,7 +11308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:9">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C49" s="4" t="s">
         <v>43</v>
       </c>
@@ -10844,7 +11331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:9">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B50" t="s">
         <v>16</v>
       </c>
@@ -10870,7 +11357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:9">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C51" s="4" t="s">
         <v>41</v>
       </c>
@@ -10893,7 +11380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:9">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C52" s="4" t="s">
         <v>42</v>
       </c>
@@ -10916,7 +11403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:9">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C53" s="4" t="s">
         <v>43</v>
       </c>
@@ -10939,7 +11426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:9">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B54" t="s">
         <v>17</v>
       </c>
@@ -10965,7 +11452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:9">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C55" s="4" t="s">
         <v>41</v>
       </c>
@@ -10988,7 +11475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:9">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C56" s="4" t="s">
         <v>42</v>
       </c>
@@ -11011,7 +11498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:9">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C57" s="4" t="s">
         <v>43</v>
       </c>
@@ -11034,7 +11521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:9">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B58" t="s">
         <v>22</v>
       </c>
@@ -11060,7 +11547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:9">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C59" s="4" t="s">
         <v>41</v>
       </c>
@@ -11083,7 +11570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:9">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C60" s="4" t="s">
         <v>42</v>
       </c>
@@ -11106,7 +11593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:9">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C61" s="4" t="s">
         <v>43</v>
       </c>
@@ -11129,7 +11616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:9">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B62" t="s">
         <v>29</v>
       </c>
@@ -11155,7 +11642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:9">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C63" s="4" t="s">
         <v>41</v>
       </c>
@@ -11178,7 +11665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:9">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C64" s="4" t="s">
         <v>42</v>
       </c>
@@ -11201,7 +11688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C65" s="4" t="s">
         <v>43</v>
       </c>
@@ -11224,7 +11711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B66" t="s">
         <v>31</v>
       </c>
@@ -11250,7 +11737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C67" s="4" t="s">
         <v>41</v>
       </c>
@@ -11273,7 +11760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C68" s="4" t="s">
         <v>42</v>
       </c>
@@ -11296,7 +11783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C69" s="4" t="s">
         <v>43</v>
       </c>
@@ -11319,7 +11806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B70" t="s">
         <v>32</v>
       </c>
@@ -11345,7 +11832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C71" s="4" t="s">
         <v>41</v>
       </c>
@@ -11368,7 +11855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C72" s="4" t="s">
         <v>42</v>
       </c>
@@ -11391,7 +11878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C73" s="4" t="s">
         <v>43</v>
       </c>
@@ -11414,7 +11901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A76" s="11" t="s">
         <v>131</v>
       </c>
@@ -11443,7 +11930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C77" s="4" t="s">
         <v>121</v>
       </c>
@@ -11466,7 +11953,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B78" t="s">
         <v>100</v>
       </c>
@@ -11492,7 +11979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C79" s="4" t="s">
         <v>121</v>
       </c>
@@ -11515,7 +12002,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B80" t="s">
         <v>101</v>
       </c>
@@ -11541,7 +12028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C81" s="4" t="s">
         <v>121</v>
       </c>
@@ -11564,7 +12051,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A84" s="11" t="s">
         <v>112</v>
       </c>
@@ -11593,7 +12080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C85" s="4" t="s">
         <v>41</v>
       </c>
@@ -11616,7 +12103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C86" s="4" t="s">
         <v>42</v>
       </c>
@@ -11639,7 +12126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C87" s="4" t="s">
         <v>43</v>
       </c>
@@ -11662,7 +12149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A90" s="11" t="s">
         <v>132</v>
       </c>
@@ -11673,11 +12160,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -11692,7 +12174,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="36.6640625" customWidth="1"/>
     <col min="2" max="2" width="64.5" customWidth="1"/>
@@ -11702,7 +12184,7 @@
     <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>52</v>
       </c>
@@ -11725,7 +12207,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
         <v>123</v>
       </c>
@@ -11746,7 +12228,7 @@
         <v>174.7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
         <v>29</v>
       </c>
@@ -11766,7 +12248,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="11" t="s">
         <v>122</v>
       </c>
@@ -11789,7 +12271,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>48</v>
       </c>
@@ -11809,7 +12291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>49</v>
       </c>
@@ -11829,7 +12311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B8" s="4" t="s">
         <v>150</v>
       </c>
@@ -11849,7 +12331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>135</v>
       </c>
@@ -11869,7 +12351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>50</v>
       </c>
@@ -11889,7 +12371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>124</v>
       </c>
@@ -11912,7 +12394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14">
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>58</v>
       </c>
@@ -11936,10 +12418,5 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added IFAS interventions in malaria areas to cost and coverages tab
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="-18500" windowWidth="24480" windowHeight="18500" tabRatio="500"/>
+    <workbookView xWindow="2920" yWindow="-18500" windowWidth="24480" windowHeight="18500" tabRatio="500" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -366,7 +366,29 @@
         </r>
       </text>
     </comment>
-    <comment ref="C21" authorId="1">
+    <comment ref="A25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+There is no unit cost for this to impact the budget.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C28" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1899,7 +1921,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="179">
   <si>
     <t>year</t>
   </si>
@@ -5049,7 +5071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -6409,7 +6431,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD17"/>
+      <selection activeCell="B11" sqref="B11:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7658,10 +7680,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7884,7 +7906,7 @@
       <c r="C16" s="35"/>
       <c r="D16" s="14"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>167</v>
       </c>
@@ -7892,7 +7914,7 @@
       <c r="C17" s="35"/>
       <c r="D17" s="14"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>168</v>
       </c>
@@ -7900,75 +7922,143 @@
       <c r="C18" s="14"/>
       <c r="D18" s="35"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>173</v>
+      </c>
+      <c r="B20" s="14"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" s="14"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>175</v>
+      </c>
+      <c r="B22" s="14"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>176</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="14"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>178</v>
+      </c>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="35"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15">
+      <c r="B26" s="14"/>
+      <c r="C26" s="15">
         <v>0.12</v>
       </c>
-      <c r="D19" s="35"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="4" t="s">
+      <c r="D26" s="35"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15">
+      <c r="B27" s="14"/>
+      <c r="C27" s="15">
         <v>0.05</v>
       </c>
-      <c r="D20" s="35"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="4" t="s">
+      <c r="D27" s="35"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15">
+      <c r="B28" s="14"/>
+      <c r="C28" s="15">
         <v>0.8</v>
       </c>
-      <c r="D21" s="35"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="4" t="s">
+      <c r="D28" s="35"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="35"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="4" t="s">
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="35"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="35"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="35"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added fictional value for bed net coverage
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Bangladesh/2017Aug/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="-18500" windowWidth="24480" windowHeight="18500" tabRatio="500" firstSheet="10" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22220" windowHeight="12640" tabRatio="500" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -28,13 +23,13 @@
     <sheet name="Interventions for children" sheetId="28" r:id="rId14"/>
     <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -407,6 +402,28 @@
           </rPr>
           <t xml:space="preserve">
 This is the fraction of the population eating these staples and belongs here.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B30" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fictional</t>
         </r>
       </text>
     </comment>
@@ -5075,13 +5092,13 @@
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="16" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>116</v>
       </c>
@@ -5092,7 +5109,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>65</v>
       </c>
@@ -5103,7 +5120,7 @@
         <v>15204000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
@@ -5111,7 +5128,7 @@
         <v>3118117</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="B4" s="34" t="s">
         <v>143</v>
       </c>
@@ -5119,7 +5136,7 @@
         <v>171684000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
@@ -5128,7 +5145,7 @@
         <v>3677298.8269880489</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="B6" s="34" t="s">
         <v>74</v>
       </c>
@@ -5136,7 +5153,7 @@
         <v>0.35199999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1">
       <c r="B7" s="4" t="s">
         <v>73</v>
       </c>
@@ -5144,7 +5161,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1">
       <c r="B8" s="34" t="s">
         <v>75</v>
       </c>
@@ -5152,11 +5169,11 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1">
       <c r="B10" s="11"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1">
       <c r="A11" s="11" t="s">
         <v>149</v>
       </c>
@@ -5167,7 +5184,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1">
       <c r="B12" t="s">
         <v>144</v>
       </c>
@@ -5175,7 +5192,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1">
       <c r="B13" t="s">
         <v>145</v>
       </c>
@@ -5183,7 +5200,7 @@
         <v>25.36</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1">
       <c r="B14" t="s">
         <v>146</v>
       </c>
@@ -5191,7 +5208,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1">
       <c r="B15" t="s">
         <v>147</v>
       </c>
@@ -5199,7 +5216,7 @@
         <v>34.68</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1">
       <c r="B16" t="s">
         <v>148</v>
       </c>
@@ -5207,11 +5224,11 @@
         <v>39.32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1">
       <c r="B18" s="11"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1">
       <c r="A19" s="11" t="s">
         <v>77</v>
       </c>
@@ -5222,7 +5239,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1">
       <c r="B20" s="34" t="s">
         <v>108</v>
       </c>
@@ -5230,7 +5247,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1">
       <c r="B21" s="34" t="s">
         <v>109</v>
       </c>
@@ -5238,7 +5255,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1">
       <c r="B22" s="34" t="s">
         <v>110</v>
       </c>
@@ -5246,7 +5263,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="B23" s="34" t="s">
         <v>78</v>
       </c>
@@ -5254,10 +5271,10 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1">
       <c r="B25" s="34"/>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="A26" s="11" t="s">
         <v>142</v>
       </c>
@@ -5268,7 +5285,7 @@
         <v>8634000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="15" customHeight="1">
       <c r="B27" s="52" t="s">
         <v>136</v>
       </c>
@@ -5276,7 +5293,7 @@
         <v>13550000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1">
       <c r="B28" s="52" t="s">
         <v>137</v>
       </c>
@@ -5284,7 +5301,7 @@
         <v>12394000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1">
       <c r="B29" s="52" t="s">
         <v>138</v>
       </c>
@@ -5292,11 +5309,11 @@
         <v>9148000</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1">
       <c r="B30" s="52"/>
       <c r="C30" s="54"/>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="A32" s="11" t="s">
         <v>130</v>
       </c>
@@ -5307,7 +5324,7 @@
         <v>0.29978973218277538</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" ht="15.75" customHeight="1">
       <c r="B33" s="51" t="s">
         <v>136</v>
       </c>
@@ -5315,7 +5332,7 @@
         <v>0.52556568434139284</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:3" ht="15.75" customHeight="1">
       <c r="B34" s="51" t="s">
         <v>137</v>
       </c>
@@ -5323,7 +5340,7 @@
         <v>0.16210210664201097</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:3" ht="15.75" customHeight="1">
       <c r="B35" s="51" t="s">
         <v>138</v>
       </c>
@@ -5335,6 +5352,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5349,12 +5371,12 @@
       <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -5371,7 +5393,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="14">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
@@ -5388,14 +5410,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -5404,6 +5426,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5415,7 +5442,7 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="43.33203125" customWidth="1"/>
@@ -5426,7 +5453,7 @@
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>87</v>
       </c>
@@ -5456,7 +5483,7 @@
       </c>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>82</v>
       </c>
@@ -5485,7 +5512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1">
       <c r="B3" s="4" t="s">
         <v>51</v>
       </c>
@@ -5511,7 +5538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1">
       <c r="B4" s="4" t="s">
         <v>58</v>
       </c>
@@ -5537,7 +5564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>169</v>
       </c>
@@ -5565,7 +5592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>86</v>
       </c>
@@ -5593,7 +5620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1">
       <c r="B7" s="4" t="s">
         <v>85</v>
       </c>
@@ -5620,7 +5647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1">
       <c r="A9" s="11" t="s">
         <v>83</v>
       </c>
@@ -5650,7 +5677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1">
       <c r="B10" t="s">
         <v>60</v>
       </c>
@@ -5676,7 +5703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1">
       <c r="B11" s="4" t="s">
         <v>88</v>
       </c>
@@ -5702,7 +5729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1">
       <c r="B12" t="s">
         <v>159</v>
       </c>
@@ -5729,7 +5756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="11" t="s">
         <v>95</v>
       </c>
@@ -5758,7 +5785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="B15" t="s">
         <v>163</v>
       </c>
@@ -5784,7 +5811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="B16" t="s">
         <v>164</v>
       </c>
@@ -5810,7 +5837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1">
       <c r="B17" t="s">
         <v>165</v>
       </c>
@@ -5836,7 +5863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1">
       <c r="B18" t="s">
         <v>166</v>
       </c>
@@ -5862,7 +5889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1">
       <c r="B19" t="s">
         <v>167</v>
       </c>
@@ -5888,7 +5915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1">
       <c r="B20" t="s">
         <v>168</v>
       </c>
@@ -5914,7 +5941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1">
       <c r="A21" s="11"/>
       <c r="B21" t="s">
         <v>172</v>
@@ -5941,7 +5968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1">
       <c r="B22" t="s">
         <v>173</v>
       </c>
@@ -5967,7 +5994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1">
       <c r="B23" t="s">
         <v>174</v>
       </c>
@@ -5993,7 +6020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1">
       <c r="B24" t="s">
         <v>175</v>
       </c>
@@ -6019,7 +6046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1">
       <c r="B25" t="s">
         <v>176</v>
       </c>
@@ -6045,7 +6072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1">
       <c r="B26" t="s">
         <v>177</v>
       </c>
@@ -6071,7 +6098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1">
       <c r="B27" t="s">
         <v>178</v>
       </c>
@@ -6097,11 +6124,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1">
       <c r="A29" s="11" t="s">
         <v>90</v>
       </c>
@@ -6135,7 +6162,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" ht="15.75" customHeight="1">
       <c r="B30" s="4" t="s">
         <v>92</v>
       </c>
@@ -6166,7 +6193,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1">
       <c r="B31" s="4" t="s">
         <v>93</v>
       </c>
@@ -6197,7 +6224,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9" ht="15.75" customHeight="1">
       <c r="B32" s="4" t="s">
         <v>111</v>
       </c>
@@ -6223,7 +6250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:9" ht="15.75" customHeight="1">
       <c r="B33" s="4" t="s">
         <v>89</v>
       </c>
@@ -6256,7 +6283,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:9" ht="15.75" customHeight="1">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
     </row>
@@ -6264,6 +6291,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6278,14 +6310,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -6305,7 +6337,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -6325,7 +6357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="B3" t="s">
         <v>55</v>
       </c>
@@ -6342,7 +6374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -6362,7 +6394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="B5" t="s">
         <v>55</v>
       </c>
@@ -6379,7 +6411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>133</v>
       </c>
@@ -6399,7 +6431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="B7" t="s">
         <v>55</v>
       </c>
@@ -6420,6 +6452,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6434,7 +6471,7 @@
       <selection activeCell="B11" sqref="B11:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="42.6640625" customWidth="1"/>
@@ -6443,7 +6480,7 @@
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="14" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>52</v>
       </c>
@@ -6490,7 +6527,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15">
       <c r="A2" s="11" t="s">
         <v>160</v>
       </c>
@@ -6537,7 +6574,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15">
       <c r="B3" t="s">
         <v>159</v>
       </c>
@@ -6581,7 +6618,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15">
       <c r="B4" t="s">
         <v>162</v>
       </c>
@@ -6625,7 +6662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15">
       <c r="B5" t="s">
         <v>163</v>
       </c>
@@ -6669,7 +6706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15">
       <c r="B6" t="s">
         <v>164</v>
       </c>
@@ -6713,7 +6750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15">
       <c r="B7" t="s">
         <v>165</v>
       </c>
@@ -6757,7 +6794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15">
       <c r="B8" t="s">
         <v>166</v>
       </c>
@@ -6801,7 +6838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15">
       <c r="B9" t="s">
         <v>167</v>
       </c>
@@ -6845,7 +6882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15">
       <c r="B10" t="s">
         <v>168</v>
       </c>
@@ -6889,7 +6926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15">
       <c r="B11" t="s">
         <v>172</v>
       </c>
@@ -6933,7 +6970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15">
       <c r="B12" t="s">
         <v>173</v>
       </c>
@@ -6977,7 +7014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15">
       <c r="B13" t="s">
         <v>174</v>
       </c>
@@ -7021,7 +7058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15">
       <c r="B14" t="s">
         <v>175</v>
       </c>
@@ -7065,7 +7102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15">
       <c r="B15" t="s">
         <v>176</v>
       </c>
@@ -7109,7 +7146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15">
       <c r="B16" t="s">
         <v>177</v>
       </c>
@@ -7153,7 +7190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15">
       <c r="B17" t="s">
         <v>178</v>
       </c>
@@ -7197,7 +7234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15">
       <c r="B18" s="4" t="s">
         <v>86</v>
       </c>
@@ -7241,7 +7278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15">
       <c r="A20" s="11" t="s">
         <v>161</v>
       </c>
@@ -7288,7 +7325,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15">
       <c r="B21" s="4" t="s">
         <v>92</v>
       </c>
@@ -7332,7 +7369,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15">
       <c r="B22" s="4" t="s">
         <v>93</v>
       </c>
@@ -7376,7 +7413,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15">
       <c r="B23" s="4" t="s">
         <v>111</v>
       </c>
@@ -7420,7 +7457,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:15">
       <c r="B24" t="s">
         <v>85</v>
       </c>
@@ -7464,7 +7501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:15">
       <c r="B25" s="4" t="s">
         <v>88</v>
       </c>
@@ -7508,23 +7545,28 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.15"/>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:2"/>
+    <row r="38" spans="2:2">
       <c r="B38" s="4"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:2">
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:2">
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:2">
       <c r="B41" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7539,7 +7581,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="27.5" customWidth="1"/>
     <col min="3" max="3" width="38.1640625" customWidth="1"/>
@@ -7549,7 +7591,7 @@
     <col min="8" max="8" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -7575,7 +7617,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>51</v>
       </c>
@@ -7601,7 +7643,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="C3" t="s">
         <v>70</v>
       </c>
@@ -7621,7 +7663,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -7643,7 +7685,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8">
       <c r="A5" s="12"/>
       <c r="B5" s="61" t="s">
         <v>171</v>
@@ -7667,7 +7709,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -7675,6 +7717,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7682,11 +7729,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="43.83203125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -7694,7 +7741,7 @@
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -7708,7 +7755,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
@@ -7725,7 +7772,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>51</v>
       </c>
@@ -7742,7 +7789,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>58</v>
       </c>
@@ -7759,7 +7806,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>169</v>
       </c>
@@ -7776,7 +7823,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>86</v>
       </c>
@@ -7787,7 +7834,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="34" t="s">
         <v>85</v>
       </c>
@@ -7798,7 +7845,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -7815,7 +7862,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -7832,7 +7879,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>88</v>
       </c>
@@ -7843,7 +7890,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" t="s">
         <v>159</v>
       </c>
@@ -7854,7 +7901,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" t="s">
         <v>162</v>
       </c>
@@ -7865,7 +7912,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" t="s">
         <v>163</v>
       </c>
@@ -7876,7 +7923,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>164</v>
       </c>
@@ -7887,7 +7934,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" t="s">
         <v>165</v>
       </c>
@@ -7898,7 +7945,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" t="s">
         <v>166</v>
       </c>
@@ -7906,7 +7953,7 @@
       <c r="C16" s="35"/>
       <c r="D16" s="14"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" t="s">
         <v>167</v>
       </c>
@@ -7914,7 +7961,7 @@
       <c r="C17" s="35"/>
       <c r="D17" s="14"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>168</v>
       </c>
@@ -7922,7 +7969,7 @@
       <c r="C18" s="14"/>
       <c r="D18" s="35"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" t="s">
         <v>172</v>
       </c>
@@ -7933,7 +7980,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" t="s">
         <v>173</v>
       </c>
@@ -7944,7 +7991,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" t="s">
         <v>174</v>
       </c>
@@ -7955,7 +8002,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" t="s">
         <v>175</v>
       </c>
@@ -7966,7 +8013,7 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" t="s">
         <v>176</v>
       </c>
@@ -7974,7 +8021,7 @@
       <c r="C23" s="35"/>
       <c r="D23" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" t="s">
         <v>177</v>
       </c>
@@ -7982,7 +8029,7 @@
       <c r="C24" s="35"/>
       <c r="D24" s="14"/>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" t="s">
         <v>178</v>
       </c>
@@ -7990,7 +8037,7 @@
       <c r="C25" s="14"/>
       <c r="D25" s="35"/>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
         <v>91</v>
       </c>
@@ -8000,7 +8047,7 @@
       </c>
       <c r="D26" s="35"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" s="4" t="s">
         <v>92</v>
       </c>
@@ -8010,7 +8057,7 @@
       </c>
       <c r="D27" s="35"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
         <v>93</v>
       </c>
@@ -8020,7 +8067,7 @@
       </c>
       <c r="D28" s="35"/>
     </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="A29" s="4" t="s">
         <v>111</v>
       </c>
@@ -8028,35 +8075,37 @@
       <c r="C29" s="14"/>
       <c r="D29" s="35"/>
     </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7" ht="15.75" customHeight="1">
       <c r="A30" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B30" s="14"/>
+      <c r="B30" s="15">
+        <v>0.2</v>
+      </c>
       <c r="C30" s="14"/>
       <c r="D30" s="35"/>
     </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:7" ht="15.75" customHeight="1">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:7" ht="15.75" customHeight="1">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:3" ht="15.75" customHeight="1">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:3" ht="15.75" customHeight="1">
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:3" ht="15.75" customHeight="1">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:3" ht="15.75" customHeight="1">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
     </row>
@@ -8064,6 +8113,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8075,7 +8129,7 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
@@ -8083,7 +8137,7 @@
     <col min="11" max="11" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8121,7 +8175,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1">
       <c r="A2" s="3">
         <v>2017</v>
       </c>
@@ -8163,7 +8217,7 @@
         <v>173766200</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1">
       <c r="A3" s="3">
         <v>2018</v>
       </c>
@@ -8205,7 +8259,7 @@
         <v>175848400</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1">
       <c r="A4" s="3">
         <v>2019</v>
       </c>
@@ -8247,7 +8301,7 @@
         <v>177930600</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1">
       <c r="A5" s="3">
         <v>2020</v>
       </c>
@@ -8289,7 +8343,7 @@
         <v>180012800</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1">
       <c r="A6" s="3">
         <v>2021</v>
       </c>
@@ -8331,7 +8385,7 @@
         <v>182095000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1">
       <c r="A7" s="3">
         <v>2022</v>
       </c>
@@ -8373,7 +8427,7 @@
         <v>183822800</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="A8" s="3">
         <v>2023</v>
       </c>
@@ -8415,7 +8469,7 @@
         <v>185550600</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1">
       <c r="A9" s="3">
         <v>2024</v>
       </c>
@@ -8457,7 +8511,7 @@
         <v>187278400</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1">
       <c r="A10" s="3">
         <v>2025</v>
       </c>
@@ -8499,7 +8553,7 @@
         <v>189006200</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1">
       <c r="A11" s="3">
         <v>2026</v>
       </c>
@@ -8541,7 +8595,7 @@
         <v>190734000</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1">
       <c r="A12" s="3">
         <v>2027</v>
       </c>
@@ -8583,7 +8637,7 @@
         <v>192287600</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1">
       <c r="A13" s="3">
         <v>2028</v>
       </c>
@@ -8625,7 +8679,7 @@
         <v>193841200</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1">
       <c r="A14" s="3">
         <v>2029</v>
       </c>
@@ -8667,7 +8721,7 @@
         <v>195394800</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1">
       <c r="A15" s="3">
         <v>2030</v>
       </c>
@@ -8713,6 +8767,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8724,12 +8783,12 @@
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -8752,7 +8811,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -8775,7 +8834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -8798,7 +8857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -8821,7 +8880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -8844,7 +8903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -8867,7 +8926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -8890,7 +8949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -8913,7 +8972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -8936,7 +8995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -8959,7 +9018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -8982,7 +9041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -9005,7 +9064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -9028,7 +9087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -9051,7 +9110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -9074,7 +9133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -9097,7 +9156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -9120,7 +9179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -9143,7 +9202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -9166,7 +9225,7 @@
         <v>2.5899999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -9189,7 +9248,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" t="s">
         <v>101</v>
       </c>
@@ -9212,7 +9271,7 @@
         <v>0.25590000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -9235,7 +9294,7 @@
         <v>0.1464</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -9258,7 +9317,7 @@
         <v>1.7600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -9281,7 +9340,7 @@
         <v>1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -9304,7 +9363,7 @@
         <v>1.14E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" t="s">
         <v>106</v>
       </c>
@@ -9327,7 +9386,7 @@
         <v>0.15129999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -9357,6 +9416,11 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9368,9 +9432,9 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
@@ -9390,7 +9454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>29</v>
       </c>
@@ -9410,7 +9474,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -9430,7 +9494,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
@@ -9453,6 +9517,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9464,7 +9533,7 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
@@ -9473,7 +9542,7 @@
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5">
       <c r="A1" s="11" t="s">
         <v>118</v>
       </c>
@@ -9490,7 +9559,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5">
       <c r="A2" s="11" t="s">
         <v>96</v>
       </c>
@@ -9505,7 +9574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5">
       <c r="A3" s="11"/>
       <c r="B3" t="s">
         <v>7</v>
@@ -9518,7 +9587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5">
       <c r="A4" s="11"/>
       <c r="B4" t="s">
         <v>8</v>
@@ -9533,7 +9602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5">
       <c r="A5" s="11"/>
       <c r="B5" t="s">
         <v>9</v>
@@ -9548,7 +9617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5">
       <c r="A6" s="11"/>
       <c r="B6" t="s">
         <v>10</v>
@@ -9563,7 +9632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="A7" s="11"/>
       <c r="B7" t="s">
         <v>84</v>
@@ -9578,7 +9647,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5">
       <c r="A8" s="11"/>
       <c r="B8" t="s">
         <v>136</v>
@@ -9593,7 +9662,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>137</v>
@@ -9608,7 +9677,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>138</v>
@@ -9623,13 +9692,13 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5">
       <c r="A11" s="11"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5">
       <c r="A12" s="11"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5">
       <c r="A13" s="11" t="s">
         <v>97</v>
       </c>
@@ -9644,7 +9713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -9656,7 +9725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5">
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -9670,7 +9739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5">
       <c r="B16" t="s">
         <v>9</v>
       </c>
@@ -9684,7 +9753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -9698,7 +9767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5">
       <c r="B18" t="s">
         <v>84</v>
       </c>
@@ -9712,7 +9781,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5">
       <c r="B19" t="s">
         <v>136</v>
       </c>
@@ -9726,7 +9795,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5">
       <c r="B20" t="s">
         <v>137</v>
       </c>
@@ -9740,7 +9809,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5">
       <c r="B21" t="s">
         <v>138</v>
       </c>
@@ -9754,7 +9823,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5">
       <c r="A24" s="11" t="s">
         <v>113</v>
       </c>
@@ -9775,6 +9844,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9786,9 +9860,9 @@
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -9811,7 +9885,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
@@ -9834,7 +9908,7 @@
         <v>25.35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
         <v>24</v>
@@ -9855,7 +9929,7 @@
         <v>33.25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="12"/>
       <c r="B4" s="13" t="s">
         <v>27</v>
@@ -9876,7 +9950,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="12"/>
       <c r="B5" s="13" t="s">
         <v>28</v>
@@ -9897,7 +9971,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
@@ -9920,7 +9994,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
@@ -9940,7 +10014,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
@@ -9960,7 +10034,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
@@ -9980,7 +10054,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
@@ -10003,7 +10077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
@@ -10023,7 +10097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="4" t="s">
         <v>42</v>
       </c>
@@ -10043,7 +10117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1">
       <c r="B17" s="4" t="s">
         <v>43</v>
       </c>
@@ -10068,6 +10142,11 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10079,12 +10158,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>119</v>
       </c>
@@ -10104,7 +10183,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>12</v>
       </c>
@@ -10125,7 +10204,7 @@
         <v>3.1128200000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="B3" t="s">
         <v>115</v>
       </c>
@@ -10140,7 +10219,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="B4" t="s">
         <v>63</v>
       </c>
@@ -10157,14 +10236,14 @@
         <v>46.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="11"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="11"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="B7" s="11" t="s">
         <v>5</v>
       </c>
@@ -10173,7 +10252,7 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="11" t="s">
         <v>61</v>
       </c>
@@ -10193,7 +10272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
@@ -10210,7 +10289,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
@@ -10227,7 +10306,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
@@ -10244,7 +10323,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
@@ -10261,7 +10340,7 @@
         <v>999.99</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1">
       <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
@@ -10278,7 +10357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
       <c r="B14" s="5" t="s">
         <v>46</v>
       </c>
@@ -10295,7 +10374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
@@ -10316,6 +10395,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10330,7 +10414,7 @@
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
@@ -10338,7 +10422,7 @@
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" s="11" t="s">
         <v>61</v>
       </c>
@@ -10367,7 +10451,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
@@ -10396,7 +10480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9">
       <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
@@ -10419,7 +10503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9">
       <c r="C4" s="4" t="s">
         <v>27</v>
       </c>
@@ -10442,7 +10526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9">
       <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
@@ -10465,7 +10549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9">
       <c r="B6" t="s">
         <v>31</v>
       </c>
@@ -10491,7 +10575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9">
       <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
@@ -10514,7 +10598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9">
       <c r="C8" s="4" t="s">
         <v>27</v>
       </c>
@@ -10537,7 +10621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9">
       <c r="C9" s="4" t="s">
         <v>28</v>
       </c>
@@ -10560,7 +10644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9">
       <c r="B10" t="s">
         <v>33</v>
       </c>
@@ -10586,7 +10670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9">
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
@@ -10609,7 +10693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9">
       <c r="C12" s="4" t="s">
         <v>27</v>
       </c>
@@ -10632,7 +10716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9">
       <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
@@ -10655,7 +10739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9">
       <c r="B14" t="s">
         <v>34</v>
       </c>
@@ -10681,7 +10765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9">
       <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
@@ -10704,7 +10788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9">
       <c r="C16" s="4" t="s">
         <v>27</v>
       </c>
@@ -10727,7 +10811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9">
       <c r="C17" s="4" t="s">
         <v>28</v>
       </c>
@@ -10750,7 +10834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9">
       <c r="B18" t="s">
         <v>38</v>
       </c>
@@ -10776,7 +10860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9">
       <c r="C19" s="4" t="s">
         <v>24</v>
       </c>
@@ -10799,7 +10883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9">
       <c r="C20" s="4" t="s">
         <v>27</v>
       </c>
@@ -10822,7 +10906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9">
       <c r="C21" s="4" t="s">
         <v>28</v>
       </c>
@@ -10845,7 +10929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9">
       <c r="A24" s="11" t="s">
         <v>30</v>
       </c>
@@ -10874,7 +10958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9">
       <c r="C25" s="4" t="s">
         <v>24</v>
       </c>
@@ -10897,7 +10981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9">
       <c r="C26" s="4" t="s">
         <v>27</v>
       </c>
@@ -10920,7 +11004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9">
       <c r="C27" s="4" t="s">
         <v>28</v>
       </c>
@@ -10943,7 +11027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9">
       <c r="B28" t="s">
         <v>31</v>
       </c>
@@ -10969,7 +11053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9">
       <c r="C29" s="4" t="s">
         <v>24</v>
       </c>
@@ -10992,7 +11076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9">
       <c r="C30" s="4" t="s">
         <v>27</v>
       </c>
@@ -11015,7 +11099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9">
       <c r="C31" s="4" t="s">
         <v>28</v>
       </c>
@@ -11038,7 +11122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9">
       <c r="B32" t="s">
         <v>33</v>
       </c>
@@ -11064,7 +11148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9">
       <c r="C33" s="4" t="s">
         <v>24</v>
       </c>
@@ -11087,7 +11171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:9">
       <c r="C34" s="4" t="s">
         <v>27</v>
       </c>
@@ -11110,7 +11194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:9">
       <c r="C35" s="4" t="s">
         <v>28</v>
       </c>
@@ -11133,7 +11217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:9">
       <c r="B36" t="s">
         <v>34</v>
       </c>
@@ -11159,7 +11243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:9">
       <c r="C37" s="4" t="s">
         <v>24</v>
       </c>
@@ -11182,7 +11266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:9">
       <c r="C38" s="4" t="s">
         <v>27</v>
       </c>
@@ -11205,7 +11289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:9">
       <c r="C39" s="4" t="s">
         <v>28</v>
       </c>
@@ -11228,7 +11312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:9">
       <c r="B40" t="s">
         <v>38</v>
       </c>
@@ -11254,7 +11338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:9">
       <c r="C41" s="4" t="s">
         <v>24</v>
       </c>
@@ -11277,7 +11361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:9">
       <c r="C42" s="4" t="s">
         <v>27</v>
       </c>
@@ -11300,7 +11384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:9">
       <c r="C43" s="4" t="s">
         <v>28</v>
       </c>
@@ -11323,7 +11407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:9">
       <c r="A46" s="11" t="s">
         <v>39</v>
       </c>
@@ -11352,7 +11436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:9">
       <c r="C47" s="4" t="s">
         <v>41</v>
       </c>
@@ -11375,7 +11459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:9">
       <c r="C48" s="4" t="s">
         <v>42</v>
       </c>
@@ -11398,7 +11482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:9">
       <c r="C49" s="4" t="s">
         <v>43</v>
       </c>
@@ -11421,7 +11505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:9">
       <c r="B50" t="s">
         <v>16</v>
       </c>
@@ -11447,7 +11531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="51" spans="2:9">
       <c r="C51" s="4" t="s">
         <v>41</v>
       </c>
@@ -11470,7 +11554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:9">
       <c r="C52" s="4" t="s">
         <v>42</v>
       </c>
@@ -11493,7 +11577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="53" spans="2:9">
       <c r="C53" s="4" t="s">
         <v>43</v>
       </c>
@@ -11516,7 +11600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="54" spans="2:9">
       <c r="B54" t="s">
         <v>17</v>
       </c>
@@ -11542,7 +11626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="55" spans="2:9">
       <c r="C55" s="4" t="s">
         <v>41</v>
       </c>
@@ -11565,7 +11649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="56" spans="2:9">
       <c r="C56" s="4" t="s">
         <v>42</v>
       </c>
@@ -11588,7 +11672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="57" spans="2:9">
       <c r="C57" s="4" t="s">
         <v>43</v>
       </c>
@@ -11611,7 +11695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="58" spans="2:9">
       <c r="B58" t="s">
         <v>22</v>
       </c>
@@ -11637,7 +11721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="59" spans="2:9">
       <c r="C59" s="4" t="s">
         <v>41</v>
       </c>
@@ -11660,7 +11744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="60" spans="2:9">
       <c r="C60" s="4" t="s">
         <v>42</v>
       </c>
@@ -11683,7 +11767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="61" spans="2:9">
       <c r="C61" s="4" t="s">
         <v>43</v>
       </c>
@@ -11706,7 +11790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="62" spans="2:9">
       <c r="B62" t="s">
         <v>29</v>
       </c>
@@ -11732,7 +11816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="63" spans="2:9">
       <c r="C63" s="4" t="s">
         <v>41</v>
       </c>
@@ -11755,7 +11839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="64" spans="2:9">
       <c r="C64" s="4" t="s">
         <v>42</v>
       </c>
@@ -11778,7 +11862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:9">
       <c r="C65" s="4" t="s">
         <v>43</v>
       </c>
@@ -11801,7 +11885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:9">
       <c r="B66" t="s">
         <v>31</v>
       </c>
@@ -11827,7 +11911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:9">
       <c r="C67" s="4" t="s">
         <v>41</v>
       </c>
@@ -11850,7 +11934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:9">
       <c r="C68" s="4" t="s">
         <v>42</v>
       </c>
@@ -11873,7 +11957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:9">
       <c r="C69" s="4" t="s">
         <v>43</v>
       </c>
@@ -11896,7 +11980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:9">
       <c r="B70" t="s">
         <v>32</v>
       </c>
@@ -11922,7 +12006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:9">
       <c r="C71" s="4" t="s">
         <v>41</v>
       </c>
@@ -11945,7 +12029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:9">
       <c r="C72" s="4" t="s">
         <v>42</v>
       </c>
@@ -11968,7 +12052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:9">
       <c r="C73" s="4" t="s">
         <v>43</v>
       </c>
@@ -11991,7 +12075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:9">
       <c r="A76" s="11" t="s">
         <v>131</v>
       </c>
@@ -12020,7 +12104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:9">
       <c r="C77" s="4" t="s">
         <v>121</v>
       </c>
@@ -12043,7 +12127,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:9">
       <c r="B78" t="s">
         <v>100</v>
       </c>
@@ -12069,7 +12153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:9">
       <c r="C79" s="4" t="s">
         <v>121</v>
       </c>
@@ -12092,7 +12176,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:9">
       <c r="B80" t="s">
         <v>101</v>
       </c>
@@ -12118,7 +12202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:9">
       <c r="C81" s="4" t="s">
         <v>121</v>
       </c>
@@ -12141,7 +12225,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:9">
       <c r="A84" s="11" t="s">
         <v>112</v>
       </c>
@@ -12170,7 +12254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:9">
       <c r="C85" s="4" t="s">
         <v>41</v>
       </c>
@@ -12193,7 +12277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:9">
       <c r="C86" s="4" t="s">
         <v>42</v>
       </c>
@@ -12216,7 +12300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:9">
       <c r="C87" s="4" t="s">
         <v>43</v>
       </c>
@@ -12239,7 +12323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:9">
       <c r="A90" s="11" t="s">
         <v>132</v>
       </c>
@@ -12250,6 +12334,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -12264,7 +12353,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="36.6640625" customWidth="1"/>
     <col min="2" max="2" width="64.5" customWidth="1"/>
@@ -12274,7 +12363,7 @@
     <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
         <v>52</v>
       </c>
@@ -12297,7 +12386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2" s="11" t="s">
         <v>123</v>
       </c>
@@ -12318,7 +12407,7 @@
         <v>174.7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="B3" s="4" t="s">
         <v>29</v>
       </c>
@@ -12338,7 +12427,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" s="11" t="s">
         <v>122</v>
       </c>
@@ -12361,7 +12450,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7">
       <c r="B6" s="4" t="s">
         <v>48</v>
       </c>
@@ -12381,7 +12470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7">
       <c r="B7" s="4" t="s">
         <v>49</v>
       </c>
@@ -12401,7 +12490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7">
       <c r="B8" s="4" t="s">
         <v>150</v>
       </c>
@@ -12421,7 +12510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7">
       <c r="B9" s="4" t="s">
         <v>135</v>
       </c>
@@ -12441,7 +12530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7">
       <c r="B10" s="4" t="s">
         <v>50</v>
       </c>
@@ -12461,7 +12550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="14">
       <c r="A12" s="11" t="s">
         <v>124</v>
       </c>
@@ -12484,7 +12573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="14">
       <c r="B13" s="4" t="s">
         <v>58</v>
       </c>
@@ -12508,5 +12597,10 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added hidden intervention coverage and cost saturation info, and added fictional values to the spreadsheet for now to avoid nans
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22220" windowHeight="12640" tabRatio="500" firstSheet="10" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22220" windowHeight="12640" tabRatio="500" firstSheet="13" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -317,6 +317,28 @@
         </r>
       </text>
     </comment>
+    <comment ref="B10" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fictional</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A11" authorId="0">
       <text>
         <r>
@@ -406,6 +428,28 @@
       </text>
     </comment>
     <comment ref="B30" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fictional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D30" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2648,7 +2692,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="517">
+  <cellStyleXfs count="519">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2660,6 +2704,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3269,7 +3315,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="517">
+  <cellStyles count="519">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3528,6 +3574,7 @@
     <cellStyle name="Followed Hyperlink" xfId="512" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="516" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="518" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3785,6 +3832,7 @@
     <cellStyle name="Hyperlink" xfId="511" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="515" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="517" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -6468,7 +6516,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B17"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -7729,8 +7777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -7883,9 +7931,15 @@
       <c r="A10" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="14"/>
+      <c r="B10" s="15">
+        <v>0</v>
+      </c>
+      <c r="C10" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="D10" s="15">
+        <v>1</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -7894,9 +7948,15 @@
       <c r="A11" t="s">
         <v>159</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="14"/>
+      <c r="B11" s="15">
+        <v>0</v>
+      </c>
+      <c r="C11" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="D11" s="15">
+        <v>1</v>
+      </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -7905,9 +7965,15 @@
       <c r="A12" t="s">
         <v>162</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="14"/>
+      <c r="B12" s="15">
+        <v>0</v>
+      </c>
+      <c r="C12" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="D12" s="15">
+        <v>1</v>
+      </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -7916,9 +7982,15 @@
       <c r="A13" t="s">
         <v>163</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="14"/>
+      <c r="B13" s="15">
+        <v>0</v>
+      </c>
+      <c r="C13" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="D13" s="15">
+        <v>1</v>
+      </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -7927,9 +7999,15 @@
       <c r="A14" t="s">
         <v>164</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="14"/>
+      <c r="B14" s="15">
+        <v>0</v>
+      </c>
+      <c r="C14" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="D14" s="15">
+        <v>1</v>
+      </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -7938,9 +8016,15 @@
       <c r="A15" t="s">
         <v>165</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="14"/>
+      <c r="B15" s="15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="D15" s="15">
+        <v>1</v>
+      </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -7949,33 +8033,57 @@
       <c r="A16" t="s">
         <v>166</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="14"/>
+      <c r="B16" s="15">
+        <v>0</v>
+      </c>
+      <c r="C16" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="D16" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" t="s">
         <v>167</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="14"/>
+      <c r="B17" s="15">
+        <v>0</v>
+      </c>
+      <c r="C17" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="D17" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>168</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="35"/>
+      <c r="B18" s="15">
+        <v>0</v>
+      </c>
+      <c r="C18" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="D18" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" t="s">
         <v>172</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="14"/>
+      <c r="B19" s="15">
+        <v>0</v>
+      </c>
+      <c r="C19" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="D19" s="15">
+        <v>1</v>
+      </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -7984,9 +8092,15 @@
       <c r="A20" t="s">
         <v>173</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="14"/>
+      <c r="B20" s="15">
+        <v>0</v>
+      </c>
+      <c r="C20" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="D20" s="15">
+        <v>1</v>
+      </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -7995,9 +8109,15 @@
       <c r="A21" t="s">
         <v>174</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="14"/>
+      <c r="B21" s="15">
+        <v>0</v>
+      </c>
+      <c r="C21" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="D21" s="15">
+        <v>1</v>
+      </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -8006,9 +8126,15 @@
       <c r="A22" t="s">
         <v>175</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="14"/>
+      <c r="B22" s="15">
+        <v>0</v>
+      </c>
+      <c r="C22" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="D22" s="15">
+        <v>1</v>
+      </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -8017,63 +8143,97 @@
       <c r="A23" t="s">
         <v>176</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="14"/>
+      <c r="B23" s="15">
+        <v>0</v>
+      </c>
+      <c r="C23" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="D23" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" t="s">
         <v>177</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="14"/>
+      <c r="B24" s="15">
+        <v>0</v>
+      </c>
+      <c r="C24" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="D24" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" t="s">
         <v>178</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="35"/>
+      <c r="B25" s="15">
+        <v>0</v>
+      </c>
+      <c r="C25" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="D25" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B26" s="14"/>
+      <c r="B26" s="15">
+        <v>0</v>
+      </c>
       <c r="C26" s="15">
         <v>0.12</v>
       </c>
-      <c r="D26" s="35"/>
+      <c r="D26" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B27" s="14"/>
+      <c r="B27" s="15">
+        <v>0</v>
+      </c>
       <c r="C27" s="15">
         <v>0.05</v>
       </c>
-      <c r="D27" s="35"/>
+      <c r="D27" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="14"/>
+      <c r="B28" s="15">
+        <v>0</v>
+      </c>
       <c r="C28" s="15">
         <v>0.8</v>
       </c>
-      <c r="D28" s="35"/>
+      <c r="D28" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="A29" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B29" s="14"/>
+      <c r="B29" s="15">
+        <v>0</v>
+      </c>
       <c r="C29" s="14"/>
-      <c r="D29" s="35"/>
+      <c r="D29" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1">
       <c r="A30" s="4" t="s">
@@ -8083,7 +8243,9 @@
         <v>0.2</v>
       </c>
       <c r="C30" s="14"/>
-      <c r="D30" s="35"/>
+      <c r="D30" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1">
       <c r="B31" s="4"/>
@@ -10410,7 +10572,7 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A65" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modified target pop for sprinkles, removed AMS:  now we have MMs and IFAS for pregnant women
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22220" windowHeight="12640" tabRatio="500" firstSheet="13" activeTab="14"/>
+    <workbookView xWindow="-73680" yWindow="-3580" windowWidth="27440" windowHeight="16760" tabRatio="500" firstSheet="12" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -1118,6 +1118,50 @@
         </r>
       </text>
     </comment>
+    <comment ref="E7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+food insecure - default poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+food insecure - default poor</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G7" authorId="0">
       <text>
         <r>
@@ -1982,7 +2026,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="178">
   <si>
     <t>year</t>
   </si>
@@ -2164,9 +2208,6 @@
     <t>Balanced energy-protein supplementation</t>
   </si>
   <si>
-    <t>Antenatal micronutrient supplementation</t>
-  </si>
-  <si>
     <t>RR of death</t>
   </si>
   <si>
@@ -2383,9 +2424,6 @@
     <t>RR of anaemia by intervention</t>
   </si>
   <si>
-    <t>IFAS for pregnant women</t>
-  </si>
-  <si>
     <t>ID anaemia prevalence</t>
   </si>
   <si>
@@ -2519,6 +2557,9 @@
   </si>
   <si>
     <t>IFAS not poor: retailer (malaria area)</t>
+  </si>
+  <si>
+    <t>Multiple micronutrient supplementation</t>
   </si>
 </sst>
 </file>
@@ -2692,7 +2733,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="519">
+  <cellStyleXfs count="521">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2704,6 +2745,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3315,7 +3358,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="519">
+  <cellStyles count="521">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3575,6 +3618,7 @@
     <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="516" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="518" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="520" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3833,6 +3877,7 @@
     <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="515" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="517" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="519" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -5148,18 +5193,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" customHeight="1">
       <c r="A1" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>116</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -5178,7 +5223,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="B4" s="34" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C4" s="55">
         <v>171684000</v>
@@ -5195,7 +5240,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="B6" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="20">
         <v>0.35199999999999998</v>
@@ -5203,7 +5248,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1">
       <c r="B7" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="18">
         <v>0.36</v>
@@ -5211,7 +5256,7 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1">
       <c r="B8" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="20">
         <v>0.1</v>
@@ -5223,10 +5268,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1">
       <c r="A11" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="20">
         <v>176</v>
@@ -5234,7 +5279,7 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1">
       <c r="B12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C12" s="20">
         <v>0.13</v>
@@ -5242,7 +5287,7 @@
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1">
       <c r="B13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C13" s="20">
         <v>25.36</v>
@@ -5250,7 +5295,7 @@
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1">
       <c r="B14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C14" s="20">
         <v>25.4</v>
@@ -5258,7 +5303,7 @@
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1">
       <c r="B15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C15" s="20">
         <v>34.68</v>
@@ -5266,7 +5311,7 @@
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1">
       <c r="B16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C16" s="20">
         <v>39.32</v>
@@ -5278,10 +5323,10 @@
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1">
       <c r="A19" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C19" s="45">
         <v>0.3</v>
@@ -5289,7 +5334,7 @@
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
       <c r="B20" s="34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C20" s="45">
         <v>0.8</v>
@@ -5297,7 +5342,7 @@
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1">
       <c r="B21" s="34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C21" s="45">
         <v>0.12</v>
@@ -5305,7 +5350,7 @@
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
       <c r="B22" s="34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C22" s="45">
         <v>0.05</v>
@@ -5313,7 +5358,7 @@
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="B23" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C23" s="45">
         <v>0.05</v>
@@ -5324,10 +5369,10 @@
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="A26" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B26" s="52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C26" s="53">
         <v>8634000</v>
@@ -5335,7 +5380,7 @@
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1">
       <c r="B27" s="52" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C27" s="53">
         <v>13550000</v>
@@ -5343,7 +5388,7 @@
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1">
       <c r="B28" s="52" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C28" s="53">
         <v>12394000</v>
@@ -5351,7 +5396,7 @@
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1">
       <c r="B29" s="52" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C29" s="53">
         <v>9148000</v>
@@ -5363,10 +5408,10 @@
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="A32" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B32" s="43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C32" s="44">
         <v>0.29978973218277538</v>
@@ -5374,7 +5419,7 @@
     </row>
     <row r="33" spans="2:3" ht="15.75" customHeight="1">
       <c r="B33" s="51" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C33" s="44">
         <v>0.52556568434139284</v>
@@ -5382,7 +5427,7 @@
     </row>
     <row r="34" spans="2:3" ht="15.75" customHeight="1">
       <c r="B34" s="51" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C34" s="44">
         <v>0.16210210664201097</v>
@@ -5390,7 +5435,7 @@
     </row>
     <row r="35" spans="2:3" ht="15.75" customHeight="1">
       <c r="B35" s="51" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C35" s="44">
         <v>1.2542476833820825E-2</v>
@@ -5487,7 +5532,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5503,7 +5548,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>47</v>
@@ -5524,16 +5569,16 @@
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>57</v>
@@ -5614,7 +5659,7 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1">
       <c r="B5" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
@@ -5642,7 +5687,7 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -5670,7 +5715,7 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1">
       <c r="B7" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" s="3">
         <v>0</v>
@@ -5678,11 +5723,13 @@
       <c r="D7" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0</v>
+      <c r="E7" s="31">
+        <f>'Baseline year demographics'!$C$7</f>
+        <v>0.36</v>
+      </c>
+      <c r="F7" s="31">
+        <f>'Baseline year demographics'!$C$7</f>
+        <v>0.36</v>
       </c>
       <c r="G7" s="31">
         <f>'Baseline year demographics'!$C$7</f>
@@ -5697,7 +5744,7 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1">
       <c r="A9" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
         <v>59</v>
@@ -5727,7 +5774,7 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1">
       <c r="B10" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
@@ -5753,7 +5800,7 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1">
       <c r="B11" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C11" s="3">
         <v>0</v>
@@ -5779,7 +5826,7 @@
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1">
       <c r="B12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C12" s="3">
         <v>0</v>
@@ -5806,10 +5853,10 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
@@ -5835,7 +5882,7 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="B15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C15" s="3">
         <v>0</v>
@@ -5861,7 +5908,7 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="B16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -5887,7 +5934,7 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1">
       <c r="B17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C17" s="3">
         <v>0</v>
@@ -5913,7 +5960,7 @@
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1">
       <c r="B18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
@@ -5939,7 +5986,7 @@
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1">
       <c r="B19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -5965,7 +6012,7 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1">
       <c r="B20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
@@ -5992,7 +6039,7 @@
     <row r="21" spans="1:9" ht="15.75" customHeight="1">
       <c r="A21" s="11"/>
       <c r="B21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
@@ -6018,7 +6065,7 @@
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1">
       <c r="B22" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
@@ -6044,7 +6091,7 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1">
       <c r="B23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
@@ -6070,7 +6117,7 @@
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1">
       <c r="B24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
@@ -6096,7 +6143,7 @@
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1">
       <c r="B25" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C25" s="3">
         <v>0</v>
@@ -6122,7 +6169,7 @@
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1">
       <c r="B26" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
@@ -6148,7 +6195,7 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1">
       <c r="B27" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C27" s="3">
         <v>0</v>
@@ -6178,10 +6225,10 @@
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1">
       <c r="A29" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
@@ -6212,7 +6259,7 @@
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1">
       <c r="B30" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C30" s="3">
         <v>0</v>
@@ -6243,7 +6290,7 @@
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1">
       <c r="B31" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C31" s="3">
         <v>0</v>
@@ -6274,7 +6321,7 @@
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1">
       <c r="B32" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C32" s="3">
         <v>0</v>
@@ -6300,7 +6347,7 @@
     </row>
     <row r="33" spans="2:9" ht="15.75" customHeight="1">
       <c r="B33" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C33" s="36">
         <f>'Baseline year demographics'!$C$8</f>
@@ -6355,7 +6402,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -6424,7 +6471,7 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="B4" t="s">
         <v>53</v>
@@ -6461,7 +6508,7 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
         <v>53</v>
@@ -6516,7 +6563,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -6551,36 +6598,36 @@
         <v>10</v>
       </c>
       <c r="H1" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>156</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -6624,7 +6671,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="B3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -6668,7 +6715,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="B4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -6712,7 +6759,7 @@
     </row>
     <row r="5" spans="1:15">
       <c r="B5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -6756,7 +6803,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="B6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -6800,7 +6847,7 @@
     </row>
     <row r="7" spans="1:15">
       <c r="B7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -6844,7 +6891,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="B8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -6888,7 +6935,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="B9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -6932,7 +6979,7 @@
     </row>
     <row r="10" spans="1:15">
       <c r="B10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -6976,7 +7023,7 @@
     </row>
     <row r="11" spans="1:15">
       <c r="B11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -7020,7 +7067,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="B12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -7064,7 +7111,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="B13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -7108,7 +7155,7 @@
     </row>
     <row r="14" spans="1:15">
       <c r="B14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -7152,7 +7199,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="B15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -7196,7 +7243,7 @@
     </row>
     <row r="16" spans="1:15">
       <c r="B16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -7240,7 +7287,7 @@
     </row>
     <row r="17" spans="1:15">
       <c r="B17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -7284,7 +7331,7 @@
     </row>
     <row r="18" spans="1:15">
       <c r="B18" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -7328,10 +7375,10 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -7375,7 +7422,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="B21" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -7419,7 +7466,7 @@
     </row>
     <row r="22" spans="1:15">
       <c r="B22" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -7463,7 +7510,7 @@
     </row>
     <row r="23" spans="1:15">
       <c r="B23" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -7507,7 +7554,7 @@
     </row>
     <row r="24" spans="1:15">
       <c r="B24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -7551,7 +7598,7 @@
     </row>
     <row r="25" spans="1:15">
       <c r="B25" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -7673,7 +7720,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
@@ -7693,7 +7740,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -7715,7 +7762,7 @@
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
@@ -7736,10 +7783,10 @@
     <row r="5" spans="1:8">
       <c r="A5" s="12"/>
       <c r="B5" s="61" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D5" s="62">
         <v>0</v>
@@ -7777,8 +7824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -7794,13 +7841,13 @@
         <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
@@ -7856,7 +7903,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B5" s="15">
         <v>0</v>
@@ -7873,7 +7920,7 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="35"/>
       <c r="C6" s="35"/>
@@ -7884,7 +7931,7 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="35"/>
       <c r="C7" s="35"/>
@@ -7912,7 +7959,7 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="B9" s="15">
         <v>0</v>
@@ -7929,7 +7976,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10" s="15">
         <v>0</v>
@@ -7946,7 +7993,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B11" s="15">
         <v>0</v>
@@ -7963,7 +8010,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B12" s="15">
         <v>0</v>
@@ -7980,7 +8027,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B13" s="15">
         <v>0</v>
@@ -7997,7 +8044,7 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B14" s="15">
         <v>0</v>
@@ -8014,7 +8061,7 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B15" s="15">
         <v>0</v>
@@ -8031,7 +8078,7 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B16" s="15">
         <v>0</v>
@@ -8045,7 +8092,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B17" s="15">
         <v>0</v>
@@ -8059,7 +8106,7 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B18" s="15">
         <v>0</v>
@@ -8073,7 +8120,7 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B19" s="15">
         <v>0</v>
@@ -8090,7 +8137,7 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B20" s="15">
         <v>0</v>
@@ -8107,7 +8154,7 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B21" s="15">
         <v>0</v>
@@ -8124,7 +8171,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B22" s="15">
         <v>0</v>
@@ -8141,7 +8188,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B23" s="15">
         <v>0</v>
@@ -8155,7 +8202,7 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B24" s="15">
         <v>0</v>
@@ -8169,7 +8216,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B25" s="15">
         <v>0</v>
@@ -8183,7 +8230,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B26" s="15">
         <v>0</v>
@@ -8197,7 +8244,7 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B27" s="15">
         <v>0</v>
@@ -8211,7 +8258,7 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B28" s="15">
         <v>0</v>
@@ -8225,7 +8272,7 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B29" s="15">
         <v>0</v>
@@ -8237,7 +8284,7 @@
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B30" s="15">
         <v>0.2</v>
@@ -8307,34 +8354,34 @@
         <v>2</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>66</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>67</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>54</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1">
@@ -8970,7 +9017,7 @@
         <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
@@ -9366,7 +9413,7 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B19" s="20">
         <v>0</v>
@@ -9389,7 +9436,7 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B20" s="20">
         <v>0</v>
@@ -9412,7 +9459,7 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B21" s="20">
         <v>0</v>
@@ -9435,7 +9482,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B22" s="20">
         <v>0</v>
@@ -9458,7 +9505,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B23" s="20">
         <v>0</v>
@@ -9481,7 +9528,7 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B24" s="20">
         <v>0</v>
@@ -9504,7 +9551,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B25" s="20">
         <v>0</v>
@@ -9527,7 +9574,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B26" s="20">
         <v>0</v>
@@ -9550,7 +9597,7 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B27" s="20">
         <v>0</v>
@@ -9638,7 +9685,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B3" s="35">
         <v>5.1999999999999998E-2</v>
@@ -9706,24 +9753,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -9797,7 +9844,7 @@
     <row r="7" spans="1:5">
       <c r="A7" s="11"/>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C7" s="20">
         <v>0</v>
@@ -9812,7 +9859,7 @@
     <row r="8" spans="1:5">
       <c r="A8" s="11"/>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C8" s="20">
         <v>0</v>
@@ -9827,7 +9874,7 @@
     <row r="9" spans="1:5">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C9" s="20">
         <v>0</v>
@@ -9842,7 +9889,7 @@
     <row r="10" spans="1:5">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C10" s="20">
         <v>0</v>
@@ -9862,7 +9909,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -9931,7 +9978,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="B18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C18" s="20">
         <v>0</v>
@@ -9945,7 +9992,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="B19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C19" s="20">
         <v>0</v>
@@ -9959,7 +10006,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="B20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C20" s="20">
         <v>0</v>
@@ -9973,7 +10020,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="B21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C21" s="20">
         <v>0</v>
@@ -9987,10 +10034,10 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" t="s">
         <v>113</v>
-      </c>
-      <c r="B24" t="s">
-        <v>114</v>
       </c>
       <c r="C24" s="41">
         <v>0.01</v>
@@ -10327,10 +10374,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C1" s="33" t="s">
         <v>45</v>
@@ -10350,7 +10397,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="21">
         <f>1-D2-E2-F2</f>
@@ -10368,7 +10415,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="B3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C3" s="46"/>
       <c r="D3" s="12">
@@ -10383,7 +10430,7 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="6">
         <v>1</v>
@@ -10416,7 +10463,7 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>11</v>
@@ -10572,7 +10619,7 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
@@ -10586,7 +10633,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -10610,7 +10657,7 @@
         <v>10</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -12239,13 +12286,13 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B76" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D76" s="4">
         <v>1</v>
@@ -12268,7 +12315,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="C77" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D77" s="4">
         <v>1</v>
@@ -12291,10 +12338,10 @@
     </row>
     <row r="78" spans="1:9">
       <c r="B78" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D78" s="4">
         <v>1</v>
@@ -12317,7 +12364,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="C79" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D79" s="4">
         <v>1</v>
@@ -12340,10 +12387,10 @@
     </row>
     <row r="80" spans="1:9">
       <c r="B80" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D80" s="4">
         <v>1</v>
@@ -12366,7 +12413,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="C81" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D81" s="4">
         <v>1</v>
@@ -12389,10 +12436,10 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>40</v>
@@ -12487,10 +12534,10 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B90" t="s">
         <v>132</v>
-      </c>
-      <c r="B90" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -12530,7 +12577,7 @@
         <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>6</v>
@@ -12550,10 +12597,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="4">
@@ -12591,7 +12638,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>56</v>
@@ -12654,7 +12701,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="B8" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -12674,7 +12721,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="B9" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -12714,7 +12761,7 @@
     </row>
     <row r="12" spans="1:7" ht="14">
       <c r="A12" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
added fake values for cost coverage of interventions to avoid nans in code
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -291,11 +291,34 @@
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Ruth</author>
     <author xml:space="preserve"> Janka Petravic</author>
-    <author>Ruth</author>
   </authors>
   <commentList>
-    <comment ref="A10" authorId="0">
+    <comment ref="D6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+made up
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="1">
       <text>
         <r>
           <rPr>
@@ -317,7 +340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="1">
+    <comment ref="B10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -339,7 +362,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0">
+    <comment ref="A11" authorId="1">
       <text>
         <r>
           <rPr>
@@ -361,7 +384,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A18" authorId="0">
+    <comment ref="A18" authorId="1">
       <text>
         <r>
           <rPr>
@@ -383,7 +406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="0">
+    <comment ref="A25" authorId="1">
       <text>
         <r>
           <rPr>
@@ -405,7 +428,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C28" authorId="1">
+    <comment ref="C28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -427,7 +450,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B30" authorId="1">
+    <comment ref="B30" authorId="0">
       <text>
         <r>
           <rPr>
@@ -449,7 +472,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D30" authorId="1">
+    <comment ref="D30" authorId="0">
       <text>
         <r>
           <rPr>
@@ -5182,7 +5205,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -7825,7 +7848,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -7922,9 +7945,15 @@
       <c r="A6" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
+      <c r="B6" s="35">
+        <v>0</v>
+      </c>
+      <c r="C6" s="35">
+        <v>0.85</v>
+      </c>
+      <c r="D6" s="35">
+        <v>50</v>
+      </c>
       <c r="E6" s="4"/>
       <c r="F6" s="9"/>
       <c r="G6" s="4"/>
@@ -7933,9 +7962,15 @@
       <c r="A7" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
+      <c r="B7" s="35">
+        <v>0</v>
+      </c>
+      <c r="C7" s="35">
+        <v>0.85</v>
+      </c>
+      <c r="D7" s="35">
+        <v>1</v>
+      </c>
       <c r="E7" s="4"/>
       <c r="F7" s="9"/>
       <c r="G7" s="4"/>
@@ -8277,7 +8312,9 @@
       <c r="B29" s="15">
         <v>0</v>
       </c>
-      <c r="C29" s="14"/>
+      <c r="C29" s="14">
+        <v>0.85</v>
+      </c>
       <c r="D29" s="20">
         <v>1</v>
       </c>
@@ -8289,7 +8326,9 @@
       <c r="B30" s="15">
         <v>0.2</v>
       </c>
-      <c r="C30" s="14"/>
+      <c r="C30" s="14">
+        <v>0.85</v>
+      </c>
       <c r="D30" s="20">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
added malaria area interventions
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-73680" yWindow="-3580" windowWidth="27440" windowHeight="16760" tabRatio="500" firstSheet="12" activeTab="14"/>
+    <workbookView xWindow="-33940" yWindow="-3600" windowWidth="27440" windowHeight="16760" tabRatio="500" firstSheet="12" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -295,7 +295,7 @@
     <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="D6" authorId="0">
+    <comment ref="D7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -318,7 +318,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="1">
+    <comment ref="A14" authorId="1">
       <text>
         <r>
           <rPr>
@@ -340,7 +340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0">
+    <comment ref="B14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -362,7 +362,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="1">
+    <comment ref="A15" authorId="1">
       <text>
         <r>
           <rPr>
@@ -384,7 +384,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A18" authorId="1">
+    <comment ref="A22" authorId="1">
       <text>
         <r>
           <rPr>
@@ -406,7 +406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="1">
+    <comment ref="A29" authorId="1">
       <text>
         <r>
           <rPr>
@@ -428,7 +428,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C28" authorId="0">
+    <comment ref="C32" authorId="0">
       <text>
         <r>
           <rPr>
@@ -450,7 +450,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B30" authorId="0">
+    <comment ref="B34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -472,7 +472,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D30" authorId="0">
+    <comment ref="D34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1097,50 +1097,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="E7" authorId="0">
       <text>
         <r>
@@ -1185,7 +1141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0">
+    <comment ref="E9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1207,7 +1163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H9" authorId="0">
+    <comment ref="F9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1229,7 +1185,51 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="1">
+    <comment ref="G9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+food insecure - default poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+food insecure - default poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1251,7 +1251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="1">
+    <comment ref="B16" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1273,7 +1273,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="1">
+    <comment ref="A18" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1295,7 +1295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I14" authorId="1">
+    <comment ref="I18" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1317,7 +1317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I15" authorId="0">
+    <comment ref="I19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1339,7 +1339,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I21" authorId="1">
+    <comment ref="I25" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1361,7 +1361,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I22" authorId="0">
+    <comment ref="I26" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1380,380 +1380,6 @@
           </rPr>
           <t xml:space="preserve">
 food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E29" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F29" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G29" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H29" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I29" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E30" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F30" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G30" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H30" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I30" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E31" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F31" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G31" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H31" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I31" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C33" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D33" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
         </r>
       </text>
     </comment>
@@ -1775,7 +1401,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-At risk from malaria</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1797,7 +1423,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-At risk from malaria</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1819,7 +1445,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-At risk from malaria</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1841,11 +1467,385 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-At risk from malaria</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
     <comment ref="I33" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E34" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F34" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G34" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H34" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I34" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E35" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F35" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G35" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H35" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I35" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C37" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D37" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E37" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F37" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G37" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H37" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I37" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2049,7 +2049,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="182">
   <si>
     <t>year</t>
   </si>
@@ -2583,6 +2583,18 @@
   </si>
   <si>
     <t>Multiple micronutrient supplementation</t>
+  </si>
+  <si>
+    <t>Public provision of complementary foods with iron (malaria area)</t>
+  </si>
+  <si>
+    <t>Sprinkles (malaria area)</t>
+  </si>
+  <si>
+    <t>Multiple micronutrient supplementation (malaria area)</t>
+  </si>
+  <si>
+    <t>Iron and folic acid supplementation for pregnant women (malaria area)</t>
   </si>
 </sst>
 </file>
@@ -2687,7 +2699,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2716,6 +2728,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -2756,7 +2774,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="521">
+  <cellStyleXfs count="537">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3278,8 +3296,24 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3380,8 +3414,12 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="521">
+  <cellStyles count="537">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3642,6 +3680,14 @@
     <cellStyle name="Followed Hyperlink" xfId="516" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="518" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="520" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="522" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="524" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="526" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="528" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="530" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="532" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="534" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="536" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3901,6 +3947,14 @@
     <cellStyle name="Hyperlink" xfId="515" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="517" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="519" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="521" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="523" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="525" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="527" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="529" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="531" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="533" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="535" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -5552,16 +5606,16 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" customWidth="1"/>
+    <col min="2" max="2" width="54.83203125" customWidth="1"/>
     <col min="3" max="6" width="13.5" customWidth="1"/>
     <col min="7" max="7" width="12.5" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" customWidth="1"/>
@@ -5719,11 +5773,9 @@
         <v>0</v>
       </c>
       <c r="E6" s="31">
-        <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
       <c r="F6" s="31">
-        <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
       <c r="G6" s="31">
@@ -5738,7 +5790,7 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1">
       <c r="B7" s="4" t="s">
-        <v>84</v>
+        <v>178</v>
       </c>
       <c r="C7" s="3">
         <v>0</v>
@@ -5755,235 +5807,238 @@
         <v>0.36</v>
       </c>
       <c r="G7" s="31">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1">
+      <c r="B8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="31">
+        <v>0.36</v>
+      </c>
+      <c r="F8" s="31">
+        <v>0.36</v>
+      </c>
+      <c r="G8" s="31">
+        <v>0.36</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1">
+      <c r="B9" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="31">
         <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
-      <c r="H7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A9" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="31">
+      <c r="F9" s="31">
         <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
+      <c r="G9" s="31">
+        <f>'Baseline year demographics'!$C$7</f>
+        <v>0.36</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
       <c r="I9" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B10" t="s">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A11" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="31">
+        <f>'Baseline year demographics'!$C$7</f>
+        <v>0.36</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A12" s="11"/>
+      <c r="B12" t="s">
         <v>177</v>
       </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3">
-        <v>1</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B11" s="4" t="s">
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1">
+      <c r="B13" t="s">
+        <v>180</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1">
+      <c r="B14" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="36">
-        <v>1</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B12" t="s">
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="36">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1">
+      <c r="B15" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="36">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1">
+      <c r="B16" t="s">
         <v>157</v>
       </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0</v>
-      </c>
-      <c r="G12" s="3">
-        <v>0</v>
-      </c>
-      <c r="H12" s="36">
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="I12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A14" s="11" t="s">
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A18" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B18" t="s">
         <v>160</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3">
-        <v>0</v>
-      </c>
-      <c r="I14" s="59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B15" t="s">
-        <v>161</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0</v>
-      </c>
-      <c r="H15" s="3">
-        <v>0</v>
-      </c>
-      <c r="I15" s="59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B16" t="s">
-        <v>162</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0</v>
-      </c>
-      <c r="H16" s="3">
-        <v>0</v>
-      </c>
-      <c r="I16" s="59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B17" t="s">
-        <v>163</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0</v>
-      </c>
-      <c r="H17" s="3">
-        <v>0</v>
-      </c>
-      <c r="I17" s="59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B18" t="s">
-        <v>164</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
@@ -6009,7 +6064,7 @@
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1">
       <c r="B19" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -6035,7 +6090,7 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1">
       <c r="B20" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
@@ -6055,14 +6110,13 @@
       <c r="H20" s="3">
         <v>0</v>
       </c>
-      <c r="I20" s="60">
+      <c r="I20" s="59">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A21" s="11"/>
       <c r="B21" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
@@ -6088,7 +6142,7 @@
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1">
       <c r="B22" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
@@ -6114,7 +6168,7 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1">
       <c r="B23" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
@@ -6140,7 +6194,7 @@
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1">
       <c r="B24" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
@@ -6160,13 +6214,14 @@
       <c r="H24" s="3">
         <v>0</v>
       </c>
-      <c r="I24" s="59">
+      <c r="I24" s="60">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A25" s="11"/>
       <c r="B25" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C25" s="3">
         <v>0</v>
@@ -6192,7 +6247,7 @@
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1">
       <c r="B26" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
@@ -6218,192 +6273,296 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1">
       <c r="B27" t="s">
+        <v>172</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+      <c r="I27" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
+      <c r="I28" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B29" t="s">
+        <v>174</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0</v>
+      </c>
+      <c r="I29" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B30" t="s">
+        <v>175</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
+      <c r="I30" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B31" t="s">
         <v>176</v>
       </c>
-      <c r="C27" s="3">
-        <v>0</v>
-      </c>
-      <c r="D27" s="3">
-        <v>0</v>
-      </c>
-      <c r="E27" s="3">
-        <v>0</v>
-      </c>
-      <c r="F27" s="3">
-        <v>0</v>
-      </c>
-      <c r="G27" s="3">
-        <v>0</v>
-      </c>
-      <c r="H27" s="3">
-        <v>0</v>
-      </c>
-      <c r="I27" s="60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A29" s="11" t="s">
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
+      <c r="I31" s="60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A33" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="3">
-        <v>0</v>
-      </c>
-      <c r="D29" s="3">
-        <v>0</v>
-      </c>
-      <c r="E29" s="36">
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="F29" s="36">
+      <c r="F33" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="G29" s="36">
+      <c r="G33" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="H29" s="36">
+      <c r="H33" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="I29" s="36">
+      <c r="I33" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B30" s="4" t="s">
+    <row r="34" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B34" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="3">
-        <v>0</v>
-      </c>
-      <c r="D30" s="3">
-        <v>0</v>
-      </c>
-      <c r="E30" s="3">
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F34" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G34" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H34" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I34" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B31" s="4" t="s">
+    <row r="35" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B35" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="3">
-        <v>0</v>
-      </c>
-      <c r="D31" s="3">
-        <v>0</v>
-      </c>
-      <c r="E31" s="3">
+      <c r="C35" s="3">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0</v>
+      </c>
+      <c r="E35" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F35" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G35" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H35" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I35" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B32" s="4" t="s">
+    <row r="36" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B36" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C32" s="3">
-        <v>0</v>
-      </c>
-      <c r="D32" s="3">
-        <v>0</v>
-      </c>
-      <c r="E32" s="36">
-        <v>1</v>
-      </c>
-      <c r="F32" s="36">
-        <v>1</v>
-      </c>
-      <c r="G32" s="36">
-        <v>1</v>
-      </c>
-      <c r="H32" s="36">
-        <v>1</v>
-      </c>
-      <c r="I32" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B33" s="4" t="s">
+      <c r="C36" s="3">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0</v>
+      </c>
+      <c r="E36" s="36">
+        <v>1</v>
+      </c>
+      <c r="F36" s="36">
+        <v>1</v>
+      </c>
+      <c r="G36" s="36">
+        <v>1</v>
+      </c>
+      <c r="H36" s="36">
+        <v>1</v>
+      </c>
+      <c r="I36" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B37" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="36">
+      <c r="C37" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="D33" s="36">
+      <c r="D37" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E37" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="F33" s="36">
+      <c r="F37" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="G33" s="36">
+      <c r="G37" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="H33" s="36">
+      <c r="H37" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="I33" s="36">
+      <c r="I37" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
+    <row r="39" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7845,15 +8004,15 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="43.83203125" customWidth="1"/>
+    <col min="1" max="1" width="56" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
@@ -7945,13 +8104,13 @@
       <c r="A6" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="35">
-        <v>0</v>
-      </c>
-      <c r="C6" s="35">
+      <c r="B6" s="64">
+        <v>0</v>
+      </c>
+      <c r="C6" s="65">
         <v>0.85</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="65">
         <v>50</v>
       </c>
       <c r="E6" s="4"/>
@@ -7959,8 +8118,8 @@
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A7" s="34" t="s">
-        <v>84</v>
+      <c r="A7" s="4" t="s">
+        <v>178</v>
       </c>
       <c r="B7" s="35">
         <v>0</v>
@@ -7969,49 +8128,49 @@
         <v>0.85</v>
       </c>
       <c r="D7" s="35">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="9"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="64">
+        <v>0</v>
+      </c>
+      <c r="C8" s="65">
+        <v>0.85</v>
+      </c>
+      <c r="D8" s="65">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A9" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" s="35">
+        <v>0</v>
+      </c>
+      <c r="C9" s="35">
+        <v>0.85</v>
+      </c>
+      <c r="D9" s="35">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A10" t="s">
         <v>59</v>
-      </c>
-      <c r="B8" s="15">
-        <v>0</v>
-      </c>
-      <c r="C8" s="15">
-        <v>0.85</v>
-      </c>
-      <c r="D8" s="15">
-        <v>25</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A9" t="s">
-        <v>177</v>
-      </c>
-      <c r="B9" s="15">
-        <v>0</v>
-      </c>
-      <c r="C9" s="15">
-        <v>0.85</v>
-      </c>
-      <c r="D9" s="15">
-        <v>1.8</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A10" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="B10" s="15">
         <v>0</v>
@@ -8020,7 +8179,7 @@
         <v>0.85</v>
       </c>
       <c r="D10" s="15">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -8028,16 +8187,16 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" t="s">
-        <v>157</v>
-      </c>
-      <c r="B11" s="15">
-        <v>0</v>
-      </c>
-      <c r="C11" s="15">
+        <v>177</v>
+      </c>
+      <c r="B11" s="66">
+        <v>0</v>
+      </c>
+      <c r="C11" s="67">
         <v>0.85</v>
       </c>
-      <c r="D11" s="15">
-        <v>1</v>
+      <c r="D11" s="67">
+        <v>1.8</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -8045,7 +8204,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="B12" s="15">
         <v>0</v>
@@ -8054,23 +8213,23 @@
         <v>0.85</v>
       </c>
       <c r="D12" s="15">
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A13" t="s">
-        <v>161</v>
-      </c>
-      <c r="B13" s="15">
-        <v>0</v>
-      </c>
-      <c r="C13" s="15">
+      <c r="A13" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="66">
+        <v>0</v>
+      </c>
+      <c r="C13" s="67">
         <v>0.85</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="67">
         <v>1</v>
       </c>
       <c r="E13" s="4"/>
@@ -8078,8 +8237,8 @@
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A14" t="s">
-        <v>162</v>
+      <c r="A14" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="B14" s="15">
         <v>0</v>
@@ -8096,7 +8255,7 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B15" s="15">
         <v>0</v>
@@ -8113,7 +8272,7 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B16" s="15">
         <v>0</v>
@@ -8124,10 +8283,13 @@
       <c r="D16" s="15">
         <v>1</v>
       </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B17" s="15">
         <v>0</v>
@@ -8138,10 +8300,13 @@
       <c r="D17" s="15">
         <v>1</v>
       </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B18" s="15">
         <v>0</v>
@@ -8149,13 +8314,16 @@
       <c r="C18" s="15">
         <v>0.85</v>
       </c>
-      <c r="D18" s="20">
-        <v>1</v>
-      </c>
+      <c r="D18" s="15">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B19" s="15">
         <v>0</v>
@@ -8172,7 +8340,7 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B20" s="15">
         <v>0</v>
@@ -8183,13 +8351,10 @@
       <c r="D20" s="15">
         <v>1</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B21" s="15">
         <v>0</v>
@@ -8200,13 +8365,10 @@
       <c r="D21" s="15">
         <v>1</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B22" s="15">
         <v>0</v>
@@ -8214,16 +8376,13 @@
       <c r="C22" s="15">
         <v>0.85</v>
       </c>
-      <c r="D22" s="15">
-        <v>1</v>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="D22" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B23" s="15">
         <v>0</v>
@@ -8234,10 +8393,13 @@
       <c r="D23" s="15">
         <v>1</v>
       </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B24" s="15">
         <v>0</v>
@@ -8248,10 +8410,13 @@
       <c r="D24" s="15">
         <v>1</v>
       </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B25" s="15">
         <v>0</v>
@@ -8259,60 +8424,66 @@
       <c r="C25" s="15">
         <v>0.85</v>
       </c>
-      <c r="D25" s="20">
-        <v>1</v>
-      </c>
+      <c r="D25" s="15">
+        <v>1</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A26" s="4" t="s">
-        <v>90</v>
+      <c r="A26" t="s">
+        <v>173</v>
       </c>
       <c r="B26" s="15">
         <v>0</v>
       </c>
       <c r="C26" s="15">
-        <v>0.12</v>
-      </c>
-      <c r="D26" s="20">
-        <v>1</v>
-      </c>
+        <v>0.85</v>
+      </c>
+      <c r="D26" s="15">
+        <v>1</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A27" s="4" t="s">
-        <v>91</v>
+      <c r="A27" t="s">
+        <v>174</v>
       </c>
       <c r="B27" s="15">
         <v>0</v>
       </c>
       <c r="C27" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="D27" s="20">
+        <v>0.85</v>
+      </c>
+      <c r="D27" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A28" s="4" t="s">
-        <v>92</v>
+      <c r="A28" t="s">
+        <v>175</v>
       </c>
       <c r="B28" s="15">
         <v>0</v>
       </c>
       <c r="C28" s="15">
-        <v>0.8</v>
-      </c>
-      <c r="D28" s="20">
+        <v>0.85</v>
+      </c>
+      <c r="D28" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A29" s="4" t="s">
-        <v>110</v>
+      <c r="A29" t="s">
+        <v>176</v>
       </c>
       <c r="B29" s="15">
         <v>0</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="15">
         <v>0.85</v>
       </c>
       <c r="D29" s="20">
@@ -8321,41 +8492,97 @@
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1">
       <c r="A30" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="15">
+        <v>0</v>
+      </c>
+      <c r="C30" s="15">
+        <v>0.12</v>
+      </c>
+      <c r="D30" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A31" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="15">
+        <v>0</v>
+      </c>
+      <c r="C31" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="D31" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A32" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="15">
+        <v>0</v>
+      </c>
+      <c r="C32" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="D32" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A33" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="15">
+        <v>0</v>
+      </c>
+      <c r="C33" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D33" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A34" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B34" s="15">
         <v>0.2</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C34" s="14">
         <v>0.85</v>
       </c>
-      <c r="D30" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-    </row>
-    <row r="33" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-    </row>
-    <row r="34" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-    </row>
-    <row r="35" spans="2:3" ht="15.75" customHeight="1">
+      <c r="D34" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" customHeight="1">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="2:3" ht="15.75" customHeight="1">
+    <row r="36" spans="1:4" ht="15.75" customHeight="1">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
multiplied malaria area target pops by malaria risk
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-33940" yWindow="-3600" windowWidth="27440" windowHeight="16760" tabRatio="500" firstSheet="12" activeTab="14"/>
+    <workbookView xWindow="-70100" yWindow="-3100" windowWidth="27440" windowHeight="16760" tabRatio="500" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -5608,8 +5608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5799,12 +5799,12 @@
         <v>0</v>
       </c>
       <c r="E7" s="31">
-        <f>'Baseline year demographics'!$C$7</f>
-        <v>0.36</v>
+        <f>'Baseline year demographics'!$C$7*'Baseline year demographics'!C8</f>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="F7" s="31">
-        <f>'Baseline year demographics'!$C$7</f>
-        <v>0.36</v>
+        <f>'Baseline year demographics'!$C$7*'Baseline year demographics'!C8</f>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="G7" s="31">
         <v>0</v>
@@ -5853,16 +5853,16 @@
         <v>0</v>
       </c>
       <c r="E9" s="31">
-        <f>'Baseline year demographics'!$C$7</f>
-        <v>0.36</v>
+        <f>'Baseline year demographics'!$C$7*'Baseline year demographics'!C8</f>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="F9" s="31">
-        <f>'Baseline year demographics'!$C$7</f>
-        <v>0.36</v>
+        <f>'Baseline year demographics'!$C$7*'Baseline year demographics'!C8</f>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="G9" s="31">
-        <f>'Baseline year demographics'!$C$7</f>
-        <v>0.36</v>
+        <f>'Baseline year demographics'!$C$7*'Baseline year demographics'!C8</f>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="H9" s="3">
         <v>0</v>
@@ -5948,7 +5948,8 @@
         <v>0</v>
       </c>
       <c r="H13" s="3">
-        <v>1</v>
+        <f>1*'Baseline year demographics'!C8</f>
+        <v>0.1</v>
       </c>
       <c r="I13" s="3">
         <v>0</v>
@@ -6000,7 +6001,8 @@
         <v>0</v>
       </c>
       <c r="H15" s="36">
-        <v>1</v>
+        <f>1*'Baseline year demographics'!C8</f>
+        <v>0.1</v>
       </c>
       <c r="I15" s="3">
         <v>0</v>
@@ -8006,7 +8008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added zinc to spreadsheet
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-70100" yWindow="-3100" windowWidth="27440" windowHeight="16760" tabRatio="500" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="-70100" yWindow="-3100" windowWidth="27440" windowHeight="16760" tabRatio="500" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -295,7 +295,7 @@
     <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="D7" authorId="0">
+    <comment ref="D8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -315,50 +315,6 @@
           <t xml:space="preserve">
 made up
 </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A14" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B14" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fictional</t>
         </r>
       </text>
     </comment>
@@ -380,11 +336,55 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Also brestfeeding women up to 6 months?</t>
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
         </r>
       </text>
     </comment>
-    <comment ref="A22" authorId="1">
+    <comment ref="B15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fictional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A16" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Also brestfeeding women up to 6 months?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A23" authorId="1">
       <text>
         <r>
           <rPr>
@@ -406,7 +406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A29" authorId="1">
+    <comment ref="A30" authorId="1">
       <text>
         <r>
           <rPr>
@@ -428,7 +428,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C32" authorId="0">
+    <comment ref="C33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -450,7 +450,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B34" authorId="0">
+    <comment ref="B35" authorId="0">
       <text>
         <r>
           <rPr>
@@ -472,7 +472,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D34" authorId="0">
+    <comment ref="D35" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1075,7 +1075,7 @@
     <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0">
+    <comment ref="E6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1097,7 +1097,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0">
+    <comment ref="E8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1119,7 +1119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="0">
+    <comment ref="F8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1141,7 +1141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0">
+    <comment ref="E10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1163,7 +1163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0">
+    <comment ref="F10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1185,7 +1185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0">
+    <comment ref="G10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1207,7 +1207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H11" authorId="0">
+    <comment ref="H12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1226,28 +1226,6 @@
           </rPr>
           <t xml:space="preserve">
 food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B15" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
         </r>
       </text>
     </comment>
@@ -1269,11 +1247,33 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Also brestfeeding women up to 6 months?</t>
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
         </r>
       </text>
     </comment>
-    <comment ref="A18" authorId="1">
+    <comment ref="B17" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Also brestfeeding women up to 6 months?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A19" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1295,7 +1295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I18" authorId="1">
+    <comment ref="I19" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1317,7 +1317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I19" authorId="0">
+    <comment ref="I20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1339,7 +1339,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I25" authorId="1">
+    <comment ref="I26" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1361,7 +1361,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I26" authorId="0">
+    <comment ref="I27" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1380,116 +1380,6 @@
           </rPr>
           <t xml:space="preserve">
 food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E33" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F33" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G33" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H33" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I33" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1511,7 +1401,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1533,7 +1423,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1555,7 +1445,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1577,7 +1467,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1599,7 +1489,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1621,7 +1511,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1643,7 +1533,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1665,7 +1555,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1687,7 +1577,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1709,11 +1599,121 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
-    <comment ref="C37" authorId="1">
+    <comment ref="E36" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F36" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G36" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H36" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I36" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C38" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1735,7 +1735,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D37" authorId="1">
+    <comment ref="D38" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1757,7 +1757,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E37" authorId="1">
+    <comment ref="E38" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1779,7 +1779,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F37" authorId="1">
+    <comment ref="F38" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1801,7 +1801,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G37" authorId="1">
+    <comment ref="G38" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1823,7 +1823,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H37" authorId="1">
+    <comment ref="H38" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1845,7 +1845,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I37" authorId="1">
+    <comment ref="I38" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2049,7 +2049,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="183">
   <si>
     <t>year</t>
   </si>
@@ -2595,6 +2595,9 @@
   </si>
   <si>
     <t>Iron and folic acid supplementation for pregnant women (malaria area)</t>
+  </si>
+  <si>
+    <t>Zinc supplementation</t>
   </si>
 </sst>
 </file>
@@ -5606,10 +5609,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5683,8 +5686,9 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A3" s="11"/>
       <c r="B3" s="4" t="s">
-        <v>51</v>
+        <v>182</v>
       </c>
       <c r="C3" s="3">
         <v>0</v>
@@ -5710,7 +5714,7 @@
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C4" s="3">
         <v>0</v>
@@ -5725,7 +5729,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="3">
         <v>0</v>
@@ -5736,48 +5740,48 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1">
       <c r="B5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+      <c r="B6" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="31">
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="31">
         <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F6" s="31">
         <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
-      <c r="G5" s="31">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B6" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="31">
-        <v>0.36</v>
-      </c>
-      <c r="F6" s="31">
-        <v>0.36</v>
-      </c>
       <c r="G6" s="31">
         <v>0</v>
       </c>
@@ -5790,50 +5794,50 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1">
       <c r="B7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="31">
+        <v>0.36</v>
+      </c>
+      <c r="F7" s="31">
+        <v>0.36</v>
+      </c>
+      <c r="G7" s="31">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1">
+      <c r="B8" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="31">
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="31">
         <f>'Baseline year demographics'!$C$7*'Baseline year demographics'!C8</f>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="F7" s="31">
+      <c r="F8" s="31">
         <f>'Baseline year demographics'!$C$7*'Baseline year demographics'!C8</f>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G7" s="31">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B8" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="31">
-        <v>0.36</v>
-      </c>
-      <c r="F8" s="31">
-        <v>0.36</v>
-      </c>
       <c r="G8" s="31">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="H8" s="3">
         <v>0</v>
@@ -5844,229 +5848,229 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1">
       <c r="B9" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="31">
+        <v>0.36</v>
+      </c>
+      <c r="F9" s="31">
+        <v>0.36</v>
+      </c>
+      <c r="G9" s="31">
+        <v>0.36</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1">
+      <c r="B10" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="31">
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="31">
         <f>'Baseline year demographics'!$C$7*'Baseline year demographics'!C8</f>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="F9" s="31">
+      <c r="F10" s="31">
         <f>'Baseline year demographics'!$C$7*'Baseline year demographics'!C8</f>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G10" s="31">
         <f>'Baseline year demographics'!$C$7*'Baseline year demographics'!C8</f>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="H9" s="3">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A11" s="11" t="s">
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A12" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="31">
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="31">
         <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
-      <c r="I11" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A12" s="11"/>
-      <c r="B12" t="s">
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A13" s="11"/>
+      <c r="B13" t="s">
         <v>177</v>
       </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0</v>
-      </c>
-      <c r="G12" s="3">
-        <v>0</v>
-      </c>
-      <c r="H12" s="3">
-        <v>1</v>
-      </c>
-      <c r="I12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B13" t="s">
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1">
+      <c r="B14" t="s">
         <v>180</v>
       </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3">
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
         <f>1*'Baseline year demographics'!C8</f>
         <v>0.1</v>
       </c>
-      <c r="I13" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B14" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0</v>
-      </c>
-      <c r="H14" s="36">
-        <v>1</v>
-      </c>
       <c r="I14" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="B15" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="36">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1">
+      <c r="B16" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0</v>
-      </c>
-      <c r="H15" s="36">
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="36">
         <f>1*'Baseline year demographics'!C8</f>
         <v>0.1</v>
       </c>
-      <c r="I15" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B16" t="s">
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B17" t="s">
         <v>157</v>
       </c>
-      <c r="C16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0</v>
-      </c>
-      <c r="H16" s="36">
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="I16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A18" s="11" t="s">
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A19" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>160</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3">
-        <v>0</v>
-      </c>
-      <c r="I18" s="59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B19" t="s">
-        <v>161</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -6092,7 +6096,7 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1">
       <c r="B20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
@@ -6118,7 +6122,7 @@
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1">
       <c r="B21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
@@ -6144,7 +6148,7 @@
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1">
       <c r="B22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
@@ -6170,7 +6174,7 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1">
       <c r="B23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
@@ -6196,60 +6200,60 @@
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1">
       <c r="B24" t="s">
+        <v>165</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B25" t="s">
         <v>166</v>
       </c>
-      <c r="C24" s="3">
-        <v>0</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0</v>
-      </c>
-      <c r="E24" s="3">
-        <v>0</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0</v>
-      </c>
-      <c r="G24" s="3">
-        <v>0</v>
-      </c>
-      <c r="H24" s="3">
-        <v>0</v>
-      </c>
-      <c r="I24" s="60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A25" s="11"/>
-      <c r="B25" t="s">
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A26" s="11"/>
+      <c r="B26" t="s">
         <v>170</v>
-      </c>
-      <c r="C25" s="3">
-        <v>0</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0</v>
-      </c>
-      <c r="E25" s="3">
-        <v>0</v>
-      </c>
-      <c r="F25" s="3">
-        <v>0</v>
-      </c>
-      <c r="G25" s="3">
-        <v>0</v>
-      </c>
-      <c r="H25" s="3">
-        <v>0</v>
-      </c>
-      <c r="I25" s="59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B26" t="s">
-        <v>171</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
@@ -6275,7 +6279,7 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1">
       <c r="B27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C27" s="3">
         <v>0</v>
@@ -6301,7 +6305,7 @@
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1">
       <c r="B28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C28" s="3">
         <v>0</v>
@@ -6327,7 +6331,7 @@
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1">
       <c r="B29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
@@ -6353,7 +6357,7 @@
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1">
       <c r="B30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C30" s="3">
         <v>0</v>
@@ -6379,192 +6383,218 @@
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1">
       <c r="B31" t="s">
+        <v>175</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
+      <c r="I31" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B32" t="s">
         <v>176</v>
       </c>
-      <c r="C31" s="3">
-        <v>0</v>
-      </c>
-      <c r="D31" s="3">
-        <v>0</v>
-      </c>
-      <c r="E31" s="3">
-        <v>0</v>
-      </c>
-      <c r="F31" s="3">
-        <v>0</v>
-      </c>
-      <c r="G31" s="3">
-        <v>0</v>
-      </c>
-      <c r="H31" s="3">
-        <v>0</v>
-      </c>
-      <c r="I31" s="60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="C32" s="3">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0</v>
+      </c>
+      <c r="I32" s="60">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A33" s="11" t="s">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A34" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="3">
-        <v>0</v>
-      </c>
-      <c r="D33" s="3">
-        <v>0</v>
-      </c>
-      <c r="E33" s="36">
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0</v>
+      </c>
+      <c r="E34" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="F33" s="36">
+      <c r="F34" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="G33" s="36">
+      <c r="G34" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="H33" s="36">
+      <c r="H34" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="I33" s="36">
+      <c r="I34" s="36">
         <f>'Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B34" s="4" t="s">
+    <row r="35" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B35" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C34" s="3">
-        <v>0</v>
-      </c>
-      <c r="D34" s="3">
-        <v>0</v>
-      </c>
-      <c r="E34" s="3">
+      <c r="C35" s="3">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0</v>
+      </c>
+      <c r="E35" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F35" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G35" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H35" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I35" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B35" s="4" t="s">
+    <row r="36" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B36" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="3">
-        <v>0</v>
-      </c>
-      <c r="D35" s="3">
-        <v>0</v>
-      </c>
-      <c r="E35" s="3">
+      <c r="C36" s="3">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0</v>
+      </c>
+      <c r="E36" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F36" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G36" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="H35" s="3">
+      <c r="H36" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I36" s="3">
         <f>'Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B36" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C36" s="3">
-        <v>0</v>
-      </c>
-      <c r="D36" s="3">
-        <v>0</v>
-      </c>
-      <c r="E36" s="36">
-        <v>1</v>
-      </c>
-      <c r="F36" s="36">
-        <v>1</v>
-      </c>
-      <c r="G36" s="36">
-        <v>1</v>
-      </c>
-      <c r="H36" s="36">
-        <v>1</v>
-      </c>
-      <c r="I36" s="36">
-        <v>1</v>
-      </c>
-    </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1">
       <c r="B37" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37" s="36">
+        <v>1</v>
+      </c>
+      <c r="F37" s="36">
+        <v>1</v>
+      </c>
+      <c r="G37" s="36">
+        <v>1</v>
+      </c>
+      <c r="H37" s="36">
+        <v>1</v>
+      </c>
+      <c r="I37" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B38" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C37" s="36">
+      <c r="C38" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="D37" s="36">
+      <c r="D38" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="E37" s="36">
+      <c r="E38" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="F37" s="36">
+      <c r="F38" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="G37" s="36">
+      <c r="G38" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="H37" s="36">
+      <c r="H38" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="I37" s="36">
+      <c r="I38" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
+    <row r="40" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8006,10 +8036,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -8053,16 +8083,16 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>51</v>
+        <v>182</v>
       </c>
       <c r="B3" s="15">
-        <v>0.621</v>
+        <v>0</v>
       </c>
       <c r="C3" s="15">
         <v>0.85</v>
       </c>
       <c r="D3" s="15">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="9"/>
@@ -8070,16 +8100,16 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B4" s="15">
-        <v>0.247</v>
+        <v>0.621</v>
       </c>
       <c r="C4" s="15">
         <v>0.85</v>
       </c>
       <c r="D4" s="15">
-        <v>3.56</v>
+        <v>0.35</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="9"/>
@@ -8087,16 +8117,16 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>167</v>
+        <v>58</v>
       </c>
       <c r="B5" s="15">
-        <v>0</v>
+        <v>0.247</v>
       </c>
       <c r="C5" s="15">
         <v>0.85</v>
       </c>
       <c r="D5" s="15">
-        <v>48</v>
+        <v>3.56</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="9"/>
@@ -8104,16 +8134,16 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="64">
-        <v>0</v>
-      </c>
-      <c r="C6" s="65">
+        <v>167</v>
+      </c>
+      <c r="B6" s="15">
+        <v>0</v>
+      </c>
+      <c r="C6" s="15">
         <v>0.85</v>
       </c>
-      <c r="D6" s="65">
-        <v>50</v>
+      <c r="D6" s="15">
+        <v>48</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="9"/>
@@ -8121,15 +8151,15 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="B7" s="35">
-        <v>0</v>
-      </c>
-      <c r="C7" s="35">
+        <v>85</v>
+      </c>
+      <c r="B7" s="64">
+        <v>0</v>
+      </c>
+      <c r="C7" s="65">
         <v>0.85</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="65">
         <v>50</v>
       </c>
       <c r="E7" s="4"/>
@@ -8138,32 +8168,32 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" s="64">
-        <v>0</v>
-      </c>
-      <c r="C8" s="65">
+        <v>178</v>
+      </c>
+      <c r="B8" s="35">
+        <v>0</v>
+      </c>
+      <c r="C8" s="35">
         <v>0.85</v>
       </c>
-      <c r="D8" s="65">
-        <v>1</v>
+      <c r="D8" s="35">
+        <v>50</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="9"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A9" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="B9" s="35">
-        <v>0</v>
-      </c>
-      <c r="C9" s="35">
+      <c r="A9" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="64">
+        <v>0</v>
+      </c>
+      <c r="C9" s="65">
         <v>0.85</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="65">
         <v>1</v>
       </c>
       <c r="E9" s="4"/>
@@ -8171,34 +8201,34 @@
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="15">
-        <v>0</v>
-      </c>
-      <c r="C10" s="15">
+      <c r="A10" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="B10" s="35">
+        <v>0</v>
+      </c>
+      <c r="C10" s="35">
         <v>0.85</v>
       </c>
-      <c r="D10" s="15">
-        <v>25</v>
+      <c r="D10" s="35">
+        <v>1</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="F10" s="9"/>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" t="s">
-        <v>177</v>
-      </c>
-      <c r="B11" s="66">
-        <v>0</v>
-      </c>
-      <c r="C11" s="67">
+        <v>59</v>
+      </c>
+      <c r="B11" s="15">
+        <v>0</v>
+      </c>
+      <c r="C11" s="15">
         <v>0.85</v>
       </c>
-      <c r="D11" s="67">
-        <v>1.8</v>
+      <c r="D11" s="15">
+        <v>25</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -8206,15 +8236,15 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" t="s">
-        <v>180</v>
-      </c>
-      <c r="B12" s="15">
-        <v>0</v>
-      </c>
-      <c r="C12" s="15">
+        <v>177</v>
+      </c>
+      <c r="B12" s="66">
+        <v>0</v>
+      </c>
+      <c r="C12" s="67">
         <v>0.85</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="67">
         <v>1.8</v>
       </c>
       <c r="E12" s="4"/>
@@ -8222,17 +8252,17 @@
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="66">
-        <v>0</v>
-      </c>
-      <c r="C13" s="67">
+      <c r="A13" t="s">
+        <v>180</v>
+      </c>
+      <c r="B13" s="15">
+        <v>0</v>
+      </c>
+      <c r="C13" s="15">
         <v>0.85</v>
       </c>
-      <c r="D13" s="67">
-        <v>1</v>
+      <c r="D13" s="15">
+        <v>1.8</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -8240,15 +8270,15 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="B14" s="15">
-        <v>0</v>
-      </c>
-      <c r="C14" s="15">
+        <v>87</v>
+      </c>
+      <c r="B14" s="66">
+        <v>0</v>
+      </c>
+      <c r="C14" s="67">
         <v>0.85</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="67">
         <v>1</v>
       </c>
       <c r="E14" s="4"/>
@@ -8256,8 +8286,8 @@
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A15" t="s">
-        <v>157</v>
+      <c r="A15" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="B15" s="15">
         <v>0</v>
@@ -8274,7 +8304,7 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B16" s="15">
         <v>0</v>
@@ -8291,7 +8321,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B17" s="15">
         <v>0</v>
@@ -8308,7 +8338,7 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B18" s="15">
         <v>0</v>
@@ -8325,7 +8355,7 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B19" s="15">
         <v>0</v>
@@ -8342,7 +8372,7 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B20" s="15">
         <v>0</v>
@@ -8353,10 +8383,13 @@
       <c r="D20" s="15">
         <v>1</v>
       </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B21" s="15">
         <v>0</v>
@@ -8370,7 +8403,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B22" s="15">
         <v>0</v>
@@ -8378,13 +8411,13 @@
       <c r="C22" s="15">
         <v>0.85</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B23" s="15">
         <v>0</v>
@@ -8392,16 +8425,13 @@
       <c r="C23" s="15">
         <v>0.85</v>
       </c>
-      <c r="D23" s="15">
-        <v>1</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="D23" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B24" s="15">
         <v>0</v>
@@ -8418,7 +8448,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B25" s="15">
         <v>0</v>
@@ -8435,7 +8465,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B26" s="15">
         <v>0</v>
@@ -8452,7 +8482,7 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B27" s="15">
         <v>0</v>
@@ -8463,10 +8493,13 @@
       <c r="D27" s="15">
         <v>1</v>
       </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1">
       <c r="A28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B28" s="15">
         <v>0</v>
@@ -8480,7 +8513,7 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="A29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B29" s="15">
         <v>0</v>
@@ -8488,19 +8521,19 @@
       <c r="C29" s="15">
         <v>0.85</v>
       </c>
-      <c r="D29" s="20">
+      <c r="D29" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A30" s="4" t="s">
-        <v>90</v>
+      <c r="A30" t="s">
+        <v>176</v>
       </c>
       <c r="B30" s="15">
         <v>0</v>
       </c>
       <c r="C30" s="15">
-        <v>0.12</v>
+        <v>0.85</v>
       </c>
       <c r="D30" s="20">
         <v>1</v>
@@ -8508,13 +8541,13 @@
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B31" s="15">
         <v>0</v>
       </c>
       <c r="C31" s="15">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
       <c r="D31" s="20">
         <v>1</v>
@@ -8522,13 +8555,13 @@
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B32" s="15">
         <v>0</v>
       </c>
       <c r="C32" s="15">
-        <v>0.8</v>
+        <v>0.05</v>
       </c>
       <c r="D32" s="20">
         <v>1</v>
@@ -8536,13 +8569,13 @@
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="B33" s="15">
         <v>0</v>
       </c>
-      <c r="C33" s="14">
-        <v>0.85</v>
+      <c r="C33" s="15">
+        <v>0.8</v>
       </c>
       <c r="D33" s="20">
         <v>1</v>
@@ -8550,10 +8583,10 @@
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="B34" s="15">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C34" s="14">
         <v>0.85</v>
@@ -8563,8 +8596,18 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1">
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
+      <c r="A35" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="C35" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D35" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1">
       <c r="B36" s="4"/>
@@ -8585,6 +8628,10 @@
     <row r="40" spans="1:4" ht="15.75" customHeight="1">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added wasting to incidences tab (possibly incorrect data)
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Bangladesh/2017Aug/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-70100" yWindow="-3100" windowWidth="27440" windowHeight="16760" tabRatio="500" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="-32760" yWindow="-19860" windowWidth="27440" windowHeight="16760" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -23,13 +28,13 @@
     <sheet name="Interventions for children" sheetId="28" r:id="rId14"/>
     <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -2030,7 +2035,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="183">
   <si>
     <t>year</t>
   </si>
@@ -5254,13 +5259,13 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" customHeight="1">
+    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>115</v>
       </c>
@@ -5271,7 +5276,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>64</v>
       </c>
@@ -5282,7 +5287,7 @@
         <v>15204000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
@@ -5290,7 +5295,7 @@
         <v>3118117</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="34" t="s">
         <v>141</v>
       </c>
@@ -5298,7 +5303,7 @@
         <v>171684000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
@@ -5307,7 +5312,7 @@
         <v>3677298.8269880489</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="34" t="s">
         <v>73</v>
       </c>
@@ -5315,7 +5320,7 @@
         <v>0.35199999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>72</v>
       </c>
@@ -5323,7 +5328,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="34" t="s">
         <v>74</v>
       </c>
@@ -5331,11 +5336,11 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="11"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="11" t="s">
         <v>147</v>
       </c>
@@ -5346,7 +5351,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>142</v>
       </c>
@@ -5354,7 +5359,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>143</v>
       </c>
@@ -5362,7 +5367,7 @@
         <v>25.36</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>144</v>
       </c>
@@ -5370,7 +5375,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>145</v>
       </c>
@@ -5378,7 +5383,7 @@
         <v>34.68</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>146</v>
       </c>
@@ -5386,11 +5391,11 @@
         <v>39.32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="11"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
         <v>76</v>
       </c>
@@ -5401,7 +5406,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="34" t="s">
         <v>107</v>
       </c>
@@ -5409,7 +5414,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="34" t="s">
         <v>108</v>
       </c>
@@ -5417,7 +5422,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="34" t="s">
         <v>109</v>
       </c>
@@ -5425,7 +5430,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="34" t="s">
         <v>77</v>
       </c>
@@ -5433,10 +5438,10 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="34"/>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>140</v>
       </c>
@@ -5447,7 +5452,7 @@
         <v>8634000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="52" t="s">
         <v>134</v>
       </c>
@@ -5455,7 +5460,7 @@
         <v>13550000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="52" t="s">
         <v>135</v>
       </c>
@@ -5463,7 +5468,7 @@
         <v>12394000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="52" t="s">
         <v>136</v>
       </c>
@@ -5471,11 +5476,11 @@
         <v>9148000</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="52"/>
       <c r="C30" s="54"/>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>129</v>
       </c>
@@ -5486,7 +5491,7 @@
         <v>0.29978973218277538</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="15.75" customHeight="1">
+    <row r="33" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="51" t="s">
         <v>134</v>
       </c>
@@ -5494,7 +5499,7 @@
         <v>0.52556568434139284</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="15.75" customHeight="1">
+    <row r="34" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="51" t="s">
         <v>135</v>
       </c>
@@ -5502,7 +5507,7 @@
         <v>0.16210210664201097</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="15.75" customHeight="1">
+    <row r="35" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="51" t="s">
         <v>136</v>
       </c>
@@ -5514,11 +5519,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5533,12 +5533,12 @@
       <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
@@ -5572,14 +5572,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -5588,11 +5588,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5600,11 +5595,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="54.83203125" customWidth="1"/>
@@ -5615,7 +5610,7 @@
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>86</v>
       </c>
@@ -5645,7 +5640,7 @@
       </c>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
         <v>81</v>
       </c>
@@ -5674,7 +5669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="11"/>
       <c r="B3" s="4" t="s">
         <v>182</v>
@@ -5701,7 +5696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4" t="s">
         <v>51</v>
       </c>
@@ -5727,7 +5722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
         <v>58</v>
       </c>
@@ -5753,7 +5748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>167</v>
       </c>
@@ -5781,7 +5776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>85</v>
       </c>
@@ -5810,7 +5805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="4" t="s">
         <v>178</v>
       </c>
@@ -5838,7 +5833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>84</v>
       </c>
@@ -5867,7 +5862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>179</v>
       </c>
@@ -5896,7 +5891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="11" t="s">
         <v>82</v>
       </c>
@@ -5926,7 +5921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="11"/>
       <c r="B13" t="s">
         <v>177</v>
@@ -5953,7 +5948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>180</v>
       </c>
@@ -5980,7 +5975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="4" t="s">
         <v>87</v>
       </c>
@@ -6006,7 +6001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="4" t="s">
         <v>181</v>
       </c>
@@ -6033,7 +6028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>157</v>
       </c>
@@ -6060,7 +6055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
         <v>94</v>
       </c>
@@ -6089,7 +6084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>161</v>
       </c>
@@ -6115,7 +6110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
         <v>162</v>
       </c>
@@ -6141,7 +6136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" t="s">
         <v>163</v>
       </c>
@@ -6167,7 +6162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" t="s">
         <v>164</v>
       </c>
@@ -6193,7 +6188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
         <v>165</v>
       </c>
@@ -6219,7 +6214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
         <v>166</v>
       </c>
@@ -6245,7 +6240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="11"/>
       <c r="B26" t="s">
         <v>170</v>
@@ -6272,7 +6267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
         <v>171</v>
       </c>
@@ -6298,7 +6293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
         <v>172</v>
       </c>
@@ -6324,7 +6319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" t="s">
         <v>173</v>
       </c>
@@ -6350,7 +6345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1">
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" t="s">
         <v>174</v>
       </c>
@@ -6376,7 +6371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" t="s">
         <v>175</v>
       </c>
@@ -6402,7 +6397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1">
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>176</v>
       </c>
@@ -6428,11 +6423,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.75" customHeight="1">
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:9" ht="15.75" customHeight="1">
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="11" t="s">
         <v>89</v>
       </c>
@@ -6466,7 +6461,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1">
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="4" t="s">
         <v>91</v>
       </c>
@@ -6497,7 +6492,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75" customHeight="1">
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="4" t="s">
         <v>92</v>
       </c>
@@ -6528,7 +6523,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.75" customHeight="1">
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="4" t="s">
         <v>110</v>
       </c>
@@ -6554,7 +6549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.75" customHeight="1">
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="4" t="s">
         <v>88</v>
       </c>
@@ -6587,7 +6582,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.75" customHeight="1">
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
     </row>
@@ -6595,11 +6590,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6614,14 +6604,14 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -6641,7 +6631,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -6661,7 +6651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>55</v>
       </c>
@@ -6678,7 +6668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>177</v>
       </c>
@@ -6698,7 +6688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>55</v>
       </c>
@@ -6715,7 +6705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -6735,7 +6725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>55</v>
       </c>
@@ -6756,11 +6746,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6775,7 +6760,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="42.6640625" customWidth="1"/>
@@ -6784,7 +6769,7 @@
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="14" customHeight="1">
+    <row r="1" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>52</v>
       </c>
@@ -6831,7 +6816,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
         <v>158</v>
       </c>
@@ -6878,7 +6863,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>157</v>
       </c>
@@ -6922,7 +6907,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>160</v>
       </c>
@@ -6966,7 +6951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>161</v>
       </c>
@@ -7010,7 +6995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>162</v>
       </c>
@@ -7054,7 +7039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>163</v>
       </c>
@@ -7098,7 +7083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
         <v>164</v>
       </c>
@@ -7142,7 +7127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
         <v>165</v>
       </c>
@@ -7186,7 +7171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>166</v>
       </c>
@@ -7230,7 +7215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
         <v>170</v>
       </c>
@@ -7274,7 +7259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>171</v>
       </c>
@@ -7318,7 +7303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>172</v>
       </c>
@@ -7362,7 +7347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>173</v>
       </c>
@@ -7406,7 +7391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>174</v>
       </c>
@@ -7450,7 +7435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>175</v>
       </c>
@@ -7494,7 +7479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>176</v>
       </c>
@@ -7538,7 +7523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B18" s="4" t="s">
         <v>85</v>
       </c>
@@ -7582,7 +7567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20" s="11" t="s">
         <v>159</v>
       </c>
@@ -7629,7 +7614,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B21" s="4" t="s">
         <v>91</v>
       </c>
@@ -7673,7 +7658,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B22" s="4" t="s">
         <v>92</v>
       </c>
@@ -7717,7 +7702,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B23" s="4" t="s">
         <v>110</v>
       </c>
@@ -7761,7 +7746,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
         <v>84</v>
       </c>
@@ -7805,7 +7790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B25" s="4" t="s">
         <v>87</v>
       </c>
@@ -7849,28 +7834,23 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="37" spans="2:2"/>
-    <row r="38" spans="2:2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.15"/>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B38" s="4"/>
     </row>
-    <row r="39" spans="2:2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="2:2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="2:2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B41" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7885,7 +7865,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="27.5" customWidth="1"/>
     <col min="3" max="3" width="38.1640625" customWidth="1"/>
@@ -7895,7 +7875,7 @@
     <col min="8" max="8" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -7921,7 +7901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>51</v>
       </c>
@@ -7947,7 +7927,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C3" t="s">
         <v>69</v>
       </c>
@@ -7967,7 +7947,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -7989,7 +7969,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="12"/>
       <c r="B5" s="61" t="s">
         <v>169</v>
@@ -8013,7 +7993,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -8021,11 +8001,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8037,7 +8012,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="56" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -8045,7 +8020,7 @@
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -8059,7 +8034,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
@@ -8076,7 +8051,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>182</v>
       </c>
@@ -8093,7 +8068,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>51</v>
       </c>
@@ -8110,7 +8085,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>58</v>
       </c>
@@ -8127,7 +8102,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>167</v>
       </c>
@@ -8144,7 +8119,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>85</v>
       </c>
@@ -8161,7 +8136,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>178</v>
       </c>
@@ -8178,7 +8153,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>84</v>
       </c>
@@ -8195,7 +8170,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="34" t="s">
         <v>179</v>
       </c>
@@ -8212,7 +8187,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -8229,7 +8204,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>177</v>
       </c>
@@ -8246,7 +8221,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>180</v>
       </c>
@@ -8263,7 +8238,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>87</v>
       </c>
@@ -8280,7 +8255,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
         <v>181</v>
       </c>
@@ -8297,7 +8272,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>157</v>
       </c>
@@ -8314,7 +8289,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>160</v>
       </c>
@@ -8331,7 +8306,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>161</v>
       </c>
@@ -8348,7 +8323,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>162</v>
       </c>
@@ -8365,7 +8340,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>163</v>
       </c>
@@ -8382,7 +8357,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>164</v>
       </c>
@@ -8396,7 +8371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>165</v>
       </c>
@@ -8410,7 +8385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>166</v>
       </c>
@@ -8424,7 +8399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>170</v>
       </c>
@@ -8441,7 +8416,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>171</v>
       </c>
@@ -8458,7 +8433,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>172</v>
       </c>
@@ -8475,7 +8450,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>173</v>
       </c>
@@ -8492,7 +8467,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>174</v>
       </c>
@@ -8506,7 +8481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>175</v>
       </c>
@@ -8520,7 +8495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1">
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>176</v>
       </c>
@@ -8534,7 +8509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1">
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>90</v>
       </c>
@@ -8548,7 +8523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1">
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>91</v>
       </c>
@@ -8562,7 +8537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1">
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>92</v>
       </c>
@@ -8576,7 +8551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1">
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>110</v>
       </c>
@@ -8590,7 +8565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1">
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
         <v>88</v>
       </c>
@@ -8604,27 +8579,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1">
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1">
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1">
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1">
+    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1">
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1">
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
     </row>
@@ -8632,11 +8607,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8648,7 +8618,7 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
@@ -8656,7 +8626,7 @@
     <col min="11" max="11" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8694,7 +8664,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>2017</v>
       </c>
@@ -8736,7 +8706,7 @@
         <v>173766200</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>2018</v>
       </c>
@@ -8778,7 +8748,7 @@
         <v>175848400</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>2019</v>
       </c>
@@ -8820,7 +8790,7 @@
         <v>177930600</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>2020</v>
       </c>
@@ -8862,7 +8832,7 @@
         <v>180012800</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>2021</v>
       </c>
@@ -8904,7 +8874,7 @@
         <v>182095000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>2022</v>
       </c>
@@ -8946,7 +8916,7 @@
         <v>183822800</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>2023</v>
       </c>
@@ -8988,7 +8958,7 @@
         <v>185550600</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>2024</v>
       </c>
@@ -9030,7 +9000,7 @@
         <v>187278400</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>2025</v>
       </c>
@@ -9072,7 +9042,7 @@
         <v>189006200</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>2026</v>
       </c>
@@ -9114,7 +9084,7 @@
         <v>190734000</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>2027</v>
       </c>
@@ -9156,7 +9126,7 @@
         <v>192287600</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>2028</v>
       </c>
@@ -9198,7 +9168,7 @@
         <v>193841200</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>2029</v>
       </c>
@@ -9240,7 +9210,7 @@
         <v>195394800</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>2030</v>
       </c>
@@ -9286,11 +9256,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9302,12 +9267,12 @@
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -9330,7 +9295,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -9353,7 +9318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -9376,7 +9341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -9399,7 +9364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -9422,7 +9387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -9445,7 +9410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -9468,7 +9433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -9491,7 +9456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -9514,7 +9479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -9537,7 +9502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -9560,7 +9525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -9583,7 +9548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -9606,7 +9571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -9629,7 +9594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -9652,7 +9617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -9675,7 +9640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -9698,7 +9663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -9721,7 +9686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>98</v>
       </c>
@@ -9744,7 +9709,7 @@
         <v>2.5899999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -9767,7 +9732,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>100</v>
       </c>
@@ -9790,7 +9755,7 @@
         <v>0.25590000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>101</v>
       </c>
@@ -9813,7 +9778,7 @@
         <v>0.1464</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>102</v>
       </c>
@@ -9836,7 +9801,7 @@
         <v>1.7600000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -9859,7 +9824,7 @@
         <v>1.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -9882,7 +9847,7 @@
         <v>1.14E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -9905,7 +9870,7 @@
         <v>0.15129999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -9935,25 +9900,20 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
@@ -9973,7 +9933,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>29</v>
       </c>
@@ -9993,7 +9953,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>128</v>
       </c>
@@ -10013,7 +9973,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
@@ -10031,16 +9991,31 @@
       </c>
       <c r="F4" s="14">
         <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="61">
+        <v>2.6</v>
+      </c>
+      <c r="C5" s="61">
+        <v>2.6</v>
+      </c>
+      <c r="D5" s="61">
+        <v>2.6</v>
+      </c>
+      <c r="E5" s="61">
+        <v>2.6</v>
+      </c>
+      <c r="F5" s="61">
+        <v>2.6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -10052,7 +10027,7 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
@@ -10061,7 +10036,7 @@
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>117</v>
       </c>
@@ -10078,7 +10053,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
         <v>95</v>
       </c>
@@ -10093,7 +10068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="11"/>
       <c r="B3" t="s">
         <v>7</v>
@@ -10106,7 +10081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="11"/>
       <c r="B4" t="s">
         <v>8</v>
@@ -10121,7 +10096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="11"/>
       <c r="B5" t="s">
         <v>9</v>
@@ -10136,7 +10111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="11"/>
       <c r="B6" t="s">
         <v>10</v>
@@ -10151,7 +10126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="11"/>
       <c r="B7" t="s">
         <v>83</v>
@@ -10166,7 +10141,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="11"/>
       <c r="B8" t="s">
         <v>134</v>
@@ -10181,7 +10156,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>135</v>
@@ -10196,7 +10171,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>136</v>
@@ -10211,13 +10186,13 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="11"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="11"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="11" t="s">
         <v>96</v>
       </c>
@@ -10232,7 +10207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -10244,7 +10219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -10258,7 +10233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>9</v>
       </c>
@@ -10272,7 +10247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -10286,7 +10261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>83</v>
       </c>
@@ -10300,7 +10275,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>134</v>
       </c>
@@ -10314,7 +10289,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>135</v>
       </c>
@@ -10328,7 +10303,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
         <v>136</v>
       </c>
@@ -10342,7 +10317,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="11" t="s">
         <v>112</v>
       </c>
@@ -10363,11 +10338,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -10376,12 +10346,12 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -10404,7 +10374,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
@@ -10427,7 +10397,7 @@
         <v>25.35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
         <v>24</v>
@@ -10448,7 +10418,7 @@
         <v>33.25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="12"/>
       <c r="B4" s="13" t="s">
         <v>27</v>
@@ -10469,7 +10439,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="12"/>
       <c r="B5" s="13" t="s">
         <v>28</v>
@@ -10490,7 +10460,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
@@ -10513,7 +10483,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
@@ -10533,7 +10503,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
@@ -10553,7 +10523,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
@@ -10573,7 +10543,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
@@ -10596,7 +10566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
@@ -10616,7 +10586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="4" t="s">
         <v>42</v>
       </c>
@@ -10636,7 +10606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="4" t="s">
         <v>43</v>
       </c>
@@ -10661,11 +10631,6 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -10677,12 +10642,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>118</v>
       </c>
@@ -10702,7 +10667,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
         <v>12</v>
       </c>
@@ -10723,7 +10688,7 @@
         <v>3.1128200000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>114</v>
       </c>
@@ -10738,7 +10703,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>62</v>
       </c>
@@ -10755,14 +10720,14 @@
         <v>46.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="11"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="11"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="11" t="s">
         <v>5</v>
       </c>
@@ -10771,7 +10736,7 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
         <v>60</v>
       </c>
@@ -10791,7 +10756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
@@ -10808,7 +10773,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
@@ -10825,7 +10790,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
@@ -10842,7 +10807,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
@@ -10859,7 +10824,7 @@
         <v>999.99</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
@@ -10876,7 +10841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>46</v>
       </c>
@@ -10893,7 +10858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
@@ -10914,11 +10879,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -10929,11 +10889,11 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
@@ -10941,7 +10901,7 @@
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>60</v>
       </c>
@@ -10970,7 +10930,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
@@ -10999,7 +10959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
@@ -11022,7 +10982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C4" s="4" t="s">
         <v>27</v>
       </c>
@@ -11045,7 +11005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
@@ -11068,7 +11028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>31</v>
       </c>
@@ -11094,7 +11054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
@@ -11117,7 +11077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C8" s="4" t="s">
         <v>27</v>
       </c>
@@ -11140,7 +11100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C9" s="4" t="s">
         <v>28</v>
       </c>
@@ -11163,7 +11123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>33</v>
       </c>
@@ -11189,7 +11149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
@@ -11212,7 +11172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C12" s="4" t="s">
         <v>27</v>
       </c>
@@ -11235,7 +11195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
@@ -11258,7 +11218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>34</v>
       </c>
@@ -11284,7 +11244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
@@ -11307,7 +11267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C16" s="4" t="s">
         <v>27</v>
       </c>
@@ -11330,7 +11290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C17" s="4" t="s">
         <v>28</v>
       </c>
@@ -11353,7 +11313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>38</v>
       </c>
@@ -11379,7 +11339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C19" s="4" t="s">
         <v>24</v>
       </c>
@@ -11402,7 +11362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C20" s="4" t="s">
         <v>27</v>
       </c>
@@ -11425,7 +11385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C21" s="4" t="s">
         <v>28</v>
       </c>
@@ -11448,7 +11408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="11" t="s">
         <v>30</v>
       </c>
@@ -11477,7 +11437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C25" s="4" t="s">
         <v>24</v>
       </c>
@@ -11500,7 +11460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C26" s="4" t="s">
         <v>27</v>
       </c>
@@ -11523,7 +11483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C27" s="4" t="s">
         <v>28</v>
       </c>
@@ -11546,7 +11506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
         <v>31</v>
       </c>
@@ -11572,7 +11532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C29" s="4" t="s">
         <v>24</v>
       </c>
@@ -11595,7 +11555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C30" s="4" t="s">
         <v>27</v>
       </c>
@@ -11618,7 +11578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C31" s="4" t="s">
         <v>28</v>
       </c>
@@ -11641,7 +11601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>33</v>
       </c>
@@ -11667,7 +11627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C33" s="4" t="s">
         <v>24</v>
       </c>
@@ -11690,7 +11650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C34" s="4" t="s">
         <v>27</v>
       </c>
@@ -11713,7 +11673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C35" s="4" t="s">
         <v>28</v>
       </c>
@@ -11736,7 +11696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B36" t="s">
         <v>34</v>
       </c>
@@ -11762,7 +11722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C37" s="4" t="s">
         <v>24</v>
       </c>
@@ -11785,7 +11745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C38" s="4" t="s">
         <v>27</v>
       </c>
@@ -11808,7 +11768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C39" s="4" t="s">
         <v>28</v>
       </c>
@@ -11831,7 +11791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B40" t="s">
         <v>38</v>
       </c>
@@ -11857,7 +11817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C41" s="4" t="s">
         <v>24</v>
       </c>
@@ -11880,7 +11840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C42" s="4" t="s">
         <v>27</v>
       </c>
@@ -11903,7 +11863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C43" s="4" t="s">
         <v>28</v>
       </c>
@@ -11926,7 +11886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="11" t="s">
         <v>39</v>
       </c>
@@ -11955,7 +11915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C47" s="4" t="s">
         <v>41</v>
       </c>
@@ -11978,7 +11938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C48" s="4" t="s">
         <v>42</v>
       </c>
@@ -12001,7 +11961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:9">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C49" s="4" t="s">
         <v>43</v>
       </c>
@@ -12024,7 +11984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:9">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B50" t="s">
         <v>16</v>
       </c>
@@ -12050,7 +12010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:9">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C51" s="4" t="s">
         <v>41</v>
       </c>
@@ -12073,7 +12033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:9">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C52" s="4" t="s">
         <v>42</v>
       </c>
@@ -12096,7 +12056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:9">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C53" s="4" t="s">
         <v>43</v>
       </c>
@@ -12119,7 +12079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:9">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B54" t="s">
         <v>17</v>
       </c>
@@ -12145,7 +12105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:9">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C55" s="4" t="s">
         <v>41</v>
       </c>
@@ -12168,7 +12128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:9">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C56" s="4" t="s">
         <v>42</v>
       </c>
@@ -12191,7 +12151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:9">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C57" s="4" t="s">
         <v>43</v>
       </c>
@@ -12214,7 +12174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:9">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B58" t="s">
         <v>22</v>
       </c>
@@ -12240,7 +12200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:9">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C59" s="4" t="s">
         <v>41</v>
       </c>
@@ -12263,7 +12223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:9">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C60" s="4" t="s">
         <v>42</v>
       </c>
@@ -12286,7 +12246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:9">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C61" s="4" t="s">
         <v>43</v>
       </c>
@@ -12309,7 +12269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:9">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B62" t="s">
         <v>29</v>
       </c>
@@ -12335,7 +12295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:9">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C63" s="4" t="s">
         <v>41</v>
       </c>
@@ -12358,7 +12318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:9">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C64" s="4" t="s">
         <v>42</v>
       </c>
@@ -12381,7 +12341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C65" s="4" t="s">
         <v>43</v>
       </c>
@@ -12404,7 +12364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B66" t="s">
         <v>31</v>
       </c>
@@ -12430,7 +12390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C67" s="4" t="s">
         <v>41</v>
       </c>
@@ -12453,7 +12413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C68" s="4" t="s">
         <v>42</v>
       </c>
@@ -12476,7 +12436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C69" s="4" t="s">
         <v>43</v>
       </c>
@@ -12499,7 +12459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B70" t="s">
         <v>32</v>
       </c>
@@ -12525,7 +12485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C71" s="4" t="s">
         <v>41</v>
       </c>
@@ -12548,7 +12508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C72" s="4" t="s">
         <v>42</v>
       </c>
@@ -12571,7 +12531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C73" s="4" t="s">
         <v>43</v>
       </c>
@@ -12594,7 +12554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A76" s="11" t="s">
         <v>130</v>
       </c>
@@ -12623,7 +12583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C77" s="4" t="s">
         <v>120</v>
       </c>
@@ -12646,7 +12606,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B78" t="s">
         <v>99</v>
       </c>
@@ -12672,7 +12632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C79" s="4" t="s">
         <v>120</v>
       </c>
@@ -12695,7 +12655,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B80" t="s">
         <v>100</v>
       </c>
@@ -12721,7 +12681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C81" s="4" t="s">
         <v>120</v>
       </c>
@@ -12744,7 +12704,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A84" s="11" t="s">
         <v>111</v>
       </c>
@@ -12773,7 +12733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C85" s="4" t="s">
         <v>41</v>
       </c>
@@ -12796,7 +12756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C86" s="4" t="s">
         <v>42</v>
       </c>
@@ -12819,7 +12779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C87" s="4" t="s">
         <v>43</v>
       </c>
@@ -12842,7 +12802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A90" s="11" t="s">
         <v>131</v>
       </c>
@@ -12853,11 +12813,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -12872,7 +12827,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="36.6640625" customWidth="1"/>
     <col min="2" max="2" width="64.5" customWidth="1"/>
@@ -12882,7 +12837,7 @@
     <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>52</v>
       </c>
@@ -12905,7 +12860,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
         <v>122</v>
       </c>
@@ -12926,7 +12881,7 @@
         <v>174.7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
         <v>29</v>
       </c>
@@ -12946,7 +12901,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="11" t="s">
         <v>121</v>
       </c>
@@ -12969,7 +12924,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>48</v>
       </c>
@@ -12989,7 +12944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>49</v>
       </c>
@@ -13009,7 +12964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B8" s="4" t="s">
         <v>148</v>
       </c>
@@ -13029,7 +12984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>133</v>
       </c>
@@ -13049,7 +13004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>50</v>
       </c>
@@ -13069,7 +13024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>123</v>
       </c>
@@ -13092,7 +13047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14">
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>58</v>
       </c>
@@ -13116,10 +13071,5 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bug fixes after testing adding coverage constraints
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-70100" yWindow="-3100" windowWidth="27440" windowHeight="16760" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-73300" yWindow="-1420" windowWidth="25600" windowHeight="14680" tabRatio="500" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -5597,8 +5597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5768,7 +5768,7 @@
         <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G6" s="59">
         <v>0</v>
       </c>
       <c r="H6" s="3">
@@ -5796,9 +5796,8 @@
         <f>'Baseline year demographics'!$C$7*(1-'Baseline year demographics'!C8)</f>
         <v>0.32400000000000001</v>
       </c>
-      <c r="G7" s="31">
-        <f>'Baseline year demographics'!$C$7*(1-'Baseline year demographics'!C8)</f>
-        <v>0.32400000000000001</v>
+      <c r="G7" s="59">
+        <v>0</v>
       </c>
       <c r="H7" s="3">
         <v>0</v>
@@ -5825,7 +5824,7 @@
         <f>'Baseline year demographics'!$C$7*'Baseline year demographics'!C8</f>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="59">
         <v>0</v>
       </c>
       <c r="H8" s="3">
@@ -9944,7 +9943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added mission interventions RR/OR to spreadsheet and started writing demo script
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-73300" yWindow="-1420" windowWidth="25600" windowHeight="14680" tabRatio="500" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23480" windowHeight="13160" tabRatio="500" firstSheet="10" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -1891,7 +1891,7 @@
     <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="E23" authorId="0">
+    <comment ref="E25" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1914,7 +1914,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G24" authorId="0">
+    <comment ref="E26" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1936,7 +1936,117 @@
         </r>
       </text>
     </comment>
-    <comment ref="B25" authorId="1">
+    <comment ref="F26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+mader this number up</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+mader this number up</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E27" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+mader this number up</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F27" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+mader this number up</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G27" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+mader this number up</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B28" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1958,7 +2068,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L25" authorId="0">
+    <comment ref="L28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1981,7 +2091,52 @@
         </r>
       </text>
     </comment>
-    <comment ref="B37" authorId="1">
+    <comment ref="B29" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+made this number up
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B40" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2003,7 +2158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B41" authorId="1">
+    <comment ref="B44" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2030,7 +2185,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="183">
   <si>
     <t>year</t>
   </si>
@@ -2576,6 +2731,9 @@
   </si>
   <si>
     <t>Zinc supplementation</t>
+  </si>
+  <si>
+    <t>Multiple micronutrient supplementation(malaria area)</t>
   </si>
 </sst>
 </file>
@@ -2755,7 +2913,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="541">
+  <cellStyleXfs count="565">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2767,6 +2925,30 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3404,7 +3586,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="541">
+  <cellStyles count="565">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3675,6 +3857,18 @@
     <cellStyle name="Followed Hyperlink" xfId="536" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="538" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="540" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="542" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="544" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="546" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="548" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="550" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="552" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="554" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="556" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="560" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3944,6 +4138,18 @@
     <cellStyle name="Hyperlink" xfId="535" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="537" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="539" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="541" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="543" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="545" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="547" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="549" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="551" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="553" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="555" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="559" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -5248,7 +5454,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5597,8 +5803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -6765,16 +6971,16 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
     <col min="3" max="3" width="18.83203125" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
@@ -6875,8 +7081,9 @@
       </c>
     </row>
     <row r="3" spans="1:15">
+      <c r="A3" s="11"/>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -6906,21 +7113,21 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.83</v>
+        <v>0.3</v>
       </c>
       <c r="M3">
-        <v>0.83</v>
+        <v>0.3</v>
       </c>
       <c r="N3">
-        <v>0.83</v>
+        <v>0.3</v>
       </c>
       <c r="O3">
-        <v>0.83</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="B4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -6938,33 +7145,33 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="B5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -7008,7 +7215,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="B6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -7052,7 +7259,7 @@
     </row>
     <row r="7" spans="1:15">
       <c r="B7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -7096,7 +7303,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="B8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -7140,7 +7347,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="B9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -7184,7 +7391,7 @@
     </row>
     <row r="10" spans="1:15">
       <c r="B10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -7228,7 +7435,7 @@
     </row>
     <row r="11" spans="1:15">
       <c r="B11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -7272,7 +7479,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="B12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -7316,7 +7523,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="B13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -7360,7 +7567,7 @@
     </row>
     <row r="14" spans="1:15">
       <c r="B14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -7404,7 +7611,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="B15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -7448,7 +7655,7 @@
     </row>
     <row r="16" spans="1:15">
       <c r="B16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -7492,7 +7699,7 @@
     </row>
     <row r="17" spans="1:15">
       <c r="B17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -7535,143 +7742,143 @@
       </c>
     </row>
     <row r="18" spans="1:15">
-      <c r="B18" s="4" t="s">
+      <c r="B18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0.73</v>
+      </c>
+      <c r="I18">
+        <v>0.73</v>
+      </c>
+      <c r="J18">
+        <v>0.73</v>
+      </c>
+      <c r="K18">
+        <v>0.73</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="B19" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" s="61">
-        <v>1</v>
-      </c>
-      <c r="F18" s="61">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18">
-        <v>1</v>
-      </c>
-      <c r="N18">
-        <v>1</v>
-      </c>
-      <c r="O18">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="61">
+        <v>0.75</v>
+      </c>
+      <c r="F19" s="61">
+        <v>0.75</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="11" t="s">
+      <c r="B20" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="61">
+        <v>0.75</v>
+      </c>
+      <c r="F20" s="61">
+        <v>0.75</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="F20" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="G20" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="H20" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="I20" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="J20" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="K20" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="L20" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="M20" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="N20" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="O20" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="B21" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="F21" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="G21" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="H21" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="I21" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="J21" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="K21" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="L21" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="M21" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="N21" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="O21" s="57">
-        <v>0.97599999999999998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
-      <c r="B22" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -7715,7 +7922,7 @@
     </row>
     <row r="23" spans="1:15">
       <c r="B23" s="4" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -7723,43 +7930,43 @@
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="E23" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="F23" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="G23" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="H23" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="I23" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="J23" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="K23" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="L23" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="M23" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="N23" s="58">
-        <v>0.9</v>
-      </c>
-      <c r="O23" s="58">
-        <v>0.9</v>
+      <c r="E23" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="F23" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="G23" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="H23" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="I23" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="J23" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="K23" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="L23" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="M23" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="N23" s="57">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="O23" s="57">
+        <v>0.97599999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:15">
-      <c r="B24" t="s">
-        <v>84</v>
+      <c r="B24" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -7768,42 +7975,42 @@
         <v>1</v>
       </c>
       <c r="E24" s="57">
-        <v>1</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="F24" s="57">
-        <v>1</v>
-      </c>
-      <c r="G24" s="58">
-        <v>0.8</v>
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="G24" s="57">
+        <v>0.97599999999999998</v>
       </c>
       <c r="H24" s="57">
-        <v>1</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="I24" s="57">
-        <v>1</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="J24" s="57">
-        <v>1</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="K24" s="57">
-        <v>1</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="L24" s="57">
-        <v>1</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="M24" s="57">
-        <v>1</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="N24" s="57">
-        <v>1</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="O24" s="57">
-        <v>1</v>
+        <v>0.97599999999999998</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="B25" s="4" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -7811,26 +8018,26 @@
       <c r="D25">
         <v>1</v>
       </c>
-      <c r="E25" s="57">
-        <v>1</v>
-      </c>
-      <c r="F25" s="57">
-        <v>1</v>
-      </c>
-      <c r="G25" s="57">
-        <v>1</v>
-      </c>
-      <c r="H25" s="57">
-        <v>1</v>
-      </c>
-      <c r="I25" s="57">
-        <v>1</v>
-      </c>
-      <c r="J25" s="57">
-        <v>1</v>
-      </c>
-      <c r="K25" s="57">
-        <v>1</v>
+      <c r="E25" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="F25" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="G25" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="H25" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="I25" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="J25" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="K25" s="58">
+        <v>0.9</v>
       </c>
       <c r="L25" s="58">
         <v>0.9</v>
@@ -7845,18 +8052,194 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="37" spans="2:2"/>
-    <row r="38" spans="2:2">
-      <c r="B38" s="4"/>
-    </row>
-    <row r="39" spans="2:2">
-      <c r="B39" s="4"/>
-    </row>
-    <row r="40" spans="2:2">
-      <c r="B40" s="4"/>
-    </row>
+    <row r="26" spans="1:15">
+      <c r="B26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="58">
+        <v>0.8</v>
+      </c>
+      <c r="F26" s="58">
+        <v>0.8</v>
+      </c>
+      <c r="G26" s="58">
+        <v>0.8</v>
+      </c>
+      <c r="H26" s="57">
+        <v>1</v>
+      </c>
+      <c r="I26" s="57">
+        <v>1</v>
+      </c>
+      <c r="J26" s="57">
+        <v>1</v>
+      </c>
+      <c r="K26" s="57">
+        <v>1</v>
+      </c>
+      <c r="L26" s="57">
+        <v>1</v>
+      </c>
+      <c r="M26" s="57">
+        <v>1</v>
+      </c>
+      <c r="N26" s="57">
+        <v>1</v>
+      </c>
+      <c r="O26" s="57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="B27" t="s">
+        <v>178</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="58">
+        <v>0.8</v>
+      </c>
+      <c r="F27" s="58">
+        <v>0.8</v>
+      </c>
+      <c r="G27" s="58">
+        <v>0.8</v>
+      </c>
+      <c r="H27" s="57">
+        <v>1</v>
+      </c>
+      <c r="I27" s="57">
+        <v>1</v>
+      </c>
+      <c r="J27" s="57">
+        <v>1</v>
+      </c>
+      <c r="K27" s="57">
+        <v>1</v>
+      </c>
+      <c r="L27" s="57">
+        <v>1</v>
+      </c>
+      <c r="M27" s="57">
+        <v>1</v>
+      </c>
+      <c r="N27" s="57">
+        <v>1</v>
+      </c>
+      <c r="O27" s="57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="B28" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" s="57">
+        <v>1</v>
+      </c>
+      <c r="F28" s="57">
+        <v>1</v>
+      </c>
+      <c r="G28" s="57">
+        <v>1</v>
+      </c>
+      <c r="H28" s="57">
+        <v>1</v>
+      </c>
+      <c r="I28" s="57">
+        <v>1</v>
+      </c>
+      <c r="J28" s="57">
+        <v>1</v>
+      </c>
+      <c r="K28" s="57">
+        <v>1</v>
+      </c>
+      <c r="L28" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="M28" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="N28" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="O28" s="58">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="B29" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" s="57">
+        <v>1</v>
+      </c>
+      <c r="F29" s="57">
+        <v>1</v>
+      </c>
+      <c r="G29" s="57">
+        <v>1</v>
+      </c>
+      <c r="H29" s="57">
+        <v>1</v>
+      </c>
+      <c r="I29" s="57">
+        <v>1</v>
+      </c>
+      <c r="J29" s="57">
+        <v>1</v>
+      </c>
+      <c r="K29" s="57">
+        <v>1</v>
+      </c>
+      <c r="L29" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="M29" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="N29" s="58">
+        <v>0.9</v>
+      </c>
+      <c r="O29" s="58">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2"/>
     <row r="41" spans="2:2">
       <c r="B41" s="4"/>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="4"/>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="4"/>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8029,8 +8412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -10925,7 +11308,7 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adjusted anemia data RR/OR values
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23480" windowHeight="13160" tabRatio="500" firstSheet="10" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23480" windowHeight="13160" tabRatio="500" firstSheet="12" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -2068,29 +2068,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="L28" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-made this number up
-</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B29" authorId="1">
       <text>
         <r>
@@ -2110,29 +2087,6 @@
           </rPr>
           <t xml:space="preserve">
 Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L29" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-made this number up
-</t>
         </r>
       </text>
     </comment>
@@ -2910,7 +2864,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="567">
+  <cellStyleXfs count="573">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2922,6 +2876,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3586,7 +3546,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="567">
+  <cellStyles count="573">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3870,6 +3830,9 @@
     <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="572" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4152,6 +4115,9 @@
     <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="571" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -5456,7 +5422,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5806,7 +5772,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -6975,8 +6941,8 @@
   </sheetPr>
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -8174,16 +8140,16 @@
         <v>1</v>
       </c>
       <c r="L28" s="58">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="M28" s="58">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="N28" s="58">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="O28" s="58">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -8218,16 +8184,16 @@
         <v>1</v>
       </c>
       <c r="L29" s="58">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="M29" s="58">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="N29" s="58">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="O29" s="58">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="40" spans="2:2"/>

</xml_diff>

<commit_message>
updated fictional values in spreadsheet
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -2864,7 +2864,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="573">
+  <cellStyleXfs count="625">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2876,6 +2876,58 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3546,7 +3598,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="573">
+  <cellStyles count="625">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3833,6 +3885,32 @@
     <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="572" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="574" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="576" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="578" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="580" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="582" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="584" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="586" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="592" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="594" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="596" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="598" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="600" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="602" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="604" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="606" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="608" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="610" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="612" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="614" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="616" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="618" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="620" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="622" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="624" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4118,6 +4196,32 @@
     <cellStyle name="Hyperlink" xfId="567" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="569" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="571" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="573" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="575" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="577" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="579" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="581" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="583" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="585" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="591" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="593" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="595" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="597" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="599" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="601" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="603" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="605" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="607" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="609" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="611" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="613" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="615" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="617" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="619" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="621" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="623" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -6941,8 +7045,8 @@
   </sheetPr>
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -7764,10 +7868,10 @@
         <v>1</v>
       </c>
       <c r="E19" s="61">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="F19" s="61">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -7808,10 +7912,10 @@
         <v>1</v>
       </c>
       <c r="E20" s="61">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="F20" s="61">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -8031,13 +8135,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="58">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="F26" s="58">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="G26" s="58">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H26" s="57">
         <v>1</v>
@@ -8075,13 +8179,13 @@
         <v>1</v>
       </c>
       <c r="E27" s="58">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="F27" s="58">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="G27" s="58">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H27" s="57">
         <v>1</v>
@@ -8380,8 +8484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
changed unit cost and saturation to lower case so that code works
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23480" windowHeight="13160" tabRatio="500" firstSheet="12" activeTab="12"/>
+    <workbookView xWindow="-71720" yWindow="-3740" windowWidth="23480" windowHeight="13160" tabRatio="500" firstSheet="12" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -2516,12 +2516,6 @@
     <t>Baseline coverage</t>
   </si>
   <si>
-    <t>Saturation coverage</t>
-  </si>
-  <si>
-    <t>Unit cost</t>
-  </si>
-  <si>
     <t>Affected fraction</t>
   </si>
   <si>
@@ -2685,6 +2679,12 @@
   </si>
   <si>
     <t>Zinc supplementation</t>
+  </si>
+  <si>
+    <t>saturation coverage</t>
+  </si>
+  <si>
+    <t>unit cost</t>
   </si>
 </sst>
 </file>
@@ -2864,7 +2864,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="625">
+  <cellStyleXfs count="627">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2876,6 +2876,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3598,7 +3600,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="625">
+  <cellStyles count="627">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3911,6 +3913,7 @@
     <cellStyle name="Followed Hyperlink" xfId="620" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="622" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="624" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="626" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4222,6 +4225,7 @@
     <cellStyle name="Hyperlink" xfId="619" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="621" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="623" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="625" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -5526,7 +5530,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5567,7 +5571,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="B4" s="34" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C4" s="55">
         <v>171684000</v>
@@ -5612,7 +5616,7 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1">
       <c r="A11" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B11" t="s">
         <v>79</v>
@@ -5623,7 +5627,7 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1">
       <c r="B12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C12" s="20">
         <v>0.13</v>
@@ -5631,7 +5635,7 @@
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1">
       <c r="B13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C13" s="20">
         <v>25.36</v>
@@ -5639,7 +5643,7 @@
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1">
       <c r="B14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C14" s="20">
         <v>25.4</v>
@@ -5647,7 +5651,7 @@
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1">
       <c r="B15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C15" s="20">
         <v>34.68</v>
@@ -5655,7 +5659,7 @@
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1">
       <c r="B16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C16" s="20">
         <v>39.32</v>
@@ -5713,7 +5717,7 @@
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="A26" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B26" s="52" t="s">
         <v>83</v>
@@ -5724,7 +5728,7 @@
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1">
       <c r="B27" s="52" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C27" s="53">
         <v>13550000</v>
@@ -5732,7 +5736,7 @@
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1">
       <c r="B28" s="52" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C28" s="53">
         <v>12394000</v>
@@ -5740,7 +5744,7 @@
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1">
       <c r="B29" s="52" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C29" s="53">
         <v>9148000</v>
@@ -5752,7 +5756,7 @@
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="A32" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B32" s="43" t="s">
         <v>83</v>
@@ -5763,7 +5767,7 @@
     </row>
     <row r="33" spans="2:3" ht="15.75" customHeight="1">
       <c r="B33" s="51" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C33" s="44">
         <v>0.52556568434139284</v>
@@ -5771,7 +5775,7 @@
     </row>
     <row r="34" spans="2:3" ht="15.75" customHeight="1">
       <c r="B34" s="51" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C34" s="44">
         <v>0.16210210664201097</v>
@@ -5779,7 +5783,7 @@
     </row>
     <row r="35" spans="2:3" ht="15.75" customHeight="1">
       <c r="B35" s="51" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C35" s="44">
         <v>1.2542476833820825E-2</v>
@@ -5952,7 +5956,7 @@
     <row r="3" spans="1:10" ht="15.75" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C3" s="3">
         <v>0</v>
@@ -6030,7 +6034,7 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -6086,7 +6090,7 @@
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1">
       <c r="B8" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
@@ -6143,7 +6147,7 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1">
       <c r="B10" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
@@ -6203,7 +6207,7 @@
     <row r="13" spans="1:10" ht="15.75" customHeight="1">
       <c r="A13" s="11"/>
       <c r="B13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C13" s="3">
         <v>0</v>
@@ -6229,7 +6233,7 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="B14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
@@ -6282,7 +6286,7 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="B16" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -6309,7 +6313,7 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1">
       <c r="B17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C17" s="3">
         <v>0</v>
@@ -6339,7 +6343,7 @@
         <v>94</v>
       </c>
       <c r="B19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -6365,7 +6369,7 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1">
       <c r="B20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
@@ -6391,7 +6395,7 @@
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1">
       <c r="B21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
@@ -6417,7 +6421,7 @@
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1">
       <c r="B22" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
@@ -6443,7 +6447,7 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1">
       <c r="B23" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
@@ -6469,7 +6473,7 @@
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1">
       <c r="B24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
@@ -6495,7 +6499,7 @@
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1">
       <c r="B25" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C25" s="3">
         <v>0</v>
@@ -6522,7 +6526,7 @@
     <row r="26" spans="1:9" ht="15.75" customHeight="1">
       <c r="A26" s="11"/>
       <c r="B26" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
@@ -6548,7 +6552,7 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1">
       <c r="B27" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C27" s="3">
         <v>0</v>
@@ -6574,7 +6578,7 @@
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1">
       <c r="B28" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C28" s="3">
         <v>0</v>
@@ -6600,7 +6604,7 @@
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1">
       <c r="B29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
@@ -6626,7 +6630,7 @@
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1">
       <c r="B30" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C30" s="3">
         <v>0</v>
@@ -6652,7 +6656,7 @@
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1">
       <c r="B31" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C31" s="3">
         <v>0</v>
@@ -6678,7 +6682,7 @@
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1">
       <c r="B32" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C32" s="3">
         <v>0</v>
@@ -6954,7 +6958,7 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B4" t="s">
         <v>53</v>
@@ -7045,7 +7049,7 @@
   </sheetPr>
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
@@ -7081,36 +7085,36 @@
         <v>10</v>
       </c>
       <c r="H1" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>153</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -7155,7 +7159,7 @@
     <row r="3" spans="1:15">
       <c r="A3" s="11"/>
       <c r="B3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -7199,7 +7203,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="B4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -7243,7 +7247,7 @@
     </row>
     <row r="5" spans="1:15">
       <c r="B5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -7287,7 +7291,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="B6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -7331,7 +7335,7 @@
     </row>
     <row r="7" spans="1:15">
       <c r="B7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -7375,7 +7379,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="B8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -7419,7 +7423,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="B9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -7463,7 +7467,7 @@
     </row>
     <row r="10" spans="1:15">
       <c r="B10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -7507,7 +7511,7 @@
     </row>
     <row r="11" spans="1:15">
       <c r="B11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -7551,7 +7555,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="B12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -7595,7 +7599,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="B13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -7639,7 +7643,7 @@
     </row>
     <row r="14" spans="1:15">
       <c r="B14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -7683,7 +7687,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="B15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -7727,7 +7731,7 @@
     </row>
     <row r="16" spans="1:15">
       <c r="B16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -7771,7 +7775,7 @@
     </row>
     <row r="17" spans="1:15">
       <c r="B17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -7815,7 +7819,7 @@
     </row>
     <row r="18" spans="1:15">
       <c r="B18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -7903,7 +7907,7 @@
     </row>
     <row r="20" spans="1:15">
       <c r="B20" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -7947,7 +7951,7 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>90</v>
@@ -8170,7 +8174,7 @@
     </row>
     <row r="27" spans="1:15">
       <c r="B27" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -8258,7 +8262,7 @@
     </row>
     <row r="29" spans="1:15">
       <c r="B29" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -8380,7 +8384,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
@@ -8443,10 +8447,10 @@
     <row r="5" spans="1:8">
       <c r="A5" s="12"/>
       <c r="B5" s="61" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D5" s="62">
         <v>0</v>
@@ -8484,8 +8488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -8504,10 +8508,10 @@
         <v>124</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>125</v>
+        <v>180</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>126</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
@@ -8529,7 +8533,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B3" s="15">
         <v>0</v>
@@ -8580,7 +8584,7 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B6" s="15">
         <v>0</v>
@@ -8614,7 +8618,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B8" s="35">
         <v>0</v>
@@ -8648,7 +8652,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="34" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B10" s="35">
         <v>0</v>
@@ -8682,7 +8686,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B12" s="66">
         <v>0</v>
@@ -8699,7 +8703,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B13" s="15">
         <v>0</v>
@@ -8733,7 +8737,7 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B15" s="15">
         <v>0</v>
@@ -8750,7 +8754,7 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B16" s="15">
         <v>0</v>
@@ -8767,7 +8771,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B17" s="15">
         <v>0</v>
@@ -8784,7 +8788,7 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B18" s="15">
         <v>0</v>
@@ -8801,7 +8805,7 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B19" s="15">
         <v>0</v>
@@ -8818,7 +8822,7 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B20" s="15">
         <v>0</v>
@@ -8835,7 +8839,7 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B21" s="15">
         <v>0</v>
@@ -8849,7 +8853,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B22" s="15">
         <v>0</v>
@@ -8863,7 +8867,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B23" s="15">
         <v>0</v>
@@ -8877,7 +8881,7 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B24" s="15">
         <v>0</v>
@@ -8894,7 +8898,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B25" s="15">
         <v>0</v>
@@ -8911,7 +8915,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B26" s="15">
         <v>0</v>
@@ -8928,7 +8932,7 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B27" s="15">
         <v>0</v>
@@ -8945,7 +8949,7 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1">
       <c r="A28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B28" s="15">
         <v>0</v>
@@ -8959,7 +8963,7 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B29" s="15">
         <v>0</v>
@@ -8973,7 +8977,7 @@
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1">
       <c r="A30" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B30" s="15">
         <v>0</v>
@@ -9118,16 +9122,16 @@
         <v>65</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>136</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>138</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>66</v>
@@ -9142,7 +9146,7 @@
         <v>93</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1">
@@ -10446,7 +10450,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B3" s="35">
         <v>5.1999999999999998E-2</v>
@@ -10620,7 +10624,7 @@
     <row r="8" spans="1:5">
       <c r="A8" s="11"/>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C8" s="20">
         <v>0</v>
@@ -10635,7 +10639,7 @@
     <row r="9" spans="1:5">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C9" s="20">
         <v>0</v>
@@ -10650,7 +10654,7 @@
     <row r="10" spans="1:5">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C10" s="20">
         <v>0</v>
@@ -10753,7 +10757,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="B19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C19" s="20">
         <v>0</v>
@@ -10767,7 +10771,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="B20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C20" s="20">
         <v>0</v>
@@ -10781,7 +10785,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="B21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C21" s="20">
         <v>0</v>
@@ -13047,7 +13051,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B76" t="s">
         <v>98</v>
@@ -13295,10 +13299,10 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B90" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -13462,7 +13466,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="B8" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -13482,7 +13486,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="B9" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
Added incidences for both high and moderate wasting separately
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-32760" yWindow="-19860" windowWidth="27440" windowHeight="16760" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -2035,7 +2035,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="185">
   <si>
     <t>year</t>
   </si>
@@ -2584,6 +2584,12 @@
   </si>
   <si>
     <t>Zinc supplementation</t>
+  </si>
+  <si>
+    <t>Wasting (moderate)</t>
+  </si>
+  <si>
+    <t>Wasting (high)</t>
   </si>
 </sst>
 </file>
@@ -9905,10 +9911,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9995,7 +10001,7 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>183</v>
       </c>
       <c r="B5" s="61">
         <v>2.6</v>
@@ -10010,6 +10016,26 @@
         <v>2.6</v>
       </c>
       <c r="F5" s="61">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B6" s="61">
+        <v>2.6</v>
+      </c>
+      <c r="C6" s="61">
+        <v>2.6</v>
+      </c>
+      <c r="D6" s="61">
+        <v>2.6</v>
+      </c>
+      <c r="E6" s="61">
+        <v>2.6</v>
+      </c>
+      <c r="F6" s="61">
         <v>2.6</v>
       </c>
     </row>
@@ -10346,7 +10372,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10890,7 +10916,7 @@
   <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Added average duration (MAM, SAM) on treatment
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0">
+    <comment ref="B13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -110,50 +110,6 @@
           </rPr>
           <t xml:space="preserve">
 per 100,000 live births</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B12" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction of pregnancies ending in spontaneous abortion</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B13" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Number of stillbirths per 1000 TOTAL births</t>
         </r>
       </text>
     </comment>
@@ -175,7 +131,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Per 1000 live births</t>
+Fraction of pregnancies ending in spontaneous abortion</t>
         </r>
       </text>
     </comment>
@@ -197,7 +153,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Per 1000 live births</t>
+Number of stillbirths per 1000 TOTAL births</t>
         </r>
       </text>
     </comment>
@@ -223,7 +179,51 @@
         </r>
       </text>
     </comment>
-    <comment ref="C18" authorId="0">
+    <comment ref="B17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Per 1000 live births</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Per 1000 live births</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -245,7 +245,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A26" authorId="0">
+    <comment ref="A28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -267,7 +267,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A32" authorId="0">
+    <comment ref="A34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2035,7 +2035,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="187">
   <si>
     <t>year</t>
   </si>
@@ -2590,6 +2590,12 @@
   </si>
   <si>
     <t>Wasting (high)</t>
+  </si>
+  <si>
+    <t>average duration wasting (moderate) on treatment</t>
+  </si>
+  <si>
+    <t>average duration wasting (high) on treatment</t>
   </si>
 </sst>
 </file>
@@ -3312,7 +3318,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3417,6 +3423,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="541">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -5259,10 +5266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5314,7 +5321,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="19">
-        <f>(C3+C3*C13/(1000-C13))/(1-C12)</f>
+        <f>(C3+C3*C15/(1000-C15))/(1-C14)</f>
         <v>3677298.8269880489</v>
       </c>
     </row>
@@ -5342,182 +5349,201 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="68" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" s="61">
+        <v>1</v>
+      </c>
+    </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="11"/>
-      <c r="C10" s="1"/>
+      <c r="B10" s="68" t="s">
+        <v>186</v>
+      </c>
+      <c r="C10" s="61">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="11" t="s">
+      <c r="B11" s="34"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="11"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C13" s="20">
         <v>176</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" t="s">
-        <v>142</v>
-      </c>
-      <c r="C12" s="20">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" t="s">
-        <v>143</v>
-      </c>
-      <c r="C13" s="20">
-        <v>25.36</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C14" s="20">
-        <v>25.4</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C15" s="20">
-        <v>34.68</v>
+        <v>25.36</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
+        <v>144</v>
+      </c>
+      <c r="C16" s="20">
+        <v>25.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C17" s="20">
+        <v>34.68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" t="s">
         <v>146</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C18" s="20">
         <v>39.32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="11"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="11" t="s">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="11"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B21" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="45">
+      <c r="C21" s="45">
         <v>0.3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="45">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="C21" s="45">
-        <v>0.12</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C22" s="45">
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="45">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="45">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="45">
+      <c r="C25" s="45">
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="34"/>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="34"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B26" s="52" t="s">
+      <c r="B28" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="53">
+      <c r="C28" s="53">
         <v>8634000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="52" t="s">
+    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="C27" s="53">
+      <c r="C29" s="53">
         <v>13550000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="52" t="s">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="C28" s="53">
+      <c r="C30" s="53">
         <v>12394000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="52" t="s">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="52" t="s">
         <v>136</v>
       </c>
-      <c r="C29" s="53">
+      <c r="C31" s="53">
         <v>9148000</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="52"/>
-      <c r="C30" s="54"/>
-    </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="11" t="s">
+      <c r="B32" s="52"/>
+      <c r="C32" s="54"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B32" s="43" t="s">
+      <c r="B34" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="44">
+      <c r="C34" s="44">
         <v>0.29978973218277538</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="51" t="s">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="C33" s="44">
+      <c r="C35" s="44">
         <v>0.52556568434139284</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="51" t="s">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="51" t="s">
         <v>135</v>
       </c>
-      <c r="C34" s="44">
+      <c r="C36" s="44">
         <v>0.16210210664201097</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="51" t="s">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="C35" s="44">
+      <c r="C37" s="44">
         <v>1.2542476833820825E-2</v>
       </c>
     </row>
@@ -6447,23 +6473,23 @@
         <v>0</v>
       </c>
       <c r="E34" s="36">
-        <f>'Baseline year demographics'!$C$21</f>
+        <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
       <c r="F34" s="36">
-        <f>'Baseline year demographics'!$C$21</f>
+        <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
       <c r="G34" s="36">
-        <f>'Baseline year demographics'!$C$21</f>
+        <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
       <c r="H34" s="36">
-        <f>'Baseline year demographics'!$C$21</f>
+        <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
       <c r="I34" s="36">
-        <f>'Baseline year demographics'!$C$21</f>
+        <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
     </row>
@@ -6478,23 +6504,23 @@
         <v>0</v>
       </c>
       <c r="E35" s="3">
-        <f>'Baseline year demographics'!$C$22</f>
+        <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
       <c r="F35" s="3">
-        <f>'Baseline year demographics'!$C$22</f>
+        <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
       <c r="G35" s="3">
-        <f>'Baseline year demographics'!$C$22</f>
+        <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
       <c r="H35" s="3">
-        <f>'Baseline year demographics'!$C$22</f>
+        <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
       <c r="I35" s="3">
-        <f>'Baseline year demographics'!$C$22</f>
+        <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
     </row>
@@ -6509,23 +6535,23 @@
         <v>0</v>
       </c>
       <c r="E36" s="3">
-        <f>'Baseline year demographics'!$C$20</f>
+        <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
       <c r="F36" s="3">
-        <f>'Baseline year demographics'!$C$20</f>
+        <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
       <c r="G36" s="3">
-        <f>'Baseline year demographics'!$C$20</f>
+        <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
       <c r="H36" s="3">
-        <f>'Baseline year demographics'!$C$20</f>
+        <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
       <c r="I36" s="3">
-        <f>'Baseline year demographics'!$C$20</f>
+        <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
     </row>
@@ -9913,7 +9939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added placeholder PPCF effectiveness & affected fraction for wasting
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="-38040" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="3" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -2035,7 +2035,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="187">
   <si>
     <t>year</t>
   </si>
@@ -2775,7 +2775,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="541">
+  <cellStyleXfs count="543">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2787,6 +2787,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3425,7 +3427,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="541">
+  <cellStyles count="543">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3696,6 +3698,7 @@
     <cellStyle name="Followed Hyperlink" xfId="536" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="538" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="540" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="542" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3965,6 +3968,7 @@
     <cellStyle name="Hyperlink" xfId="535" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="537" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="539" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="541" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -5268,7 +5272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -7891,10 +7895,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R51" sqref="R51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8026,9 +8030,133 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="A6" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="62">
+        <v>0</v>
+      </c>
+      <c r="E6" s="62">
+        <v>0</v>
+      </c>
+      <c r="F6" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G6" s="63">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H6" s="63">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="62">
+        <v>0</v>
+      </c>
+      <c r="E7" s="62">
+        <v>0</v>
+      </c>
+      <c r="F7" s="62">
+        <v>0.3</v>
+      </c>
+      <c r="G7" s="62">
+        <v>0.3</v>
+      </c>
+      <c r="H7" s="62">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="C8" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="62">
+        <v>0</v>
+      </c>
+      <c r="E8" s="62">
+        <v>0</v>
+      </c>
+      <c r="F8" s="62">
+        <v>0.62</v>
+      </c>
+      <c r="G8" s="62">
+        <v>0.62</v>
+      </c>
+      <c r="H8" s="62">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="62">
+        <v>0</v>
+      </c>
+      <c r="E9" s="62">
+        <v>0</v>
+      </c>
+      <c r="F9" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G9" s="63">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H9" s="63">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="62">
+        <v>0</v>
+      </c>
+      <c r="E10" s="62">
+        <v>0</v>
+      </c>
+      <c r="F10" s="62">
+        <v>0.3</v>
+      </c>
+      <c r="G10" s="62">
+        <v>0.3</v>
+      </c>
+      <c r="H10" s="62">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="C11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="62">
+        <v>0</v>
+      </c>
+      <c r="E11" s="62">
+        <v>0</v>
+      </c>
+      <c r="F11" s="62">
+        <v>0.62</v>
+      </c>
+      <c r="G11" s="62">
+        <v>0.62</v>
+      </c>
+      <c r="H11" s="62">
+        <v>0.62</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8041,7 +8169,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Added OR wasting for birth outcomes
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38040" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="3" activeTab="13"/>
+    <workbookView xWindow="-38040" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -2035,7 +2035,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="189">
   <si>
     <t>year</t>
   </si>
@@ -2596,6 +2596,12 @@
   </si>
   <si>
     <t>average duration wasting (high) on treatment</t>
+  </si>
+  <si>
+    <t>OR wasting (high)</t>
+  </si>
+  <si>
+    <t>OR wasting (moderate)</t>
   </si>
 </sst>
 </file>
@@ -2775,7 +2781,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="543">
+  <cellStyleXfs count="545">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3319,8 +3325,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3426,8 +3434,11 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="543">
+  <cellStyles count="545">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3699,6 +3710,7 @@
     <cellStyle name="Followed Hyperlink" xfId="538" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="540" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="542" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="544" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3969,6 +3981,7 @@
     <cellStyle name="Hyperlink" xfId="537" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="539" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="541" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="543" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -7897,8 +7910,8 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R51" sqref="R51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10526,7 +10539,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G8" sqref="G8:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10816,10 +10829,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10900,79 +10913,79 @@
         <v>46.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="11"/>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="11"/>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" s="69">
+        <v>1</v>
+      </c>
+      <c r="D5" s="69">
+        <v>1</v>
+      </c>
+      <c r="E5" s="69">
+        <v>1</v>
+      </c>
+      <c r="F5" s="69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="69">
+        <v>1</v>
+      </c>
+      <c r="D6" s="69">
+        <v>1</v>
+      </c>
+      <c r="E6" s="69">
+        <v>1</v>
+      </c>
+      <c r="F6" s="69">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="11"/>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="11" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="5">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="E9" s="5">
-        <v>3.39</v>
-      </c>
-      <c r="F9" s="5">
-        <v>11.89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="C10" s="5">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>2.0099999999999998</v>
+        <v>1</v>
       </c>
       <c r="E10" s="5">
-        <v>3.39</v>
+        <v>1</v>
       </c>
       <c r="F10" s="5">
-        <v>11.89</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C11" s="5">
         <v>1</v>
@@ -10989,41 +11002,41 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="E12" s="5">
-        <v>999.99</v>
+        <v>3.39</v>
       </c>
       <c r="F12" s="5">
-        <v>999.99</v>
+        <v>11.89</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="E13" s="5">
-        <v>1</v>
+        <v>3.39</v>
       </c>
       <c r="F13" s="5">
-        <v>1</v>
+        <v>11.89</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="C14" s="5">
         <v>1</v>
@@ -11032,26 +11045,60 @@
         <v>1</v>
       </c>
       <c r="E14" s="5">
-        <v>1</v>
+        <v>999.99</v>
       </c>
       <c r="F14" s="5">
-        <v>1</v>
+        <v>999.99</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="5">
+        <v>1</v>
+      </c>
+      <c r="F16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="5">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="5">
-        <v>1</v>
-      </c>
-      <c r="F15" s="5">
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5">
+        <v>1</v>
+      </c>
+      <c r="F17" s="5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added PPCF to OR tab for wasting (treatment intervention) and cash transfers as prevention intervention
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="3" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -2144,7 +2144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="190">
   <si>
     <t>year</t>
   </si>
@@ -2708,6 +2708,12 @@
   </si>
   <si>
     <t>unit cost</t>
+  </si>
+  <si>
+    <t>OR wasting by intervention</t>
+  </si>
+  <si>
+    <t>Cash transfers</t>
   </si>
 </sst>
 </file>
@@ -2812,7 +2818,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2846,6 +2852,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -2887,7 +2899,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="545">
+  <cellStyleXfs count="547">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3433,8 +3445,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3543,8 +3557,12 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="545">
+  <cellStyles count="547">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3817,6 +3835,7 @@
     <cellStyle name="Followed Hyperlink" xfId="540" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="542" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="544" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="546" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4088,6 +4107,7 @@
     <cellStyle name="Hyperlink" xfId="539" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="541" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="543" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="545" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -8190,10 +8210,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8453,6 +8473,135 @@
         <v>0.62</v>
       </c>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B12" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="62">
+        <v>0</v>
+      </c>
+      <c r="E12" s="62">
+        <v>0</v>
+      </c>
+      <c r="F12" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G12" s="63">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H12" s="63">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="62">
+        <v>0</v>
+      </c>
+      <c r="E13" s="62">
+        <v>0</v>
+      </c>
+      <c r="F13" s="62">
+        <v>0.3</v>
+      </c>
+      <c r="G13" s="62">
+        <v>0.3</v>
+      </c>
+      <c r="H13" s="62">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="C14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="62">
+        <v>0</v>
+      </c>
+      <c r="E14" s="62">
+        <v>0</v>
+      </c>
+      <c r="F14" s="62">
+        <v>0.62</v>
+      </c>
+      <c r="G14" s="62">
+        <v>0.62</v>
+      </c>
+      <c r="H14" s="62">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B15" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="70">
+        <v>0</v>
+      </c>
+      <c r="E15" s="70">
+        <v>0</v>
+      </c>
+      <c r="F15" s="70">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G15" s="71">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H15" s="71">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="70">
+        <v>0</v>
+      </c>
+      <c r="E16" s="70">
+        <v>0</v>
+      </c>
+      <c r="F16" s="70">
+        <v>0.3</v>
+      </c>
+      <c r="G16" s="70">
+        <v>0.3</v>
+      </c>
+      <c r="H16" s="70">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="C17" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="70">
+        <v>0</v>
+      </c>
+      <c r="E17" s="70">
+        <v>0</v>
+      </c>
+      <c r="F17" s="70">
+        <v>0.62</v>
+      </c>
+      <c r="G17" s="70">
+        <v>0.62</v>
+      </c>
+      <c r="H17" s="70">
+        <v>0.62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -8463,8 +8612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9035,8 +9184,18 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
+      <c r="A36" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B36" s="15">
+        <v>0</v>
+      </c>
+      <c r="C36" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D36" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="4"/>
@@ -10362,7 +10521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -11398,7 +11557,7 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -13330,10 +13489,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13576,6 +13735,29 @@
         <v>1</v>
       </c>
     </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C15" s="61">
+        <v>1</v>
+      </c>
+      <c r="D15" s="61">
+        <v>1</v>
+      </c>
+      <c r="E15" s="61">
+        <v>1</v>
+      </c>
+      <c r="F15" s="61">
+        <v>1</v>
+      </c>
+      <c r="G15" s="61">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added cash transfers to target pop
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="3" activeTab="14"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -1193,7 +1193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H12" authorId="0">
+    <comment ref="H13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1212,28 +1212,6 @@
           </rPr>
           <t xml:space="preserve">
 food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B16" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
         </r>
       </text>
     </comment>
@@ -1255,11 +1233,33 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Also brestfeeding women up to 6 months?</t>
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="2">
+    <comment ref="B18" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Also brestfeeding women up to 6 months?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A20" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1281,7 +1281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I19" authorId="2">
+    <comment ref="I20" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1303,7 +1303,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I20" authorId="0">
+    <comment ref="I21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1325,7 +1325,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I26" authorId="2">
+    <comment ref="I27" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1347,7 +1347,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I27" authorId="0">
+    <comment ref="I28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1366,116 +1366,6 @@
           </rPr>
           <t xml:space="preserve">
 food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E34" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F34" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G34" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H34" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I34" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1497,7 +1387,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1519,7 +1409,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1541,7 +1431,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1563,7 +1453,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1585,7 +1475,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Fraction eating maize</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1607,7 +1497,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1629,7 +1519,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1651,7 +1541,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1673,7 +1563,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1695,11 +1585,121 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
-    <comment ref="C38" authorId="2">
+    <comment ref="E37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C39" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1721,7 +1721,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D38" authorId="2">
+    <comment ref="D39" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1743,7 +1743,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E38" authorId="2">
+    <comment ref="E39" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1765,7 +1765,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F38" authorId="2">
+    <comment ref="F39" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1787,7 +1787,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G38" authorId="2">
+    <comment ref="G39" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1809,7 +1809,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H38" authorId="2">
+    <comment ref="H39" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1831,7 +1831,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I38" authorId="2">
+    <comment ref="I39" authorId="2">
       <text>
         <r>
           <rPr>
@@ -2144,7 +2144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="190">
   <si>
     <t>year</t>
   </si>
@@ -3448,7 +3448,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3560,6 +3560,9 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="547">
@@ -5768,10 +5771,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6066,202 +6069,202 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="11" t="s">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="72">
+        <v>1</v>
+      </c>
+      <c r="E11" s="72">
+        <v>1</v>
+      </c>
+      <c r="F11" s="72">
+        <v>1</v>
+      </c>
+      <c r="G11" s="72">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0</v>
-      </c>
-      <c r="G12" s="3">
-        <v>0</v>
-      </c>
-      <c r="H12" s="31">
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="31">
         <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
-      <c r="I12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="11"/>
-      <c r="B13" t="s">
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="11"/>
+      <c r="B14" t="s">
         <v>174</v>
       </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3">
-        <v>1</v>
-      </c>
-      <c r="I13" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" t="s">
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" t="s">
         <v>177</v>
       </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3">
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
         <f>1*'Baseline year demographics'!C8</f>
         <v>0.1</v>
       </c>
-      <c r="I14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0</v>
-      </c>
-      <c r="H15" s="36">
-        <v>1</v>
-      </c>
       <c r="I15" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="36">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0</v>
-      </c>
-      <c r="H16" s="36">
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="36">
         <f>1*'Baseline year demographics'!C8</f>
         <v>0.1</v>
       </c>
-      <c r="I16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" t="s">
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" t="s">
         <v>154</v>
       </c>
-      <c r="C17" s="3">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0</v>
-      </c>
-      <c r="H17" s="36">
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="I17" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="11" t="s">
+      <c r="I18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>157</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0</v>
-      </c>
-      <c r="E19" s="3">
-        <v>0</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0</v>
-      </c>
-      <c r="H19" s="3">
-        <v>0</v>
-      </c>
-      <c r="I19" s="59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" t="s">
-        <v>158</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
@@ -6287,7 +6290,7 @@
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
@@ -6313,7 +6316,7 @@
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
@@ -6339,7 +6342,7 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
@@ -6365,7 +6368,7 @@
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
@@ -6391,60 +6394,60 @@
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
+        <v>162</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" t="s">
         <v>163</v>
       </c>
-      <c r="C25" s="3">
-        <v>0</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0</v>
-      </c>
-      <c r="E25" s="3">
-        <v>0</v>
-      </c>
-      <c r="F25" s="3">
-        <v>0</v>
-      </c>
-      <c r="G25" s="3">
-        <v>0</v>
-      </c>
-      <c r="H25" s="3">
-        <v>0</v>
-      </c>
-      <c r="I25" s="60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="11"/>
-      <c r="B26" t="s">
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
+      <c r="I26" s="60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="11"/>
+      <c r="B27" t="s">
         <v>167</v>
-      </c>
-      <c r="C26" s="3">
-        <v>0</v>
-      </c>
-      <c r="D26" s="3">
-        <v>0</v>
-      </c>
-      <c r="E26" s="3">
-        <v>0</v>
-      </c>
-      <c r="F26" s="3">
-        <v>0</v>
-      </c>
-      <c r="G26" s="3">
-        <v>0</v>
-      </c>
-      <c r="H26" s="3">
-        <v>0</v>
-      </c>
-      <c r="I26" s="59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" t="s">
-        <v>168</v>
       </c>
       <c r="C27" s="3">
         <v>0</v>
@@ -6470,7 +6473,7 @@
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C28" s="3">
         <v>0</v>
@@ -6496,7 +6499,7 @@
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
@@ -6522,7 +6525,7 @@
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C30" s="3">
         <v>0</v>
@@ -6548,7 +6551,7 @@
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C31" s="3">
         <v>0</v>
@@ -6574,192 +6577,218 @@
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
+        <v>172</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0</v>
+      </c>
+      <c r="I32" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B33" t="s">
         <v>173</v>
       </c>
-      <c r="C32" s="3">
-        <v>0</v>
-      </c>
-      <c r="D32" s="3">
-        <v>0</v>
-      </c>
-      <c r="E32" s="3">
-        <v>0</v>
-      </c>
-      <c r="F32" s="3">
-        <v>0</v>
-      </c>
-      <c r="G32" s="3">
-        <v>0</v>
-      </c>
-      <c r="H32" s="3">
-        <v>0</v>
-      </c>
-      <c r="I32" s="60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
+      <c r="I33" s="60">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="11" t="s">
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C34" s="3">
-        <v>0</v>
-      </c>
-      <c r="D34" s="3">
-        <v>0</v>
-      </c>
-      <c r="E34" s="36">
+      <c r="C35" s="3">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0</v>
+      </c>
+      <c r="E35" s="36">
         <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
-      <c r="F34" s="36">
+      <c r="F35" s="36">
         <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
-      <c r="G34" s="36">
+      <c r="G35" s="36">
         <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
-      <c r="H34" s="36">
+      <c r="H35" s="36">
         <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
-      <c r="I34" s="36">
+      <c r="I35" s="36">
         <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B35" s="4" t="s">
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B36" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="3">
-        <v>0</v>
-      </c>
-      <c r="D35" s="3">
-        <v>0</v>
-      </c>
-      <c r="E35" s="3">
+      <c r="C36" s="3">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0</v>
+      </c>
+      <c r="E36" s="3">
         <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F36" s="3">
         <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G36" s="3">
         <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
-      <c r="H35" s="3">
+      <c r="H36" s="3">
         <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I36" s="3">
         <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B36" s="4" t="s">
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="3">
-        <v>0</v>
-      </c>
-      <c r="D36" s="3">
-        <v>0</v>
-      </c>
-      <c r="E36" s="3">
+      <c r="C37" s="3">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F37" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G37" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H37" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I37" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C37" s="3">
-        <v>0</v>
-      </c>
-      <c r="D37" s="3">
-        <v>0</v>
-      </c>
-      <c r="E37" s="36">
-        <v>1</v>
-      </c>
-      <c r="F37" s="36">
-        <v>1</v>
-      </c>
-      <c r="G37" s="36">
-        <v>1</v>
-      </c>
-      <c r="H37" s="36">
-        <v>1</v>
-      </c>
-      <c r="I37" s="36">
-        <v>1</v>
-      </c>
-    </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0</v>
+      </c>
+      <c r="E38" s="36">
+        <v>1</v>
+      </c>
+      <c r="F38" s="36">
+        <v>1</v>
+      </c>
+      <c r="G38" s="36">
+        <v>1</v>
+      </c>
+      <c r="H38" s="36">
+        <v>1</v>
+      </c>
+      <c r="I38" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B39" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C38" s="36">
+      <c r="C39" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="D38" s="36">
+      <c r="D39" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="E38" s="36">
+      <c r="E39" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="F38" s="36">
+      <c r="F39" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="G38" s="36">
+      <c r="G39" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="H38" s="36">
+      <c r="H39" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="I38" s="36">
+      <c r="I39" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
+    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8612,7 +8641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added treatment of SAM and MAM to spreadsheet (placeholder OR)
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -300,6 +300,260 @@
     <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
+    <comment ref="E25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+made this number up
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+mader this number up</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+mader this number up</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+mader this number up</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E27" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+mader this number up</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F27" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+mader this number up</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G27" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+mader this number up</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B28" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B29" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B39" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Also brestfeeding women up to 6 months?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B43" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+There is no unit cost for this to impact the budget.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Ruth</author>
+    <author xml:space="preserve"> Janka Petravic</author>
+  </authors>
+  <commentList>
     <comment ref="D8" authorId="0">
       <text>
         <r>
@@ -582,336 +836,28 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author xml:space="preserve"> Janka Petravic</author>
+    <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-no data for 2 lowest age groups</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-no data for 2 lowest age groups</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-WHO database from 2001; hemoglobin &lt;110 g/L, includes mild (all-cause anemia). Consistent with Khan 2016 70.8% anemia in 6-23 months and Stevens overall ~51%</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-WHO database from 2001</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Khan 2016</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-LiST - &lt;120 g/L, includes mild</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-LiST &lt; 110 g/L, includes mild</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A13" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Default should be ~50%</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C15" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Stevens: 42% of global childhood anemia is ID</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D18" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-LiST, includes mild</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E18" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-LiST, includes mild</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C24" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Stevens</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D24" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Stevens, LiST has different values from the same source (?)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E24" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Stevens; WHO definition of &lt;70g/L, LiST is has different numbers but the same source</t>
+From Jakub's book, annual incidence of severe acute wasting is annual prevalence * 1.6  (p. 147). Assuming the same to be true for moderate wasting.</t>
         </r>
       </text>
     </comment>
@@ -922,19 +868,336 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author/>
+    <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="E16" authorId="0">
+    <comment ref="A2" authorId="0">
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Nick:
-Any breastfeeding. Other categories don't matter for this age upwards as relative risks are the same.</t>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+no data for 2 lowest age groups</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+no data for 2 lowest age groups</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+WHO database from 2001; hemoglobin &lt;110 g/L, includes mild (all-cause anemia). Consistent with Khan 2016 70.8% anemia in 6-23 months and Stevens overall ~51%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+WHO database from 2001</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Khan 2016</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+LiST - &lt;120 g/L, includes mild</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+LiST &lt; 110 g/L, includes mild</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Default should be ~50%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Stevens: 42% of global childhood anemia is ID</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+LiST, includes mild</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+LiST, includes mild</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Stevens</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Stevens, LiST has different values from the same source (?)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Stevens; WHO definition of &lt;70g/L, LiST is has different numbers but the same source</t>
         </r>
       </text>
     </comment>
@@ -945,50 +1208,19 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author xml:space="preserve"> Janka Petravic</author>
+    <author/>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="E16" authorId="0">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Term AGA should be given by a formula in the spreadsheet. The result should be greyed to indicate that it is calculated.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Kozuki 2012, for hematocrit &lt;90g/L</t>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Nick:
+Any breastfeeding. Other categories don't matter for this age upwards as relative risks are the same.</t>
         </r>
       </text>
     </comment>
@@ -999,11 +1231,10 @@
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Janka Petravic</author>
     <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="F5" authorId="0">
+    <comment ref="B2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1012,7 +1243,7 @@
             <color indexed="81"/>
             <rFont val="Arial"/>
           </rPr>
-          <t>Janka Petravic:</t>
+          <t xml:space="preserve"> Janka Petravic:</t>
         </r>
         <r>
           <rPr>
@@ -1021,11 +1252,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-LiST: 1.11</t>
+Term AGA should be given by a formula in the spreadsheet. The result should be greyed to indicate that it is calculated.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="1">
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1043,29 +1274,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-This should be changed later I guess</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B13" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-This should be changed later I guess</t>
+Kozuki 2012, for hematocrit &lt;90g/L</t>
         </r>
       </text>
     </comment>
@@ -1077,11 +1286,11 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Janka Petravic</author>
-    <author>Ruth</author>
     <author xml:space="preserve"> Janka Petravic</author>
+    <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="E6" authorId="0">
+    <comment ref="F5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1099,11 +1308,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-food insecure - default poor</t>
+LiST: 1.11</t>
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="1">
+    <comment ref="B12" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1112,7 +1321,7 @@
             <color indexed="81"/>
             <rFont val="Arial"/>
           </rPr>
-          <t>Ruth:</t>
+          <t xml:space="preserve"> Janka Petravic:</t>
         </r>
         <r>
           <rPr>
@@ -1121,12 +1330,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-poor, not in malaria area
-</t>
+This should be changed later I guess</t>
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="1">
+    <comment ref="B13" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1135,7 +1343,7 @@
             <color indexed="81"/>
             <rFont val="Arial"/>
           </rPr>
-          <t>Ruth:</t>
+          <t xml:space="preserve"> Janka Petravic:</t>
         </r>
         <r>
           <rPr>
@@ -1144,712 +1352,29 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-poor, in malaria area
-</t>
+This should be changed later I guess</t>
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="1">
+    <comment ref="B15" authorId="2">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
-poor, not in malaria area</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E10" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-poor, in malaria area</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H13" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B17" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B18" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Also brestfeeding women up to 6 months?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A20" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Coverage of these interventions is mutually exclusive</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I20" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-In baseline year, assuming only non-pregnant go to school</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I21" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I27" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-In baseline year, assuming only non-pregnant go to school</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I28" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E35" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F35" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G35" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H35" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I35" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E36" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F36" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G36" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H36" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I36" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E37" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F37" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G37" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H37" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I37" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C39" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D39" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E39" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F39" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G39" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H39" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I39" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
+Putting this here only to test out code, no idea if PPCF should be a treatment intervention for wasting</t>
         </r>
       </text>
     </comment>
@@ -1860,10 +1385,12 @@
 <file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Janka Petravic</author>
+    <author>Ruth</author>
     <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0">
+    <comment ref="E6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1872,6 +1399,140 @@
             <color indexed="81"/>
             <rFont val="Arial"/>
           </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+food insecure - default poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E7" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+poor, not in malaria area
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+poor, in malaria area
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+poor, not in malaria area</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E10" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+poor, in malaria area</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+food insecure - default poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
         <r>
@@ -1881,7 +1542,623 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Poor pregnant women - all target population</t>
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Also brestfeeding women up to 6 months?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A20" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Coverage of these interventions is mutually exclusive</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I20" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+In baseline year, assuming only non-pregnant go to school</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+food insecure - default poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I27" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+In baseline year, assuming only non-pregnant go to school</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I28" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+food insecure - default poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E35" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F35" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G35" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H35" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I35" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E36" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F36" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G36" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H36" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I36" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C39" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D39" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E39" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F39" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G39" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H39" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I39" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
         </r>
       </text>
     </comment>
@@ -1892,11 +2169,10 @@
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Ruth</author>
     <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="E25" authorId="0">
+    <comment ref="C3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1905,7 +2181,7 @@
             <color indexed="81"/>
             <rFont val="Arial"/>
           </rPr>
-          <t>Ruth:</t>
+          <t xml:space="preserve"> Janka Petravic:</t>
         </r>
         <r>
           <rPr>
@@ -1914,228 +2190,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-made this number up
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E26" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-mader this number up</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F26" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-mader this number up</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G26" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-mader this number up</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E27" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-mader this number up</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F27" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-mader this number up</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G27" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-mader this number up</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B28" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B29" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B39" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Also brestfeeding women up to 6 months?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B43" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-There is no unit cost for this to impact the budget.</t>
+Poor pregnant women - all target population</t>
         </r>
       </text>
     </comment>
@@ -2144,7 +2199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="192">
   <si>
     <t>year</t>
   </si>
@@ -2714,6 +2769,12 @@
   </si>
   <si>
     <t>Cash transfers</t>
+  </si>
+  <si>
+    <t>Treatment of wasting (moderate)</t>
+  </si>
+  <si>
+    <t>Treatment of wasting (high)</t>
   </si>
 </sst>
 </file>
@@ -2729,7 +2790,7 @@
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2816,6 +2877,17 @@
       <sz val="10"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="8">
@@ -5415,7 +5487,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5773,8 +5845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6073,8 +6145,8 @@
       <c r="B11" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C11" s="3">
-        <v>0</v>
+      <c r="C11" s="72">
+        <v>1</v>
       </c>
       <c r="D11" s="72">
         <v>1</v>
@@ -10547,11 +10619,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10641,19 +10713,24 @@
         <v>180</v>
       </c>
       <c r="B5" s="61">
-        <v>2.6</v>
+        <f>Distributions!C10/100 * 1.6</f>
+        <v>0.24</v>
       </c>
       <c r="C5" s="61">
-        <v>2.6</v>
+        <f>Distributions!D10/100 * 1.6</f>
+        <v>0.24</v>
       </c>
       <c r="D5" s="61">
-        <v>2.6</v>
+        <f>Distributions!E10/100 * 1.6</f>
+        <v>0.20640000000000003</v>
       </c>
       <c r="E5" s="61">
-        <v>2.6</v>
+        <f>Distributions!F10/100 * 1.6</f>
+        <v>0.17600000000000002</v>
       </c>
       <c r="F5" s="61">
-        <v>2.6</v>
+        <f>Distributions!G10/100 * 1.6</f>
+        <v>0.16800000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10661,24 +10738,30 @@
         <v>181</v>
       </c>
       <c r="B6" s="61">
-        <v>2.6</v>
+        <f>Distributions!C11/100 * 1.6</f>
+        <v>7.8400000000000011E-2</v>
       </c>
       <c r="C6" s="61">
-        <v>2.6</v>
+        <f>Distributions!D11/100 * 1.6</f>
+        <v>7.8400000000000011E-2</v>
       </c>
       <c r="D6" s="61">
-        <v>2.6</v>
+        <f>Distributions!E11/100 * 1.6</f>
+        <v>8.48E-2</v>
       </c>
       <c r="E6" s="61">
-        <v>2.6</v>
+        <f>Distributions!F11/100 * 1.6</f>
+        <v>6.5599999999999992E-2</v>
       </c>
       <c r="F6" s="61">
-        <v>2.6</v>
+        <f>Distributions!G11/100 * 1.6</f>
+        <v>3.3600000000000005E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11009,7 +11092,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:G11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -11586,7 +11669,7 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -13518,10 +13601,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13768,23 +13851,43 @@
       <c r="A15" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>164</v>
+      <c r="B15" s="62" t="s">
+        <v>190</v>
       </c>
       <c r="C15" s="61">
         <v>1</v>
       </c>
       <c r="D15" s="61">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="E15" s="61">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="F15" s="61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15" s="61">
-        <v>1</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B16" s="61" t="s">
+        <v>191</v>
+      </c>
+      <c r="C16" s="61">
+        <v>1</v>
+      </c>
+      <c r="D16" s="61">
+        <v>1.6</v>
+      </c>
+      <c r="E16" s="61">
+        <v>1.6</v>
+      </c>
+      <c r="F16" s="61">
+        <v>2</v>
+      </c>
+      <c r="G16" s="61">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added interventions for wasting
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,9 @@
     <sheet name="Interventions target population" sheetId="21" r:id="rId11"/>
     <sheet name="Interventions birth outcomes" sheetId="22" r:id="rId12"/>
     <sheet name="Interventions anemia" sheetId="30" r:id="rId13"/>
-    <sheet name="Interventions for children" sheetId="28" r:id="rId14"/>
-    <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId15"/>
+    <sheet name="Interventions wasting" sheetId="31" r:id="rId14"/>
+    <sheet name="Interventions for children" sheetId="28" r:id="rId15"/>
+    <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId16"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -550,6 +551,38 @@
 <file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
+    <comment ref="B4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Putting this here only to test out code, no idea if PPCF should be a treatment intervention for wasting</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
     <author>Ruth</author>
     <author xml:space="preserve"> Janka Petravic</author>
   </authors>
@@ -1287,7 +1320,6 @@
   <authors>
     <author>Janka Petravic</author>
     <author xml:space="preserve"> Janka Petravic</author>
-    <author>Sam</author>
   </authors>
   <commentList>
     <comment ref="F5" authorId="0">
@@ -1353,28 +1385,6 @@
           </rPr>
           <t xml:space="preserve">
 This should be changed later I guess</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B15" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Putting this here only to test out code, no idea if PPCF should be a treatment intervention for wasting</t>
         </r>
       </text>
     </comment>
@@ -1502,7 +1512,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H13" authorId="0">
+    <comment ref="H15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1524,7 +1534,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="2">
+    <comment ref="B19" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1546,7 +1556,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="2">
+    <comment ref="B20" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1568,7 +1578,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="2">
+    <comment ref="A22" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1590,7 +1600,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I20" authorId="2">
+    <comment ref="I22" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1612,7 +1622,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I21" authorId="0">
+    <comment ref="I23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1634,7 +1644,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I27" authorId="2">
+    <comment ref="I29" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1656,7 +1666,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I28" authorId="0">
+    <comment ref="I30" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1675,226 +1685,6 @@
           </rPr>
           <t xml:space="preserve">
 food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E35" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F35" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G35" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H35" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I35" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E36" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F36" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G36" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H36" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I36" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -1916,7 +1706,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1938,7 +1728,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1960,7 +1750,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -1982,7 +1772,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
@@ -2004,11 +1794,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-fraction eating rice</t>
+Fraction eating wheat</t>
         </r>
       </text>
     </comment>
-    <comment ref="C39" authorId="2">
+    <comment ref="E38" authorId="2">
       <text>
         <r>
           <rPr>
@@ -2026,11 +1816,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-At risk from malaria</t>
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
-    <comment ref="D39" authorId="2">
+    <comment ref="F38" authorId="2">
       <text>
         <r>
           <rPr>
@@ -2048,7 +1838,73 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-At risk from malaria</t>
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G38" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H38" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I38" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
         </r>
       </text>
     </comment>
@@ -2070,7 +1926,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-At risk from malaria</t>
+fraction eating rice</t>
         </r>
       </text>
     </comment>
@@ -2092,7 +1948,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-At risk from malaria</t>
+fraction eating rice</t>
         </r>
       </text>
     </comment>
@@ -2114,7 +1970,7 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-At risk from malaria</t>
+fraction eating rice</t>
         </r>
       </text>
     </comment>
@@ -2136,11 +1992,165 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-At risk from malaria</t>
+fraction eating rice</t>
         </r>
       </text>
     </comment>
     <comment ref="I39" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I41" authorId="2">
       <text>
         <r>
           <rPr>
@@ -2199,7 +2209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="195">
   <si>
     <t>year</t>
   </si>
@@ -2765,9 +2775,6 @@
     <t>unit cost</t>
   </si>
   <si>
-    <t>OR wasting by intervention</t>
-  </si>
-  <si>
     <t>Cash transfers</t>
   </si>
   <si>
@@ -2775,6 +2782,18 @@
   </si>
   <si>
     <t>Treatment of wasting (high)</t>
+  </si>
+  <si>
+    <t>OR severe wasting by intervention</t>
+  </si>
+  <si>
+    <t>OR moderate wasting by intervention</t>
+  </si>
+  <si>
+    <t>OR severe wasting by condition</t>
+  </si>
+  <si>
+    <t>OR moderate wasting by condition</t>
   </si>
 </sst>
 </file>
@@ -5843,10 +5862,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6143,252 +6162,252 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C11" s="72">
+        <v>1</v>
+      </c>
+      <c r="D11" s="72">
+        <v>1</v>
+      </c>
+      <c r="E11" s="72">
+        <v>1</v>
+      </c>
+      <c r="F11" s="72">
+        <v>1</v>
+      </c>
+      <c r="G11" s="72">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C11" s="72">
-        <v>1</v>
-      </c>
-      <c r="D11" s="72">
-        <v>1</v>
-      </c>
-      <c r="E11" s="72">
-        <v>1</v>
-      </c>
-      <c r="F11" s="72">
-        <v>1</v>
-      </c>
-      <c r="G11" s="72">
-        <v>1</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0</v>
-      </c>
-      <c r="I11" s="3">
+      <c r="C12" s="72">
+        <v>1</v>
+      </c>
+      <c r="D12" s="72">
+        <v>1</v>
+      </c>
+      <c r="E12" s="72">
+        <v>1</v>
+      </c>
+      <c r="F12" s="72">
+        <v>1</v>
+      </c>
+      <c r="G12" s="72">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="11" t="s">
+      <c r="B13" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" s="72">
+        <v>1</v>
+      </c>
+      <c r="D13" s="72">
+        <v>1</v>
+      </c>
+      <c r="E13" s="72">
+        <v>1</v>
+      </c>
+      <c r="F13" s="72">
+        <v>1</v>
+      </c>
+      <c r="G13" s="72">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0</v>
-      </c>
-      <c r="H13" s="31">
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="31">
         <f>'Baseline year demographics'!$C$7</f>
         <v>0.36</v>
       </c>
-      <c r="I13" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="11"/>
-      <c r="B14" t="s">
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="11"/>
+      <c r="B16" t="s">
         <v>174</v>
       </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3">
-        <v>1</v>
-      </c>
-      <c r="I14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" t="s">
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
         <v>177</v>
       </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0</v>
-      </c>
-      <c r="H15" s="3">
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
         <f>1*'Baseline year demographics'!C8</f>
         <v>0.1</v>
       </c>
-      <c r="I15" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="4" t="s">
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0</v>
-      </c>
-      <c r="H16" s="36">
-        <v>1</v>
-      </c>
-      <c r="I16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="4" t="s">
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="36">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C17" s="3">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0</v>
-      </c>
-      <c r="H17" s="36">
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="36">
         <f>1*'Baseline year demographics'!C8</f>
         <v>0.1</v>
       </c>
-      <c r="I17" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" t="s">
+      <c r="I19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" t="s">
         <v>154</v>
       </c>
-      <c r="C18" s="3">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0</v>
-      </c>
-      <c r="H18" s="36">
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+      <c r="H20" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="I18" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="11" t="s">
+      <c r="I20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>157</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0</v>
-      </c>
-      <c r="D20" s="3">
-        <v>0</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0</v>
-      </c>
-      <c r="H20" s="3">
-        <v>0</v>
-      </c>
-      <c r="I20" s="59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" t="s">
-        <v>158</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0</v>
-      </c>
-      <c r="E21" s="3">
-        <v>0</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0</v>
-      </c>
-      <c r="G21" s="3">
-        <v>0</v>
-      </c>
-      <c r="H21" s="3">
-        <v>0</v>
-      </c>
-      <c r="I21" s="59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" t="s">
-        <v>159</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
@@ -6414,7 +6433,7 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
@@ -6440,7 +6459,7 @@
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
@@ -6466,7 +6485,7 @@
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C25" s="3">
         <v>0</v>
@@ -6492,7 +6511,7 @@
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
@@ -6512,14 +6531,13 @@
       <c r="H26" s="3">
         <v>0</v>
       </c>
-      <c r="I26" s="60">
+      <c r="I26" s="59">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="11"/>
       <c r="B27" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C27" s="3">
         <v>0</v>
@@ -6545,7 +6563,7 @@
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C28" s="3">
         <v>0</v>
@@ -6565,13 +6583,14 @@
       <c r="H28" s="3">
         <v>0</v>
       </c>
-      <c r="I28" s="59">
+      <c r="I28" s="60">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="11"/>
       <c r="B29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
@@ -6597,7 +6616,7 @@
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C30" s="3">
         <v>0</v>
@@ -6623,7 +6642,7 @@
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C31" s="3">
         <v>0</v>
@@ -6649,7 +6668,7 @@
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C32" s="3">
         <v>0</v>
@@ -6675,192 +6694,254 @@
     </row>
     <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" t="s">
+        <v>171</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
+      <c r="I33" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B34" t="s">
+        <v>172</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0</v>
+      </c>
+      <c r="I34" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" t="s">
         <v>173</v>
       </c>
-      <c r="C33" s="3">
-        <v>0</v>
-      </c>
-      <c r="D33" s="3">
-        <v>0</v>
-      </c>
-      <c r="E33" s="3">
-        <v>0</v>
-      </c>
-      <c r="F33" s="3">
-        <v>0</v>
-      </c>
-      <c r="G33" s="3">
-        <v>0</v>
-      </c>
-      <c r="H33" s="3">
-        <v>0</v>
-      </c>
-      <c r="I33" s="60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="11" t="s">
+      <c r="C35" s="3">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0</v>
+      </c>
+      <c r="G35" s="3">
+        <v>0</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0</v>
+      </c>
+      <c r="I35" s="60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="3">
-        <v>0</v>
-      </c>
-      <c r="D35" s="3">
-        <v>0</v>
-      </c>
-      <c r="E35" s="36">
+      <c r="C37" s="3">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37" s="36">
         <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
-      <c r="F35" s="36">
+      <c r="F37" s="36">
         <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
-      <c r="G35" s="36">
+      <c r="G37" s="36">
         <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
-      <c r="H35" s="36">
+      <c r="H37" s="36">
         <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
-      <c r="I35" s="36">
+      <c r="I37" s="36">
         <f>'Baseline year demographics'!$C$23</f>
         <v>0.12</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B36" s="4" t="s">
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B38" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C36" s="3">
-        <v>0</v>
-      </c>
-      <c r="D36" s="3">
-        <v>0</v>
-      </c>
-      <c r="E36" s="3">
+      <c r="C38" s="3">
+        <v>0</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0</v>
+      </c>
+      <c r="E38" s="3">
         <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F38" s="3">
         <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G38" s="3">
         <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H38" s="3">
         <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I38" s="3">
         <f>'Baseline year demographics'!$C$24</f>
         <v>0.05</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="4" t="s">
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B39" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="3">
-        <v>0</v>
-      </c>
-      <c r="D37" s="3">
-        <v>0</v>
-      </c>
-      <c r="E37" s="3">
+      <c r="C39" s="3">
+        <v>0</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0</v>
+      </c>
+      <c r="E39" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F39" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G39" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H39" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I39" s="3">
         <f>'Baseline year demographics'!$C$22</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B38" s="4" t="s">
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B40" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C38" s="3">
-        <v>0</v>
-      </c>
-      <c r="D38" s="3">
-        <v>0</v>
-      </c>
-      <c r="E38" s="36">
-        <v>1</v>
-      </c>
-      <c r="F38" s="36">
-        <v>1</v>
-      </c>
-      <c r="G38" s="36">
-        <v>1</v>
-      </c>
-      <c r="H38" s="36">
-        <v>1</v>
-      </c>
-      <c r="I38" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B39" s="4" t="s">
+      <c r="C40" s="3">
+        <v>0</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0</v>
+      </c>
+      <c r="E40" s="36">
+        <v>1</v>
+      </c>
+      <c r="F40" s="36">
+        <v>1</v>
+      </c>
+      <c r="G40" s="36">
+        <v>1</v>
+      </c>
+      <c r="H40" s="36">
+        <v>1</v>
+      </c>
+      <c r="I40" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B41" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="36">
+      <c r="C41" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="D39" s="36">
+      <c r="D41" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="E39" s="36">
+      <c r="E41" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="F39" s="36">
+      <c r="F41" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="G39" s="36">
+      <c r="G41" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="H39" s="36">
+      <c r="H41" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
-      <c r="I39" s="36">
+      <c r="I41" s="36">
         <f>'Baseline year demographics'!$C$8</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
+    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B48" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B49" s="4" t="s">
+        <v>190</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8307,19 +8388,112 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P58" sqref="P58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="32.83203125" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="61" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="61">
+        <v>1</v>
+      </c>
+      <c r="D2" s="61">
+        <v>0.9</v>
+      </c>
+      <c r="E2" s="61">
+        <v>0.9</v>
+      </c>
+      <c r="F2" s="61">
+        <v>0.6</v>
+      </c>
+      <c r="G2" s="61">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" s="62" t="s">
+        <v>189</v>
+      </c>
+      <c r="C4" s="61">
+        <v>1</v>
+      </c>
+      <c r="D4" s="61">
+        <v>0.9</v>
+      </c>
+      <c r="E4" s="61">
+        <v>0.9</v>
+      </c>
+      <c r="F4" s="61">
+        <v>0.6</v>
+      </c>
+      <c r="G4" s="61">
+        <v>0.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="27.5" customWidth="1"/>
+    <col min="1" max="1" width="39.1640625" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
     <col min="3" max="3" width="38.1640625" customWidth="1"/>
     <col min="4" max="4" width="13.5" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" customWidth="1"/>
@@ -8575,10 +8749,10 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>189</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="A12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>181</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -8647,19 +8821,19 @@
       <c r="C15" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D15" s="70">
-        <v>0</v>
-      </c>
-      <c r="E15" s="70">
-        <v>0</v>
-      </c>
-      <c r="F15" s="70">
+      <c r="D15" s="62">
+        <v>0</v>
+      </c>
+      <c r="E15" s="62">
+        <v>0</v>
+      </c>
+      <c r="F15" s="62">
         <v>0.33500000000000002</v>
       </c>
-      <c r="G15" s="71">
+      <c r="G15" s="63">
         <v>0.33500000000000002</v>
       </c>
-      <c r="H15" s="71">
+      <c r="H15" s="63">
         <v>0.33500000000000002</v>
       </c>
     </row>
@@ -8667,39 +8841,168 @@
       <c r="C16" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="70">
-        <v>0</v>
-      </c>
-      <c r="E16" s="70">
-        <v>0</v>
-      </c>
-      <c r="F16" s="70">
+      <c r="D16" s="62">
+        <v>0</v>
+      </c>
+      <c r="E16" s="62">
+        <v>0</v>
+      </c>
+      <c r="F16" s="62">
         <v>0.3</v>
       </c>
-      <c r="G16" s="70">
+      <c r="G16" s="62">
         <v>0.3</v>
       </c>
-      <c r="H16" s="70">
+      <c r="H16" s="62">
         <v>0.3</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C17" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="70">
-        <v>0</v>
-      </c>
-      <c r="E17" s="70">
-        <v>0</v>
-      </c>
-      <c r="F17" s="70">
+      <c r="D17" s="62">
+        <v>0</v>
+      </c>
+      <c r="E17" s="62">
+        <v>0</v>
+      </c>
+      <c r="F17" s="62">
         <v>0.62</v>
       </c>
-      <c r="G17" s="70">
+      <c r="G17" s="62">
         <v>0.62</v>
       </c>
-      <c r="H17" s="70">
+      <c r="H17" s="62">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B18" t="s">
+        <v>181</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" s="62">
+        <v>0</v>
+      </c>
+      <c r="E18" s="62">
+        <v>0</v>
+      </c>
+      <c r="F18" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G18" s="63">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H18" s="63">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="62">
+        <v>0</v>
+      </c>
+      <c r="E19" s="62">
+        <v>0</v>
+      </c>
+      <c r="F19" s="62">
+        <v>0.3</v>
+      </c>
+      <c r="G19" s="62">
+        <v>0.3</v>
+      </c>
+      <c r="H19" s="62">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="C20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="62">
+        <v>0</v>
+      </c>
+      <c r="E20" s="62">
+        <v>0</v>
+      </c>
+      <c r="F20" s="62">
+        <v>0.62</v>
+      </c>
+      <c r="G20" s="62">
+        <v>0.62</v>
+      </c>
+      <c r="H20" s="62">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B21" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" s="70">
+        <v>0</v>
+      </c>
+      <c r="E21" s="70">
+        <v>0</v>
+      </c>
+      <c r="F21" s="70">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G21" s="71">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H21" s="71">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="70">
+        <v>0</v>
+      </c>
+      <c r="E22" s="70">
+        <v>0</v>
+      </c>
+      <c r="F22" s="70">
+        <v>0.3</v>
+      </c>
+      <c r="G22" s="70">
+        <v>0.3</v>
+      </c>
+      <c r="H22" s="70">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="C23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="70">
+        <v>0</v>
+      </c>
+      <c r="E23" s="70">
+        <v>0</v>
+      </c>
+      <c r="F23" s="70">
+        <v>0.62</v>
+      </c>
+      <c r="G23" s="70">
+        <v>0.62</v>
+      </c>
+      <c r="H23" s="70">
         <v>0.62</v>
       </c>
     </row>
@@ -8709,12 +9012,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9286,7 +9589,7 @@
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B36" s="15">
         <v>0</v>
@@ -9299,12 +9602,32 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
+      <c r="A37" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B37" s="15">
+        <v>0</v>
+      </c>
+      <c r="C37" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D37" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
+      <c r="A38" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B38" s="15">
+        <v>0</v>
+      </c>
+      <c r="C38" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="D38" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="4"/>
@@ -11385,7 +11708,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13601,10 +13924,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13847,47 +14170,51 @@
         <v>1</v>
       </c>
     </row>
+    <row r="14" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="B15" s="62" t="s">
-        <v>190</v>
+        <v>193</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C15" s="61">
-        <v>1</v>
+        <v>1.04</v>
       </c>
       <c r="D15" s="61">
-        <v>1.6</v>
+        <v>1.04</v>
       </c>
       <c r="E15" s="61">
-        <v>1.6</v>
+        <v>1.04</v>
       </c>
       <c r="F15" s="61">
-        <v>2</v>
+        <v>1.04</v>
       </c>
       <c r="G15" s="61">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B16" s="61" t="s">
-        <v>191</v>
-      </c>
-      <c r="C16" s="61">
-        <v>1</v>
-      </c>
-      <c r="D16" s="61">
-        <v>1.6</v>
-      </c>
-      <c r="E16" s="61">
-        <v>1.6</v>
-      </c>
-      <c r="F16" s="61">
-        <v>2</v>
-      </c>
-      <c r="G16" s="61">
-        <v>2</v>
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="61">
+        <v>1.04</v>
+      </c>
+      <c r="D17" s="61">
+        <v>1.04</v>
+      </c>
+      <c r="E17" s="61">
+        <v>1.04</v>
+      </c>
+      <c r="F17" s="61">
+        <v>1.04</v>
+      </c>
+      <c r="G17" s="61">
+        <v>1.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Delete some extraneous text
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Aug/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -2209,7 +2209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="195">
   <si>
     <t>year</t>
   </si>
@@ -5864,8 +5864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6934,14 +6934,10 @@
       <c r="C43" s="4"/>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B48" s="4" t="s">
-        <v>189</v>
-      </c>
+      <c r="B48" s="4"/>
     </row>
     <row r="49" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B49" s="4" t="s">
-        <v>190</v>
-      </c>
+      <c r="B49" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13926,7 +13922,7 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>

</xml_diff>